<commit_message>
Update: finished simulation results for partial and full vertical dimension reduction. Final results to be updated
</commit_message>
<xml_diff>
--- a/Sampling_Resolution_Calculator.xlsx
+++ b/Sampling_Resolution_Calculator.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nanw0\GoogleDrive\SLAC\SLAC-Diling\11. 21 Winter\DXS optics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B963B881-01B5-458B-93A3-116B589A23E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3DAFA7-FF22-45EE-B15A-24ED02D6B55D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="720" windowWidth="25485" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="150" yWindow="630" windowWidth="28500" windowHeight="14820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9481" sheetId="1" r:id="rId1"/>
-    <sheet name="9481 reduced" sheetId="2" r:id="rId2"/>
+    <sheet name="9481 2D" sheetId="3" r:id="rId2"/>
+    <sheet name="9481 reduced" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="48">
   <si>
     <t>T (fs)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -233,6 +234,10 @@
   </si>
   <si>
     <t>Ny reduced</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -285,12 +290,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -298,15 +297,21 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -591,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -617,14 +622,14 @@
       <c r="A1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="L1" s="6" t="s">
+      <c r="E1" s="10"/>
+      <c r="L1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="6"/>
+      <c r="M1" s="10"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -633,10 +638,10 @@
       <c r="B2">
         <v>9481</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="6"/>
+      <c r="E2" s="10"/>
       <c r="F2">
         <v>19.909876918386299</v>
       </c>
@@ -644,13 +649,13 @@
         <v>23</v>
       </c>
       <c r="I2" s="2">
-        <f>ROUND(F4,0)</f>
+        <f>MAX(ROUND(1/F4,0),ROUND(F4,0))</f>
         <v>12</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="6"/>
+      <c r="M2" s="10"/>
       <c r="N2">
         <v>42.926477759350803</v>
       </c>
@@ -658,7 +663,7 @@
         <v>23</v>
       </c>
       <c r="Q2" s="2">
-        <f>ROUND(1/N4,0)</f>
+        <f>MAX(ROUND(1/N4,0),ROUND(N4,0))</f>
         <v>4</v>
       </c>
     </row>
@@ -667,12 +672,12 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>800</v>
-      </c>
-      <c r="D3" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="10"/>
       <c r="F3">
         <v>17</v>
       </c>
@@ -683,10 +688,10 @@
         <f>$B4*F5/300000000*1000000000000000</f>
         <v>52300.882458116022</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="6"/>
+      <c r="M3" s="10"/>
       <c r="N3">
         <v>-29.5</v>
       </c>
@@ -705,10 +710,10 @@
       <c r="B4" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="10"/>
       <c r="F4">
         <f>SIN(RADIANS(F2+F3))/SIN(RADIANS(F2-F3))</f>
         <v>11.830135875287004</v>
@@ -718,12 +723,12 @@
       </c>
       <c r="I4" s="2">
         <f>MAX(ROUND(I3/$B7,0),1)</f>
-        <v>2</v>
-      </c>
-      <c r="L4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="6"/>
+      <c r="M4" s="10"/>
       <c r="N4">
         <f>SIN(RADIANS(N2+N3))/SIN(RADIANS(N2-N3))</f>
         <v>0.24356450463759297</v>
@@ -733,7 +738,7 @@
       </c>
       <c r="Q4" s="2">
         <f>MAX(ROUND(Q3/$B7,0),1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
@@ -743,18 +748,18 @@
       <c r="B5" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="E5" s="10"/>
       <c r="F5">
         <f>ABS((COS(RADIANS(F2-F3))-COS(RADIANS(F2+F3)))/SIN(RADIANS(F2-F3)))</f>
         <v>3.9225661843587014</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="6"/>
+      <c r="M5" s="10"/>
       <c r="N5">
         <f>ABS((COS(RADIANS(N2-N3))-COS(RADIANS(N2+N3)))/SIN(RADIANS(N2-N3)))</f>
         <v>0.70357494464450898</v>
@@ -769,7 +774,7 @@
       </c>
       <c r="B7">
         <f>B3*40</f>
-        <v>32000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
@@ -778,12 +783,12 @@
       </c>
       <c r="B8">
         <f>B3/10</f>
-        <v>80</v>
-      </c>
-      <c r="D8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="6"/>
+      <c r="E8" s="10"/>
       <c r="F8" s="1">
         <v>5.9999999999999997E-7</v>
       </c>
@@ -801,15 +806,15 @@
       </c>
       <c r="B9">
         <f>4/B8</f>
-        <v>0.05</v>
-      </c>
-      <c r="D9" s="6" t="s">
+        <v>0.4</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="11" cm="1">
+      <c r="E9" s="10"/>
+      <c r="F9" s="7" cm="1">
         <f t="array" ref="F9">IFERROR(LOOKUP(1,0/(25:25&lt;&gt;""),25:25),"")</f>
-        <v>2.9673244444444438E-2</v>
+        <v>0.14436124444444448</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
@@ -818,30 +823,30 @@
       </c>
       <c r="B10">
         <f>B9/B14</f>
-        <v>1.25E-4</v>
-      </c>
-      <c r="D10" s="6" t="s">
+        <v>1E-3</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="11">
+      <c r="E10" s="10"/>
+      <c r="F10" s="7">
         <f>X25-J25</f>
-        <v>1.2014933333333328E-2</v>
+        <v>3.0583466666666698E-2</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B12">
         <v>256</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="5"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B13">
@@ -851,11 +856,11 @@
         <v>46</v>
       </c>
       <c r="E13">
-        <v>8</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B14">
@@ -864,59 +869,59 @@
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6" t="s">
+      <c r="C16" s="10"/>
+      <c r="D16" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6" t="s">
+      <c r="E16" s="10"/>
+      <c r="F16" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6" t="s">
+      <c r="G16" s="10"/>
+      <c r="H16" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6" t="s">
+      <c r="I16" s="10"/>
+      <c r="J16" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6" t="s">
+      <c r="K16" s="10"/>
+      <c r="L16" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6" t="s">
+      <c r="M16" s="10"/>
+      <c r="N16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6" t="s">
+      <c r="O16" s="10"/>
+      <c r="P16" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6" t="s">
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6" t="s">
+      <c r="S16" s="10"/>
+      <c r="T16" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="U16" s="6"/>
-      <c r="V16" s="6" t="s">
+      <c r="U16" s="10"/>
+      <c r="V16" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="W16" s="6"/>
-      <c r="X16" s="6" t="s">
+      <c r="W16" s="10"/>
+      <c r="X16" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="Y16" s="6"/>
-      <c r="Z16" s="6"/>
-      <c r="AA16" s="6"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="10"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="2">
@@ -940,7 +945,7 @@
         <v>48000</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" ref="G17:I17" si="0">F17/F21</f>
+        <f t="shared" ref="G17:G19" si="0">F17/F21</f>
         <v>15.625</v>
       </c>
       <c r="H17" s="2">
@@ -948,7 +953,7 @@
         <v>48000</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" ref="I17" si="1">H17/H21</f>
+        <f t="shared" ref="I17:I19" si="1">H17/H21</f>
         <v>15.625</v>
       </c>
       <c r="J17" s="2">
@@ -980,7 +985,7 @@
         <v>16000</v>
       </c>
       <c r="Q17" s="2">
-        <f t="shared" ref="Q17:Y17" si="3">P17/P21</f>
+        <f t="shared" ref="Q17:Q19" si="3">P17/P21</f>
         <v>5.208333333333333</v>
       </c>
       <c r="R17" s="2">
@@ -988,7 +993,7 @@
         <v>16000</v>
       </c>
       <c r="S17" s="2">
-        <f t="shared" ref="S17:Y17" si="5">R17/R21</f>
+        <f t="shared" ref="S17:S19" si="5">R17/R21</f>
         <v>5.208333333333333</v>
       </c>
       <c r="T17" s="2">
@@ -996,7 +1001,7 @@
         <v>16000</v>
       </c>
       <c r="U17" s="2">
-        <f t="shared" ref="U17:Y17" si="7">T17/T21</f>
+        <f t="shared" ref="U17:U19" si="7">T17/T21</f>
         <v>5.208333333333333</v>
       </c>
       <c r="V17" s="2">
@@ -1004,8 +1009,8 @@
         <v>4000</v>
       </c>
       <c r="W17" s="2">
-        <f t="shared" ref="W17:Y17" si="8">V17/V21</f>
-        <v>5.208333333333333</v>
+        <f t="shared" ref="W17:W19" si="8">V17/V21</f>
+        <v>1.3020833333333333</v>
       </c>
       <c r="X17" s="2">
         <f t="shared" ref="X17:X19" si="9">V17</f>
@@ -1013,13 +1018,13 @@
       </c>
       <c r="Y17" s="2">
         <f t="shared" ref="Y17:Y19" si="10">X17/X21</f>
-        <v>5.208333333333333</v>
+        <v>1.3020833333333333</v>
       </c>
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="2">
@@ -1043,19 +1048,19 @@
         <v>4000</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" ref="G18:I18" si="12">F18/F22</f>
+        <f t="shared" si="0"/>
         <v>15.625</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" ref="H18" si="13">F18</f>
+        <f t="shared" ref="H18" si="12">F18</f>
         <v>4000</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" ref="I18" si="14">H18/H22</f>
+        <f t="shared" si="1"/>
         <v>15.625</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" ref="J18" si="15">H18</f>
+        <f t="shared" ref="J18" si="13">H18</f>
         <v>4000</v>
       </c>
       <c r="K18" s="2">
@@ -1063,7 +1068,7 @@
         <v>15.625</v>
       </c>
       <c r="L18" s="2">
-        <f t="shared" ref="L18" si="16">J18</f>
+        <f t="shared" ref="L18" si="14">J18</f>
         <v>4000</v>
       </c>
       <c r="M18" s="2">
@@ -1071,7 +1076,7 @@
         <v>15.625</v>
       </c>
       <c r="N18" s="2">
-        <f t="shared" ref="N18" si="17">L18</f>
+        <f t="shared" ref="N18" si="15">L18</f>
         <v>4000</v>
       </c>
       <c r="O18" s="2">
@@ -1083,7 +1088,7 @@
         <v>4000</v>
       </c>
       <c r="Q18" s="2">
-        <f t="shared" ref="Q18:Y18" si="18">P18/P22</f>
+        <f t="shared" si="3"/>
         <v>15.625</v>
       </c>
       <c r="R18" s="2">
@@ -1091,7 +1096,7 @@
         <v>4000</v>
       </c>
       <c r="S18" s="2">
-        <f t="shared" ref="S18:Y18" si="19">R18/R22</f>
+        <f t="shared" si="5"/>
         <v>15.625</v>
       </c>
       <c r="T18" s="2">
@@ -1099,15 +1104,15 @@
         <v>4000</v>
       </c>
       <c r="U18" s="2">
-        <f t="shared" ref="U18:Y18" si="20">T18/T22</f>
+        <f t="shared" si="7"/>
         <v>15.625</v>
       </c>
       <c r="V18" s="2">
-        <f t="shared" ref="V17:V19" si="21">T18</f>
+        <f t="shared" ref="V18:V19" si="16">T18</f>
         <v>4000</v>
       </c>
       <c r="W18" s="2">
-        <f t="shared" ref="W18:Y18" si="22">V18/V22</f>
+        <f t="shared" si="8"/>
         <v>15.625</v>
       </c>
       <c r="X18" s="2">
@@ -1122,562 +1127,619 @@
       <c r="AA18" s="2"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="2">
         <f>B7</f>
-        <v>32000</v>
+        <v>4000</v>
       </c>
       <c r="C19" s="2">
         <f>B8</f>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="D19" s="2">
         <f>B19*$I4</f>
-        <v>64000</v>
+        <v>52000</v>
       </c>
       <c r="E19" s="2">
         <f>D19/D23</f>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="F19" s="2">
         <f>D19</f>
-        <v>64000</v>
+        <v>52000</v>
       </c>
       <c r="G19" s="2">
-        <f t="shared" ref="G19:I19" si="23">F19/F23</f>
-        <v>80</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="H19" s="2">
         <f>F19</f>
-        <v>64000</v>
+        <v>52000</v>
       </c>
       <c r="I19" s="2">
-        <f t="shared" ref="I19" si="24">H19/H23</f>
-        <v>80</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="J19" s="2">
         <f>H19</f>
-        <v>64000</v>
+        <v>52000</v>
       </c>
       <c r="K19" s="2">
         <f>J19/J23</f>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="L19" s="2">
         <f>J19/I4*Q4</f>
-        <v>32000</v>
+        <v>8000</v>
       </c>
       <c r="M19" s="2">
         <f>L19/L23</f>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="N19" s="2">
         <f>L19</f>
-        <v>32000</v>
+        <v>8000</v>
       </c>
       <c r="O19" s="2">
         <f>N19/N23</f>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="P19" s="2">
         <f t="shared" si="2"/>
-        <v>32000</v>
+        <v>8000</v>
       </c>
       <c r="Q19" s="2">
-        <f t="shared" ref="Q19:Y19" si="25">P19/P23</f>
-        <v>80</v>
+        <f t="shared" si="3"/>
+        <v>10</v>
       </c>
       <c r="R19" s="2">
         <f t="shared" si="4"/>
-        <v>32000</v>
+        <v>8000</v>
       </c>
       <c r="S19" s="2">
-        <f t="shared" ref="S19:Y19" si="26">R19/R23</f>
-        <v>80</v>
+        <f t="shared" si="5"/>
+        <v>10</v>
       </c>
       <c r="T19" s="2">
         <f t="shared" si="6"/>
-        <v>32000</v>
+        <v>8000</v>
       </c>
       <c r="U19" s="2">
-        <f t="shared" ref="U19:Y19" si="27">T19/T23</f>
-        <v>80</v>
+        <f t="shared" si="7"/>
+        <v>10</v>
       </c>
       <c r="V19" s="2">
-        <f t="shared" si="21"/>
-        <v>32000</v>
+        <f t="shared" si="16"/>
+        <v>8000</v>
       </c>
       <c r="W19" s="2">
-        <f t="shared" ref="W19:Y19" si="28">V19/V23</f>
-        <v>80</v>
+        <f t="shared" si="8"/>
+        <v>10</v>
       </c>
       <c r="X19" s="2">
         <f t="shared" si="9"/>
-        <v>32000</v>
+        <v>8000</v>
       </c>
       <c r="Y19" s="2">
         <f t="shared" si="10"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="2">
         <f>B9*1000</f>
-        <v>50</v>
+        <v>400</v>
       </c>
       <c r="C20" s="2">
         <f>B10*1000</f>
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="D20" s="2">
         <f>$B20*$C19/E19</f>
-        <v>50</v>
+        <v>400</v>
       </c>
       <c r="E20" s="2">
         <f>$B19*$C20/D19</f>
-        <v>6.25E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="F20" s="2">
         <f>$B20*$C19/G19</f>
-        <v>50</v>
+        <v>400</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" ref="G20" si="29">$B19*$C20/F19</f>
-        <v>6.25E-2</v>
+        <f t="shared" ref="G20" si="17">$B19*$C20/F19</f>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="H20" s="2">
         <f>$B20*$C19/I19</f>
-        <v>50</v>
+        <v>400</v>
       </c>
       <c r="I20" s="2">
-        <f t="shared" ref="I20" si="30">$B19*$C20/H19</f>
-        <v>6.25E-2</v>
+        <f t="shared" ref="I20" si="18">$B19*$C20/H19</f>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="J20" s="2">
         <f>$B20*$C19/K19</f>
-        <v>50</v>
+        <v>400</v>
       </c>
       <c r="K20" s="2">
         <f>$B19*$C20/J19</f>
-        <v>6.25E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="L20" s="2">
         <f>$B20*$C19/M19</f>
-        <v>50</v>
+        <v>400</v>
       </c>
       <c r="M20" s="2">
         <f>$B19*$C20/L19</f>
-        <v>0.125</v>
+        <v>0.5</v>
       </c>
       <c r="N20" s="2">
         <f>$B20*$C19/O19</f>
-        <v>50</v>
+        <v>400</v>
       </c>
       <c r="O20" s="2">
         <f>$B19*$C20/N19</f>
-        <v>0.125</v>
+        <v>0.5</v>
       </c>
       <c r="P20" s="2">
-        <f t="shared" ref="P20" si="31">$B20*$C19/Q19</f>
-        <v>50</v>
+        <f t="shared" ref="P20" si="19">$B20*$C19/Q19</f>
+        <v>400</v>
       </c>
       <c r="Q20" s="2">
-        <f t="shared" ref="Q20" si="32">$B19*$C20/P19</f>
-        <v>0.125</v>
+        <f t="shared" ref="Q20" si="20">$B19*$C20/P19</f>
+        <v>0.5</v>
       </c>
       <c r="R20" s="2">
-        <f t="shared" ref="R20" si="33">$B20*$C19/S19</f>
-        <v>50</v>
+        <f t="shared" ref="R20" si="21">$B20*$C19/S19</f>
+        <v>400</v>
       </c>
       <c r="S20" s="2">
-        <f t="shared" ref="S20" si="34">$B19*$C20/R19</f>
-        <v>0.125</v>
+        <f t="shared" ref="S20" si="22">$B19*$C20/R19</f>
+        <v>0.5</v>
       </c>
       <c r="T20" s="2">
-        <f t="shared" ref="T20" si="35">$B20*$C19/U19</f>
-        <v>50</v>
+        <f t="shared" ref="T20" si="23">$B20*$C19/U19</f>
+        <v>400</v>
       </c>
       <c r="U20" s="2">
-        <f t="shared" ref="U20" si="36">$B19*$C20/T19</f>
-        <v>0.125</v>
+        <f t="shared" ref="U20" si="24">$B19*$C20/T19</f>
+        <v>0.5</v>
       </c>
       <c r="V20" s="2">
-        <f t="shared" ref="V20" si="37">$B20*$C19/W19</f>
-        <v>50</v>
+        <f t="shared" ref="V20" si="25">$B20*$C19/W19</f>
+        <v>400</v>
       </c>
       <c r="W20" s="2">
-        <f t="shared" ref="W20" si="38">$B19*$C20/V19</f>
-        <v>0.125</v>
+        <f t="shared" ref="W20" si="26">$B19*$C20/V19</f>
+        <v>0.5</v>
       </c>
       <c r="X20" s="2">
-        <f t="shared" ref="X20" si="39">$B20*$C19/Y19</f>
-        <v>50</v>
+        <f t="shared" ref="X20" si="27">$B20*$C19/Y19</f>
+        <v>400</v>
       </c>
       <c r="Y20" s="2">
-        <f t="shared" ref="Y20" si="40">$B19*$C20/X19</f>
-        <v>0.125</v>
+        <f t="shared" ref="Y20" si="28">$B19*$C20/X19</f>
+        <v>0.5</v>
       </c>
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="9">
         <f>B12</f>
         <v>256</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7">
+      <c r="C21" s="9"/>
+      <c r="D21" s="9">
         <f>B21*$I2</f>
         <v>3072</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7">
+      <c r="E21" s="9"/>
+      <c r="F21" s="9">
         <f>D21</f>
         <v>3072</v>
       </c>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7">
+      <c r="G21" s="9"/>
+      <c r="H21" s="9">
         <f>F21</f>
         <v>3072</v>
       </c>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7">
+      <c r="I21" s="9"/>
+      <c r="J21" s="9">
         <f>H21</f>
         <v>3072</v>
       </c>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7">
+      <c r="K21" s="9"/>
+      <c r="L21" s="9">
         <f>J21</f>
         <v>3072</v>
       </c>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7">
+      <c r="M21" s="9"/>
+      <c r="N21" s="9">
         <f>J21</f>
         <v>3072</v>
       </c>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7">
+      <c r="O21" s="9"/>
+      <c r="P21" s="9">
         <f>N21</f>
         <v>3072</v>
       </c>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7">
-        <f t="shared" ref="R21" si="41">P21</f>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9">
+        <f t="shared" ref="R21:R23" si="29">P21</f>
         <v>3072</v>
       </c>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7">
-        <f t="shared" ref="T21" si="42">R21</f>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9">
+        <f t="shared" ref="T21:T23" si="30">R21</f>
         <v>3072</v>
       </c>
-      <c r="U21" s="7"/>
-      <c r="V21" s="7">
-        <f>T21/Q2</f>
-        <v>768</v>
-      </c>
-      <c r="W21" s="7"/>
-      <c r="X21" s="7">
-        <f t="shared" ref="X21:X23" si="43">V21</f>
-        <v>768</v>
-      </c>
-      <c r="Y21" s="7"/>
-      <c r="Z21" s="7"/>
-      <c r="AA21" s="7"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9">
+        <f>T21</f>
+        <v>3072</v>
+      </c>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9">
+        <f t="shared" ref="X21:X23" si="31">V21</f>
+        <v>3072</v>
+      </c>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="9">
         <f>B13</f>
         <v>256</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7">
-        <f>B22</f>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9">
+        <f>E13</f>
         <v>256</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7">
-        <f t="shared" ref="F22" si="44">D22</f>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9">
+        <f t="shared" ref="F22" si="32">D22</f>
         <v>256</v>
       </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7">
-        <f t="shared" ref="H22:H23" si="45">F22</f>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9">
+        <f t="shared" ref="H22:H23" si="33">F22</f>
         <v>256</v>
       </c>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7">
+      <c r="I22" s="9"/>
+      <c r="J22" s="9">
         <f>H22</f>
         <v>256</v>
       </c>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7">
+      <c r="K22" s="9"/>
+      <c r="L22" s="9">
+        <f t="shared" ref="L22" si="34">J22</f>
+        <v>256</v>
+      </c>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9">
+        <f t="shared" ref="N22" si="35">L22</f>
+        <v>256</v>
+      </c>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9">
         <f>B13</f>
         <v>256</v>
       </c>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7">
-        <f t="shared" ref="N22" si="46">L22</f>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9">
+        <f t="shared" si="29"/>
         <v>256</v>
       </c>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7">
-        <f t="shared" ref="P22" si="47">N22</f>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9">
+        <f t="shared" si="30"/>
         <v>256</v>
       </c>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7">
-        <f t="shared" ref="R22" si="48">P22</f>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9">
+        <f>E13</f>
         <v>256</v>
       </c>
-      <c r="S22" s="7"/>
-      <c r="T22" s="7">
-        <f t="shared" ref="T22" si="49">R22</f>
+      <c r="W22" s="9"/>
+      <c r="X22" s="9">
+        <f t="shared" si="31"/>
         <v>256</v>
       </c>
-      <c r="U22" s="7"/>
-      <c r="V22" s="7">
-        <f t="shared" ref="V22" si="50">T22</f>
-        <v>256</v>
-      </c>
-      <c r="W22" s="7"/>
-      <c r="X22" s="7">
-        <f t="shared" si="43"/>
-        <v>256</v>
-      </c>
-      <c r="Y22" s="7"/>
-      <c r="Z22" s="7"/>
-      <c r="AA22" s="7"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+      <c r="AA22" s="9"/>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="9">
         <f>B14</f>
         <v>400</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7">
+      <c r="C23" s="9"/>
+      <c r="D23" s="9">
         <f>B23*$I4</f>
+        <v>5200</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9">
+        <f>D23</f>
+        <v>5200</v>
+      </c>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9">
+        <f t="shared" si="33"/>
+        <v>5200</v>
+      </c>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9">
+        <f t="shared" ref="J23" si="36">H23</f>
+        <v>5200</v>
+      </c>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9">
+        <f>J23/I4*Q4</f>
         <v>800</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7">
-        <f>D23</f>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9">
+        <f>L23</f>
         <v>800</v>
       </c>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7">
-        <f t="shared" si="45"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9">
+        <f t="shared" ref="P23" si="37">N23</f>
         <v>800</v>
       </c>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7">
-        <f t="shared" ref="J22:J23" si="51">H23</f>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9">
+        <f t="shared" si="29"/>
         <v>800</v>
       </c>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7">
-        <f>J23/I4*Q4</f>
-        <v>400</v>
-      </c>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7">
-        <f>L23</f>
-        <v>400</v>
-      </c>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7">
-        <f t="shared" ref="P22:P23" si="52">N23</f>
-        <v>400</v>
-      </c>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7">
-        <f t="shared" ref="R22:R23" si="53">P23</f>
-        <v>400</v>
-      </c>
-      <c r="S23" s="7"/>
-      <c r="T23" s="7">
-        <f t="shared" ref="T23" si="54">R23</f>
-        <v>400</v>
-      </c>
-      <c r="U23" s="7"/>
-      <c r="V23" s="7">
-        <f t="shared" ref="V22:V23" si="55">T23</f>
-        <v>400</v>
-      </c>
-      <c r="W23" s="7"/>
-      <c r="X23" s="7">
-        <f t="shared" si="43"/>
-        <v>400</v>
-      </c>
-      <c r="Y23" s="7"/>
-      <c r="Z23" s="7"/>
-      <c r="AA23" s="7"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9">
+        <f t="shared" si="30"/>
+        <v>800</v>
+      </c>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9">
+        <f t="shared" ref="V23" si="38">T23</f>
+        <v>800</v>
+      </c>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9">
+        <f t="shared" si="31"/>
+        <v>800</v>
+      </c>
+      <c r="Y23" s="9"/>
+      <c r="Z23" s="9"/>
+      <c r="AA23" s="9"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="12">
         <f>B21*B22*B23</f>
         <v>26214400</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8">
-        <f t="shared" ref="D24" si="56">D21*D22*D23</f>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12">
+        <f t="shared" ref="D24" si="39">D21*D22*D23</f>
+        <v>4089446400</v>
+      </c>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12">
+        <f t="shared" ref="F24" si="40">F21*F22*F23</f>
+        <v>4089446400</v>
+      </c>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12">
+        <f t="shared" ref="H24" si="41">H21*H22*H23</f>
+        <v>4089446400</v>
+      </c>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12">
+        <f t="shared" ref="J24" si="42">J21*J22*J23</f>
+        <v>4089446400</v>
+      </c>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12">
+        <f t="shared" ref="L24" si="43">L21*L22*L23</f>
         <v>629145600</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8">
-        <f t="shared" ref="F24" si="57">F21*F22*F23</f>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12">
+        <f t="shared" ref="N24" si="44">N21*N22*N23</f>
         <v>629145600</v>
       </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8">
-        <f t="shared" ref="H24" si="58">H21*H22*H23</f>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12">
+        <f t="shared" ref="P24" si="45">P21*P22*P23</f>
         <v>629145600</v>
       </c>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8">
-        <f t="shared" ref="J24" si="59">J21*J22*J23</f>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12">
+        <f t="shared" ref="R24" si="46">R21*R22*R23</f>
         <v>629145600</v>
       </c>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8">
-        <f t="shared" ref="L24" si="60">L21*L22*L23</f>
-        <v>314572800</v>
-      </c>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8">
-        <f t="shared" ref="N24" si="61">N21*N22*N23</f>
-        <v>314572800</v>
-      </c>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8">
-        <f t="shared" ref="P24" si="62">P21*P22*P23</f>
-        <v>314572800</v>
-      </c>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8">
-        <f t="shared" ref="R24" si="63">R21*R22*R23</f>
-        <v>314572800</v>
-      </c>
-      <c r="S24" s="8"/>
-      <c r="T24" s="8">
-        <f t="shared" ref="T24" si="64">T21*T22*T23</f>
-        <v>314572800</v>
-      </c>
-      <c r="U24" s="8"/>
-      <c r="V24" s="8">
-        <f t="shared" ref="V24" si="65">V21*V22*V23</f>
-        <v>78643200</v>
-      </c>
-      <c r="W24" s="8"/>
-      <c r="X24" s="8">
-        <f t="shared" ref="X24" si="66">X21*X22*X23</f>
-        <v>78643200</v>
-      </c>
-      <c r="Y24" s="8"/>
-      <c r="Z24" s="4"/>
-      <c r="AA24" s="4"/>
+      <c r="S24" s="12"/>
+      <c r="T24" s="12">
+        <f t="shared" ref="T24" si="47">T21*T22*T23</f>
+        <v>629145600</v>
+      </c>
+      <c r="U24" s="12"/>
+      <c r="V24" s="12">
+        <f t="shared" ref="V24" si="48">V21*V22*V23</f>
+        <v>629145600</v>
+      </c>
+      <c r="W24" s="12"/>
+      <c r="X24" s="12">
+        <f t="shared" ref="X24" si="49">X21*X22*X23</f>
+        <v>629145600</v>
+      </c>
+      <c r="Y24" s="12"/>
+      <c r="Z24" s="5"/>
+      <c r="AA24" s="5"/>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25" s="11">
         <f>B24*$F8/86400</f>
         <v>1.8204444444444443E-4</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12">
+      <c r="C25" s="11"/>
+      <c r="D25" s="11">
         <f>D24*$F8/86400+B25</f>
-        <v>4.5511111111111099E-3</v>
-      </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12">
-        <f t="shared" ref="F25" si="67">F24*$F8/86400+D25</f>
-        <v>8.9201777777777758E-3</v>
-      </c>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12">
-        <f t="shared" ref="H25" si="68">H24*$F8/86400+F25</f>
-        <v>1.3289244444444442E-2</v>
-      </c>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12">
-        <f t="shared" ref="J25" si="69">J24*$F8/86400+H25</f>
-        <v>1.7658311111111109E-2</v>
-      </c>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12">
-        <f t="shared" ref="L25" si="70">L24*$F8/86400+J25</f>
-        <v>1.9842844444444441E-2</v>
-      </c>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12">
-        <f t="shared" ref="N25" si="71">N24*$F8/86400+L25</f>
-        <v>2.2027377777777774E-2</v>
-      </c>
-      <c r="O25" s="12"/>
-      <c r="P25" s="12">
-        <f t="shared" ref="P25" si="72">P24*$F8/86400+N25</f>
-        <v>2.4211911111111106E-2</v>
-      </c>
-      <c r="Q25" s="12"/>
-      <c r="R25" s="12">
-        <f t="shared" ref="R25" si="73">R24*$F8/86400+P25</f>
-        <v>2.6396444444444438E-2</v>
-      </c>
-      <c r="S25" s="12"/>
-      <c r="T25" s="12">
-        <f t="shared" ref="T25" si="74">T24*$F8/86400+R25</f>
-        <v>2.858097777777777E-2</v>
-      </c>
-      <c r="U25" s="12"/>
-      <c r="V25" s="12">
-        <f t="shared" ref="V25" si="75">V24*$F8/86400+T25</f>
-        <v>2.9127111111111104E-2</v>
-      </c>
-      <c r="W25" s="12"/>
-      <c r="X25" s="12">
-        <f t="shared" ref="X25" si="76">X24*$F8/86400+V25</f>
-        <v>2.9673244444444438E-2</v>
-      </c>
-      <c r="Y25" s="12"/>
-      <c r="Z25" s="9"/>
-      <c r="AA25" s="9"/>
+        <v>2.858097777777778E-2</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11">
+        <f t="shared" ref="F25" si="50">F24*$F8/86400+D25</f>
+        <v>5.6979911111111115E-2</v>
+      </c>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11">
+        <f t="shared" ref="H25" si="51">H24*$F8/86400+F25</f>
+        <v>8.5378844444444449E-2</v>
+      </c>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11">
+        <f t="shared" ref="J25" si="52">J24*$F8/86400+H25</f>
+        <v>0.11377777777777778</v>
+      </c>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11">
+        <f t="shared" ref="L25" si="53">L24*$F8/86400+J25</f>
+        <v>0.11814684444444445</v>
+      </c>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11">
+        <f t="shared" ref="N25" si="54">N24*$F8/86400+L25</f>
+        <v>0.12251591111111113</v>
+      </c>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11">
+        <f t="shared" ref="P25" si="55">P24*$F8/86400+N25</f>
+        <v>0.1268849777777778</v>
+      </c>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11">
+        <f t="shared" ref="R25" si="56">R24*$F8/86400+P25</f>
+        <v>0.13125404444444447</v>
+      </c>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11">
+        <f t="shared" ref="T25" si="57">T24*$F8/86400+R25</f>
+        <v>0.13562311111111114</v>
+      </c>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11">
+        <f t="shared" ref="V25" si="58">V24*$F8/86400+T25</f>
+        <v>0.13999217777777781</v>
+      </c>
+      <c r="W25" s="11"/>
+      <c r="X25" s="11">
+        <f t="shared" ref="X25" si="59">X24*$F8/86400+V25</f>
+        <v>0.14436124444444448</v>
+      </c>
+      <c r="Y25" s="11"/>
+      <c r="Z25" s="8"/>
+      <c r="AA25" s="8"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="E31" s="10"/>
+      <c r="E31" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="90">
-    <mergeCell ref="Z25:AA25"/>
-    <mergeCell ref="Z22:AA22"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="Z23:AA23"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="T21:U21"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="X21:Y21"/>
-    <mergeCell ref="Z21:AA21"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="R23:S23"/>
     <mergeCell ref="P25:Q25"/>
     <mergeCell ref="R25:S25"/>
     <mergeCell ref="T16:U16"/>
@@ -1694,85 +1756,30 @@
     <mergeCell ref="T24:U24"/>
     <mergeCell ref="V24:W24"/>
     <mergeCell ref="X24:Y24"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="T21:U21"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="X21:Y21"/>
+    <mergeCell ref="Z21:AA21"/>
+    <mergeCell ref="Z25:AA25"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="Z23:AA23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="E20" formula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B7FF28-7221-43C9-AFD5-E9B2F94032D2}">
-  <dimension ref="A1:Y25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6D17F22-0533-4A13-BFFA-7902E7E4E321}">
+  <dimension ref="A1:AA31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1793,30 +1800,30 @@
     <col min="16" max="16" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="L1" s="6" t="s">
+      <c r="E1" s="10"/>
+      <c r="L1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="6"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="M1" s="10"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>9481</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="6"/>
+      <c r="E2" s="10"/>
       <c r="F2">
         <v>19.909876918386299</v>
       </c>
@@ -1824,13 +1831,13 @@
         <v>23</v>
       </c>
       <c r="I2" s="2">
-        <f>ROUND(F4,0)</f>
+        <f>MAX(ROUND(1/F4,0),ROUND(F4,0))</f>
         <v>12</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="6"/>
+      <c r="M2" s="10"/>
       <c r="N2">
         <v>42.926477759350803</v>
       </c>
@@ -1838,21 +1845,21 @@
         <v>23</v>
       </c>
       <c r="Q2" s="2">
-        <f>ROUND(1/N4,0)</f>
+        <f>MAX(ROUND(1/N4,0),ROUND(N4,0))</f>
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3">
-        <v>20</v>
-      </c>
-      <c r="D3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="10"/>
       <c r="F3">
         <v>17</v>
       </c>
@@ -1863,10 +1870,10 @@
         <f>$B4*F5/300000000*1000000000000000</f>
         <v>52300.882458116022</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="6"/>
+      <c r="M3" s="10"/>
       <c r="N3">
         <v>-29.5</v>
       </c>
@@ -1878,17 +1885,17 @@
         <v>9380.9992619267869</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="10"/>
       <c r="F4">
         <f>SIN(RADIANS(F2+F3))/SIN(RADIANS(F2-F3))</f>
         <v>11.830135875287004</v>
@@ -1898,12 +1905,12 @@
       </c>
       <c r="I4" s="2">
         <f>MAX(ROUND(I3/$B7,0),1)</f>
-        <v>65</v>
-      </c>
-      <c r="L4" s="6" t="s">
+        <v>1308</v>
+      </c>
+      <c r="L4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="6"/>
+      <c r="M4" s="10"/>
       <c r="N4">
         <f>SIN(RADIANS(N2+N3))/SIN(RADIANS(N2-N3))</f>
         <v>0.24356450463759297</v>
@@ -1913,57 +1920,57 @@
       </c>
       <c r="Q4" s="2">
         <f>MAX(ROUND(Q3/$B7,0),1)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="E5" s="10"/>
       <c r="F5">
         <f>ABS((COS(RADIANS(F2-F3))-COS(RADIANS(F2+F3)))/SIN(RADIANS(F2-F3)))</f>
         <v>3.9225661843587014</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="6"/>
+      <c r="M5" s="10"/>
       <c r="N5">
         <f>ABS((COS(RADIANS(N2-N3))-COS(RADIANS(N2+N3)))/SIN(RADIANS(N2-N3)))</f>
         <v>0.70357494464450898</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="B7">
         <f>B3*40</f>
-        <v>800</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
       <c r="B8">
         <f>B3/10</f>
-        <v>2</v>
-      </c>
-      <c r="D8" s="6" t="s">
+        <v>0.1</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="6"/>
+      <c r="E8" s="10"/>
       <c r="F8" s="1">
         <v>5.9999999999999997E-7</v>
       </c>
@@ -1975,57 +1982,57 @@
         <v>2048000000</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9">
         <f>4/B8</f>
-        <v>2</v>
-      </c>
-      <c r="D9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="11" cm="1">
+      <c r="E9" s="10"/>
+      <c r="F9" s="7" cm="1">
         <f t="array" ref="F9">IFERROR(LOOKUP(1,0/(25:25&lt;&gt;""),25:25),"")</f>
-        <v>9.8622577777777776E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+        <v>0.98222648888888864</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10">
         <f>B9/B14</f>
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D10" s="6" t="s">
+        <v>0.1</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="11">
+      <c r="E10" s="10"/>
+      <c r="F10" s="7">
         <f>X25-J25</f>
-        <v>8.0691199999999991E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+        <v>0.62504959999999976</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B12">
         <v>256</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B13">
-        <v>256</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
         <v>46</v>
@@ -2034,8 +2041,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B14">
@@ -2043,58 +2050,60 @@
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B16" s="6" t="s">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B16" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6" t="s">
+      <c r="C16" s="10"/>
+      <c r="D16" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6" t="s">
+      <c r="E16" s="10"/>
+      <c r="F16" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6" t="s">
+      <c r="G16" s="10"/>
+      <c r="H16" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6" t="s">
+      <c r="I16" s="10"/>
+      <c r="J16" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6" t="s">
+      <c r="K16" s="10"/>
+      <c r="L16" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6" t="s">
+      <c r="M16" s="10"/>
+      <c r="N16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6" t="s">
+      <c r="O16" s="10"/>
+      <c r="P16" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6" t="s">
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6" t="s">
+      <c r="S16" s="10"/>
+      <c r="T16" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="U16" s="6"/>
-      <c r="V16" s="6" t="s">
+      <c r="U16" s="10"/>
+      <c r="V16" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="W16" s="6"/>
-      <c r="X16" s="6" t="s">
+      <c r="W16" s="10"/>
+      <c r="X16" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="Y16" s="6"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="10"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="2">
@@ -2118,7 +2127,7 @@
         <v>48000</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" ref="G17:I19" si="0">F17/F21</f>
+        <f t="shared" ref="G17:G19" si="0">F17/F21</f>
         <v>15.625</v>
       </c>
       <c r="H17" s="2">
@@ -2158,7 +2167,7 @@
         <v>16000</v>
       </c>
       <c r="Q17" s="2">
-        <f t="shared" ref="Q17:Y19" si="3">P17/P21</f>
+        <f t="shared" ref="Q17:Q19" si="3">P17/P21</f>
         <v>5.208333333333333</v>
       </c>
       <c r="R17" s="2">
@@ -2166,7 +2175,7 @@
         <v>16000</v>
       </c>
       <c r="S17" s="2">
-        <f t="shared" ref="S17:Y19" si="5">R17/R21</f>
+        <f t="shared" ref="S17:S19" si="5">R17/R21</f>
         <v>5.208333333333333</v>
       </c>
       <c r="T17" s="2">
@@ -2174,7 +2183,7 @@
         <v>16000</v>
       </c>
       <c r="U17" s="2">
-        <f t="shared" ref="U17:Y19" si="7">T17/T21</f>
+        <f t="shared" ref="U17:U19" si="7">T17/T21</f>
         <v>5.208333333333333</v>
       </c>
       <c r="V17" s="2">
@@ -2182,8 +2191,8 @@
         <v>4000</v>
       </c>
       <c r="W17" s="2">
-        <f t="shared" ref="W17:Y19" si="8">V17/V21</f>
-        <v>5.208333333333333</v>
+        <f t="shared" ref="W17:W19" si="8">V17/V21</f>
+        <v>1.3020833333333333</v>
       </c>
       <c r="X17" s="2">
         <f t="shared" ref="X17:X19" si="9">V17</f>
@@ -2191,11 +2200,13 @@
       </c>
       <c r="Y17" s="2">
         <f t="shared" ref="Y17:Y19" si="10">X17/X21</f>
-        <v>5.208333333333333</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+        <v>1.3020833333333333</v>
+      </c>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="2">
@@ -2204,7 +2215,7 @@
       </c>
       <c r="C18" s="2">
         <f>B18/B22</f>
-        <v>15.625</v>
+        <v>500</v>
       </c>
       <c r="D18" s="2">
         <f>B18</f>
@@ -2260,7 +2271,7 @@
       </c>
       <c r="Q18" s="2">
         <f t="shared" si="3"/>
-        <v>15.625</v>
+        <v>500</v>
       </c>
       <c r="R18" s="2">
         <f t="shared" si="4"/>
@@ -2268,7 +2279,7 @@
       </c>
       <c r="S18" s="2">
         <f t="shared" si="5"/>
-        <v>15.625</v>
+        <v>500</v>
       </c>
       <c r="T18" s="2">
         <f t="shared" si="6"/>
@@ -2276,10 +2287,10 @@
       </c>
       <c r="U18" s="2">
         <f t="shared" si="7"/>
-        <v>15.625</v>
+        <v>500</v>
       </c>
       <c r="V18" s="2">
-        <f t="shared" ref="V18:V20" si="16">T18</f>
+        <f t="shared" ref="V18:V19" si="16">T18</f>
         <v>4000</v>
       </c>
       <c r="W18" s="2">
@@ -2294,551 +2305,1801 @@
         <f t="shared" si="10"/>
         <v>500</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="2">
         <f>B7</f>
-        <v>800</v>
+        <v>40</v>
       </c>
       <c r="C19" s="2">
         <f>B8</f>
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="D19" s="2">
         <f>B19*$I4</f>
-        <v>52000</v>
+        <v>52320</v>
       </c>
       <c r="E19" s="2">
         <f>D19/D23</f>
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="F19" s="2">
         <f>D19</f>
-        <v>52000</v>
+        <v>52320</v>
       </c>
       <c r="G19" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="H19" s="2">
         <f>F19</f>
-        <v>52000</v>
+        <v>52320</v>
       </c>
       <c r="I19" s="2">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="J19" s="2">
         <f>H19</f>
-        <v>52000</v>
+        <v>52320</v>
       </c>
       <c r="K19" s="2">
         <f>J19/J23</f>
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="L19" s="2">
         <f>J19/I4*Q4</f>
-        <v>9600</v>
+        <v>9400</v>
       </c>
       <c r="M19" s="2">
         <f>L19/L23</f>
-        <v>2</v>
+        <v>1.7966360856269112E-2</v>
       </c>
       <c r="N19" s="2">
         <f>L19</f>
-        <v>9600</v>
+        <v>9400</v>
       </c>
       <c r="O19" s="2">
         <f>N19/N23</f>
-        <v>2</v>
+        <v>1.7966360856269112E-2</v>
       </c>
       <c r="P19" s="2">
         <f t="shared" si="2"/>
-        <v>9600</v>
+        <v>9400</v>
       </c>
       <c r="Q19" s="2">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.7966360856269112E-2</v>
       </c>
       <c r="R19" s="2">
         <f t="shared" si="4"/>
-        <v>9600</v>
+        <v>9400</v>
       </c>
       <c r="S19" s="2">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1.7966360856269112E-2</v>
       </c>
       <c r="T19" s="2">
         <f t="shared" si="6"/>
-        <v>9600</v>
+        <v>9400</v>
       </c>
       <c r="U19" s="2">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1.7966360856269112E-2</v>
       </c>
       <c r="V19" s="2">
         <f t="shared" si="16"/>
-        <v>9600</v>
+        <v>9400</v>
       </c>
       <c r="W19" s="2">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1.7966360856269112E-2</v>
       </c>
       <c r="X19" s="2">
         <f t="shared" si="9"/>
-        <v>9600</v>
+        <v>9400</v>
       </c>
       <c r="Y19" s="2">
         <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+        <v>1.7966360856269112E-2</v>
+      </c>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="2">
         <f>B9*1000</f>
-        <v>2000</v>
+        <v>40000</v>
       </c>
       <c r="C20" s="2">
         <f>B10*1000</f>
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D20" s="2">
         <f>$B20*$C19/E19</f>
-        <v>2000</v>
+        <v>40000</v>
       </c>
       <c r="E20" s="2">
         <f>$B19*$C20/D19</f>
-        <v>7.6923076923076927E-2</v>
+        <v>7.64525993883792E-2</v>
       </c>
       <c r="F20" s="2">
         <f>$B20*$C19/G19</f>
-        <v>2000</v>
+        <v>40000</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" ref="G20" si="17">$B19*$C20/F19</f>
-        <v>7.6923076923076927E-2</v>
+        <v>7.64525993883792E-2</v>
       </c>
       <c r="H20" s="2">
         <f>$B20*$C19/I19</f>
-        <v>2000</v>
+        <v>40000</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" ref="I20" si="18">$B19*$C20/H19</f>
-        <v>7.6923076923076927E-2</v>
+        <v>7.64525993883792E-2</v>
       </c>
       <c r="J20" s="2">
         <f>$B20*$C19/K19</f>
-        <v>2000</v>
+        <v>40000</v>
       </c>
       <c r="K20" s="2">
         <f>$B19*$C20/J19</f>
-        <v>7.6923076923076927E-2</v>
+        <v>7.64525993883792E-2</v>
       </c>
       <c r="L20" s="2">
         <f>$B20*$C19/M19</f>
-        <v>2000</v>
+        <v>222638.29787234045</v>
       </c>
       <c r="M20" s="2">
         <f>$B19*$C20/L19</f>
-        <v>0.41666666666666669</v>
+        <v>0.42553191489361702</v>
       </c>
       <c r="N20" s="2">
         <f>$B20*$C19/O19</f>
-        <v>2000</v>
+        <v>222638.29787234045</v>
       </c>
       <c r="O20" s="2">
         <f>$B19*$C20/N19</f>
-        <v>0.41666666666666669</v>
+        <v>0.42553191489361702</v>
       </c>
       <c r="P20" s="2">
         <f t="shared" ref="P20" si="19">$B20*$C19/Q19</f>
-        <v>2000</v>
+        <v>222638.29787234045</v>
       </c>
       <c r="Q20" s="2">
         <f t="shared" ref="Q20" si="20">$B19*$C20/P19</f>
-        <v>0.41666666666666669</v>
+        <v>0.42553191489361702</v>
       </c>
       <c r="R20" s="2">
         <f t="shared" ref="R20" si="21">$B20*$C19/S19</f>
-        <v>2000</v>
+        <v>222638.29787234045</v>
       </c>
       <c r="S20" s="2">
         <f t="shared" ref="S20" si="22">$B19*$C20/R19</f>
-        <v>0.41666666666666669</v>
+        <v>0.42553191489361702</v>
       </c>
       <c r="T20" s="2">
         <f t="shared" ref="T20" si="23">$B20*$C19/U19</f>
-        <v>2000</v>
+        <v>222638.29787234045</v>
       </c>
       <c r="U20" s="2">
         <f t="shared" ref="U20" si="24">$B19*$C20/T19</f>
-        <v>0.41666666666666669</v>
+        <v>0.42553191489361702</v>
       </c>
       <c r="V20" s="2">
         <f t="shared" ref="V20" si="25">$B20*$C19/W19</f>
-        <v>2000</v>
+        <v>222638.29787234045</v>
       </c>
       <c r="W20" s="2">
         <f t="shared" ref="W20" si="26">$B19*$C20/V19</f>
-        <v>0.41666666666666669</v>
+        <v>0.42553191489361702</v>
       </c>
       <c r="X20" s="2">
         <f t="shared" ref="X20" si="27">$B20*$C19/Y19</f>
-        <v>2000</v>
+        <v>222638.29787234045</v>
       </c>
       <c r="Y20" s="2">
         <f t="shared" ref="Y20" si="28">$B19*$C20/X19</f>
-        <v>0.41666666666666669</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+        <v>0.42553191489361702</v>
+      </c>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="9">
         <f>B12</f>
         <v>256</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7">
+      <c r="C21" s="9"/>
+      <c r="D21" s="9">
         <f>B21*$I2</f>
         <v>3072</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7">
+      <c r="E21" s="9"/>
+      <c r="F21" s="9">
         <f>D21</f>
         <v>3072</v>
       </c>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7">
+      <c r="G21" s="9"/>
+      <c r="H21" s="9">
         <f>F21</f>
         <v>3072</v>
       </c>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7">
+      <c r="I21" s="9"/>
+      <c r="J21" s="9">
         <f>H21</f>
         <v>3072</v>
       </c>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7">
+      <c r="K21" s="9"/>
+      <c r="L21" s="9">
         <f>J21</f>
         <v>3072</v>
       </c>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7">
+      <c r="M21" s="9"/>
+      <c r="N21" s="9">
         <f>J21</f>
         <v>3072</v>
       </c>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7">
+      <c r="O21" s="9"/>
+      <c r="P21" s="9">
         <f>N21</f>
         <v>3072</v>
       </c>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7">
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9">
         <f t="shared" ref="R21:R23" si="29">P21</f>
         <v>3072</v>
       </c>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7">
+      <c r="S21" s="9"/>
+      <c r="T21" s="9">
         <f t="shared" ref="T21:T23" si="30">R21</f>
         <v>3072</v>
       </c>
-      <c r="U21" s="7"/>
-      <c r="V21" s="7">
-        <f>T21/Q2</f>
-        <v>768</v>
-      </c>
-      <c r="W21" s="7"/>
-      <c r="X21" s="7">
+      <c r="U21" s="9"/>
+      <c r="V21" s="9">
+        <f>T21</f>
+        <v>3072</v>
+      </c>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9">
         <f t="shared" ref="X21:X23" si="31">V21</f>
-        <v>768</v>
-      </c>
-      <c r="Y21" s="7"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+        <v>3072</v>
+      </c>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="9">
         <f>B13</f>
-        <v>256</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7">
+        <v>8</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9">
         <f>E13</f>
         <v>8</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7">
+      <c r="E22" s="9"/>
+      <c r="F22" s="9">
         <f t="shared" ref="F22" si="32">D22</f>
         <v>8</v>
       </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7">
+      <c r="G22" s="9"/>
+      <c r="H22" s="9">
         <f t="shared" ref="H22:H23" si="33">F22</f>
         <v>8</v>
       </c>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7">
+      <c r="I22" s="9"/>
+      <c r="J22" s="9">
         <f>H22</f>
         <v>8</v>
       </c>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7">
-        <f>J22</f>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9">
+        <f t="shared" ref="L22" si="34">J22</f>
         <v>8</v>
       </c>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7">
-        <f t="shared" ref="N22" si="34">L22</f>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9">
+        <f t="shared" ref="N22" si="35">L22</f>
         <v>8</v>
       </c>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7">
+      <c r="O22" s="9"/>
+      <c r="P22" s="9">
         <f>B13</f>
-        <v>256</v>
-      </c>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7">
-        <f>P22</f>
-        <v>256</v>
-      </c>
-      <c r="S22" s="7"/>
-      <c r="T22" s="7">
+        <v>8</v>
+      </c>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9">
+        <f t="shared" si="29"/>
+        <v>8</v>
+      </c>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9">
         <f t="shared" si="30"/>
-        <v>256</v>
-      </c>
-      <c r="U22" s="7"/>
-      <c r="V22" s="7">
+        <v>8</v>
+      </c>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9">
         <f>E13</f>
         <v>8</v>
       </c>
-      <c r="W22" s="7"/>
-      <c r="X22" s="7">
+      <c r="W22" s="9"/>
+      <c r="X22" s="9">
         <f t="shared" si="31"/>
         <v>8</v>
       </c>
-      <c r="Y22" s="7"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+      <c r="AA22" s="9"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="9">
         <f>B14</f>
         <v>400</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7">
+      <c r="C23" s="9"/>
+      <c r="D23" s="9">
         <f>B23*$I4</f>
-        <v>26000</v>
-      </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7">
+        <v>523200</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9">
         <f>D23</f>
-        <v>26000</v>
-      </c>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7">
+        <v>523200</v>
+      </c>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9">
         <f t="shared" si="33"/>
-        <v>26000</v>
-      </c>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7">
-        <f t="shared" ref="J23:J24" si="35">H23</f>
-        <v>26000</v>
-      </c>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7">
-        <f>J23/I4*Q4</f>
-        <v>4800</v>
-      </c>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7">
+        <v>523200</v>
+      </c>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9">
+        <f t="shared" ref="J23" si="36">H23</f>
+        <v>523200</v>
+      </c>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9">
+        <f>J23</f>
+        <v>523200</v>
+      </c>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9">
         <f>L23</f>
-        <v>4800</v>
-      </c>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7">
-        <f t="shared" ref="P22:P23" si="36">N23</f>
-        <v>4800</v>
-      </c>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7">
+        <v>523200</v>
+      </c>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9">
+        <f t="shared" ref="P23" si="37">N23</f>
+        <v>523200</v>
+      </c>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9">
         <f t="shared" si="29"/>
-        <v>4800</v>
-      </c>
-      <c r="S23" s="7"/>
-      <c r="T23" s="7">
+        <v>523200</v>
+      </c>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9">
         <f t="shared" si="30"/>
-        <v>4800</v>
-      </c>
-      <c r="U23" s="7"/>
-      <c r="V23" s="7">
-        <f t="shared" ref="V22:V23" si="37">T23</f>
-        <v>4800</v>
-      </c>
-      <c r="W23" s="7"/>
-      <c r="X23" s="7">
+        <v>523200</v>
+      </c>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9">
+        <f t="shared" ref="V23" si="38">T23</f>
+        <v>523200</v>
+      </c>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9">
         <f t="shared" si="31"/>
-        <v>4800</v>
-      </c>
-      <c r="Y23" s="7"/>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+        <v>523200</v>
+      </c>
+      <c r="Y23" s="9"/>
+      <c r="Z23" s="9"/>
+      <c r="AA23" s="9"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="12">
         <f>B21*B22*B23</f>
-        <v>26214400</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8">
-        <f t="shared" ref="D24" si="38">D21*D22*D23</f>
-        <v>638976000</v>
-      </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8">
-        <f t="shared" ref="F24" si="39">F21*F22*F23</f>
-        <v>638976000</v>
-      </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8">
-        <f t="shared" ref="H24" si="40">H21*H22*H23</f>
-        <v>638976000</v>
-      </c>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8">
-        <f t="shared" ref="J24" si="41">J21*J22*J23</f>
-        <v>638976000</v>
-      </c>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8">
-        <f t="shared" ref="L24" si="42">L21*L22*L23</f>
-        <v>117964800</v>
-      </c>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8">
-        <f t="shared" ref="N24" si="43">N21*N22*N23</f>
-        <v>117964800</v>
-      </c>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8">
-        <f t="shared" ref="P24" si="44">P21*P22*P23</f>
-        <v>3774873600</v>
-      </c>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8">
-        <f t="shared" ref="R24" si="45">R21*R22*R23</f>
-        <v>3774873600</v>
-      </c>
-      <c r="S24" s="8"/>
-      <c r="T24" s="8">
-        <f t="shared" ref="T24" si="46">T21*T22*T23</f>
-        <v>3774873600</v>
-      </c>
-      <c r="U24" s="8"/>
-      <c r="V24" s="8">
-        <f t="shared" ref="V24" si="47">V21*V22*V23</f>
-        <v>29491200</v>
-      </c>
-      <c r="W24" s="8"/>
-      <c r="X24" s="8">
-        <f t="shared" ref="X24" si="48">X21*X22*X23</f>
-        <v>29491200</v>
-      </c>
-      <c r="Y24" s="8"/>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+        <v>819200</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12">
+        <f t="shared" ref="D24" si="39">D21*D22*D23</f>
+        <v>12858163200</v>
+      </c>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12">
+        <f t="shared" ref="F24" si="40">F21*F22*F23</f>
+        <v>12858163200</v>
+      </c>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12">
+        <f t="shared" ref="H24" si="41">H21*H22*H23</f>
+        <v>12858163200</v>
+      </c>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12">
+        <f t="shared" ref="J24" si="42">J21*J22*J23</f>
+        <v>12858163200</v>
+      </c>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12">
+        <f t="shared" ref="L24" si="43">L21*L22*L23</f>
+        <v>12858163200</v>
+      </c>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12">
+        <f t="shared" ref="N24" si="44">N21*N22*N23</f>
+        <v>12858163200</v>
+      </c>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12">
+        <f t="shared" ref="P24" si="45">P21*P22*P23</f>
+        <v>12858163200</v>
+      </c>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12">
+        <f t="shared" ref="R24" si="46">R21*R22*R23</f>
+        <v>12858163200</v>
+      </c>
+      <c r="S24" s="12"/>
+      <c r="T24" s="12">
+        <f t="shared" ref="T24" si="47">T21*T22*T23</f>
+        <v>12858163200</v>
+      </c>
+      <c r="U24" s="12"/>
+      <c r="V24" s="12">
+        <f t="shared" ref="V24" si="48">V21*V22*V23</f>
+        <v>12858163200</v>
+      </c>
+      <c r="W24" s="12"/>
+      <c r="X24" s="12">
+        <f t="shared" ref="X24" si="49">X21*X22*X23</f>
+        <v>12858163200</v>
+      </c>
+      <c r="Y24" s="12"/>
+      <c r="Z24" s="5"/>
+      <c r="AA24" s="5"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25" s="11">
         <f>B24*$F8/86400</f>
-        <v>1.8204444444444443E-4</v>
-      </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12">
+        <v>5.6888888888888884E-6</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11">
         <f>D24*$F8/86400+B25</f>
-        <v>4.6193777777777771E-3</v>
-      </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12">
-        <f t="shared" ref="F25" si="49">F24*$F8/86400+D25</f>
-        <v>9.0567111111111102E-3</v>
-      </c>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12">
-        <f t="shared" ref="H25" si="50">H24*$F8/86400+F25</f>
-        <v>1.3494044444444443E-2</v>
-      </c>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12">
-        <f t="shared" ref="J25" si="51">J24*$F8/86400+H25</f>
-        <v>1.7931377777777778E-2</v>
-      </c>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12">
-        <f t="shared" ref="L25" si="52">L24*$F8/86400+J25</f>
-        <v>1.8750577777777777E-2</v>
-      </c>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12">
-        <f t="shared" ref="N25" si="53">N24*$F8/86400+L25</f>
-        <v>1.9569777777777776E-2</v>
-      </c>
-      <c r="O25" s="12"/>
-      <c r="P25" s="12">
-        <f t="shared" ref="P25" si="54">P24*$F8/86400+N25</f>
-        <v>4.5784177777777775E-2</v>
-      </c>
-      <c r="Q25" s="12"/>
-      <c r="R25" s="12">
-        <f t="shared" ref="R25" si="55">R24*$F8/86400+P25</f>
-        <v>7.1998577777777767E-2</v>
-      </c>
-      <c r="S25" s="12"/>
-      <c r="T25" s="12">
-        <f t="shared" ref="T25" si="56">T24*$F8/86400+R25</f>
-        <v>9.8212977777777766E-2</v>
-      </c>
-      <c r="U25" s="12"/>
-      <c r="V25" s="12">
-        <f t="shared" ref="V25" si="57">V24*$F8/86400+T25</f>
-        <v>9.8417777777777771E-2</v>
-      </c>
-      <c r="W25" s="12"/>
-      <c r="X25" s="12">
-        <f t="shared" ref="X25" si="58">X24*$F8/86400+V25</f>
-        <v>9.8622577777777776E-2</v>
-      </c>
-      <c r="Y25" s="12"/>
+        <v>8.9298488888888874E-2</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11">
+        <f t="shared" ref="F25" si="50">F24*$F8/86400+D25</f>
+        <v>0.17859128888888887</v>
+      </c>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11">
+        <f t="shared" ref="H25" si="51">H24*$F8/86400+F25</f>
+        <v>0.26788408888888887</v>
+      </c>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11">
+        <f t="shared" ref="J25" si="52">J24*$F8/86400+H25</f>
+        <v>0.35717688888888888</v>
+      </c>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11">
+        <f t="shared" ref="L25" si="53">L24*$F8/86400+J25</f>
+        <v>0.44646968888888888</v>
+      </c>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11">
+        <f t="shared" ref="N25" si="54">N24*$F8/86400+L25</f>
+        <v>0.53576248888888889</v>
+      </c>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11">
+        <f t="shared" ref="P25" si="55">P24*$F8/86400+N25</f>
+        <v>0.62505528888888884</v>
+      </c>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11">
+        <f t="shared" ref="R25" si="56">R24*$F8/86400+P25</f>
+        <v>0.71434808888888879</v>
+      </c>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11">
+        <f t="shared" ref="T25" si="57">T24*$F8/86400+R25</f>
+        <v>0.80364088888888874</v>
+      </c>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11">
+        <f t="shared" ref="V25" si="58">V24*$F8/86400+T25</f>
+        <v>0.89293368888888869</v>
+      </c>
+      <c r="W25" s="11"/>
+      <c r="X25" s="11">
+        <f t="shared" ref="X25" si="59">X24*$F8/86400+V25</f>
+        <v>0.98222648888888864</v>
+      </c>
+      <c r="Y25" s="11"/>
+      <c r="Z25" s="8"/>
+      <c r="AA25" s="8"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="E31" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="85">
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="R25:S25"/>
-    <mergeCell ref="T25:U25"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="X25:Y25"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="X24:Y24"/>
+  <mergeCells count="90">
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="F25:G25"/>
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="J25:K25"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="Z23:AA23"/>
     <mergeCell ref="L25:M25"/>
     <mergeCell ref="N25:O25"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="R25:S25"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="T25:U25"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="X25:Y25"/>
+    <mergeCell ref="Z25:AA25"/>
+    <mergeCell ref="X24:Y24"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="T21:U21"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="X21:Y21"/>
+    <mergeCell ref="Z21:AA21"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="X16:Y16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="L3:M3"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B7FF28-7221-43C9-AFD5-E9B2F94032D2}">
+  <dimension ref="A1:AA31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="10"/>
+      <c r="L1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="10"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>9481</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2">
+        <v>19.909876918386299</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="2">
+        <f>MAX(ROUND(1/F4,0),ROUND(F4,0))</f>
+        <v>12</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="10"/>
+      <c r="N2">
+        <v>42.926477759350803</v>
+      </c>
+      <c r="P2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="2">
+        <f>MAX(ROUND(1/N4,0),ROUND(N4,0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="2">
+        <f>$B4*F5/300000000*1000000000000000</f>
+        <v>52300.882458116022</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="10"/>
+      <c r="N3">
+        <v>-29.5</v>
+      </c>
+      <c r="P3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" s="2">
+        <f>$B4*N5/300000000*1000000000000000</f>
+        <v>9380.9992619267869</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4">
+        <f>SIN(RADIANS(F2+F3))/SIN(RADIANS(F2-F3))</f>
+        <v>11.830135875287004</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="2">
+        <f>MAX(ROUND(I3/$B7,0),1)</f>
+        <v>65</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="10"/>
+      <c r="N4">
+        <f>SIN(RADIANS(N2+N3))/SIN(RADIANS(N2-N3))</f>
+        <v>0.24356450463759297</v>
+      </c>
+      <c r="P4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="2">
+        <f>MAX(ROUND(Q3/$B7,0),1)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5">
+        <f>ABS((COS(RADIANS(F2-F3))-COS(RADIANS(F2+F3)))/SIN(RADIANS(F2-F3)))</f>
+        <v>3.9225661843587014</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="10"/>
+      <c r="N5">
+        <f>ABS((COS(RADIANS(N2-N3))-COS(RADIANS(N2+N3)))/SIN(RADIANS(N2-N3)))</f>
+        <v>0.70357494464450898</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <f>B3*40</f>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <f>B3/10</f>
+        <v>2</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="1">
+        <v>5.9999999999999997E-7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="1">
+        <f>2048*2*500000</f>
+        <v>2048000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <f>4/B8</f>
+        <v>2</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="7" cm="1">
+        <f t="array" ref="F9">IFERROR(LOOKUP(1,0/(25:25&lt;&gt;""),25:25),"")</f>
+        <v>9.9851377777777778E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <f>B9/B14</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="7">
+        <f>X25-J25</f>
+        <v>8.1919999999999993E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>256</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>256</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <f>B7/B8</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B16" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="W16" s="10"/>
+      <c r="X16" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="10"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2">
+        <f>B4*1000000</f>
+        <v>4000</v>
+      </c>
+      <c r="C17" s="2">
+        <f>B17/B21</f>
+        <v>15.625</v>
+      </c>
+      <c r="D17" s="2">
+        <f>B17*$I2</f>
+        <v>48000</v>
+      </c>
+      <c r="E17" s="2">
+        <f>D17/D21</f>
+        <v>15.625</v>
+      </c>
+      <c r="F17" s="2">
+        <f>D17</f>
+        <v>48000</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" ref="G17:G19" si="0">F17/F21</f>
+        <v>15.625</v>
+      </c>
+      <c r="H17" s="2">
+        <f>F17</f>
+        <v>48000</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" ref="I17:I19" si="1">H17/H21</f>
+        <v>15.625</v>
+      </c>
+      <c r="J17" s="2">
+        <f>H17/I2</f>
+        <v>4000</v>
+      </c>
+      <c r="K17" s="2">
+        <f>J17/J21</f>
+        <v>1.3020833333333333</v>
+      </c>
+      <c r="L17" s="2">
+        <f>J17</f>
+        <v>4000</v>
+      </c>
+      <c r="M17" s="2">
+        <f>L17/L21</f>
+        <v>1.3020833333333333</v>
+      </c>
+      <c r="N17" s="2">
+        <f>L17*Q2</f>
+        <v>16000</v>
+      </c>
+      <c r="O17" s="2">
+        <f>N17/N21</f>
+        <v>5.208333333333333</v>
+      </c>
+      <c r="P17" s="2">
+        <f t="shared" ref="P17:P19" si="2">N17</f>
+        <v>16000</v>
+      </c>
+      <c r="Q17" s="2">
+        <f t="shared" ref="Q17:Q19" si="3">P17/P21</f>
+        <v>5.208333333333333</v>
+      </c>
+      <c r="R17" s="2">
+        <f t="shared" ref="R17:R19" si="4">P17</f>
+        <v>16000</v>
+      </c>
+      <c r="S17" s="2">
+        <f t="shared" ref="S17:S19" si="5">R17/R21</f>
+        <v>5.208333333333333</v>
+      </c>
+      <c r="T17" s="2">
+        <f t="shared" ref="T17:T19" si="6">R17</f>
+        <v>16000</v>
+      </c>
+      <c r="U17" s="2">
+        <f t="shared" ref="U17:U19" si="7">T17/T21</f>
+        <v>5.208333333333333</v>
+      </c>
+      <c r="V17" s="2">
+        <f>T17/Q2</f>
+        <v>4000</v>
+      </c>
+      <c r="W17" s="2">
+        <f t="shared" ref="W17:W19" si="8">V17/V21</f>
+        <v>1.3020833333333333</v>
+      </c>
+      <c r="X17" s="2">
+        <f t="shared" ref="X17:X19" si="9">V17</f>
+        <v>4000</v>
+      </c>
+      <c r="Y17" s="2">
+        <f t="shared" ref="Y17:Y19" si="10">X17/X21</f>
+        <v>1.3020833333333333</v>
+      </c>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="2">
+        <f>B5*1000000</f>
+        <v>4000</v>
+      </c>
+      <c r="C18" s="2">
+        <f>B18/B22</f>
+        <v>15.625</v>
+      </c>
+      <c r="D18" s="2">
+        <f>B18</f>
+        <v>4000</v>
+      </c>
+      <c r="E18" s="2">
+        <f>D18/D22</f>
+        <v>500</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" ref="F18" si="11">D18</f>
+        <v>4000</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" ref="H18" si="12">F18</f>
+        <v>4000</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" ref="J18" si="13">H18</f>
+        <v>4000</v>
+      </c>
+      <c r="K18" s="2">
+        <f>J18/J22</f>
+        <v>500</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" ref="L18" si="14">J18</f>
+        <v>4000</v>
+      </c>
+      <c r="M18" s="2">
+        <f>L18/L22</f>
+        <v>500</v>
+      </c>
+      <c r="N18" s="2">
+        <f t="shared" ref="N18" si="15">L18</f>
+        <v>4000</v>
+      </c>
+      <c r="O18" s="2">
+        <f>N18/N22</f>
+        <v>500</v>
+      </c>
+      <c r="P18" s="2">
+        <f t="shared" si="2"/>
+        <v>4000</v>
+      </c>
+      <c r="Q18" s="2">
+        <f t="shared" si="3"/>
+        <v>15.625</v>
+      </c>
+      <c r="R18" s="2">
+        <f t="shared" si="4"/>
+        <v>4000</v>
+      </c>
+      <c r="S18" s="2">
+        <f t="shared" si="5"/>
+        <v>15.625</v>
+      </c>
+      <c r="T18" s="2">
+        <f t="shared" si="6"/>
+        <v>4000</v>
+      </c>
+      <c r="U18" s="2">
+        <f t="shared" si="7"/>
+        <v>15.625</v>
+      </c>
+      <c r="V18" s="2">
+        <f t="shared" ref="V18:V19" si="16">T18</f>
+        <v>4000</v>
+      </c>
+      <c r="W18" s="2">
+        <f t="shared" si="8"/>
+        <v>500</v>
+      </c>
+      <c r="X18" s="2">
+        <f t="shared" si="9"/>
+        <v>4000</v>
+      </c>
+      <c r="Y18" s="2">
+        <f t="shared" si="10"/>
+        <v>500</v>
+      </c>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="2">
+        <f>B7</f>
+        <v>800</v>
+      </c>
+      <c r="C19" s="2">
+        <f>B8</f>
+        <v>2</v>
+      </c>
+      <c r="D19" s="2">
+        <f>B19*$I4</f>
+        <v>52000</v>
+      </c>
+      <c r="E19" s="2">
+        <f>D19/D23</f>
+        <v>2</v>
+      </c>
+      <c r="F19" s="2">
+        <f>D19</f>
+        <v>52000</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H19" s="2">
+        <f>F19</f>
+        <v>52000</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J19" s="2">
+        <f>H19</f>
+        <v>52000</v>
+      </c>
+      <c r="K19" s="2">
+        <f>J19/J23</f>
+        <v>2</v>
+      </c>
+      <c r="L19" s="2">
+        <f>J19/I4*Q4</f>
+        <v>9600</v>
+      </c>
+      <c r="M19" s="2">
+        <f>L19/L23</f>
+        <v>2</v>
+      </c>
+      <c r="N19" s="2">
+        <f>L19</f>
+        <v>9600</v>
+      </c>
+      <c r="O19" s="2">
+        <f>N19/N23</f>
+        <v>2</v>
+      </c>
+      <c r="P19" s="2">
+        <f t="shared" si="2"/>
+        <v>9600</v>
+      </c>
+      <c r="Q19" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="R19" s="2">
+        <f t="shared" si="4"/>
+        <v>9600</v>
+      </c>
+      <c r="S19" s="2">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="T19" s="2">
+        <f t="shared" si="6"/>
+        <v>9600</v>
+      </c>
+      <c r="U19" s="2">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="V19" s="2">
+        <f t="shared" si="16"/>
+        <v>9600</v>
+      </c>
+      <c r="W19" s="2">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="X19" s="2">
+        <f t="shared" si="9"/>
+        <v>9600</v>
+      </c>
+      <c r="Y19" s="2">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="2">
+        <f>B9*1000</f>
+        <v>2000</v>
+      </c>
+      <c r="C20" s="2">
+        <f>B10*1000</f>
+        <v>5</v>
+      </c>
+      <c r="D20" s="2">
+        <f>$B20*$C19/E19</f>
+        <v>2000</v>
+      </c>
+      <c r="E20" s="2">
+        <f>$B19*$C20/D19</f>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F20" s="2">
+        <f>$B20*$C19/G19</f>
+        <v>2000</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" ref="G20" si="17">$B19*$C20/F19</f>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H20" s="2">
+        <f>$B20*$C19/I19</f>
+        <v>2000</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" ref="I20" si="18">$B19*$C20/H19</f>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="J20" s="2">
+        <f>$B20*$C19/K19</f>
+        <v>2000</v>
+      </c>
+      <c r="K20" s="2">
+        <f>$B19*$C20/J19</f>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="L20" s="2">
+        <f>$B20*$C19/M19</f>
+        <v>2000</v>
+      </c>
+      <c r="M20" s="2">
+        <f>$B19*$C20/L19</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="N20" s="2">
+        <f>$B20*$C19/O19</f>
+        <v>2000</v>
+      </c>
+      <c r="O20" s="2">
+        <f>$B19*$C20/N19</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="P20" s="2">
+        <f t="shared" ref="P20" si="19">$B20*$C19/Q19</f>
+        <v>2000</v>
+      </c>
+      <c r="Q20" s="2">
+        <f t="shared" ref="Q20" si="20">$B19*$C20/P19</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="R20" s="2">
+        <f t="shared" ref="R20" si="21">$B20*$C19/S19</f>
+        <v>2000</v>
+      </c>
+      <c r="S20" s="2">
+        <f t="shared" ref="S20" si="22">$B19*$C20/R19</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="T20" s="2">
+        <f t="shared" ref="T20" si="23">$B20*$C19/U19</f>
+        <v>2000</v>
+      </c>
+      <c r="U20" s="2">
+        <f t="shared" ref="U20" si="24">$B19*$C20/T19</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="V20" s="2">
+        <f t="shared" ref="V20" si="25">$B20*$C19/W19</f>
+        <v>2000</v>
+      </c>
+      <c r="W20" s="2">
+        <f t="shared" ref="W20" si="26">$B19*$C20/V19</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="X20" s="2">
+        <f t="shared" ref="X20" si="27">$B20*$C19/Y19</f>
+        <v>2000</v>
+      </c>
+      <c r="Y20" s="2">
+        <f t="shared" ref="Y20" si="28">$B19*$C20/X19</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="9">
+        <f>B12</f>
+        <v>256</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9">
+        <f>B21*$I2</f>
+        <v>3072</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9">
+        <f>D21</f>
+        <v>3072</v>
+      </c>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9">
+        <f>F21</f>
+        <v>3072</v>
+      </c>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9">
+        <f>H21</f>
+        <v>3072</v>
+      </c>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9">
+        <f>J21</f>
+        <v>3072</v>
+      </c>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9">
+        <f>J21</f>
+        <v>3072</v>
+      </c>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9">
+        <f>N21</f>
+        <v>3072</v>
+      </c>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9">
+        <f t="shared" ref="R21:R23" si="29">P21</f>
+        <v>3072</v>
+      </c>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9">
+        <f t="shared" ref="T21:T23" si="30">R21</f>
+        <v>3072</v>
+      </c>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9">
+        <f>T21</f>
+        <v>3072</v>
+      </c>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9">
+        <f t="shared" ref="X21:X23" si="31">V21</f>
+        <v>3072</v>
+      </c>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="9">
+        <f>B13</f>
+        <v>256</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9">
+        <f>E13</f>
+        <v>8</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9">
+        <f t="shared" ref="F22" si="32">D22</f>
+        <v>8</v>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9">
+        <f t="shared" ref="H22:H23" si="33">F22</f>
+        <v>8</v>
+      </c>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9">
+        <f>H22</f>
+        <v>8</v>
+      </c>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9">
+        <f t="shared" ref="L22" si="34">J22</f>
+        <v>8</v>
+      </c>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9">
+        <f t="shared" ref="N22" si="35">L22</f>
+        <v>8</v>
+      </c>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9">
+        <f>B13</f>
+        <v>256</v>
+      </c>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9">
+        <f t="shared" si="29"/>
+        <v>256</v>
+      </c>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9">
+        <f t="shared" si="30"/>
+        <v>256</v>
+      </c>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9">
+        <f>E13</f>
+        <v>8</v>
+      </c>
+      <c r="W22" s="9"/>
+      <c r="X22" s="9">
+        <f t="shared" si="31"/>
+        <v>8</v>
+      </c>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+      <c r="AA22" s="9"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="9">
+        <f>B14</f>
+        <v>400</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9">
+        <f>B23*$I4</f>
+        <v>26000</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9">
+        <f>D23</f>
+        <v>26000</v>
+      </c>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9">
+        <f t="shared" si="33"/>
+        <v>26000</v>
+      </c>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9">
+        <f t="shared" ref="J23" si="36">H23</f>
+        <v>26000</v>
+      </c>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9">
+        <f>J23/I4*Q4</f>
+        <v>4800</v>
+      </c>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9">
+        <f>L23</f>
+        <v>4800</v>
+      </c>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9">
+        <f t="shared" ref="P23" si="37">N23</f>
+        <v>4800</v>
+      </c>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9">
+        <f t="shared" si="29"/>
+        <v>4800</v>
+      </c>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9">
+        <f t="shared" si="30"/>
+        <v>4800</v>
+      </c>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9">
+        <f t="shared" ref="V23" si="38">T23</f>
+        <v>4800</v>
+      </c>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9">
+        <f t="shared" si="31"/>
+        <v>4800</v>
+      </c>
+      <c r="Y23" s="9"/>
+      <c r="Z23" s="9"/>
+      <c r="AA23" s="9"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="12">
+        <f>B21*B22*B23</f>
+        <v>26214400</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12">
+        <f t="shared" ref="D24" si="39">D21*D22*D23</f>
+        <v>638976000</v>
+      </c>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12">
+        <f t="shared" ref="F24" si="40">F21*F22*F23</f>
+        <v>638976000</v>
+      </c>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12">
+        <f t="shared" ref="H24" si="41">H21*H22*H23</f>
+        <v>638976000</v>
+      </c>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12">
+        <f t="shared" ref="J24" si="42">J21*J22*J23</f>
+        <v>638976000</v>
+      </c>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12">
+        <f t="shared" ref="L24" si="43">L21*L22*L23</f>
+        <v>117964800</v>
+      </c>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12">
+        <f t="shared" ref="N24" si="44">N21*N22*N23</f>
+        <v>117964800</v>
+      </c>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12">
+        <f t="shared" ref="P24" si="45">P21*P22*P23</f>
+        <v>3774873600</v>
+      </c>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12">
+        <f t="shared" ref="R24" si="46">R21*R22*R23</f>
+        <v>3774873600</v>
+      </c>
+      <c r="S24" s="12"/>
+      <c r="T24" s="12">
+        <f t="shared" ref="T24" si="47">T21*T22*T23</f>
+        <v>3774873600</v>
+      </c>
+      <c r="U24" s="12"/>
+      <c r="V24" s="12">
+        <f t="shared" ref="V24" si="48">V21*V22*V23</f>
+        <v>117964800</v>
+      </c>
+      <c r="W24" s="12"/>
+      <c r="X24" s="12">
+        <f t="shared" ref="X24" si="49">X21*X22*X23</f>
+        <v>117964800</v>
+      </c>
+      <c r="Y24" s="12"/>
+      <c r="Z24" s="5"/>
+      <c r="AA24" s="5"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="11">
+        <f>B24*$F8/86400</f>
+        <v>1.8204444444444443E-4</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11">
+        <f>D24*$F8/86400+B25</f>
+        <v>4.6193777777777771E-3</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11">
+        <f t="shared" ref="F25" si="50">F24*$F8/86400+D25</f>
+        <v>9.0567111111111102E-3</v>
+      </c>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11">
+        <f t="shared" ref="H25" si="51">H24*$F8/86400+F25</f>
+        <v>1.3494044444444443E-2</v>
+      </c>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11">
+        <f t="shared" ref="J25" si="52">J24*$F8/86400+H25</f>
+        <v>1.7931377777777778E-2</v>
+      </c>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11">
+        <f t="shared" ref="L25" si="53">L24*$F8/86400+J25</f>
+        <v>1.8750577777777777E-2</v>
+      </c>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11">
+        <f t="shared" ref="N25" si="54">N24*$F8/86400+L25</f>
+        <v>1.9569777777777776E-2</v>
+      </c>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11">
+        <f t="shared" ref="P25" si="55">P24*$F8/86400+N25</f>
+        <v>4.5784177777777775E-2</v>
+      </c>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11">
+        <f t="shared" ref="R25" si="56">R24*$F8/86400+P25</f>
+        <v>7.1998577777777767E-2</v>
+      </c>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11">
+        <f t="shared" ref="T25" si="57">T24*$F8/86400+R25</f>
+        <v>9.8212977777777766E-2</v>
+      </c>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11">
+        <f t="shared" ref="V25" si="58">V24*$F8/86400+T25</f>
+        <v>9.9032177777777772E-2</v>
+      </c>
+      <c r="W25" s="11"/>
+      <c r="X25" s="11">
+        <f t="shared" ref="X25" si="59">X24*$F8/86400+V25</f>
+        <v>9.9851377777777778E-2</v>
+      </c>
+      <c r="Y25" s="11"/>
+      <c r="Z25" s="8"/>
+      <c r="AA25" s="8"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="E31" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="90">
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="Z21:AA21"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="Z23:AA23"/>
+    <mergeCell ref="Z25:AA25"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="X16:Y16"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="T21:U21"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="X21:Y21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
     <mergeCell ref="X23:Y23"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="D24:E24"/>
@@ -2855,62 +4116,24 @@
     <mergeCell ref="R23:S23"/>
     <mergeCell ref="T23:U23"/>
     <mergeCell ref="V23:W23"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="X22:Y22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="T21:U21"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="X21:Y21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="X16:Y16"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="X24:Y24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="R25:S25"/>
+    <mergeCell ref="T25:U25"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="X25:Y25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update: tolerance simulation with variable inputs updated
argparse variables for looping
</commit_message>
<xml_diff>
--- a/Sampling_Resolution_Calculator.xlsx
+++ b/Sampling_Resolution_Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nanw0\GoogleDrive\SLAC\SLAC-Diling\11. 21 Winter\DXS optics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3DAFA7-FF22-45EE-B15A-24ED02D6B55D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280D99DE-50ED-4E23-8257-AD2BD90888E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="630" windowWidth="28500" windowHeight="14820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="555" windowWidth="25200" windowHeight="20370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9481" sheetId="1" r:id="rId1"/>
@@ -299,19 +299,19 @@
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -622,14 +622,14 @@
       <c r="A1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="L1" s="10" t="s">
+      <c r="E1" s="8"/>
+      <c r="L1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="10"/>
+      <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -638,10 +638,10 @@
       <c r="B2">
         <v>9481</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="10"/>
+      <c r="E2" s="8"/>
       <c r="F2">
         <v>19.909876918386299</v>
       </c>
@@ -652,10 +652,10 @@
         <f>MAX(ROUND(1/F4,0),ROUND(F4,0))</f>
         <v>12</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="10"/>
+      <c r="M2" s="8"/>
       <c r="N2">
         <v>42.926477759350803</v>
       </c>
@@ -674,10 +674,10 @@
       <c r="B3">
         <v>100</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="8"/>
       <c r="F3">
         <v>17</v>
       </c>
@@ -688,10 +688,10 @@
         <f>$B4*F5/300000000*1000000000000000</f>
         <v>52300.882458116022</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="10"/>
+      <c r="M3" s="8"/>
       <c r="N3">
         <v>-29.5</v>
       </c>
@@ -710,10 +710,10 @@
       <c r="B4" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="10"/>
+      <c r="E4" s="8"/>
       <c r="F4">
         <f>SIN(RADIANS(F2+F3))/SIN(RADIANS(F2-F3))</f>
         <v>11.830135875287004</v>
@@ -725,10 +725,10 @@
         <f>MAX(ROUND(I3/$B7,0),1)</f>
         <v>13</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="10"/>
+      <c r="M4" s="8"/>
       <c r="N4">
         <f>SIN(RADIANS(N2+N3))/SIN(RADIANS(N2-N3))</f>
         <v>0.24356450463759297</v>
@@ -748,18 +748,18 @@
       <c r="B5" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="E5" s="8"/>
       <c r="F5">
         <f>ABS((COS(RADIANS(F2-F3))-COS(RADIANS(F2+F3)))/SIN(RADIANS(F2-F3)))</f>
         <v>3.9225661843587014</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="10"/>
+      <c r="M5" s="8"/>
       <c r="N5">
         <f>ABS((COS(RADIANS(N2-N3))-COS(RADIANS(N2+N3)))/SIN(RADIANS(N2-N3)))</f>
         <v>0.70357494464450898</v>
@@ -785,10 +785,10 @@
         <f>B3/10</f>
         <v>10</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="10"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="1">
         <v>5.9999999999999997E-7</v>
       </c>
@@ -808,10 +808,10 @@
         <f>4/B8</f>
         <v>0.4</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="10"/>
+      <c r="E9" s="8"/>
       <c r="F9" s="7" cm="1">
         <f t="array" ref="F9">IFERROR(LOOKUP(1,0/(25:25&lt;&gt;""),25:25),"")</f>
         <v>0.14436124444444448</v>
@@ -825,10 +825,10 @@
         <f>B9/B14</f>
         <v>1E-3</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="10"/>
+      <c r="E10" s="8"/>
       <c r="F10" s="7">
         <f>X25-J25</f>
         <v>3.0583466666666698E-2</v>
@@ -869,56 +869,56 @@
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10" t="s">
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10" t="s">
+      <c r="E16" s="8"/>
+      <c r="F16" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10" t="s">
+      <c r="G16" s="8"/>
+      <c r="H16" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10" t="s">
+      <c r="I16" s="8"/>
+      <c r="J16" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10" t="s">
+      <c r="K16" s="8"/>
+      <c r="L16" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10" t="s">
+      <c r="M16" s="8"/>
+      <c r="N16" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10" t="s">
+      <c r="O16" s="8"/>
+      <c r="P16" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10" t="s">
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10" t="s">
+      <c r="S16" s="8"/>
+      <c r="T16" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10" t="s">
+      <c r="U16" s="8"/>
+      <c r="V16" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="W16" s="10"/>
-      <c r="X16" s="10" t="s">
+      <c r="W16" s="8"/>
+      <c r="X16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Y16" s="10"/>
-      <c r="Z16" s="10"/>
-      <c r="AA16" s="10"/>
+      <c r="Y16" s="8"/>
+      <c r="Z16" s="8"/>
+      <c r="AA16" s="8"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
@@ -1537,66 +1537,66 @@
       <c r="A24" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="11">
         <f>B21*B22*B23</f>
         <v>26214400</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12">
+      <c r="C24" s="11"/>
+      <c r="D24" s="11">
         <f t="shared" ref="D24" si="39">D21*D22*D23</f>
         <v>4089446400</v>
       </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12">
+      <c r="E24" s="11"/>
+      <c r="F24" s="11">
         <f t="shared" ref="F24" si="40">F21*F22*F23</f>
         <v>4089446400</v>
       </c>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12">
+      <c r="G24" s="11"/>
+      <c r="H24" s="11">
         <f t="shared" ref="H24" si="41">H21*H22*H23</f>
         <v>4089446400</v>
       </c>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12">
+      <c r="I24" s="11"/>
+      <c r="J24" s="11">
         <f t="shared" ref="J24" si="42">J21*J22*J23</f>
         <v>4089446400</v>
       </c>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12">
+      <c r="K24" s="11"/>
+      <c r="L24" s="11">
         <f t="shared" ref="L24" si="43">L21*L22*L23</f>
         <v>629145600</v>
       </c>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12">
+      <c r="M24" s="11"/>
+      <c r="N24" s="11">
         <f t="shared" ref="N24" si="44">N21*N22*N23</f>
         <v>629145600</v>
       </c>
-      <c r="O24" s="12"/>
-      <c r="P24" s="12">
+      <c r="O24" s="11"/>
+      <c r="P24" s="11">
         <f t="shared" ref="P24" si="45">P21*P22*P23</f>
         <v>629145600</v>
       </c>
-      <c r="Q24" s="12"/>
-      <c r="R24" s="12">
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11">
         <f t="shared" ref="R24" si="46">R21*R22*R23</f>
         <v>629145600</v>
       </c>
-      <c r="S24" s="12"/>
-      <c r="T24" s="12">
+      <c r="S24" s="11"/>
+      <c r="T24" s="11">
         <f t="shared" ref="T24" si="47">T21*T22*T23</f>
         <v>629145600</v>
       </c>
-      <c r="U24" s="12"/>
-      <c r="V24" s="12">
+      <c r="U24" s="11"/>
+      <c r="V24" s="11">
         <f t="shared" ref="V24" si="48">V21*V22*V23</f>
         <v>629145600</v>
       </c>
-      <c r="W24" s="12"/>
-      <c r="X24" s="12">
+      <c r="W24" s="11"/>
+      <c r="X24" s="11">
         <f t="shared" ref="X24" si="49">X21*X22*X23</f>
         <v>629145600</v>
       </c>
-      <c r="Y24" s="12"/>
+      <c r="Y24" s="11"/>
       <c r="Z24" s="5"/>
       <c r="AA24" s="5"/>
     </row>
@@ -1604,68 +1604,68 @@
       <c r="A25" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="10">
         <f>B24*$F8/86400</f>
         <v>1.8204444444444443E-4</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11">
+      <c r="C25" s="10"/>
+      <c r="D25" s="10">
         <f>D24*$F8/86400+B25</f>
         <v>2.858097777777778E-2</v>
       </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11">
+      <c r="E25" s="10"/>
+      <c r="F25" s="10">
         <f t="shared" ref="F25" si="50">F24*$F8/86400+D25</f>
         <v>5.6979911111111115E-2</v>
       </c>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11">
+      <c r="G25" s="10"/>
+      <c r="H25" s="10">
         <f t="shared" ref="H25" si="51">H24*$F8/86400+F25</f>
         <v>8.5378844444444449E-2</v>
       </c>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11">
+      <c r="I25" s="10"/>
+      <c r="J25" s="10">
         <f t="shared" ref="J25" si="52">J24*$F8/86400+H25</f>
         <v>0.11377777777777778</v>
       </c>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11">
+      <c r="K25" s="10"/>
+      <c r="L25" s="10">
         <f t="shared" ref="L25" si="53">L24*$F8/86400+J25</f>
         <v>0.11814684444444445</v>
       </c>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11">
+      <c r="M25" s="10"/>
+      <c r="N25" s="10">
         <f t="shared" ref="N25" si="54">N24*$F8/86400+L25</f>
         <v>0.12251591111111113</v>
       </c>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11">
+      <c r="O25" s="10"/>
+      <c r="P25" s="10">
         <f t="shared" ref="P25" si="55">P24*$F8/86400+N25</f>
         <v>0.1268849777777778</v>
       </c>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11">
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10">
         <f t="shared" ref="R25" si="56">R24*$F8/86400+P25</f>
         <v>0.13125404444444447</v>
       </c>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11">
+      <c r="S25" s="10"/>
+      <c r="T25" s="10">
         <f t="shared" ref="T25" si="57">T24*$F8/86400+R25</f>
         <v>0.13562311111111114</v>
       </c>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11">
+      <c r="U25" s="10"/>
+      <c r="V25" s="10">
         <f t="shared" ref="V25" si="58">V24*$F8/86400+T25</f>
         <v>0.13999217777777781</v>
       </c>
-      <c r="W25" s="11"/>
-      <c r="X25" s="11">
+      <c r="W25" s="10"/>
+      <c r="X25" s="10">
         <f t="shared" ref="X25" si="59">X24*$F8/86400+V25</f>
         <v>0.14436124444444448</v>
       </c>
-      <c r="Y25" s="11"/>
-      <c r="Z25" s="8"/>
-      <c r="AA25" s="8"/>
+      <c r="Y25" s="10"/>
+      <c r="Z25" s="12"/>
+      <c r="AA25" s="12"/>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="G30" t="s">
@@ -1677,26 +1677,59 @@
     </row>
   </sheetData>
   <mergeCells count="90">
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="Z25:AA25"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="Z23:AA23"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="T21:U21"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="X21:Y21"/>
+    <mergeCell ref="Z21:AA21"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="R25:S25"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="X16:Y16"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="T25:U25"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="X25:Y25"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="X24:Y24"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L4:M4"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="B25:C25"/>
@@ -1713,60 +1746,27 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
     <mergeCell ref="J25:K25"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="R25:S25"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="X16:Y16"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="X22:Y22"/>
-    <mergeCell ref="T25:U25"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="X25:Y25"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="R24:S24"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="X24:Y24"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="T21:U21"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="X21:Y21"/>
-    <mergeCell ref="Z21:AA21"/>
-    <mergeCell ref="Z25:AA25"/>
-    <mergeCell ref="Z22:AA22"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="Z23:AA23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1779,7 +1779,7 @@
   <dimension ref="A1:AA31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1804,14 +1804,14 @@
       <c r="A1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="L1" s="10" t="s">
+      <c r="E1" s="8"/>
+      <c r="L1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="10"/>
+      <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1820,10 +1820,10 @@
       <c r="B2">
         <v>9481</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="10"/>
+      <c r="E2" s="8"/>
       <c r="F2">
         <v>19.909876918386299</v>
       </c>
@@ -1834,10 +1834,10 @@
         <f>MAX(ROUND(1/F4,0),ROUND(F4,0))</f>
         <v>12</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="10"/>
+      <c r="M2" s="8"/>
       <c r="N2">
         <v>42.926477759350803</v>
       </c>
@@ -1854,12 +1854,12 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="8"/>
       <c r="F3">
         <v>17</v>
       </c>
@@ -1870,10 +1870,10 @@
         <f>$B4*F5/300000000*1000000000000000</f>
         <v>52300.882458116022</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="10"/>
+      <c r="M3" s="8"/>
       <c r="N3">
         <v>-29.5</v>
       </c>
@@ -1892,10 +1892,10 @@
       <c r="B4" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="10"/>
+      <c r="E4" s="8"/>
       <c r="F4">
         <f>SIN(RADIANS(F2+F3))/SIN(RADIANS(F2-F3))</f>
         <v>11.830135875287004</v>
@@ -1905,12 +1905,12 @@
       </c>
       <c r="I4" s="2">
         <f>MAX(ROUND(I3/$B7,0),1)</f>
-        <v>1308</v>
-      </c>
-      <c r="L4" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="10"/>
+      <c r="M4" s="8"/>
       <c r="N4">
         <f>SIN(RADIANS(N2+N3))/SIN(RADIANS(N2-N3))</f>
         <v>0.24356450463759297</v>
@@ -1920,7 +1920,7 @@
       </c>
       <c r="Q4" s="2">
         <f>MAX(ROUND(Q3/$B7,0),1)</f>
-        <v>235</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
@@ -1930,18 +1930,18 @@
       <c r="B5" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="E5" s="8"/>
       <c r="F5">
         <f>ABS((COS(RADIANS(F2-F3))-COS(RADIANS(F2+F3)))/SIN(RADIANS(F2-F3)))</f>
         <v>3.9225661843587014</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="10"/>
+      <c r="M5" s="8"/>
       <c r="N5">
         <f>ABS((COS(RADIANS(N2-N3))-COS(RADIANS(N2+N3)))/SIN(RADIANS(N2-N3)))</f>
         <v>0.70357494464450898</v>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="B7">
         <f>B3*40</f>
-        <v>40</v>
+        <v>800</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
@@ -1965,12 +1965,12 @@
       </c>
       <c r="B8">
         <f>B3/10</f>
-        <v>0.1</v>
-      </c>
-      <c r="D8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="10"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="1">
         <v>5.9999999999999997E-7</v>
       </c>
@@ -1988,15 +1988,15 @@
       </c>
       <c r="B9">
         <f>4/B8</f>
-        <v>40</v>
-      </c>
-      <c r="D9" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="10"/>
+      <c r="E9" s="8"/>
       <c r="F9" s="7" cm="1">
         <f t="array" ref="F9">IFERROR(LOOKUP(1,0/(25:25&lt;&gt;""),25:25),"")</f>
-        <v>0.98222648888888864</v>
+        <v>4.8816355555555566E-2</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
@@ -2005,15 +2005,15 @@
       </c>
       <c r="B10">
         <f>B9/B14</f>
-        <v>0.1</v>
-      </c>
-      <c r="D10" s="10" t="s">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="10"/>
+      <c r="E10" s="8"/>
       <c r="F10" s="7">
         <f>X25-J25</f>
-        <v>0.62504959999999976</v>
+        <v>3.1061333333333344E-2</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
@@ -2051,56 +2051,56 @@
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10" t="s">
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10" t="s">
+      <c r="E16" s="8"/>
+      <c r="F16" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10" t="s">
+      <c r="G16" s="8"/>
+      <c r="H16" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10" t="s">
+      <c r="I16" s="8"/>
+      <c r="J16" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10" t="s">
+      <c r="K16" s="8"/>
+      <c r="L16" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10" t="s">
+      <c r="M16" s="8"/>
+      <c r="N16" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10" t="s">
+      <c r="O16" s="8"/>
+      <c r="P16" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10" t="s">
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10" t="s">
+      <c r="S16" s="8"/>
+      <c r="T16" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10" t="s">
+      <c r="U16" s="8"/>
+      <c r="V16" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="W16" s="10"/>
-      <c r="X16" s="10" t="s">
+      <c r="W16" s="8"/>
+      <c r="X16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Y16" s="10"/>
-      <c r="Z16" s="10"/>
-      <c r="AA16" s="10"/>
+      <c r="Y16" s="8"/>
+      <c r="Z16" s="8"/>
+      <c r="AA16" s="8"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
@@ -2314,99 +2314,99 @@
       </c>
       <c r="B19" s="2">
         <f>B7</f>
-        <v>40</v>
+        <v>800</v>
       </c>
       <c r="C19" s="2">
         <f>B8</f>
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="D19" s="2">
         <f>B19*$I4</f>
-        <v>52320</v>
+        <v>52000</v>
       </c>
       <c r="E19" s="2">
         <f>D19/D23</f>
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="F19" s="2">
         <f>D19</f>
-        <v>52320</v>
+        <v>52000</v>
       </c>
       <c r="G19" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="H19" s="2">
         <f>F19</f>
-        <v>52320</v>
+        <v>52000</v>
       </c>
       <c r="I19" s="2">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="J19" s="2">
         <f>H19</f>
-        <v>52320</v>
+        <v>52000</v>
       </c>
       <c r="K19" s="2">
         <f>J19/J23</f>
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="L19" s="2">
         <f>J19/I4*Q4</f>
-        <v>9400</v>
+        <v>9600</v>
       </c>
       <c r="M19" s="2">
         <f>L19/L23</f>
-        <v>1.7966360856269112E-2</v>
+        <v>0.36923076923076925</v>
       </c>
       <c r="N19" s="2">
         <f>L19</f>
-        <v>9400</v>
+        <v>9600</v>
       </c>
       <c r="O19" s="2">
         <f>N19/N23</f>
-        <v>1.7966360856269112E-2</v>
+        <v>0.36923076923076925</v>
       </c>
       <c r="P19" s="2">
         <f t="shared" si="2"/>
-        <v>9400</v>
+        <v>9600</v>
       </c>
       <c r="Q19" s="2">
         <f t="shared" si="3"/>
-        <v>1.7966360856269112E-2</v>
+        <v>0.36923076923076925</v>
       </c>
       <c r="R19" s="2">
         <f t="shared" si="4"/>
-        <v>9400</v>
+        <v>9600</v>
       </c>
       <c r="S19" s="2">
         <f t="shared" si="5"/>
-        <v>1.7966360856269112E-2</v>
+        <v>0.36923076923076925</v>
       </c>
       <c r="T19" s="2">
         <f t="shared" si="6"/>
-        <v>9400</v>
+        <v>9600</v>
       </c>
       <c r="U19" s="2">
         <f t="shared" si="7"/>
-        <v>1.7966360856269112E-2</v>
+        <v>0.36923076923076925</v>
       </c>
       <c r="V19" s="2">
         <f t="shared" si="16"/>
-        <v>9400</v>
+        <v>9600</v>
       </c>
       <c r="W19" s="2">
         <f t="shared" si="8"/>
-        <v>1.7966360856269112E-2</v>
+        <v>0.36923076923076925</v>
       </c>
       <c r="X19" s="2">
         <f t="shared" si="9"/>
-        <v>9400</v>
+        <v>9600</v>
       </c>
       <c r="Y19" s="2">
         <f t="shared" si="10"/>
-        <v>1.7966360856269112E-2</v>
+        <v>0.36923076923076925</v>
       </c>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
@@ -2417,99 +2417,99 @@
       </c>
       <c r="B20" s="2">
         <f>B9*1000</f>
-        <v>40000</v>
+        <v>2000</v>
       </c>
       <c r="C20" s="2">
         <f>B10*1000</f>
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="D20" s="2">
         <f>$B20*$C19/E19</f>
-        <v>40000</v>
+        <v>2000</v>
       </c>
       <c r="E20" s="2">
         <f>$B19*$C20/D19</f>
-        <v>7.64525993883792E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="F20" s="2">
         <f>$B20*$C19/G19</f>
-        <v>40000</v>
+        <v>2000</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" ref="G20" si="17">$B19*$C20/F19</f>
-        <v>7.64525993883792E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="H20" s="2">
         <f>$B20*$C19/I19</f>
-        <v>40000</v>
+        <v>2000</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" ref="I20" si="18">$B19*$C20/H19</f>
-        <v>7.64525993883792E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="J20" s="2">
         <f>$B20*$C19/K19</f>
-        <v>40000</v>
+        <v>2000</v>
       </c>
       <c r="K20" s="2">
         <f>$B19*$C20/J19</f>
-        <v>7.64525993883792E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="L20" s="2">
         <f>$B20*$C19/M19</f>
-        <v>222638.29787234045</v>
+        <v>10833.333333333332</v>
       </c>
       <c r="M20" s="2">
         <f>$B19*$C20/L19</f>
-        <v>0.42553191489361702</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="N20" s="2">
         <f>$B20*$C19/O19</f>
-        <v>222638.29787234045</v>
+        <v>10833.333333333332</v>
       </c>
       <c r="O20" s="2">
         <f>$B19*$C20/N19</f>
-        <v>0.42553191489361702</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="P20" s="2">
         <f t="shared" ref="P20" si="19">$B20*$C19/Q19</f>
-        <v>222638.29787234045</v>
+        <v>10833.333333333332</v>
       </c>
       <c r="Q20" s="2">
         <f t="shared" ref="Q20" si="20">$B19*$C20/P19</f>
-        <v>0.42553191489361702</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="R20" s="2">
         <f t="shared" ref="R20" si="21">$B20*$C19/S19</f>
-        <v>222638.29787234045</v>
+        <v>10833.333333333332</v>
       </c>
       <c r="S20" s="2">
         <f t="shared" ref="S20" si="22">$B19*$C20/R19</f>
-        <v>0.42553191489361702</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="T20" s="2">
         <f t="shared" ref="T20" si="23">$B20*$C19/U19</f>
-        <v>222638.29787234045</v>
+        <v>10833.333333333332</v>
       </c>
       <c r="U20" s="2">
         <f t="shared" ref="U20" si="24">$B19*$C20/T19</f>
-        <v>0.42553191489361702</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="V20" s="2">
         <f t="shared" ref="V20" si="25">$B20*$C19/W19</f>
-        <v>222638.29787234045</v>
+        <v>10833.333333333332</v>
       </c>
       <c r="W20" s="2">
         <f t="shared" ref="W20" si="26">$B19*$C20/V19</f>
-        <v>0.42553191489361702</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="X20" s="2">
         <f t="shared" ref="X20" si="27">$B20*$C19/Y19</f>
-        <v>222638.29787234045</v>
+        <v>10833.333333333332</v>
       </c>
       <c r="Y20" s="2">
         <f t="shared" ref="Y20" si="28">$B19*$C20/X19</f>
-        <v>0.42553191489361702</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
@@ -2659,57 +2659,57 @@
       <c r="C23" s="9"/>
       <c r="D23" s="9">
         <f>B23*$I4</f>
-        <v>523200</v>
+        <v>26000</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="9">
         <f>D23</f>
-        <v>523200</v>
+        <v>26000</v>
       </c>
       <c r="G23" s="9"/>
       <c r="H23" s="9">
         <f t="shared" si="33"/>
-        <v>523200</v>
+        <v>26000</v>
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="9">
         <f t="shared" ref="J23" si="36">H23</f>
-        <v>523200</v>
+        <v>26000</v>
       </c>
       <c r="K23" s="9"/>
       <c r="L23" s="9">
         <f>J23</f>
-        <v>523200</v>
+        <v>26000</v>
       </c>
       <c r="M23" s="9"/>
       <c r="N23" s="9">
         <f>L23</f>
-        <v>523200</v>
+        <v>26000</v>
       </c>
       <c r="O23" s="9"/>
       <c r="P23" s="9">
         <f t="shared" ref="P23" si="37">N23</f>
-        <v>523200</v>
+        <v>26000</v>
       </c>
       <c r="Q23" s="9"/>
       <c r="R23" s="9">
         <f t="shared" si="29"/>
-        <v>523200</v>
+        <v>26000</v>
       </c>
       <c r="S23" s="9"/>
       <c r="T23" s="9">
         <f t="shared" si="30"/>
-        <v>523200</v>
+        <v>26000</v>
       </c>
       <c r="U23" s="9"/>
       <c r="V23" s="9">
         <f t="shared" ref="V23" si="38">T23</f>
-        <v>523200</v>
+        <v>26000</v>
       </c>
       <c r="W23" s="9"/>
       <c r="X23" s="9">
         <f t="shared" si="31"/>
-        <v>523200</v>
+        <v>26000</v>
       </c>
       <c r="Y23" s="9"/>
       <c r="Z23" s="9"/>
@@ -2719,66 +2719,66 @@
       <c r="A24" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="11">
         <f>B21*B22*B23</f>
         <v>819200</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12">
+      <c r="C24" s="11"/>
+      <c r="D24" s="11">
         <f t="shared" ref="D24" si="39">D21*D22*D23</f>
-        <v>12858163200</v>
-      </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12">
+        <v>638976000</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11">
         <f t="shared" ref="F24" si="40">F21*F22*F23</f>
-        <v>12858163200</v>
-      </c>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12">
+        <v>638976000</v>
+      </c>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11">
         <f t="shared" ref="H24" si="41">H21*H22*H23</f>
-        <v>12858163200</v>
-      </c>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12">
+        <v>638976000</v>
+      </c>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11">
         <f t="shared" ref="J24" si="42">J21*J22*J23</f>
-        <v>12858163200</v>
-      </c>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12">
+        <v>638976000</v>
+      </c>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11">
         <f t="shared" ref="L24" si="43">L21*L22*L23</f>
-        <v>12858163200</v>
-      </c>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12">
+        <v>638976000</v>
+      </c>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11">
         <f t="shared" ref="N24" si="44">N21*N22*N23</f>
-        <v>12858163200</v>
-      </c>
-      <c r="O24" s="12"/>
-      <c r="P24" s="12">
+        <v>638976000</v>
+      </c>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11">
         <f t="shared" ref="P24" si="45">P21*P22*P23</f>
-        <v>12858163200</v>
-      </c>
-      <c r="Q24" s="12"/>
-      <c r="R24" s="12">
+        <v>638976000</v>
+      </c>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11">
         <f t="shared" ref="R24" si="46">R21*R22*R23</f>
-        <v>12858163200</v>
-      </c>
-      <c r="S24" s="12"/>
-      <c r="T24" s="12">
+        <v>638976000</v>
+      </c>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11">
         <f t="shared" ref="T24" si="47">T21*T22*T23</f>
-        <v>12858163200</v>
-      </c>
-      <c r="U24" s="12"/>
-      <c r="V24" s="12">
+        <v>638976000</v>
+      </c>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11">
         <f t="shared" ref="V24" si="48">V21*V22*V23</f>
-        <v>12858163200</v>
-      </c>
-      <c r="W24" s="12"/>
-      <c r="X24" s="12">
+        <v>638976000</v>
+      </c>
+      <c r="W24" s="11"/>
+      <c r="X24" s="11">
         <f t="shared" ref="X24" si="49">X21*X22*X23</f>
-        <v>12858163200</v>
-      </c>
-      <c r="Y24" s="12"/>
+        <v>638976000</v>
+      </c>
+      <c r="Y24" s="11"/>
       <c r="Z24" s="5"/>
       <c r="AA24" s="5"/>
     </row>
@@ -2786,68 +2786,68 @@
       <c r="A25" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="10">
         <f>B24*$F8/86400</f>
         <v>5.6888888888888884E-6</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11">
+      <c r="C25" s="10"/>
+      <c r="D25" s="10">
         <f>D24*$F8/86400+B25</f>
-        <v>8.9298488888888874E-2</v>
-      </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11">
+        <v>4.443022222222222E-3</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10">
         <f t="shared" ref="F25" si="50">F24*$F8/86400+D25</f>
-        <v>0.17859128888888887</v>
-      </c>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11">
+        <v>8.8803555555555559E-3</v>
+      </c>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10">
         <f t="shared" ref="H25" si="51">H24*$F8/86400+F25</f>
-        <v>0.26788408888888887</v>
-      </c>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11">
+        <v>1.3317688888888889E-2</v>
+      </c>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10">
         <f t="shared" ref="J25" si="52">J24*$F8/86400+H25</f>
-        <v>0.35717688888888888</v>
-      </c>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11">
+        <v>1.7755022222222222E-2</v>
+      </c>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10">
         <f t="shared" ref="L25" si="53">L24*$F8/86400+J25</f>
-        <v>0.44646968888888888</v>
-      </c>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11">
+        <v>2.2192355555555557E-2</v>
+      </c>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10">
         <f t="shared" ref="N25" si="54">N24*$F8/86400+L25</f>
-        <v>0.53576248888888889</v>
-      </c>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11">
+        <v>2.6629688888888892E-2</v>
+      </c>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10">
         <f t="shared" ref="P25" si="55">P24*$F8/86400+N25</f>
-        <v>0.62505528888888884</v>
-      </c>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11">
+        <v>3.1067022222222226E-2</v>
+      </c>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10">
         <f t="shared" ref="R25" si="56">R24*$F8/86400+P25</f>
-        <v>0.71434808888888879</v>
-      </c>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11">
+        <v>3.5504355555555561E-2</v>
+      </c>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10">
         <f t="shared" ref="T25" si="57">T24*$F8/86400+R25</f>
-        <v>0.80364088888888874</v>
-      </c>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11">
+        <v>3.9941688888888896E-2</v>
+      </c>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10">
         <f t="shared" ref="V25" si="58">V24*$F8/86400+T25</f>
-        <v>0.89293368888888869</v>
-      </c>
-      <c r="W25" s="11"/>
-      <c r="X25" s="11">
+        <v>4.4379022222222231E-2</v>
+      </c>
+      <c r="W25" s="10"/>
+      <c r="X25" s="10">
         <f t="shared" ref="X25" si="59">X24*$F8/86400+V25</f>
-        <v>0.98222648888888864</v>
-      </c>
-      <c r="Y25" s="11"/>
-      <c r="Z25" s="8"/>
-      <c r="AA25" s="8"/>
+        <v>4.8816355555555566E-2</v>
+      </c>
+      <c r="Y25" s="10"/>
+      <c r="Z25" s="12"/>
+      <c r="AA25" s="12"/>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="G30" t="s">
@@ -2859,11 +2859,75 @@
     </row>
   </sheetData>
   <mergeCells count="90">
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="X16:Y16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="T21:U21"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="X21:Y21"/>
+    <mergeCell ref="Z21:AA21"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="L22:M22"/>
     <mergeCell ref="X23:Y23"/>
     <mergeCell ref="Z23:AA23"/>
     <mergeCell ref="L25:M25"/>
@@ -2880,75 +2944,11 @@
     <mergeCell ref="Z25:AA25"/>
     <mergeCell ref="X24:Y24"/>
     <mergeCell ref="T24:U24"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="T21:U21"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="X21:Y21"/>
-    <mergeCell ref="Z21:AA21"/>
-    <mergeCell ref="X22:Y22"/>
-    <mergeCell ref="Z22:AA22"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="X16:Y16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2986,14 +2986,14 @@
       <c r="A1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="L1" s="10" t="s">
+      <c r="E1" s="8"/>
+      <c r="L1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="10"/>
+      <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -3002,10 +3002,10 @@
       <c r="B2">
         <v>9481</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="10"/>
+      <c r="E2" s="8"/>
       <c r="F2">
         <v>19.909876918386299</v>
       </c>
@@ -3016,10 +3016,10 @@
         <f>MAX(ROUND(1/F4,0),ROUND(F4,0))</f>
         <v>12</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="10"/>
+      <c r="M2" s="8"/>
       <c r="N2">
         <v>42.926477759350803</v>
       </c>
@@ -3038,10 +3038,10 @@
       <c r="B3">
         <v>20</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="8"/>
       <c r="F3">
         <v>17</v>
       </c>
@@ -3052,10 +3052,10 @@
         <f>$B4*F5/300000000*1000000000000000</f>
         <v>52300.882458116022</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="10"/>
+      <c r="M3" s="8"/>
       <c r="N3">
         <v>-29.5</v>
       </c>
@@ -3074,10 +3074,10 @@
       <c r="B4" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="10"/>
+      <c r="E4" s="8"/>
       <c r="F4">
         <f>SIN(RADIANS(F2+F3))/SIN(RADIANS(F2-F3))</f>
         <v>11.830135875287004</v>
@@ -3089,10 +3089,10 @@
         <f>MAX(ROUND(I3/$B7,0),1)</f>
         <v>65</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="10"/>
+      <c r="M4" s="8"/>
       <c r="N4">
         <f>SIN(RADIANS(N2+N3))/SIN(RADIANS(N2-N3))</f>
         <v>0.24356450463759297</v>
@@ -3112,18 +3112,18 @@
       <c r="B5" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="E5" s="8"/>
       <c r="F5">
         <f>ABS((COS(RADIANS(F2-F3))-COS(RADIANS(F2+F3)))/SIN(RADIANS(F2-F3)))</f>
         <v>3.9225661843587014</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="10"/>
+      <c r="M5" s="8"/>
       <c r="N5">
         <f>ABS((COS(RADIANS(N2-N3))-COS(RADIANS(N2+N3)))/SIN(RADIANS(N2-N3)))</f>
         <v>0.70357494464450898</v>
@@ -3149,10 +3149,10 @@
         <f>B3/10</f>
         <v>2</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="10"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="1">
         <v>5.9999999999999997E-7</v>
       </c>
@@ -3172,10 +3172,10 @@
         <f>4/B8</f>
         <v>2</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="10"/>
+      <c r="E9" s="8"/>
       <c r="F9" s="7" cm="1">
         <f t="array" ref="F9">IFERROR(LOOKUP(1,0/(25:25&lt;&gt;""),25:25),"")</f>
         <v>9.9851377777777778E-2</v>
@@ -3189,10 +3189,10 @@
         <f>B9/B14</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="10"/>
+      <c r="E10" s="8"/>
       <c r="F10" s="7">
         <f>X25-J25</f>
         <v>8.1919999999999993E-2</v>
@@ -3233,56 +3233,56 @@
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10" t="s">
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10" t="s">
+      <c r="E16" s="8"/>
+      <c r="F16" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10" t="s">
+      <c r="G16" s="8"/>
+      <c r="H16" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10" t="s">
+      <c r="I16" s="8"/>
+      <c r="J16" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10" t="s">
+      <c r="K16" s="8"/>
+      <c r="L16" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10" t="s">
+      <c r="M16" s="8"/>
+      <c r="N16" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10" t="s">
+      <c r="O16" s="8"/>
+      <c r="P16" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10" t="s">
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10" t="s">
+      <c r="S16" s="8"/>
+      <c r="T16" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10" t="s">
+      <c r="U16" s="8"/>
+      <c r="V16" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="W16" s="10"/>
-      <c r="X16" s="10" t="s">
+      <c r="W16" s="8"/>
+      <c r="X16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Y16" s="10"/>
-      <c r="Z16" s="10"/>
-      <c r="AA16" s="10"/>
+      <c r="Y16" s="8"/>
+      <c r="Z16" s="8"/>
+      <c r="AA16" s="8"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
@@ -3901,66 +3901,66 @@
       <c r="A24" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="11">
         <f>B21*B22*B23</f>
         <v>26214400</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12">
+      <c r="C24" s="11"/>
+      <c r="D24" s="11">
         <f t="shared" ref="D24" si="39">D21*D22*D23</f>
         <v>638976000</v>
       </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12">
+      <c r="E24" s="11"/>
+      <c r="F24" s="11">
         <f t="shared" ref="F24" si="40">F21*F22*F23</f>
         <v>638976000</v>
       </c>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12">
+      <c r="G24" s="11"/>
+      <c r="H24" s="11">
         <f t="shared" ref="H24" si="41">H21*H22*H23</f>
         <v>638976000</v>
       </c>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12">
+      <c r="I24" s="11"/>
+      <c r="J24" s="11">
         <f t="shared" ref="J24" si="42">J21*J22*J23</f>
         <v>638976000</v>
       </c>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12">
+      <c r="K24" s="11"/>
+      <c r="L24" s="11">
         <f t="shared" ref="L24" si="43">L21*L22*L23</f>
         <v>117964800</v>
       </c>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12">
+      <c r="M24" s="11"/>
+      <c r="N24" s="11">
         <f t="shared" ref="N24" si="44">N21*N22*N23</f>
         <v>117964800</v>
       </c>
-      <c r="O24" s="12"/>
-      <c r="P24" s="12">
+      <c r="O24" s="11"/>
+      <c r="P24" s="11">
         <f t="shared" ref="P24" si="45">P21*P22*P23</f>
         <v>3774873600</v>
       </c>
-      <c r="Q24" s="12"/>
-      <c r="R24" s="12">
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11">
         <f t="shared" ref="R24" si="46">R21*R22*R23</f>
         <v>3774873600</v>
       </c>
-      <c r="S24" s="12"/>
-      <c r="T24" s="12">
+      <c r="S24" s="11"/>
+      <c r="T24" s="11">
         <f t="shared" ref="T24" si="47">T21*T22*T23</f>
         <v>3774873600</v>
       </c>
-      <c r="U24" s="12"/>
-      <c r="V24" s="12">
+      <c r="U24" s="11"/>
+      <c r="V24" s="11">
         <f t="shared" ref="V24" si="48">V21*V22*V23</f>
         <v>117964800</v>
       </c>
-      <c r="W24" s="12"/>
-      <c r="X24" s="12">
+      <c r="W24" s="11"/>
+      <c r="X24" s="11">
         <f t="shared" ref="X24" si="49">X21*X22*X23</f>
         <v>117964800</v>
       </c>
-      <c r="Y24" s="12"/>
+      <c r="Y24" s="11"/>
       <c r="Z24" s="5"/>
       <c r="AA24" s="5"/>
     </row>
@@ -3968,68 +3968,68 @@
       <c r="A25" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="10">
         <f>B24*$F8/86400</f>
         <v>1.8204444444444443E-4</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11">
+      <c r="C25" s="10"/>
+      <c r="D25" s="10">
         <f>D24*$F8/86400+B25</f>
         <v>4.6193777777777771E-3</v>
       </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11">
+      <c r="E25" s="10"/>
+      <c r="F25" s="10">
         <f t="shared" ref="F25" si="50">F24*$F8/86400+D25</f>
         <v>9.0567111111111102E-3</v>
       </c>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11">
+      <c r="G25" s="10"/>
+      <c r="H25" s="10">
         <f t="shared" ref="H25" si="51">H24*$F8/86400+F25</f>
         <v>1.3494044444444443E-2</v>
       </c>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11">
+      <c r="I25" s="10"/>
+      <c r="J25" s="10">
         <f t="shared" ref="J25" si="52">J24*$F8/86400+H25</f>
         <v>1.7931377777777778E-2</v>
       </c>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11">
+      <c r="K25" s="10"/>
+      <c r="L25" s="10">
         <f t="shared" ref="L25" si="53">L24*$F8/86400+J25</f>
         <v>1.8750577777777777E-2</v>
       </c>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11">
+      <c r="M25" s="10"/>
+      <c r="N25" s="10">
         <f t="shared" ref="N25" si="54">N24*$F8/86400+L25</f>
         <v>1.9569777777777776E-2</v>
       </c>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11">
+      <c r="O25" s="10"/>
+      <c r="P25" s="10">
         <f t="shared" ref="P25" si="55">P24*$F8/86400+N25</f>
         <v>4.5784177777777775E-2</v>
       </c>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11">
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10">
         <f t="shared" ref="R25" si="56">R24*$F8/86400+P25</f>
         <v>7.1998577777777767E-2</v>
       </c>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11">
+      <c r="S25" s="10"/>
+      <c r="T25" s="10">
         <f t="shared" ref="T25" si="57">T24*$F8/86400+R25</f>
         <v>9.8212977777777766E-2</v>
       </c>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11">
+      <c r="U25" s="10"/>
+      <c r="V25" s="10">
         <f t="shared" ref="V25" si="58">V24*$F8/86400+T25</f>
         <v>9.9032177777777772E-2</v>
       </c>
-      <c r="W25" s="11"/>
-      <c r="X25" s="11">
+      <c r="W25" s="10"/>
+      <c r="X25" s="10">
         <f t="shared" ref="X25" si="59">X24*$F8/86400+V25</f>
         <v>9.9851377777777778E-2</v>
       </c>
-      <c r="Y25" s="11"/>
-      <c r="Z25" s="8"/>
-      <c r="AA25" s="8"/>
+      <c r="Y25" s="10"/>
+      <c r="Z25" s="12"/>
+      <c r="AA25" s="12"/>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="G30" t="s">
@@ -4041,44 +4041,42 @@
     </row>
   </sheetData>
   <mergeCells count="90">
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="Z21:AA21"/>
-    <mergeCell ref="Z22:AA22"/>
-    <mergeCell ref="Z23:AA23"/>
-    <mergeCell ref="Z25:AA25"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="X16:Y16"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="X24:Y24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="R25:S25"/>
+    <mergeCell ref="T25:U25"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="X25:Y25"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
     <mergeCell ref="T21:U21"/>
     <mergeCell ref="V21:W21"/>
     <mergeCell ref="X21:Y21"/>
@@ -4095,42 +4093,44 @@
     <mergeCell ref="V22:W22"/>
     <mergeCell ref="X22:Y22"/>
     <mergeCell ref="L21:M21"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="R24:S24"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="X24:Y24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="R25:S25"/>
-    <mergeCell ref="T25:U25"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="X25:Y25"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="X16:Y16"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="Z21:AA21"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="Z23:AA23"/>
+    <mergeCell ref="Z25:AA25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update: added beam diagnostics for parameter scans. f1_scan submitted at NERSC
</commit_message>
<xml_diff>
--- a/Sampling_Resolution_Calculator.xlsx
+++ b/Sampling_Resolution_Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nanw0\GoogleDrive\SLAC\SLAC-Diling\11. 21 Winter\DXS optics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEB7962-69E2-4683-B5E6-09B818838D92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC53D04A-EA9B-4E04-94FD-ABEC322E7CEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="555" windowWidth="25200" windowHeight="20370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="285" windowWidth="38640" windowHeight="20865" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HHLM" sheetId="10" r:id="rId1"/>
@@ -1630,7 +1630,7 @@
   <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1643,14 +1643,14 @@
     <col min="6" max="6" width="12.75" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.75" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1694,7 +1694,7 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>25</v>
@@ -1708,7 +1708,7 @@
       </c>
       <c r="I3" s="2">
         <f>$B4*F5/300000000*1000000000000000</f>
-        <v>9380.9992619267869</v>
+        <v>11726.249077408484</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -1716,7 +1716,8 @@
         <v>9</v>
       </c>
       <c r="B4" s="1">
-        <v>4.0000000000000001E-3</v>
+        <f>0.005</f>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>21</v>
@@ -1730,12 +1731,12 @@
         <v>19</v>
       </c>
       <c r="I4" s="2">
-        <f>MAX(ROUND(I3/$B7,0),1)</f>
-        <v>2</v>
+        <f>MAX(ROUND(2*I3/$B7,0),1)</f>
+        <v>1</v>
       </c>
       <c r="J4">
         <f>I3/$B7</f>
-        <v>2.3452498154816968</v>
+        <v>0.36644528366901513</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -1743,7 +1744,8 @@
         <v>10</v>
       </c>
       <c r="B5" s="1">
-        <v>4.0000000000000001E-3</v>
+        <f>0.005</f>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>22</v>
@@ -1763,7 +1765,7 @@
       </c>
       <c r="B7">
         <f>B8*B14</f>
-        <v>4000</v>
+        <v>32000</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
@@ -1772,7 +1774,7 @@
       </c>
       <c r="B8">
         <f>B3/10</f>
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>20</v>
@@ -1786,7 +1788,7 @@
       </c>
       <c r="I8" s="9">
         <f>22122874/1024/1024/3072/8/26000*MAX(25:25)</f>
-        <v>13.848954577323717</v>
+        <v>6.9244772886618584</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
@@ -1795,7 +1797,7 @@
       </c>
       <c r="B9">
         <f>4/B8</f>
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>52</v>
@@ -1803,7 +1805,7 @@
       <c r="E9" s="16"/>
       <c r="F9" s="7">
         <f>SUM(28:28)/86400</f>
-        <v>1.3293055555555556E-3</v>
+        <v>1.2159490740740739E-3</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
@@ -1811,8 +1813,8 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <f>MIN(B9/400,0.001)</f>
-        <v>1E-3</v>
+        <f>MIN(B9/800,0.001)</f>
+        <v>1.25E-4</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>53</v>
@@ -1820,7 +1822,7 @@
       <c r="E10" s="16"/>
       <c r="F10" s="7">
         <f>SUM(31:31)-F9</f>
-        <v>1.2573466435185187E-2</v>
+        <v>1.1049305555555555E-2</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
@@ -1830,7 +1832,7 @@
       <c r="E11" s="16"/>
       <c r="F11" s="10">
         <f>SUM(31:31)</f>
-        <v>1.3902771990740742E-2</v>
+        <v>1.2265254629629629E-2</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
@@ -1838,7 +1840,7 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>512</v>
+        <v>1024</v>
       </c>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
@@ -1858,7 +1860,7 @@
       </c>
       <c r="B14">
         <f>B9/B10</f>
-        <v>400</v>
+        <v>800</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
@@ -1906,7 +1908,7 @@
       </c>
       <c r="B17" s="2">
         <f>B22*C17</f>
-        <v>4008.96</v>
+        <v>8017.92</v>
       </c>
       <c r="C17" s="2">
         <f>7.83</f>
@@ -1914,7 +1916,7 @@
       </c>
       <c r="D17" s="2">
         <f>D22*E17</f>
-        <v>4008.96</v>
+        <v>8017.92</v>
       </c>
       <c r="E17" s="2">
         <f>C17</f>
@@ -1977,67 +1979,67 @@
       </c>
       <c r="B18" s="2">
         <f>B5*1000000</f>
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="C18" s="2">
         <f>B18/B23</f>
-        <v>500</v>
+        <v>625</v>
       </c>
       <c r="D18" s="2">
         <f>B18</f>
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="E18" s="2">
         <f>D18/D23</f>
-        <v>500</v>
+        <v>625</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" ref="F18" si="1">D18</f>
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="G18" s="2">
         <f>F18/F23</f>
-        <v>500</v>
+        <v>625</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" ref="H18" si="2">F18</f>
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="I18" s="2">
         <f>H18/H23</f>
-        <v>500</v>
+        <v>625</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" ref="J18" si="3">H18</f>
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="K18" s="2">
         <f>J18/J23</f>
-        <v>500</v>
+        <v>625</v>
       </c>
       <c r="L18" s="2">
         <f t="shared" ref="L18" si="4">J18</f>
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="M18" s="2">
         <f>L18/L23</f>
-        <v>500</v>
+        <v>625</v>
       </c>
       <c r="N18" s="2">
         <f t="shared" ref="N18" si="5">L18</f>
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="O18" s="2">
         <f>N18/N23</f>
-        <v>500</v>
+        <v>625</v>
       </c>
       <c r="P18" s="2">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="Q18" s="2">
         <f>P18/P23</f>
-        <v>500</v>
+        <v>625</v>
       </c>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
@@ -2048,67 +2050,67 @@
       </c>
       <c r="B19" s="2">
         <f>B7</f>
-        <v>4000</v>
+        <v>32000</v>
       </c>
       <c r="C19" s="2">
         <f>B8</f>
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D19" s="2">
         <f>E19*D24</f>
-        <v>4000</v>
+        <v>32000</v>
       </c>
       <c r="E19" s="2">
         <f>C19</f>
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="F19" s="2">
         <f>G19*F24</f>
-        <v>8000</v>
+        <v>32000</v>
       </c>
       <c r="G19" s="2">
         <f>E19</f>
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="H19" s="2">
         <f>I19*H24</f>
-        <v>8000</v>
+        <v>32000</v>
       </c>
       <c r="I19" s="2">
         <f>G19</f>
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="J19" s="2">
         <f>K19*J24</f>
-        <v>8000</v>
+        <v>32000</v>
       </c>
       <c r="K19" s="2">
         <f>I19</f>
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="L19" s="2">
         <f>M19*L24</f>
-        <v>8000</v>
+        <v>32000</v>
       </c>
       <c r="M19" s="2">
         <f>K19</f>
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="N19" s="2">
         <f>O19*N24</f>
-        <v>8000</v>
+        <v>32000</v>
       </c>
       <c r="O19" s="2">
         <f>M19</f>
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="P19" s="2">
         <f>Q19*P24</f>
-        <v>16000</v>
+        <v>32000</v>
       </c>
       <c r="Q19" s="2">
         <f>O19</f>
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
@@ -2119,67 +2121,67 @@
       </c>
       <c r="B20" s="2">
         <f>B9*1000</f>
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="C20" s="2">
         <f>B10*1000</f>
-        <v>1</v>
+        <v>0.125</v>
       </c>
       <c r="D20" s="2">
         <f>$B20*$C19/E19</f>
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="E20" s="2">
         <f>$B19*$C20/D19</f>
-        <v>1</v>
+        <v>0.125</v>
       </c>
       <c r="F20" s="2">
         <f>$B20*$C19/G19</f>
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="G20" s="2">
         <f>$B19*$C20/F19</f>
-        <v>0.5</v>
+        <v>0.125</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" ref="H20" si="6">$B20*$C19/I19</f>
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" ref="I20" si="7">$B19*$C20/H19</f>
-        <v>0.5</v>
+        <v>0.125</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" ref="J20" si="8">$B20*$C19/K19</f>
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="K20" s="2">
         <f t="shared" ref="K20" si="9">$B19*$C20/J19</f>
-        <v>0.5</v>
+        <v>0.125</v>
       </c>
       <c r="L20" s="2">
         <f t="shared" ref="L20" si="10">$B20*$C19/M19</f>
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="M20" s="2">
         <f t="shared" ref="M20" si="11">$B19*$C20/L19</f>
-        <v>0.5</v>
+        <v>0.125</v>
       </c>
       <c r="N20" s="2">
         <f t="shared" ref="N20" si="12">$B20*$C19/O19</f>
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="O20" s="2">
         <f t="shared" ref="O20" si="13">$B19*$C20/N19</f>
-        <v>0.5</v>
+        <v>0.125</v>
       </c>
       <c r="P20" s="2">
         <f t="shared" ref="P20" si="14">$B20*$C19/Q19</f>
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="Q20" s="2">
         <f t="shared" ref="Q20" si="15">$B19*$C20/P19</f>
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
@@ -2229,16 +2231,16 @@
       </c>
       <c r="B22" s="18">
         <f>B12</f>
-        <v>512</v>
+        <v>1024</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="18">
         <f>B22</f>
-        <v>512</v>
+        <v>1024</v>
       </c>
       <c r="E22" s="18"/>
       <c r="F22" s="18">
-        <f>D22*I2*4*4</f>
+        <f>D22*I2*8</f>
         <v>32768</v>
       </c>
       <c r="G22" s="18"/>
@@ -2323,12 +2325,12 @@
       </c>
       <c r="B24" s="18">
         <f>B14</f>
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="18">
         <f t="shared" si="19"/>
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="E24" s="18"/>
       <c r="F24" s="18">
@@ -2357,8 +2359,8 @@
       </c>
       <c r="O24" s="18"/>
       <c r="P24" s="18">
-        <f>N24*2</f>
-        <v>1600</v>
+        <f>N24</f>
+        <v>800</v>
       </c>
       <c r="Q24" s="18"/>
       <c r="R24" s="18"/>
@@ -2370,12 +2372,12 @@
       </c>
       <c r="B25" s="19">
         <f>B22*B23*B24</f>
-        <v>1638400</v>
+        <v>6553600</v>
       </c>
       <c r="C25" s="19"/>
       <c r="D25" s="19">
         <f>D22*D23*D24</f>
-        <v>1638400</v>
+        <v>6553600</v>
       </c>
       <c r="E25" s="19"/>
       <c r="F25" s="19">
@@ -2405,7 +2407,7 @@
       <c r="O25" s="19"/>
       <c r="P25" s="19">
         <f t="shared" ref="P25" si="28">P22*P23*P24</f>
-        <v>419430400</v>
+        <v>209715200</v>
       </c>
       <c r="Q25" s="19"/>
       <c r="R25" s="13"/>
@@ -2496,12 +2498,12 @@
       </c>
       <c r="B28" s="17">
         <f>B26/512/8/1600*B$25</f>
-        <v>1.6840000000000002</v>
+        <v>6.7360000000000007</v>
       </c>
       <c r="C28" s="17"/>
       <c r="D28" s="17">
         <f>D26/512/8/1600*D$25</f>
-        <v>0.28799999999999998</v>
+        <v>1.1519999999999999</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="17">
@@ -2531,7 +2533,7 @@
       <c r="O28" s="17"/>
       <c r="P28" s="17">
         <f t="shared" ref="P28" si="33">P26/4096/8/3200*P$25</f>
-        <v>31.42</v>
+        <v>15.71</v>
       </c>
       <c r="Q28" s="17"/>
     </row>
@@ -2541,12 +2543,12 @@
       </c>
       <c r="B29" s="17">
         <f>B27/512/8/1600*B$25</f>
-        <v>3.8224999999999993</v>
+        <v>15.289999999999997</v>
       </c>
       <c r="C29" s="17"/>
       <c r="D29" s="17">
         <f>D27/512/8/1600*D$25</f>
-        <v>5.915</v>
+        <v>23.66</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="17">
@@ -2576,7 +2578,7 @@
       <c r="O29" s="17"/>
       <c r="P29" s="17">
         <f t="shared" ref="P29" si="38">P27/4096/8/3200*P$25</f>
-        <v>321.8</v>
+        <v>160.9</v>
       </c>
       <c r="Q29" s="17"/>
     </row>
@@ -2623,12 +2625,12 @@
       </c>
       <c r="B31" s="21">
         <f>(B28+B29*B30)/86400</f>
-        <v>6.3732638888888875E-5</v>
+        <v>2.549305555555555E-4</v>
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="21">
         <f t="shared" ref="D31:F31" si="39">(D28+D29*D30)/86400</f>
-        <v>7.1793981481481492E-5</v>
+        <v>2.8717592592592597E-4</v>
       </c>
       <c r="E31" s="21"/>
       <c r="F31" s="21">
@@ -2658,7 +2660,7 @@
       <c r="O31" s="21"/>
       <c r="P31" s="21">
         <f t="shared" si="40"/>
-        <v>4.0881944444444446E-3</v>
+        <v>2.0440972222222223E-3</v>
       </c>
       <c r="Q31" s="21"/>
       <c r="R31" s="17"/>
@@ -2684,6 +2686,15 @@
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="F29:G29"/>
     <mergeCell ref="L27:M27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
     <mergeCell ref="R31:S31"/>
     <mergeCell ref="H30:I30"/>
     <mergeCell ref="J30:K30"/>
@@ -2701,18 +2712,9 @@
     <mergeCell ref="P30:Q30"/>
     <mergeCell ref="N31:O31"/>
     <mergeCell ref="P31:Q31"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
     <mergeCell ref="H28:I28"/>
     <mergeCell ref="J28:K28"/>
     <mergeCell ref="L28:M28"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="F26:G26"/>

</xml_diff>

<commit_message>
Update: Strehl Ratio for crystal thermal deformation
</commit_message>
<xml_diff>
--- a/Sampling_Resolution_Calculator.xlsx
+++ b/Sampling_Resolution_Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nanw0\GoogleDrive\SLAC\SLAC-Diling\11. 21 Winter\DXS optics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC53D04A-EA9B-4E04-94FD-ABEC322E7CEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DC94C7-E1EC-4D96-8598-30183B5B3C96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="285" windowWidth="38640" windowHeight="20865" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5070" yWindow="5070" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HHLM" sheetId="10" r:id="rId1"/>
@@ -482,22 +482,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -808,10 +808,10 @@
       <c r="A1" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="16"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -820,10 +820,10 @@
       <c r="B2">
         <v>9481</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="16"/>
+      <c r="E2" s="21"/>
       <c r="F2">
         <v>19.909876918386299</v>
       </c>
@@ -846,10 +846,10 @@
       <c r="B3">
         <v>20</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="16"/>
+      <c r="E3" s="21"/>
       <c r="F3">
         <v>17</v>
       </c>
@@ -868,10 +868,10 @@
       <c r="B4" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="16"/>
+      <c r="E4" s="21"/>
       <c r="F4">
         <f>SIN(RADIANS(F2+F3))/SIN(RADIANS(F2-F3))</f>
         <v>11.830135875287004</v>
@@ -895,10 +895,10 @@
       <c r="B5" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="16"/>
+      <c r="E5" s="21"/>
       <c r="F5">
         <f>ABS((COS(RADIANS(F2-F3))-COS(RADIANS(F2+F3)))/SIN(RADIANS(F2-F3)))</f>
         <v>3.9225661843587014</v>
@@ -924,10 +924,10 @@
         <f>B3/10</f>
         <v>2</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="16"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="1">
         <v>5.9999999999999997E-7</v>
       </c>
@@ -947,10 +947,10 @@
         <f>4/B8</f>
         <v>2</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="16"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="7">
         <f>SUM(28:28)/86400</f>
         <v>6.0394444444444445E-3</v>
@@ -964,20 +964,20 @@
         <f>MIN(B9/400,0.001)</f>
         <v>1E-3</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="16"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="7">
         <f>SUM(31:31)-F9</f>
         <v>4.7264062499999995E-2</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="16"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="10">
         <f>SUM(31:31)</f>
         <v>5.330350694444444E-2</v>
@@ -1015,26 +1015,26 @@
       <c r="A16" t="s">
         <v>89</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16" t="s">
+      <c r="C16" s="21"/>
+      <c r="D16" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16" t="s">
+      <c r="E16" s="21"/>
+      <c r="F16" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16" t="s">
+      <c r="G16" s="21"/>
+      <c r="H16" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16" t="s">
+      <c r="I16" s="21"/>
+      <c r="J16" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="K16" s="16"/>
+      <c r="K16" s="21"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
@@ -1228,317 +1228,317 @@
       <c r="A21" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="17">
+      <c r="B21" s="18">
         <v>722.7</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17">
+      <c r="C21" s="18"/>
+      <c r="D21" s="18">
         <f>B21*J2</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17">
+      <c r="E21" s="18"/>
+      <c r="F21" s="18">
         <f>D21</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17">
+      <c r="G21" s="18"/>
+      <c r="H21" s="18">
         <f>F21</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17">
+      <c r="I21" s="18"/>
+      <c r="J21" s="18">
         <f>H21/J2</f>
         <v>722.7</v>
       </c>
-      <c r="K21" s="17"/>
+      <c r="K21" s="18"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="17">
         <f>B12</f>
         <v>512</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18">
+      <c r="C22" s="17"/>
+      <c r="D22" s="17">
         <f>B22*I2</f>
         <v>6144</v>
       </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18">
+      <c r="E22" s="17"/>
+      <c r="F22" s="17">
         <f>D22</f>
         <v>6144</v>
       </c>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18">
+      <c r="G22" s="17"/>
+      <c r="H22" s="17">
         <f>F22</f>
         <v>6144</v>
       </c>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18">
+      <c r="I22" s="17"/>
+      <c r="J22" s="17">
         <f t="shared" ref="J22:J24" si="7">H22</f>
         <v>6144</v>
       </c>
-      <c r="K22" s="18"/>
+      <c r="K22" s="17"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="17">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18">
+      <c r="C23" s="17"/>
+      <c r="D23" s="17">
         <f t="shared" ref="D23" si="8">B23</f>
         <v>8</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18">
+      <c r="E23" s="17"/>
+      <c r="F23" s="17">
         <f t="shared" ref="F23" si="9">D23</f>
         <v>8</v>
       </c>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18">
+      <c r="G23" s="17"/>
+      <c r="H23" s="17">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18">
+      <c r="I23" s="17"/>
+      <c r="J23" s="17">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="K23" s="18"/>
+      <c r="K23" s="17"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="17">
         <f>B14</f>
         <v>2000</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18">
+      <c r="C24" s="17"/>
+      <c r="D24" s="17">
         <f>B24*I4</f>
         <v>26000</v>
       </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18">
+      <c r="E24" s="17"/>
+      <c r="F24" s="17">
         <f>D24</f>
         <v>26000</v>
       </c>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18">
+      <c r="G24" s="17"/>
+      <c r="H24" s="17">
         <f t="shared" ref="H24" si="10">F24</f>
         <v>26000</v>
       </c>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18">
+      <c r="I24" s="17"/>
+      <c r="J24" s="17">
         <f t="shared" si="7"/>
         <v>26000</v>
       </c>
-      <c r="K24" s="18"/>
+      <c r="K24" s="17"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="20">
         <f>B22*B23*B24</f>
         <v>8192000</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19">
+      <c r="C25" s="20"/>
+      <c r="D25" s="20">
         <f>D22*D23*D24</f>
         <v>1277952000</v>
       </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19">
+      <c r="E25" s="20"/>
+      <c r="F25" s="20">
         <f t="shared" ref="F25" si="11">F22*F23*F24</f>
         <v>1277952000</v>
       </c>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19">
+      <c r="G25" s="20"/>
+      <c r="H25" s="20">
         <f t="shared" ref="H25" si="12">H22*H23*H24</f>
         <v>1277952000</v>
       </c>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19">
+      <c r="I25" s="20"/>
+      <c r="J25" s="20">
         <f t="shared" ref="J25" si="13">J22*J23*J24</f>
         <v>1277952000</v>
       </c>
-      <c r="K25" s="19"/>
+      <c r="K25" s="20"/>
     </row>
     <row r="26" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" s="19">
         <f>0.191+9.964+1.804+1.666</f>
         <v>13.625000000000002</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20">
+      <c r="C26" s="19"/>
+      <c r="D26" s="19">
         <v>25.887</v>
       </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20">
+      <c r="E26" s="19"/>
+      <c r="F26" s="19">
         <v>21.568000000000001</v>
       </c>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20">
+      <c r="G26" s="19"/>
+      <c r="H26" s="19">
         <v>21.541</v>
       </c>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20">
+      <c r="I26" s="19"/>
+      <c r="J26" s="19">
         <v>9.1859999999999999</v>
       </c>
-      <c r="K26" s="20"/>
+      <c r="K26" s="19"/>
     </row>
     <row r="27" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="20">
+      <c r="B27" s="19">
         <f>19.37+17.15</f>
         <v>36.519999999999996</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20">
+      <c r="C27" s="19"/>
+      <c r="D27" s="19">
         <v>146.75</v>
       </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20">
+      <c r="E27" s="19"/>
+      <c r="F27" s="19">
         <v>180.85</v>
       </c>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20">
+      <c r="G27" s="19"/>
+      <c r="H27" s="19">
         <v>166.69</v>
       </c>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20">
+      <c r="I27" s="19"/>
+      <c r="J27" s="19">
         <v>128.34</v>
       </c>
-      <c r="K27" s="20"/>
+      <c r="K27" s="19"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="17">
+      <c r="B28" s="18">
         <f>B26/512/8/2000*B$25</f>
         <v>13.625000000000002</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17">
+      <c r="C28" s="18"/>
+      <c r="D28" s="18">
         <f>D26/6144/8/4000*D$25</f>
         <v>168.2655</v>
       </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17">
+      <c r="E28" s="18"/>
+      <c r="F28" s="18">
         <f t="shared" ref="F28" si="14">F26/6144/8/4000*F$25</f>
         <v>140.19200000000001</v>
       </c>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17">
+      <c r="G28" s="18"/>
+      <c r="H28" s="18">
         <f t="shared" ref="H28" si="15">H26/6144/8/4000*H$25</f>
         <v>140.01650000000001</v>
       </c>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17">
+      <c r="I28" s="18"/>
+      <c r="J28" s="18">
         <f t="shared" ref="J28" si="16">J26/6144/8/4000*J$25</f>
         <v>59.708999999999996</v>
       </c>
-      <c r="K28" s="17"/>
+      <c r="K28" s="18"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="17">
+      <c r="B29" s="18">
         <f>B27/512/8/2000*B$25</f>
         <v>36.519999999999996</v>
       </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17">
+      <c r="C29" s="18"/>
+      <c r="D29" s="18">
         <f>D27/6144/8/4000*D$25</f>
         <v>953.875</v>
       </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17">
+      <c r="E29" s="18"/>
+      <c r="F29" s="18">
         <f t="shared" ref="F29" si="17">F27/6144/8/4000*F$25</f>
         <v>1175.5250000000001</v>
       </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17">
+      <c r="G29" s="18"/>
+      <c r="H29" s="18">
         <f t="shared" ref="H29" si="18">H27/6144/8/4000*H$25</f>
         <v>1083.4849999999999</v>
       </c>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17">
+      <c r="I29" s="18"/>
+      <c r="J29" s="18">
         <f t="shared" ref="J29" si="19">J27/6144/8/4000*J$25</f>
         <v>834.20999999999992</v>
       </c>
-      <c r="K29" s="17"/>
+      <c r="K29" s="18"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="18">
+      <c r="B30" s="17">
         <v>1</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18">
+      <c r="C30" s="17"/>
+      <c r="D30" s="17">
         <v>1</v>
       </c>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18">
+      <c r="E30" s="17"/>
+      <c r="F30" s="17">
         <v>1</v>
       </c>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18">
+      <c r="G30" s="17"/>
+      <c r="H30" s="17">
         <v>1</v>
       </c>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18">
+      <c r="I30" s="17"/>
+      <c r="J30" s="17">
         <v>1</v>
       </c>
-      <c r="K30" s="18"/>
+      <c r="K30" s="17"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="21">
+      <c r="B31" s="16">
         <f>(B28+B29*B30)/86400</f>
         <v>5.8038194444444435E-4</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21">
+      <c r="C31" s="16"/>
+      <c r="D31" s="16">
         <f t="shared" ref="D31:F31" si="20">(D28+D29*D30)/86400</f>
         <v>1.2987737268518517E-2</v>
       </c>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21">
+      <c r="E31" s="16"/>
+      <c r="F31" s="16">
         <f t="shared" si="20"/>
         <v>1.5228206018518519E-2</v>
       </c>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21">
+      <c r="G31" s="16"/>
+      <c r="H31" s="16">
         <f t="shared" ref="H31" si="21">(H28+H29*H30)/86400</f>
         <v>1.4160896990740739E-2</v>
       </c>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21">
+      <c r="I31" s="16"/>
+      <c r="J31" s="16">
         <f t="shared" ref="J31" si="22">(J28+J29*J30)/86400</f>
         <v>1.034628472222222E-2</v>
       </c>
-      <c r="K31" s="21"/>
+      <c r="K31" s="16"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="E32" s="6"/>
@@ -1550,66 +1550,6 @@
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="F16:G16"/>
@@ -1619,6 +1559,66 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D8:E8"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1630,7 +1630,7 @@
   <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1658,10 +1658,10 @@
       <c r="A1" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="16"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1670,10 +1670,10 @@
       <c r="B2">
         <v>9481</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="16"/>
+      <c r="E2" s="21"/>
       <c r="F2">
         <v>42.926477759350803</v>
       </c>
@@ -1694,12 +1694,12 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>400</v>
-      </c>
-      <c r="D3" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="16"/>
+      <c r="E3" s="21"/>
       <c r="F3">
         <v>-29.5</v>
       </c>
@@ -1719,10 +1719,10 @@
         <f>0.005</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="16"/>
+      <c r="E4" s="21"/>
       <c r="F4">
         <f>SIN(RADIANS(F2+F3))/SIN(RADIANS(F2-F3))</f>
         <v>0.24356450463759297</v>
@@ -1732,11 +1732,11 @@
       </c>
       <c r="I4" s="2">
         <f>MAX(ROUND(2*I3/$B7,0),1)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J4">
         <f>I3/$B7</f>
-        <v>0.36644528366901513</v>
+        <v>1.4657811346760605</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -1747,10 +1747,10 @@
         <f>0.005</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="16"/>
+      <c r="E5" s="21"/>
       <c r="F5">
         <f>ABS((COS(RADIANS(F2-F3))-COS(RADIANS(F2+F3)))/SIN(RADIANS(F2-F3)))</f>
         <v>0.70357494464450898</v>
@@ -1765,7 +1765,7 @@
       </c>
       <c r="B7">
         <f>B8*B14</f>
-        <v>32000</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
@@ -1774,12 +1774,12 @@
       </c>
       <c r="B8">
         <f>B3/10</f>
-        <v>40</v>
-      </c>
-      <c r="D8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="16"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="1">
         <v>5.9999999999999997E-7</v>
       </c>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="I8" s="9">
         <f>22122874/1024/1024/3072/8/26000*MAX(25:25)</f>
-        <v>6.9244772886618584</v>
+        <v>20.773431865985575</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
@@ -1797,15 +1797,15 @@
       </c>
       <c r="B9">
         <f>4/B8</f>
-        <v>0.1</v>
-      </c>
-      <c r="D9" s="16" t="s">
+        <v>0.4</v>
+      </c>
+      <c r="D9" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="16"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="7">
         <f>SUM(28:28)/86400</f>
-        <v>1.2159490740740739E-3</v>
+        <v>3.4652546296296298E-3</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
@@ -1814,25 +1814,25 @@
       </c>
       <c r="B10">
         <f>MIN(B9/800,0.001)</f>
-        <v>1.25E-4</v>
-      </c>
-      <c r="D10" s="16" t="s">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D10" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="16"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="7">
         <f>SUM(31:31)-F9</f>
-        <v>1.1049305555555555E-2</v>
+        <v>3.2246296296296301E-2</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="16"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="10">
         <f>SUM(31:31)</f>
-        <v>1.2265254629629629E-2</v>
+        <v>3.5711550925925928E-2</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
@@ -1867,40 +1867,40 @@
       <c r="A16" t="s">
         <v>88</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16" t="s">
+      <c r="C16" s="21"/>
+      <c r="D16" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16" t="s">
+      <c r="E16" s="21"/>
+      <c r="F16" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16" t="s">
+      <c r="G16" s="21"/>
+      <c r="H16" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16" t="s">
+      <c r="I16" s="21"/>
+      <c r="J16" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16" t="s">
+      <c r="K16" s="21"/>
+      <c r="L16" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16" t="s">
+      <c r="M16" s="21"/>
+      <c r="N16" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16" t="s">
+      <c r="O16" s="21"/>
+      <c r="P16" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="16"/>
-      <c r="S16" s="16"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="21"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
@@ -2050,67 +2050,67 @@
       </c>
       <c r="B19" s="2">
         <f>B7</f>
-        <v>32000</v>
+        <v>8000</v>
       </c>
       <c r="C19" s="2">
         <f>B8</f>
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D19" s="2">
         <f>E19*D24</f>
-        <v>32000</v>
+        <v>8000</v>
       </c>
       <c r="E19" s="2">
         <f>C19</f>
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="F19" s="2">
         <f>G19*F24</f>
-        <v>32000</v>
+        <v>24000</v>
       </c>
       <c r="G19" s="2">
         <f>E19</f>
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="H19" s="2">
         <f>I19*H24</f>
-        <v>32000</v>
+        <v>24000</v>
       </c>
       <c r="I19" s="2">
         <f>G19</f>
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="J19" s="2">
         <f>K19*J24</f>
-        <v>32000</v>
+        <v>24000</v>
       </c>
       <c r="K19" s="2">
         <f>I19</f>
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="L19" s="2">
         <f>M19*L24</f>
-        <v>32000</v>
+        <v>24000</v>
       </c>
       <c r="M19" s="2">
         <f>K19</f>
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="N19" s="2">
         <f>O19*N24</f>
-        <v>32000</v>
+        <v>24000</v>
       </c>
       <c r="O19" s="2">
         <f>M19</f>
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="P19" s="2">
         <f>Q19*P24</f>
-        <v>32000</v>
+        <v>24000</v>
       </c>
       <c r="Q19" s="2">
         <f>O19</f>
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
@@ -2121,67 +2121,67 @@
       </c>
       <c r="B20" s="2">
         <f>B9*1000</f>
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="C20" s="2">
         <f>B10*1000</f>
-        <v>0.125</v>
+        <v>0.5</v>
       </c>
       <c r="D20" s="2">
         <f>$B20*$C19/E19</f>
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="E20" s="2">
         <f>$B19*$C20/D19</f>
-        <v>0.125</v>
+        <v>0.5</v>
       </c>
       <c r="F20" s="2">
         <f>$B20*$C19/G19</f>
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G20" s="2">
         <f>$B19*$C20/F19</f>
-        <v>0.125</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" ref="H20" si="6">$B20*$C19/I19</f>
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" ref="I20" si="7">$B19*$C20/H19</f>
-        <v>0.125</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" ref="J20" si="8">$B20*$C19/K19</f>
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="K20" s="2">
         <f t="shared" ref="K20" si="9">$B19*$C20/J19</f>
-        <v>0.125</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="L20" s="2">
         <f t="shared" ref="L20" si="10">$B20*$C19/M19</f>
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="M20" s="2">
         <f t="shared" ref="M20" si="11">$B19*$C20/L19</f>
-        <v>0.125</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="N20" s="2">
         <f t="shared" ref="N20" si="12">$B20*$C19/O19</f>
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="O20" s="2">
         <f t="shared" ref="O20" si="13">$B19*$C20/N19</f>
-        <v>0.125</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="P20" s="2">
         <f t="shared" ref="P20" si="14">$B20*$C19/Q19</f>
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="Q20" s="2">
         <f t="shared" ref="Q20" si="15">$B19*$C20/P19</f>
-        <v>0.125</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
@@ -2190,38 +2190,38 @@
       <c r="A21" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="17">
+      <c r="B21" s="18">
         <v>726.57</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17">
+      <c r="C21" s="18"/>
+      <c r="D21" s="18">
         <v>722.86</v>
       </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17">
+      <c r="E21" s="18"/>
+      <c r="F21" s="18">
         <v>722.85</v>
       </c>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17">
+      <c r="G21" s="18"/>
+      <c r="H21" s="18">
         <v>176.54</v>
       </c>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17">
+      <c r="I21" s="18"/>
+      <c r="J21" s="18">
         <v>14.28</v>
       </c>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17">
+      <c r="K21" s="18"/>
+      <c r="L21" s="18">
         <v>175.15</v>
       </c>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17">
+      <c r="M21" s="18"/>
+      <c r="N21" s="18">
         <v>173.04</v>
       </c>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17">
+      <c r="O21" s="18"/>
+      <c r="P21" s="18">
         <v>173.07</v>
       </c>
-      <c r="Q21" s="17"/>
+      <c r="Q21" s="18"/>
       <c r="R21" s="12"/>
       <c r="S21" s="12"/>
     </row>
@@ -2229,187 +2229,187 @@
       <c r="A22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="17">
         <f>B12</f>
         <v>1024</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18">
+      <c r="C22" s="17"/>
+      <c r="D22" s="17">
         <f>B22</f>
         <v>1024</v>
       </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18">
+      <c r="E22" s="17"/>
+      <c r="F22" s="17">
         <f>D22*I2*8</f>
         <v>32768</v>
       </c>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18">
+      <c r="G22" s="17"/>
+      <c r="H22" s="17">
         <f>F22</f>
         <v>32768</v>
       </c>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18">
+      <c r="I22" s="17"/>
+      <c r="J22" s="17">
         <f t="shared" ref="J22:J24" si="16">H22</f>
         <v>32768</v>
       </c>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18">
+      <c r="K22" s="17"/>
+      <c r="L22" s="17">
         <f t="shared" ref="L22:L24" si="17">J22</f>
         <v>32768</v>
       </c>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18">
+      <c r="M22" s="17"/>
+      <c r="N22" s="17">
         <f>L22</f>
         <v>32768</v>
       </c>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18">
+      <c r="O22" s="17"/>
+      <c r="P22" s="17">
         <f t="shared" ref="P22:P23" si="18">N22</f>
         <v>32768</v>
       </c>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="S22" s="17"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="17">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18">
+      <c r="C23" s="17"/>
+      <c r="D23" s="17">
         <f t="shared" ref="D23:D24" si="19">B23</f>
         <v>8</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18">
+      <c r="E23" s="17"/>
+      <c r="F23" s="17">
         <f t="shared" ref="F23" si="20">D23</f>
         <v>8</v>
       </c>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18">
+      <c r="G23" s="17"/>
+      <c r="H23" s="17">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18">
+      <c r="I23" s="17"/>
+      <c r="J23" s="17">
         <f t="shared" si="16"/>
         <v>8</v>
       </c>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18">
+      <c r="K23" s="17"/>
+      <c r="L23" s="17">
         <f t="shared" si="17"/>
         <v>8</v>
       </c>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18">
+      <c r="M23" s="17"/>
+      <c r="N23" s="17">
         <f>L23</f>
         <v>8</v>
       </c>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18">
+      <c r="O23" s="17"/>
+      <c r="P23" s="17">
         <f t="shared" si="18"/>
         <v>8</v>
       </c>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="17"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="17">
         <f>B14</f>
         <v>800</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18">
+      <c r="C24" s="17"/>
+      <c r="D24" s="17">
         <f t="shared" si="19"/>
         <v>800</v>
       </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18">
+      <c r="E24" s="17"/>
+      <c r="F24" s="17">
         <f>D24*I4</f>
-        <v>800</v>
-      </c>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18">
+        <v>2400</v>
+      </c>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17">
         <f t="shared" ref="H24" si="21">F24</f>
-        <v>800</v>
-      </c>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18">
+        <v>2400</v>
+      </c>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17">
         <f t="shared" si="16"/>
-        <v>800</v>
-      </c>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18">
+        <v>2400</v>
+      </c>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17">
         <f t="shared" si="17"/>
-        <v>800</v>
-      </c>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18">
+        <v>2400</v>
+      </c>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17">
         <f t="shared" ref="N24" si="22">L24</f>
-        <v>800</v>
-      </c>
-      <c r="O24" s="18"/>
-      <c r="P24" s="18">
+        <v>2400</v>
+      </c>
+      <c r="O24" s="17"/>
+      <c r="P24" s="17">
         <f>N24</f>
-        <v>800</v>
-      </c>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18"/>
-      <c r="S24" s="18"/>
+        <v>2400</v>
+      </c>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="17"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="20">
         <f>B22*B23*B24</f>
         <v>6553600</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19">
+      <c r="C25" s="20"/>
+      <c r="D25" s="20">
         <f>D22*D23*D24</f>
         <v>6553600</v>
       </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19">
+      <c r="E25" s="20"/>
+      <c r="F25" s="20">
         <f t="shared" ref="F25" si="23">F22*F23*F24</f>
-        <v>209715200</v>
-      </c>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19">
+        <v>629145600</v>
+      </c>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20">
         <f t="shared" ref="H25" si="24">H22*H23*H24</f>
-        <v>209715200</v>
-      </c>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19">
+        <v>629145600</v>
+      </c>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20">
         <f t="shared" ref="J25" si="25">J22*J23*J24</f>
-        <v>209715200</v>
-      </c>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19">
+        <v>629145600</v>
+      </c>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20">
         <f t="shared" ref="L25" si="26">L22*L23*L24</f>
-        <v>209715200</v>
-      </c>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19">
+        <v>629145600</v>
+      </c>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20">
         <f t="shared" ref="N25" si="27">N22*N23*N24</f>
-        <v>209715200</v>
-      </c>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19">
+        <v>629145600</v>
+      </c>
+      <c r="O25" s="20"/>
+      <c r="P25" s="20">
         <f t="shared" ref="P25" si="28">P22*P23*P24</f>
-        <v>209715200</v>
-      </c>
-      <c r="Q25" s="19"/>
+        <v>629145600</v>
+      </c>
+      <c r="Q25" s="20"/>
       <c r="R25" s="13"/>
       <c r="S25" s="13"/>
     </row>
@@ -2417,40 +2417,40 @@
       <c r="A26" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" s="19">
         <f>0.154+3.252+1.863+1.467</f>
         <v>6.7360000000000007</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20">
+      <c r="C26" s="19"/>
+      <c r="D26" s="19">
         <v>1.1519999999999999</v>
       </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20">
+      <c r="E26" s="19"/>
+      <c r="F26" s="19">
         <v>14.536</v>
       </c>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20">
+      <c r="G26" s="19"/>
+      <c r="H26" s="19">
         <v>5.0839999999999996</v>
       </c>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20">
+      <c r="I26" s="19"/>
+      <c r="J26" s="19">
         <f>0.874+3.15</f>
         <v>4.024</v>
       </c>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20">
+      <c r="K26" s="19"/>
+      <c r="L26" s="19">
         <v>5.891</v>
       </c>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20">
+      <c r="M26" s="19"/>
+      <c r="N26" s="19">
         <v>11.195</v>
       </c>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20">
+      <c r="O26" s="19"/>
+      <c r="P26" s="19">
         <v>7.8550000000000004</v>
       </c>
-      <c r="Q26" s="20"/>
+      <c r="Q26" s="19"/>
       <c r="R26" s="14"/>
       <c r="S26" s="14"/>
     </row>
@@ -2458,219 +2458,305 @@
       <c r="A27" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="20">
+      <c r="B27" s="19">
         <f>6.36+8.93</f>
         <v>15.29</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20">
+      <c r="C27" s="19"/>
+      <c r="D27" s="19">
         <v>23.66</v>
       </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20">
+      <c r="E27" s="19"/>
+      <c r="F27" s="19">
         <v>108.08</v>
       </c>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20">
+      <c r="G27" s="19"/>
+      <c r="H27" s="19">
         <v>62.75</v>
       </c>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20">
+      <c r="I27" s="19"/>
+      <c r="J27" s="19">
         <v>56.74</v>
       </c>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20">
+      <c r="K27" s="19"/>
+      <c r="L27" s="19">
         <v>67.02</v>
       </c>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20">
+      <c r="M27" s="19"/>
+      <c r="N27" s="19">
         <v>72.900000000000006</v>
       </c>
-      <c r="O27" s="20"/>
-      <c r="P27" s="20">
+      <c r="O27" s="19"/>
+      <c r="P27" s="19">
         <v>80.45</v>
       </c>
-      <c r="Q27" s="20"/>
+      <c r="Q27" s="19"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="17">
+      <c r="B28" s="18">
         <f>B26/512/8/1600*B$25</f>
         <v>6.7360000000000007</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17">
+      <c r="C28" s="18"/>
+      <c r="D28" s="18">
         <f>D26/512/8/1600*D$25</f>
         <v>1.1519999999999999</v>
       </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17">
+      <c r="E28" s="18"/>
+      <c r="F28" s="18">
         <f>F26/4096/8/3200*F$25</f>
-        <v>29.071999999999999</v>
-      </c>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17">
+        <v>87.215999999999994</v>
+      </c>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18">
         <f t="shared" ref="H28" si="29">H26/4096/8/3200*H$25</f>
-        <v>10.167999999999999</v>
-      </c>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17">
+        <v>30.503999999999998</v>
+      </c>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18">
         <f t="shared" ref="J28" si="30">J26/4096/8/3200*J$25</f>
-        <v>8.048</v>
-      </c>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17">
+        <v>24.143999999999998</v>
+      </c>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18">
         <f t="shared" ref="L28" si="31">L26/4096/8/3200*L$25</f>
-        <v>11.782</v>
-      </c>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17">
+        <v>35.345999999999997</v>
+      </c>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18">
         <f t="shared" ref="N28" si="32">N26/4096/8/3200*N$25</f>
-        <v>22.39</v>
-      </c>
-      <c r="O28" s="17"/>
-      <c r="P28" s="17">
+        <v>67.17</v>
+      </c>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18">
         <f t="shared" ref="P28" si="33">P26/4096/8/3200*P$25</f>
-        <v>15.71</v>
-      </c>
-      <c r="Q28" s="17"/>
+        <v>47.13</v>
+      </c>
+      <c r="Q28" s="18"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="17">
+      <c r="B29" s="18">
         <f>B27/512/8/1600*B$25</f>
         <v>15.289999999999997</v>
       </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17">
+      <c r="C29" s="18"/>
+      <c r="D29" s="18">
         <f>D27/512/8/1600*D$25</f>
         <v>23.66</v>
       </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17">
+      <c r="E29" s="18"/>
+      <c r="F29" s="18">
         <f>F27/4096/8/3200*F$25</f>
-        <v>216.16</v>
-      </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17">
+        <v>648.48</v>
+      </c>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18">
         <f t="shared" ref="H29" si="34">H27/4096/8/3200*H$25</f>
-        <v>125.49999999999999</v>
-      </c>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17">
+        <v>376.49999999999994</v>
+      </c>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18">
         <f t="shared" ref="J29" si="35">J27/4096/8/3200*J$25</f>
-        <v>113.48</v>
-      </c>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17">
+        <v>340.44</v>
+      </c>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18">
         <f t="shared" ref="L29" si="36">L27/4096/8/3200*L$25</f>
-        <v>134.04</v>
-      </c>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17">
+        <v>402.11999999999995</v>
+      </c>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18">
         <f t="shared" ref="N29" si="37">N27/4096/8/3200*N$25</f>
-        <v>145.80000000000001</v>
-      </c>
-      <c r="O29" s="17"/>
-      <c r="P29" s="17">
+        <v>437.40000000000003</v>
+      </c>
+      <c r="O29" s="18"/>
+      <c r="P29" s="18">
         <f t="shared" ref="P29" si="38">P27/4096/8/3200*P$25</f>
-        <v>160.9</v>
-      </c>
-      <c r="Q29" s="17"/>
+        <v>482.7</v>
+      </c>
+      <c r="Q29" s="18"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="18">
+      <c r="B30" s="17">
         <v>1</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18">
+      <c r="C30" s="17"/>
+      <c r="D30" s="17">
         <v>1</v>
       </c>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18">
+      <c r="E30" s="17"/>
+      <c r="F30" s="17">
         <v>1</v>
       </c>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18">
+      <c r="G30" s="17"/>
+      <c r="H30" s="17">
         <v>1</v>
       </c>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18">
+      <c r="I30" s="17"/>
+      <c r="J30" s="17">
         <v>1</v>
       </c>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18">
+      <c r="K30" s="17"/>
+      <c r="L30" s="17">
         <v>1</v>
       </c>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18">
+      <c r="M30" s="17"/>
+      <c r="N30" s="17">
         <v>1</v>
       </c>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18">
+      <c r="O30" s="17"/>
+      <c r="P30" s="17">
         <v>1</v>
       </c>
-      <c r="Q30" s="18"/>
+      <c r="Q30" s="17"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="21">
+      <c r="B31" s="16">
         <f>(B28+B29*B30)/86400</f>
         <v>2.549305555555555E-4</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21">
+      <c r="C31" s="16"/>
+      <c r="D31" s="16">
         <f t="shared" ref="D31:F31" si="39">(D28+D29*D30)/86400</f>
         <v>2.8717592592592597E-4</v>
       </c>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21">
+      <c r="E31" s="16"/>
+      <c r="F31" s="16">
         <f t="shared" si="39"/>
-        <v>2.8383333333333333E-3</v>
-      </c>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21">
+        <v>8.515E-3</v>
+      </c>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16">
         <f>(H28+H29*H30+J28)/86400</f>
-        <v>1.6633796296296295E-3</v>
-      </c>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21">
+        <v>4.9901388888888886E-3</v>
+      </c>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16">
         <f>(J28+J29*J30+L28)/86400</f>
-        <v>1.5429398148148149E-3</v>
-      </c>
-      <c r="K31" s="21"/>
-      <c r="L31" s="21">
+        <v>4.628819444444445E-3</v>
+      </c>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16">
         <f t="shared" ref="L31:P31" si="40">(L28+L29*L30)/86400</f>
-        <v>1.6877546296296298E-3</v>
-      </c>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21">
+        <v>5.063263888888888E-3</v>
+      </c>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16">
         <f t="shared" si="40"/>
-        <v>1.9466435185185186E-3</v>
-      </c>
-      <c r="O31" s="21"/>
-      <c r="P31" s="21">
+        <v>5.8399305555555565E-3</v>
+      </c>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16">
         <f t="shared" si="40"/>
-        <v>2.0440972222222223E-3</v>
-      </c>
-      <c r="Q31" s="21"/>
-      <c r="R31" s="17"/>
-      <c r="S31" s="17"/>
+        <v>6.132291666666667E-3</v>
+      </c>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="18"/>
+      <c r="S31" s="18"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="E32" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="110">
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="P31:Q31"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
     <mergeCell ref="N26:O26"/>
     <mergeCell ref="N27:O27"/>
     <mergeCell ref="P26:Q26"/>
@@ -2695,92 +2781,6 @@
     <mergeCell ref="F27:G27"/>
     <mergeCell ref="H27:I27"/>
     <mergeCell ref="J27:K27"/>
-    <mergeCell ref="R31:S31"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="P31:Q31"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="R24:S24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2829,14 +2829,14 @@
       <c r="A1" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="L1" s="16" t="s">
+      <c r="E1" s="21"/>
+      <c r="L1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="16"/>
+      <c r="M1" s="21"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2845,10 +2845,10 @@
       <c r="B2">
         <v>9481</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="16"/>
+      <c r="E2" s="21"/>
       <c r="F2">
         <v>19.909876918386299</v>
       </c>
@@ -2863,10 +2863,10 @@
         <f>MAX(F4,1/F4)</f>
         <v>11.830135875287004</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="16"/>
+      <c r="M2" s="21"/>
       <c r="N2">
         <v>42.926477759350803</v>
       </c>
@@ -2889,10 +2889,10 @@
       <c r="B3">
         <v>20</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="16"/>
+      <c r="E3" s="21"/>
       <c r="F3">
         <v>17</v>
       </c>
@@ -2903,10 +2903,10 @@
         <f>$B4*F5/300000000*1000000000000000</f>
         <v>52300.882458116022</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="L3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="16"/>
+      <c r="M3" s="21"/>
       <c r="N3">
         <v>-29.5</v>
       </c>
@@ -2925,10 +2925,10 @@
       <c r="B4" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="16"/>
+      <c r="E4" s="21"/>
       <c r="F4">
         <f>SIN(RADIANS(F2+F3))/SIN(RADIANS(F2-F3))</f>
         <v>11.830135875287004</v>
@@ -2944,10 +2944,10 @@
         <f>I3/$B7</f>
         <v>13.075220614529005</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="L4" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="16"/>
+      <c r="M4" s="21"/>
       <c r="N4">
         <f>SIN(RADIANS(N2+N3))/SIN(RADIANS(N2-N3))</f>
         <v>0.24356450463759297</v>
@@ -2971,18 +2971,18 @@
       <c r="B5" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="16"/>
+      <c r="E5" s="21"/>
       <c r="F5">
         <f>ABS((COS(RADIANS(F2-F3))-COS(RADIANS(F2+F3)))/SIN(RADIANS(F2-F3)))</f>
         <v>3.9225661843587014</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="L5" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="16"/>
+      <c r="M5" s="21"/>
       <c r="N5">
         <f>ABS((COS(RADIANS(N2-N3))-COS(RADIANS(N2+N3)))/SIN(RADIANS(N2-N3)))</f>
         <v>0.70357494464450898</v>
@@ -3008,10 +3008,10 @@
         <f>B3/10</f>
         <v>2</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="16"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="1">
         <v>5.9999999999999997E-7</v>
       </c>
@@ -3031,10 +3031,10 @@
         <f>4/B8</f>
         <v>2</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="16"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="7">
         <f>SUM(28:28)/86400</f>
         <v>0.1360213888888889</v>
@@ -3048,20 +3048,20 @@
         <f>MIN(B9/400,0.001)</f>
         <v>1E-3</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="16"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="7">
         <f>SUM(31:31)-F9</f>
         <v>1.3155878472222222</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="16"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="10">
         <f>SUM(31:31)</f>
         <v>1.451609236111111</v>
@@ -3096,56 +3096,56 @@
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16" t="s">
+      <c r="C16" s="21"/>
+      <c r="D16" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16" t="s">
+      <c r="E16" s="21"/>
+      <c r="F16" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16" t="s">
+      <c r="G16" s="21"/>
+      <c r="H16" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16" t="s">
+      <c r="I16" s="21"/>
+      <c r="J16" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16" t="s">
+      <c r="K16" s="21"/>
+      <c r="L16" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16" t="s">
+      <c r="M16" s="21"/>
+      <c r="N16" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16" t="s">
+      <c r="O16" s="21"/>
+      <c r="P16" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="16" t="s">
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="S16" s="16"/>
-      <c r="T16" s="16" t="s">
+      <c r="S16" s="21"/>
+      <c r="T16" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="U16" s="16"/>
-      <c r="V16" s="16" t="s">
+      <c r="U16" s="21"/>
+      <c r="V16" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="W16" s="16"/>
-      <c r="X16" s="16" t="s">
+      <c r="W16" s="21"/>
+      <c r="X16" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="Y16" s="16"/>
-      <c r="Z16" s="16"/>
-      <c r="AA16" s="16"/>
+      <c r="Y16" s="21"/>
+      <c r="Z16" s="21"/>
+      <c r="AA16" s="21"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
@@ -3563,259 +3563,259 @@
       <c r="A21" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="17">
+      <c r="B21" s="18">
         <v>722.7</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17">
+      <c r="C21" s="18"/>
+      <c r="D21" s="18">
         <f>B21*J2</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17">
+      <c r="E21" s="18"/>
+      <c r="F21" s="18">
         <f>D21</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17">
+      <c r="G21" s="18"/>
+      <c r="H21" s="18">
         <f>F21</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17">
+      <c r="I21" s="18"/>
+      <c r="J21" s="18">
         <f>H21/J2</f>
         <v>722.7</v>
       </c>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17">
+      <c r="K21" s="18"/>
+      <c r="L21" s="18">
         <v>722.86</v>
       </c>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17">
+      <c r="M21" s="18"/>
+      <c r="N21" s="18">
         <v>722.85</v>
       </c>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17">
+      <c r="O21" s="18"/>
+      <c r="P21" s="18">
         <v>176.54</v>
       </c>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="17">
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18">
         <v>14.28</v>
       </c>
-      <c r="S21" s="17"/>
-      <c r="T21" s="17">
+      <c r="S21" s="18"/>
+      <c r="T21" s="18">
         <v>175.15</v>
       </c>
-      <c r="U21" s="17"/>
-      <c r="V21" s="17">
+      <c r="U21" s="18"/>
+      <c r="V21" s="18">
         <v>173.04</v>
       </c>
-      <c r="W21" s="17"/>
-      <c r="X21" s="17">
+      <c r="W21" s="18"/>
+      <c r="X21" s="18">
         <v>173.07</v>
       </c>
-      <c r="Y21" s="17"/>
-      <c r="Z21" s="18"/>
-      <c r="AA21" s="18"/>
+      <c r="Y21" s="18"/>
+      <c r="Z21" s="17"/>
+      <c r="AA21" s="17"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="17">
         <f>B12</f>
         <v>512</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18">
+      <c r="C22" s="17"/>
+      <c r="D22" s="17">
         <f>B22*I2</f>
         <v>6144</v>
       </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18">
+      <c r="E22" s="17"/>
+      <c r="F22" s="17">
         <f>D22</f>
         <v>6144</v>
       </c>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18">
+      <c r="G22" s="17"/>
+      <c r="H22" s="17">
         <f>F22</f>
         <v>6144</v>
       </c>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18">
+      <c r="I22" s="17"/>
+      <c r="J22" s="17">
         <f t="shared" ref="J22:J24" si="23">H22</f>
         <v>6144</v>
       </c>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18">
+      <c r="K22" s="17"/>
+      <c r="L22" s="17">
         <f>J22</f>
         <v>6144</v>
       </c>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18">
+      <c r="M22" s="17"/>
+      <c r="N22" s="17">
         <f>L22*Q2*4</f>
         <v>98304</v>
       </c>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18">
+      <c r="O22" s="17"/>
+      <c r="P22" s="17">
         <f>N22</f>
         <v>98304</v>
       </c>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18">
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17">
         <f t="shared" ref="R22:R24" si="24">P22</f>
         <v>98304</v>
       </c>
-      <c r="S22" s="18"/>
-      <c r="T22" s="18">
+      <c r="S22" s="17"/>
+      <c r="T22" s="17">
         <f t="shared" ref="T22:T24" si="25">R22</f>
         <v>98304</v>
       </c>
-      <c r="U22" s="18"/>
-      <c r="V22" s="18">
+      <c r="U22" s="17"/>
+      <c r="V22" s="17">
         <f>T22</f>
         <v>98304</v>
       </c>
-      <c r="W22" s="18"/>
-      <c r="X22" s="18">
+      <c r="W22" s="17"/>
+      <c r="X22" s="17">
         <f t="shared" ref="X22:X23" si="26">V22</f>
         <v>98304</v>
       </c>
-      <c r="Y22" s="18"/>
-      <c r="Z22" s="18"/>
-      <c r="AA22" s="18"/>
+      <c r="Y22" s="17"/>
+      <c r="Z22" s="17"/>
+      <c r="AA22" s="17"/>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="17">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18">
+      <c r="C23" s="17"/>
+      <c r="D23" s="17">
         <f t="shared" ref="D23" si="27">B23</f>
         <v>8</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18">
+      <c r="E23" s="17"/>
+      <c r="F23" s="17">
         <f t="shared" ref="F23" si="28">D23</f>
         <v>8</v>
       </c>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18">
+      <c r="G23" s="17"/>
+      <c r="H23" s="17">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18">
+      <c r="I23" s="17"/>
+      <c r="J23" s="17">
         <f t="shared" si="23"/>
         <v>8</v>
       </c>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18">
+      <c r="K23" s="17"/>
+      <c r="L23" s="17">
         <f t="shared" ref="L23:L24" si="29">J23</f>
         <v>8</v>
       </c>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18">
+      <c r="M23" s="17"/>
+      <c r="N23" s="17">
         <f t="shared" ref="N23" si="30">L23</f>
         <v>8</v>
       </c>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18">
+      <c r="O23" s="17"/>
+      <c r="P23" s="17">
         <f>N23</f>
         <v>8</v>
       </c>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18">
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17">
         <f t="shared" si="24"/>
         <v>8</v>
       </c>
-      <c r="S23" s="18"/>
-      <c r="T23" s="18">
+      <c r="S23" s="17"/>
+      <c r="T23" s="17">
         <f t="shared" si="25"/>
         <v>8</v>
       </c>
-      <c r="U23" s="18"/>
-      <c r="V23" s="18">
+      <c r="U23" s="17"/>
+      <c r="V23" s="17">
         <f>T23</f>
         <v>8</v>
       </c>
-      <c r="W23" s="18"/>
-      <c r="X23" s="18">
+      <c r="W23" s="17"/>
+      <c r="X23" s="17">
         <f t="shared" si="26"/>
         <v>8</v>
       </c>
-      <c r="Y23" s="18"/>
-      <c r="Z23" s="18"/>
-      <c r="AA23" s="18"/>
+      <c r="Y23" s="17"/>
+      <c r="Z23" s="17"/>
+      <c r="AA23" s="17"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="17">
         <f>B14</f>
         <v>2000</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18">
+      <c r="C24" s="17"/>
+      <c r="D24" s="17">
         <f>B24*I4</f>
         <v>26000</v>
       </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18">
+      <c r="E24" s="17"/>
+      <c r="F24" s="17">
         <f>D24</f>
         <v>26000</v>
       </c>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18">
+      <c r="G24" s="17"/>
+      <c r="H24" s="17">
         <f t="shared" ref="H24" si="31">F24</f>
         <v>26000</v>
       </c>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18">
+      <c r="I24" s="17"/>
+      <c r="J24" s="17">
         <f t="shared" si="23"/>
         <v>26000</v>
       </c>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18">
+      <c r="K24" s="17"/>
+      <c r="L24" s="17">
         <f t="shared" si="29"/>
         <v>26000</v>
       </c>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18">
+      <c r="M24" s="17"/>
+      <c r="N24" s="17">
         <f>L24</f>
         <v>26000</v>
       </c>
-      <c r="O24" s="18"/>
-      <c r="P24" s="18">
+      <c r="O24" s="17"/>
+      <c r="P24" s="17">
         <f t="shared" ref="P24" si="32">N24</f>
         <v>26000</v>
       </c>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18">
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17">
         <f t="shared" si="24"/>
         <v>26000</v>
       </c>
-      <c r="S24" s="18"/>
-      <c r="T24" s="18">
+      <c r="S24" s="17"/>
+      <c r="T24" s="17">
         <f t="shared" si="25"/>
         <v>26000</v>
       </c>
-      <c r="U24" s="18"/>
-      <c r="V24" s="18">
+      <c r="U24" s="17"/>
+      <c r="V24" s="17">
         <f t="shared" ref="V24" si="33">T24</f>
         <v>26000</v>
       </c>
-      <c r="W24" s="18"/>
-      <c r="X24" s="18">
+      <c r="W24" s="17"/>
+      <c r="X24" s="17">
         <f>V24*2</f>
         <v>52000</v>
       </c>
-      <c r="Y24" s="18"/>
+      <c r="Y24" s="17"/>
       <c r="Z24" s="5"/>
       <c r="AA24" s="5"/>
     </row>
@@ -3823,66 +3823,66 @@
       <c r="A25" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="20">
         <f>B22*B23*B24</f>
         <v>8192000</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19">
+      <c r="C25" s="20"/>
+      <c r="D25" s="20">
         <f>D22*D23*D24</f>
         <v>1277952000</v>
       </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19">
+      <c r="E25" s="20"/>
+      <c r="F25" s="20">
         <f t="shared" ref="F25" si="34">F22*F23*F24</f>
         <v>1277952000</v>
       </c>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19">
+      <c r="G25" s="20"/>
+      <c r="H25" s="20">
         <f t="shared" ref="H25" si="35">H22*H23*H24</f>
         <v>1277952000</v>
       </c>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19">
+      <c r="I25" s="20"/>
+      <c r="J25" s="20">
         <f t="shared" ref="J25" si="36">J22*J23*J24</f>
         <v>1277952000</v>
       </c>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19">
+      <c r="K25" s="20"/>
+      <c r="L25" s="20">
         <f>L22*L23*L24</f>
         <v>1277952000</v>
       </c>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19">
+      <c r="M25" s="20"/>
+      <c r="N25" s="20">
         <f t="shared" ref="N25:X25" si="37">N22*N23*N24</f>
         <v>20447232000</v>
       </c>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19">
+      <c r="O25" s="20"/>
+      <c r="P25" s="20">
         <f t="shared" si="37"/>
         <v>20447232000</v>
       </c>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="19">
+      <c r="Q25" s="20"/>
+      <c r="R25" s="20">
         <f t="shared" si="37"/>
         <v>20447232000</v>
       </c>
-      <c r="S25" s="19"/>
-      <c r="T25" s="19">
+      <c r="S25" s="20"/>
+      <c r="T25" s="20">
         <f t="shared" si="37"/>
         <v>20447232000</v>
       </c>
-      <c r="U25" s="19"/>
-      <c r="V25" s="19">
+      <c r="U25" s="20"/>
+      <c r="V25" s="20">
         <f t="shared" si="37"/>
         <v>20447232000</v>
       </c>
-      <c r="W25" s="19"/>
-      <c r="X25" s="19">
+      <c r="W25" s="20"/>
+      <c r="X25" s="20">
         <f t="shared" si="37"/>
         <v>40894464000</v>
       </c>
-      <c r="Y25" s="19"/>
+      <c r="Y25" s="20"/>
       <c r="Z25" s="8"/>
       <c r="AA25" s="8"/>
     </row>
@@ -3890,410 +3890,455 @@
       <c r="A26" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" s="19">
         <f>0.191+9.964+1.804+1.666</f>
         <v>13.625000000000002</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20">
+      <c r="C26" s="19"/>
+      <c r="D26" s="19">
         <v>25.887</v>
       </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20">
+      <c r="E26" s="19"/>
+      <c r="F26" s="19">
         <v>21.568000000000001</v>
       </c>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20">
+      <c r="G26" s="19"/>
+      <c r="H26" s="19">
         <v>21.541</v>
       </c>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20">
+      <c r="I26" s="19"/>
+      <c r="J26" s="19">
         <v>9.1859999999999999</v>
       </c>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20">
+      <c r="K26" s="19"/>
+      <c r="L26" s="19">
         <v>1.1519999999999999</v>
       </c>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20">
+      <c r="M26" s="19"/>
+      <c r="N26" s="19">
         <v>14.536</v>
       </c>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20">
+      <c r="O26" s="19"/>
+      <c r="P26" s="19">
         <v>5.0839999999999996</v>
       </c>
-      <c r="Q26" s="20"/>
-      <c r="R26" s="20">
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19">
         <f>0.874+3.15</f>
         <v>4.024</v>
       </c>
-      <c r="S26" s="20"/>
-      <c r="T26" s="20">
+      <c r="S26" s="19"/>
+      <c r="T26" s="19">
         <v>5.891</v>
       </c>
-      <c r="U26" s="20"/>
-      <c r="V26" s="20">
+      <c r="U26" s="19"/>
+      <c r="V26" s="19">
         <v>11.195</v>
       </c>
-      <c r="W26" s="20"/>
-      <c r="X26" s="20">
+      <c r="W26" s="19"/>
+      <c r="X26" s="19">
         <v>7.8550000000000004</v>
       </c>
-      <c r="Y26" s="20"/>
+      <c r="Y26" s="19"/>
     </row>
     <row r="27" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="20">
+      <c r="B27" s="19">
         <f>19.37+17.15</f>
         <v>36.519999999999996</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20">
+      <c r="C27" s="19"/>
+      <c r="D27" s="19">
         <v>146.75</v>
       </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20">
+      <c r="E27" s="19"/>
+      <c r="F27" s="19">
         <v>180.85</v>
       </c>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20">
+      <c r="G27" s="19"/>
+      <c r="H27" s="19">
         <v>166.69</v>
       </c>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20">
+      <c r="I27" s="19"/>
+      <c r="J27" s="19">
         <v>128.34</v>
       </c>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20">
+      <c r="K27" s="19"/>
+      <c r="L27" s="19">
         <v>23.66</v>
       </c>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20">
+      <c r="M27" s="19"/>
+      <c r="N27" s="19">
         <v>108.08</v>
       </c>
-      <c r="O27" s="20"/>
-      <c r="P27" s="20">
+      <c r="O27" s="19"/>
+      <c r="P27" s="19">
         <v>62.75</v>
       </c>
-      <c r="Q27" s="20"/>
-      <c r="R27" s="20">
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19">
         <v>56.74</v>
       </c>
-      <c r="S27" s="20"/>
-      <c r="T27" s="20">
+      <c r="S27" s="19"/>
+      <c r="T27" s="19">
         <v>67.02</v>
       </c>
-      <c r="U27" s="20"/>
-      <c r="V27" s="20">
+      <c r="U27" s="19"/>
+      <c r="V27" s="19">
         <v>72.900000000000006</v>
       </c>
-      <c r="W27" s="20"/>
-      <c r="X27" s="20">
+      <c r="W27" s="19"/>
+      <c r="X27" s="19">
         <v>80.45</v>
       </c>
-      <c r="Y27" s="20"/>
+      <c r="Y27" s="19"/>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="17">
+      <c r="B28" s="18">
         <f>B26/512/8/2000*B$25</f>
         <v>13.625000000000002</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17">
+      <c r="C28" s="18"/>
+      <c r="D28" s="18">
         <f>D26/6144/8/4000*D$25</f>
         <v>168.2655</v>
       </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17">
+      <c r="E28" s="18"/>
+      <c r="F28" s="18">
         <f t="shared" ref="F28:F29" si="38">F26/6144/8/4000*F$25</f>
         <v>140.19200000000001</v>
       </c>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17">
+      <c r="G28" s="18"/>
+      <c r="H28" s="18">
         <f t="shared" ref="H28:H29" si="39">H26/6144/8/4000*H$25</f>
         <v>140.01650000000001</v>
       </c>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17">
+      <c r="I28" s="18"/>
+      <c r="J28" s="18">
         <f t="shared" ref="J28:J29" si="40">J26/6144/8/4000*J$25</f>
         <v>59.708999999999996</v>
       </c>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17">
+      <c r="K28" s="18"/>
+      <c r="L28" s="18">
         <f>L26/512/8/1600*L$25</f>
         <v>224.64</v>
       </c>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17">
+      <c r="M28" s="18"/>
+      <c r="N28" s="18">
         <f>N26/4096/8/3200*N$25</f>
         <v>2834.52</v>
       </c>
-      <c r="O28" s="17"/>
-      <c r="P28" s="17">
+      <c r="O28" s="18"/>
+      <c r="P28" s="18">
         <f t="shared" ref="P28:P29" si="41">P26/4096/8/3200*P$25</f>
         <v>991.37999999999988</v>
       </c>
-      <c r="Q28" s="17"/>
-      <c r="R28" s="17">
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18">
         <f t="shared" ref="R28:R29" si="42">R26/4096/8/3200*R$25</f>
         <v>784.68</v>
       </c>
-      <c r="S28" s="17"/>
-      <c r="T28" s="17">
+      <c r="S28" s="18"/>
+      <c r="T28" s="18">
         <f t="shared" ref="T28:T29" si="43">T26/4096/8/3200*T$25</f>
         <v>1148.7449999999999</v>
       </c>
-      <c r="U28" s="17"/>
-      <c r="V28" s="17">
+      <c r="U28" s="18"/>
+      <c r="V28" s="18">
         <f t="shared" ref="V28:V29" si="44">V26/4096/8/3200*V$25</f>
         <v>2183.0250000000001</v>
       </c>
-      <c r="W28" s="17"/>
-      <c r="X28" s="17">
+      <c r="W28" s="18"/>
+      <c r="X28" s="18">
         <f t="shared" ref="X28:X29" si="45">X26/4096/8/3200*X$25</f>
         <v>3063.4500000000003</v>
       </c>
-      <c r="Y28" s="17"/>
+      <c r="Y28" s="18"/>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="17">
+      <c r="B29" s="18">
         <f>B27/512/8/2000*B$25</f>
         <v>36.519999999999996</v>
       </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17">
+      <c r="C29" s="18"/>
+      <c r="D29" s="18">
         <f>D27/6144/8/4000*D$25</f>
         <v>953.875</v>
       </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17">
+      <c r="E29" s="18"/>
+      <c r="F29" s="18">
         <f t="shared" si="38"/>
         <v>1175.5250000000001</v>
       </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17">
+      <c r="G29" s="18"/>
+      <c r="H29" s="18">
         <f t="shared" si="39"/>
         <v>1083.4849999999999</v>
       </c>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17">
+      <c r="I29" s="18"/>
+      <c r="J29" s="18">
         <f t="shared" si="40"/>
         <v>834.20999999999992</v>
       </c>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17">
+      <c r="K29" s="18"/>
+      <c r="L29" s="18">
         <f>L27/512/8/1600*L$25</f>
         <v>4613.7</v>
       </c>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17">
+      <c r="M29" s="18"/>
+      <c r="N29" s="18">
         <f>N27/4096/8/3200*N$25</f>
         <v>21075.599999999999</v>
       </c>
-      <c r="O29" s="17"/>
-      <c r="P29" s="17">
+      <c r="O29" s="18"/>
+      <c r="P29" s="18">
         <f t="shared" si="41"/>
         <v>12236.249999999998</v>
       </c>
-      <c r="Q29" s="17"/>
-      <c r="R29" s="17">
+      <c r="Q29" s="18"/>
+      <c r="R29" s="18">
         <f t="shared" si="42"/>
         <v>11064.300000000001</v>
       </c>
-      <c r="S29" s="17"/>
-      <c r="T29" s="17">
+      <c r="S29" s="18"/>
+      <c r="T29" s="18">
         <f t="shared" si="43"/>
         <v>13068.899999999998</v>
       </c>
-      <c r="U29" s="17"/>
-      <c r="V29" s="17">
+      <c r="U29" s="18"/>
+      <c r="V29" s="18">
         <f t="shared" si="44"/>
         <v>14215.500000000002</v>
       </c>
-      <c r="W29" s="17"/>
-      <c r="X29" s="17">
+      <c r="W29" s="18"/>
+      <c r="X29" s="18">
         <f t="shared" si="45"/>
         <v>31375.5</v>
       </c>
-      <c r="Y29" s="17"/>
+      <c r="Y29" s="18"/>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="18">
+      <c r="B30" s="17">
         <v>1</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18">
+      <c r="C30" s="17"/>
+      <c r="D30" s="17">
         <v>1</v>
       </c>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18">
+      <c r="E30" s="17"/>
+      <c r="F30" s="17">
         <v>1</v>
       </c>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18">
+      <c r="G30" s="17"/>
+      <c r="H30" s="17">
         <v>1</v>
       </c>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18">
+      <c r="I30" s="17"/>
+      <c r="J30" s="17">
         <v>1</v>
       </c>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18">
+      <c r="K30" s="17"/>
+      <c r="L30" s="17">
         <v>1</v>
       </c>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18">
+      <c r="M30" s="17"/>
+      <c r="N30" s="17">
         <v>1</v>
       </c>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18">
+      <c r="O30" s="17"/>
+      <c r="P30" s="17">
         <v>1</v>
       </c>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="18">
+      <c r="Q30" s="17"/>
+      <c r="R30" s="17">
         <v>1</v>
       </c>
-      <c r="S30" s="18"/>
-      <c r="T30" s="18">
+      <c r="S30" s="17"/>
+      <c r="T30" s="17">
         <v>1</v>
       </c>
-      <c r="U30" s="18"/>
-      <c r="V30" s="18">
+      <c r="U30" s="17"/>
+      <c r="V30" s="17">
         <v>1</v>
       </c>
-      <c r="W30" s="18"/>
-      <c r="X30" s="18">
+      <c r="W30" s="17"/>
+      <c r="X30" s="17">
         <v>1</v>
       </c>
-      <c r="Y30" s="18"/>
-      <c r="Z30" s="17"/>
-      <c r="AA30" s="17"/>
+      <c r="Y30" s="17"/>
+      <c r="Z30" s="18"/>
+      <c r="AA30" s="18"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="21">
+      <c r="B31" s="16">
         <f>(B28+B29*B30)/86400</f>
         <v>5.8038194444444435E-4</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21">
+      <c r="C31" s="16"/>
+      <c r="D31" s="16">
         <f t="shared" ref="D31:F31" si="46">(D28+D29*D30)/86400</f>
         <v>1.2987737268518517E-2</v>
       </c>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21">
+      <c r="E31" s="16"/>
+      <c r="F31" s="16">
         <f t="shared" si="46"/>
         <v>1.5228206018518519E-2</v>
       </c>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21">
+      <c r="G31" s="16"/>
+      <c r="H31" s="16">
         <f t="shared" ref="H31" si="47">(H28+H29*H30)/86400</f>
         <v>1.4160896990740739E-2</v>
       </c>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21">
+      <c r="I31" s="16"/>
+      <c r="J31" s="16">
         <f t="shared" ref="J31" si="48">(J28+J29*J30)/86400</f>
         <v>1.034628472222222E-2</v>
       </c>
-      <c r="K31" s="21"/>
-      <c r="L31" s="21">
+      <c r="K31" s="16"/>
+      <c r="L31" s="16">
         <f t="shared" ref="L31:N31" si="49">(L28+L29*L30)/86400</f>
         <v>5.5999305555555559E-2</v>
       </c>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21">
+      <c r="M31" s="16"/>
+      <c r="N31" s="16">
         <f t="shared" si="49"/>
         <v>0.27673749999999997</v>
       </c>
-      <c r="O31" s="21"/>
-      <c r="P31" s="21">
+      <c r="O31" s="16"/>
+      <c r="P31" s="16">
         <f>(P28+P29*P30+R28)/86400</f>
         <v>0.16217951388888885</v>
       </c>
-      <c r="Q31" s="21"/>
-      <c r="R31" s="21">
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16">
         <f>(R28+R29*R30+T28)/86400</f>
         <v>0.15043663194444448</v>
       </c>
-      <c r="S31" s="21"/>
-      <c r="T31" s="21">
+      <c r="S31" s="16"/>
+      <c r="T31" s="16">
         <f t="shared" ref="T31:X31" si="50">(T28+T29*T30)/86400</f>
         <v>0.16455607638888886</v>
       </c>
-      <c r="U31" s="21"/>
-      <c r="V31" s="21">
+      <c r="U31" s="16"/>
+      <c r="V31" s="16">
         <f t="shared" si="50"/>
         <v>0.18979774305555558</v>
       </c>
-      <c r="W31" s="21"/>
-      <c r="X31" s="21">
+      <c r="W31" s="16"/>
+      <c r="X31" s="16">
         <f t="shared" si="50"/>
         <v>0.39859895833333331</v>
       </c>
-      <c r="Y31" s="21"/>
+      <c r="Y31" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="163">
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="P31:Q31"/>
-    <mergeCell ref="R31:S31"/>
-    <mergeCell ref="T31:U31"/>
-    <mergeCell ref="V31:W31"/>
-    <mergeCell ref="X31:Y31"/>
-    <mergeCell ref="V28:W28"/>
-    <mergeCell ref="X28:Y28"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="R29:S29"/>
-    <mergeCell ref="V29:W29"/>
-    <mergeCell ref="X29:Y29"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="R30:S30"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="X30:Y30"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="X25:Y25"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="R26:S26"/>
-    <mergeCell ref="V26:W26"/>
-    <mergeCell ref="X26:Y26"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="R27:S27"/>
-    <mergeCell ref="V27:W27"/>
-    <mergeCell ref="X27:Y27"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="X16:Y16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="T21:U21"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="X21:Y21"/>
+    <mergeCell ref="Z21:AA21"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="Z23:AA23"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="Z30:AA30"/>
+    <mergeCell ref="X24:Y24"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="T25:U25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="D29:E29"/>
@@ -4318,98 +4363,53 @@
     <mergeCell ref="N28:O28"/>
     <mergeCell ref="P28:Q28"/>
     <mergeCell ref="R28:S28"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="Z23:AA23"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="R24:S24"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="Z30:AA30"/>
-    <mergeCell ref="X24:Y24"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="T25:U25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="T21:U21"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="X21:Y21"/>
-    <mergeCell ref="Z21:AA21"/>
-    <mergeCell ref="X22:Y22"/>
-    <mergeCell ref="Z22:AA22"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="X16:Y16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="X25:Y25"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="R26:S26"/>
+    <mergeCell ref="V26:W26"/>
+    <mergeCell ref="X26:Y26"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="R27:S27"/>
+    <mergeCell ref="V27:W27"/>
+    <mergeCell ref="X27:Y27"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="P31:Q31"/>
+    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="T31:U31"/>
+    <mergeCell ref="V31:W31"/>
+    <mergeCell ref="X31:Y31"/>
+    <mergeCell ref="V28:W28"/>
+    <mergeCell ref="X28:Y28"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="R29:S29"/>
+    <mergeCell ref="V29:W29"/>
+    <mergeCell ref="X29:Y29"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="R30:S30"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="X30:Y30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update: demo code for Oleg
</commit_message>
<xml_diff>
--- a/Sampling_Resolution_Calculator.xlsx
+++ b/Sampling_Resolution_Calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nanw0\GoogleDrive\SLAC\SLAC-Diling\11. 21 Winter\DXS optics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DC94C7-E1EC-4D96-8598-30183B5B3C96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C425473C-AFF6-47E7-ABAA-7E280437DDEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="5070" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="735" windowWidth="17580" windowHeight="15090" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HHLM" sheetId="10" r:id="rId1"/>
@@ -482,22 +482,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -808,10 +808,10 @@
       <c r="A1" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="21"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -820,10 +820,10 @@
       <c r="B2">
         <v>9481</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="21"/>
+      <c r="E2" s="16"/>
       <c r="F2">
         <v>19.909876918386299</v>
       </c>
@@ -846,10 +846,10 @@
       <c r="B3">
         <v>20</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="21"/>
+      <c r="E3" s="16"/>
       <c r="F3">
         <v>17</v>
       </c>
@@ -868,10 +868,10 @@
       <c r="B4" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="21"/>
+      <c r="E4" s="16"/>
       <c r="F4">
         <f>SIN(RADIANS(F2+F3))/SIN(RADIANS(F2-F3))</f>
         <v>11.830135875287004</v>
@@ -895,10 +895,10 @@
       <c r="B5" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="21"/>
+      <c r="E5" s="16"/>
       <c r="F5">
         <f>ABS((COS(RADIANS(F2-F3))-COS(RADIANS(F2+F3)))/SIN(RADIANS(F2-F3)))</f>
         <v>3.9225661843587014</v>
@@ -924,10 +924,10 @@
         <f>B3/10</f>
         <v>2</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="21"/>
+      <c r="E8" s="16"/>
       <c r="F8" s="1">
         <v>5.9999999999999997E-7</v>
       </c>
@@ -947,10 +947,10 @@
         <f>4/B8</f>
         <v>2</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="21"/>
+      <c r="E9" s="16"/>
       <c r="F9" s="7">
         <f>SUM(28:28)/86400</f>
         <v>6.0394444444444445E-3</v>
@@ -964,20 +964,20 @@
         <f>MIN(B9/400,0.001)</f>
         <v>1E-3</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="21"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="7">
         <f>SUM(31:31)-F9</f>
         <v>4.7264062499999995E-2</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="21"/>
+      <c r="E11" s="16"/>
       <c r="F11" s="10">
         <f>SUM(31:31)</f>
         <v>5.330350694444444E-2</v>
@@ -1015,26 +1015,26 @@
       <c r="A16" t="s">
         <v>89</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21" t="s">
+      <c r="C16" s="16"/>
+      <c r="D16" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21" t="s">
+      <c r="E16" s="16"/>
+      <c r="F16" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21" t="s">
+      <c r="G16" s="16"/>
+      <c r="H16" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21" t="s">
+      <c r="I16" s="16"/>
+      <c r="J16" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="K16" s="21"/>
+      <c r="K16" s="16"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
@@ -1228,317 +1228,317 @@
       <c r="A21" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="17">
         <v>722.7</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18">
+      <c r="C21" s="17"/>
+      <c r="D21" s="17">
         <f>B21*J2</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18">
+      <c r="E21" s="17"/>
+      <c r="F21" s="17">
         <f>D21</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18">
+      <c r="G21" s="17"/>
+      <c r="H21" s="17">
         <f>F21</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18">
+      <c r="I21" s="17"/>
+      <c r="J21" s="17">
         <f>H21/J2</f>
         <v>722.7</v>
       </c>
-      <c r="K21" s="18"/>
+      <c r="K21" s="17"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="17">
+      <c r="B22" s="18">
         <f>B12</f>
         <v>512</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17">
+      <c r="C22" s="18"/>
+      <c r="D22" s="18">
         <f>B22*I2</f>
         <v>6144</v>
       </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17">
+      <c r="E22" s="18"/>
+      <c r="F22" s="18">
         <f>D22</f>
         <v>6144</v>
       </c>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17">
+      <c r="G22" s="18"/>
+      <c r="H22" s="18">
         <f>F22</f>
         <v>6144</v>
       </c>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17">
+      <c r="I22" s="18"/>
+      <c r="J22" s="18">
         <f t="shared" ref="J22:J24" si="7">H22</f>
         <v>6144</v>
       </c>
-      <c r="K22" s="17"/>
+      <c r="K22" s="18"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="18">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17">
+      <c r="C23" s="18"/>
+      <c r="D23" s="18">
         <f t="shared" ref="D23" si="8">B23</f>
         <v>8</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17">
+      <c r="E23" s="18"/>
+      <c r="F23" s="18">
         <f t="shared" ref="F23" si="9">D23</f>
         <v>8</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17">
+      <c r="G23" s="18"/>
+      <c r="H23" s="18">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17">
+      <c r="I23" s="18"/>
+      <c r="J23" s="18">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="K23" s="17"/>
+      <c r="K23" s="18"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="17">
+      <c r="B24" s="18">
         <f>B14</f>
         <v>2000</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17">
+      <c r="C24" s="18"/>
+      <c r="D24" s="18">
         <f>B24*I4</f>
         <v>26000</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17">
+      <c r="E24" s="18"/>
+      <c r="F24" s="18">
         <f>D24</f>
         <v>26000</v>
       </c>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17">
+      <c r="G24" s="18"/>
+      <c r="H24" s="18">
         <f t="shared" ref="H24" si="10">F24</f>
         <v>26000</v>
       </c>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17">
+      <c r="I24" s="18"/>
+      <c r="J24" s="18">
         <f t="shared" si="7"/>
         <v>26000</v>
       </c>
-      <c r="K24" s="17"/>
+      <c r="K24" s="18"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="20">
+      <c r="B25" s="19">
         <f>B22*B23*B24</f>
         <v>8192000</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20">
+      <c r="C25" s="19"/>
+      <c r="D25" s="19">
         <f>D22*D23*D24</f>
         <v>1277952000</v>
       </c>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20">
+      <c r="E25" s="19"/>
+      <c r="F25" s="19">
         <f t="shared" ref="F25" si="11">F22*F23*F24</f>
         <v>1277952000</v>
       </c>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20">
+      <c r="G25" s="19"/>
+      <c r="H25" s="19">
         <f t="shared" ref="H25" si="12">H22*H23*H24</f>
         <v>1277952000</v>
       </c>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20">
+      <c r="I25" s="19"/>
+      <c r="J25" s="19">
         <f t="shared" ref="J25" si="13">J22*J23*J24</f>
         <v>1277952000</v>
       </c>
-      <c r="K25" s="20"/>
+      <c r="K25" s="19"/>
     </row>
     <row r="26" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="19">
+      <c r="B26" s="20">
         <f>0.191+9.964+1.804+1.666</f>
         <v>13.625000000000002</v>
       </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19">
+      <c r="C26" s="20"/>
+      <c r="D26" s="20">
         <v>25.887</v>
       </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19">
+      <c r="E26" s="20"/>
+      <c r="F26" s="20">
         <v>21.568000000000001</v>
       </c>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19">
+      <c r="G26" s="20"/>
+      <c r="H26" s="20">
         <v>21.541</v>
       </c>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19">
+      <c r="I26" s="20"/>
+      <c r="J26" s="20">
         <v>9.1859999999999999</v>
       </c>
-      <c r="K26" s="19"/>
+      <c r="K26" s="20"/>
     </row>
     <row r="27" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="19">
+      <c r="B27" s="20">
         <f>19.37+17.15</f>
         <v>36.519999999999996</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19">
+      <c r="C27" s="20"/>
+      <c r="D27" s="20">
         <v>146.75</v>
       </c>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19">
+      <c r="E27" s="20"/>
+      <c r="F27" s="20">
         <v>180.85</v>
       </c>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19">
+      <c r="G27" s="20"/>
+      <c r="H27" s="20">
         <v>166.69</v>
       </c>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19">
+      <c r="I27" s="20"/>
+      <c r="J27" s="20">
         <v>128.34</v>
       </c>
-      <c r="K27" s="19"/>
+      <c r="K27" s="20"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="17">
         <f>B26/512/8/2000*B$25</f>
         <v>13.625000000000002</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18">
+      <c r="C28" s="17"/>
+      <c r="D28" s="17">
         <f>D26/6144/8/4000*D$25</f>
         <v>168.2655</v>
       </c>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18">
+      <c r="E28" s="17"/>
+      <c r="F28" s="17">
         <f t="shared" ref="F28" si="14">F26/6144/8/4000*F$25</f>
         <v>140.19200000000001</v>
       </c>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18">
+      <c r="G28" s="17"/>
+      <c r="H28" s="17">
         <f t="shared" ref="H28" si="15">H26/6144/8/4000*H$25</f>
         <v>140.01650000000001</v>
       </c>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18">
+      <c r="I28" s="17"/>
+      <c r="J28" s="17">
         <f t="shared" ref="J28" si="16">J26/6144/8/4000*J$25</f>
         <v>59.708999999999996</v>
       </c>
-      <c r="K28" s="18"/>
+      <c r="K28" s="17"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="18">
+      <c r="B29" s="17">
         <f>B27/512/8/2000*B$25</f>
         <v>36.519999999999996</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18">
+      <c r="C29" s="17"/>
+      <c r="D29" s="17">
         <f>D27/6144/8/4000*D$25</f>
         <v>953.875</v>
       </c>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18">
+      <c r="E29" s="17"/>
+      <c r="F29" s="17">
         <f t="shared" ref="F29" si="17">F27/6144/8/4000*F$25</f>
         <v>1175.5250000000001</v>
       </c>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18">
+      <c r="G29" s="17"/>
+      <c r="H29" s="17">
         <f t="shared" ref="H29" si="18">H27/6144/8/4000*H$25</f>
         <v>1083.4849999999999</v>
       </c>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18">
+      <c r="I29" s="17"/>
+      <c r="J29" s="17">
         <f t="shared" ref="J29" si="19">J27/6144/8/4000*J$25</f>
         <v>834.20999999999992</v>
       </c>
-      <c r="K29" s="18"/>
+      <c r="K29" s="17"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="17">
+      <c r="B30" s="18">
         <v>1</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17">
+      <c r="C30" s="18"/>
+      <c r="D30" s="18">
         <v>1</v>
       </c>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17">
+      <c r="E30" s="18"/>
+      <c r="F30" s="18">
         <v>1</v>
       </c>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17">
+      <c r="G30" s="18"/>
+      <c r="H30" s="18">
         <v>1</v>
       </c>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17">
+      <c r="I30" s="18"/>
+      <c r="J30" s="18">
         <v>1</v>
       </c>
-      <c r="K30" s="17"/>
+      <c r="K30" s="18"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="16">
+      <c r="B31" s="21">
         <f>(B28+B29*B30)/86400</f>
         <v>5.8038194444444435E-4</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16">
+      <c r="C31" s="21"/>
+      <c r="D31" s="21">
         <f t="shared" ref="D31:F31" si="20">(D28+D29*D30)/86400</f>
         <v>1.2987737268518517E-2</v>
       </c>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16">
+      <c r="E31" s="21"/>
+      <c r="F31" s="21">
         <f t="shared" si="20"/>
         <v>1.5228206018518519E-2</v>
       </c>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16">
+      <c r="G31" s="21"/>
+      <c r="H31" s="21">
         <f t="shared" ref="H31" si="21">(H28+H29*H30)/86400</f>
         <v>1.4160896990740739E-2</v>
       </c>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16">
+      <c r="I31" s="21"/>
+      <c r="J31" s="21">
         <f t="shared" ref="J31" si="22">(J28+J29*J30)/86400</f>
         <v>1.034628472222222E-2</v>
       </c>
-      <c r="K31" s="16"/>
+      <c r="K31" s="21"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="E32" s="6"/>
@@ -1550,6 +1550,66 @@
     </row>
   </sheetData>
   <mergeCells count="69">
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="F16:G16"/>
@@ -1559,66 +1619,6 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:K31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1630,7 +1630,7 @@
   <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1658,10 +1658,10 @@
       <c r="A1" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="21"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1670,10 +1670,10 @@
       <c r="B2">
         <v>9481</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="21"/>
+      <c r="E2" s="16"/>
       <c r="F2">
         <v>42.926477759350803</v>
       </c>
@@ -1694,12 +1694,12 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>100</v>
-      </c>
-      <c r="D3" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="21"/>
+      <c r="E3" s="16"/>
       <c r="F3">
         <v>-29.5</v>
       </c>
@@ -1719,10 +1719,10 @@
         <f>0.005</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="21"/>
+      <c r="E4" s="16"/>
       <c r="F4">
         <f>SIN(RADIANS(F2+F3))/SIN(RADIANS(F2-F3))</f>
         <v>0.24356450463759297</v>
@@ -1732,11 +1732,11 @@
       </c>
       <c r="I4" s="2">
         <f>MAX(ROUND(2*I3/$B7,0),1)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J4">
         <f>I3/$B7</f>
-        <v>1.4657811346760605</v>
+        <v>2.9315622693521211</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -1747,10 +1747,10 @@
         <f>0.005</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="21"/>
+      <c r="E5" s="16"/>
       <c r="F5">
         <f>ABS((COS(RADIANS(F2-F3))-COS(RADIANS(F2+F3)))/SIN(RADIANS(F2-F3)))</f>
         <v>0.70357494464450898</v>
@@ -1765,7 +1765,7 @@
       </c>
       <c r="B7">
         <f>B8*B14</f>
-        <v>8000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
@@ -1774,12 +1774,12 @@
       </c>
       <c r="B8">
         <f>B3/10</f>
-        <v>10</v>
-      </c>
-      <c r="D8" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="21"/>
+      <c r="E8" s="16"/>
       <c r="F8" s="1">
         <v>5.9999999999999997E-7</v>
       </c>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="I8" s="9">
         <f>22122874/1024/1024/3072/8/26000*MAX(25:25)</f>
-        <v>20.773431865985575</v>
+        <v>103.86715932992787</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
@@ -1797,15 +1797,15 @@
       </c>
       <c r="B9">
         <f>4/B8</f>
-        <v>0.4</v>
-      </c>
-      <c r="D9" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="21"/>
+      <c r="E9" s="16"/>
       <c r="F9" s="7">
         <f>SUM(28:28)/86400</f>
-        <v>3.4652546296296298E-3</v>
+        <v>1.7098032407407406E-2</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
@@ -1814,25 +1814,25 @@
       </c>
       <c r="B10">
         <f>MIN(B9/800,0.001)</f>
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="D10" s="21" t="s">
+        <v>1E-3</v>
+      </c>
+      <c r="D10" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="21"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="7">
         <f>SUM(31:31)-F9</f>
-        <v>3.2246296296296301E-2</v>
+        <v>0.16010445601851853</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="21"/>
+      <c r="E11" s="16"/>
       <c r="F11" s="10">
         <f>SUM(31:31)</f>
-        <v>3.5711550925925928E-2</v>
+        <v>0.17720248842592592</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
@@ -1860,47 +1860,47 @@
       </c>
       <c r="B14">
         <f>B9/B10</f>
-        <v>800</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>88</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21" t="s">
+      <c r="C16" s="16"/>
+      <c r="D16" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21" t="s">
+      <c r="E16" s="16"/>
+      <c r="F16" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21" t="s">
+      <c r="G16" s="16"/>
+      <c r="H16" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21" t="s">
+      <c r="I16" s="16"/>
+      <c r="J16" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21" t="s">
+      <c r="K16" s="16"/>
+      <c r="L16" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21" t="s">
+      <c r="M16" s="16"/>
+      <c r="N16" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="O16" s="21"/>
-      <c r="P16" s="21" t="s">
+      <c r="O16" s="16"/>
+      <c r="P16" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="21"/>
-      <c r="S16" s="21"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
@@ -2050,19 +2050,19 @@
       </c>
       <c r="B19" s="2">
         <f>B7</f>
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="C19" s="2">
         <f>B8</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D19" s="2">
         <f>E19*D24</f>
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="E19" s="2">
         <f>C19</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F19" s="2">
         <f>G19*F24</f>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="G19" s="2">
         <f>E19</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H19" s="2">
         <f>I19*H24</f>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="I19" s="2">
         <f>G19</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J19" s="2">
         <f>K19*J24</f>
@@ -2086,7 +2086,7 @@
       </c>
       <c r="K19" s="2">
         <f>I19</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="L19" s="2">
         <f>M19*L24</f>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="M19" s="2">
         <f>K19</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="N19" s="2">
         <f>O19*N24</f>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="O19" s="2">
         <f>M19</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="P19" s="2">
         <f>Q19*P24</f>
@@ -2110,7 +2110,7 @@
       </c>
       <c r="Q19" s="2">
         <f>O19</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
@@ -2121,23 +2121,23 @@
       </c>
       <c r="B20" s="2">
         <f>B9*1000</f>
-        <v>400</v>
+        <v>2000</v>
       </c>
       <c r="C20" s="2">
         <f>B10*1000</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D20" s="2">
         <f>$B20*$C19/E19</f>
-        <v>400</v>
+        <v>2000</v>
       </c>
       <c r="E20" s="2">
         <f>$B19*$C20/D19</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F20" s="2">
         <f>$B20*$C19/G19</f>
-        <v>400</v>
+        <v>2000</v>
       </c>
       <c r="G20" s="2">
         <f>$B19*$C20/F19</f>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="H20" s="2">
         <f t="shared" ref="H20" si="6">$B20*$C19/I19</f>
-        <v>400</v>
+        <v>2000</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" ref="I20" si="7">$B19*$C20/H19</f>
@@ -2153,7 +2153,7 @@
       </c>
       <c r="J20" s="2">
         <f t="shared" ref="J20" si="8">$B20*$C19/K19</f>
-        <v>400</v>
+        <v>2000</v>
       </c>
       <c r="K20" s="2">
         <f t="shared" ref="K20" si="9">$B19*$C20/J19</f>
@@ -2161,7 +2161,7 @@
       </c>
       <c r="L20" s="2">
         <f t="shared" ref="L20" si="10">$B20*$C19/M19</f>
-        <v>400</v>
+        <v>2000</v>
       </c>
       <c r="M20" s="2">
         <f t="shared" ref="M20" si="11">$B19*$C20/L19</f>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="N20" s="2">
         <f t="shared" ref="N20" si="12">$B20*$C19/O19</f>
-        <v>400</v>
+        <v>2000</v>
       </c>
       <c r="O20" s="2">
         <f t="shared" ref="O20" si="13">$B19*$C20/N19</f>
@@ -2177,7 +2177,7 @@
       </c>
       <c r="P20" s="2">
         <f t="shared" ref="P20" si="14">$B20*$C19/Q19</f>
-        <v>400</v>
+        <v>2000</v>
       </c>
       <c r="Q20" s="2">
         <f t="shared" ref="Q20" si="15">$B19*$C20/P19</f>
@@ -2190,38 +2190,38 @@
       <c r="A21" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="17">
         <v>726.57</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18">
+      <c r="C21" s="17"/>
+      <c r="D21" s="17">
         <v>722.86</v>
       </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18">
+      <c r="E21" s="17"/>
+      <c r="F21" s="17">
         <v>722.85</v>
       </c>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18">
+      <c r="G21" s="17"/>
+      <c r="H21" s="17">
         <v>176.54</v>
       </c>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18">
+      <c r="I21" s="17"/>
+      <c r="J21" s="17">
         <v>14.28</v>
       </c>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18">
+      <c r="K21" s="17"/>
+      <c r="L21" s="17">
         <v>175.15</v>
       </c>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18">
+      <c r="M21" s="17"/>
+      <c r="N21" s="17">
         <v>173.04</v>
       </c>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18">
+      <c r="O21" s="17"/>
+      <c r="P21" s="17">
         <v>173.07</v>
       </c>
-      <c r="Q21" s="18"/>
+      <c r="Q21" s="17"/>
       <c r="R21" s="12"/>
       <c r="S21" s="12"/>
     </row>
@@ -2229,187 +2229,187 @@
       <c r="A22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="17">
+      <c r="B22" s="18">
         <f>B12</f>
         <v>1024</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17">
+      <c r="C22" s="18"/>
+      <c r="D22" s="18">
         <f>B22</f>
         <v>1024</v>
       </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17">
+      <c r="E22" s="18"/>
+      <c r="F22" s="18">
         <f>D22*I2*8</f>
         <v>32768</v>
       </c>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17">
+      <c r="G22" s="18"/>
+      <c r="H22" s="18">
         <f>F22</f>
         <v>32768</v>
       </c>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17">
+      <c r="I22" s="18"/>
+      <c r="J22" s="18">
         <f t="shared" ref="J22:J24" si="16">H22</f>
         <v>32768</v>
       </c>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17">
+      <c r="K22" s="18"/>
+      <c r="L22" s="18">
         <f t="shared" ref="L22:L24" si="17">J22</f>
         <v>32768</v>
       </c>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17">
+      <c r="M22" s="18"/>
+      <c r="N22" s="18">
         <f>L22</f>
         <v>32768</v>
       </c>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17">
+      <c r="O22" s="18"/>
+      <c r="P22" s="18">
         <f t="shared" ref="P22:P23" si="18">N22</f>
         <v>32768</v>
       </c>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="17"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="18"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="18">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17">
+      <c r="C23" s="18"/>
+      <c r="D23" s="18">
         <f t="shared" ref="D23:D24" si="19">B23</f>
         <v>8</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17">
+      <c r="E23" s="18"/>
+      <c r="F23" s="18">
         <f t="shared" ref="F23" si="20">D23</f>
         <v>8</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17">
+      <c r="G23" s="18"/>
+      <c r="H23" s="18">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17">
+      <c r="I23" s="18"/>
+      <c r="J23" s="18">
         <f t="shared" si="16"/>
         <v>8</v>
       </c>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17">
+      <c r="K23" s="18"/>
+      <c r="L23" s="18">
         <f t="shared" si="17"/>
         <v>8</v>
       </c>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17">
+      <c r="M23" s="18"/>
+      <c r="N23" s="18">
         <f>L23</f>
         <v>8</v>
       </c>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17">
+      <c r="O23" s="18"/>
+      <c r="P23" s="18">
         <f t="shared" si="18"/>
         <v>8</v>
       </c>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="17"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="17">
+      <c r="B24" s="18">
         <f>B14</f>
-        <v>800</v>
-      </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17">
+        <v>2000</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18">
         <f t="shared" si="19"/>
-        <v>800</v>
-      </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17">
+        <v>2000</v>
+      </c>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18">
         <f>D24*I4</f>
-        <v>2400</v>
-      </c>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17">
+        <v>12000</v>
+      </c>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18">
         <f t="shared" ref="H24" si="21">F24</f>
-        <v>2400</v>
-      </c>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17">
+        <v>12000</v>
+      </c>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18">
         <f t="shared" si="16"/>
-        <v>2400</v>
-      </c>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17">
+        <v>12000</v>
+      </c>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18">
         <f t="shared" si="17"/>
-        <v>2400</v>
-      </c>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17">
+        <v>12000</v>
+      </c>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18">
         <f t="shared" ref="N24" si="22">L24</f>
-        <v>2400</v>
-      </c>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17">
+        <v>12000</v>
+      </c>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18">
         <f>N24</f>
-        <v>2400</v>
-      </c>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="17"/>
-      <c r="S24" s="17"/>
+        <v>12000</v>
+      </c>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="20">
+      <c r="B25" s="19">
         <f>B22*B23*B24</f>
-        <v>6553600</v>
-      </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20">
+        <v>16384000</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19">
         <f>D22*D23*D24</f>
-        <v>6553600</v>
-      </c>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20">
+        <v>16384000</v>
+      </c>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19">
         <f t="shared" ref="F25" si="23">F22*F23*F24</f>
-        <v>629145600</v>
-      </c>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20">
+        <v>3145728000</v>
+      </c>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19">
         <f t="shared" ref="H25" si="24">H22*H23*H24</f>
-        <v>629145600</v>
-      </c>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20">
+        <v>3145728000</v>
+      </c>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19">
         <f t="shared" ref="J25" si="25">J22*J23*J24</f>
-        <v>629145600</v>
-      </c>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20">
+        <v>3145728000</v>
+      </c>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19">
         <f t="shared" ref="L25" si="26">L22*L23*L24</f>
-        <v>629145600</v>
-      </c>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20">
+        <v>3145728000</v>
+      </c>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19">
         <f t="shared" ref="N25" si="27">N22*N23*N24</f>
-        <v>629145600</v>
-      </c>
-      <c r="O25" s="20"/>
-      <c r="P25" s="20">
+        <v>3145728000</v>
+      </c>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19">
         <f t="shared" ref="P25" si="28">P22*P23*P24</f>
-        <v>629145600</v>
-      </c>
-      <c r="Q25" s="20"/>
+        <v>3145728000</v>
+      </c>
+      <c r="Q25" s="19"/>
       <c r="R25" s="13"/>
       <c r="S25" s="13"/>
     </row>
@@ -2417,40 +2417,40 @@
       <c r="A26" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="19">
+      <c r="B26" s="20">
         <f>0.154+3.252+1.863+1.467</f>
         <v>6.7360000000000007</v>
       </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19">
+      <c r="C26" s="20"/>
+      <c r="D26" s="20">
         <v>1.1519999999999999</v>
       </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19">
+      <c r="E26" s="20"/>
+      <c r="F26" s="20">
         <v>14.536</v>
       </c>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19">
+      <c r="G26" s="20"/>
+      <c r="H26" s="20">
         <v>5.0839999999999996</v>
       </c>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19">
+      <c r="I26" s="20"/>
+      <c r="J26" s="20">
         <f>0.874+3.15</f>
         <v>4.024</v>
       </c>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19">
+      <c r="K26" s="20"/>
+      <c r="L26" s="20">
         <v>5.891</v>
       </c>
-      <c r="M26" s="19"/>
-      <c r="N26" s="19">
+      <c r="M26" s="20"/>
+      <c r="N26" s="20">
         <v>11.195</v>
       </c>
-      <c r="O26" s="19"/>
-      <c r="P26" s="19">
+      <c r="O26" s="20"/>
+      <c r="P26" s="20">
         <v>7.8550000000000004</v>
       </c>
-      <c r="Q26" s="19"/>
+      <c r="Q26" s="20"/>
       <c r="R26" s="14"/>
       <c r="S26" s="14"/>
     </row>
@@ -2458,261 +2458,263 @@
       <c r="A27" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="19">
+      <c r="B27" s="20">
         <f>6.36+8.93</f>
         <v>15.29</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19">
+      <c r="C27" s="20"/>
+      <c r="D27" s="20">
         <v>23.66</v>
       </c>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19">
+      <c r="E27" s="20"/>
+      <c r="F27" s="20">
         <v>108.08</v>
       </c>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19">
+      <c r="G27" s="20"/>
+      <c r="H27" s="20">
         <v>62.75</v>
       </c>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19">
+      <c r="I27" s="20"/>
+      <c r="J27" s="20">
         <v>56.74</v>
       </c>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19">
+      <c r="K27" s="20"/>
+      <c r="L27" s="20">
         <v>67.02</v>
       </c>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19">
+      <c r="M27" s="20"/>
+      <c r="N27" s="20">
         <v>72.900000000000006</v>
       </c>
-      <c r="O27" s="19"/>
-      <c r="P27" s="19">
+      <c r="O27" s="20"/>
+      <c r="P27" s="20">
         <v>80.45</v>
       </c>
-      <c r="Q27" s="19"/>
+      <c r="Q27" s="20"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="17">
         <f>B26/512/8/1600*B$25</f>
-        <v>6.7360000000000007</v>
-      </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18">
+        <v>16.84</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17">
         <f>D26/512/8/1600*D$25</f>
-        <v>1.1519999999999999</v>
-      </c>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18">
+        <v>2.88</v>
+      </c>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17">
         <f>F26/4096/8/3200*F$25</f>
-        <v>87.215999999999994</v>
-      </c>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18">
+        <v>436.08</v>
+      </c>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17">
         <f t="shared" ref="H28" si="29">H26/4096/8/3200*H$25</f>
-        <v>30.503999999999998</v>
-      </c>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18">
+        <v>152.51999999999998</v>
+      </c>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17">
         <f t="shared" ref="J28" si="30">J26/4096/8/3200*J$25</f>
-        <v>24.143999999999998</v>
-      </c>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18">
+        <v>120.72</v>
+      </c>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17">
         <f t="shared" ref="L28" si="31">L26/4096/8/3200*L$25</f>
-        <v>35.345999999999997</v>
-      </c>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18">
+        <v>176.73</v>
+      </c>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17">
         <f t="shared" ref="N28" si="32">N26/4096/8/3200*N$25</f>
-        <v>67.17</v>
-      </c>
-      <c r="O28" s="18"/>
-      <c r="P28" s="18">
+        <v>335.85</v>
+      </c>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17">
         <f t="shared" ref="P28" si="33">P26/4096/8/3200*P$25</f>
-        <v>47.13</v>
-      </c>
-      <c r="Q28" s="18"/>
+        <v>235.65000000000003</v>
+      </c>
+      <c r="Q28" s="17"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="18">
+      <c r="B29" s="17">
         <f>B27/512/8/1600*B$25</f>
-        <v>15.289999999999997</v>
-      </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18">
+        <v>38.224999999999994</v>
+      </c>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17">
         <f>D27/512/8/1600*D$25</f>
-        <v>23.66</v>
-      </c>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18">
+        <v>59.15</v>
+      </c>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17">
         <f>F27/4096/8/3200*F$25</f>
-        <v>648.48</v>
-      </c>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18">
+        <v>3242.4</v>
+      </c>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17">
         <f t="shared" ref="H29" si="34">H27/4096/8/3200*H$25</f>
-        <v>376.49999999999994</v>
-      </c>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18">
+        <v>1882.4999999999998</v>
+      </c>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17">
         <f t="shared" ref="J29" si="35">J27/4096/8/3200*J$25</f>
-        <v>340.44</v>
-      </c>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18">
+        <v>1702.2</v>
+      </c>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17">
         <f t="shared" ref="L29" si="36">L27/4096/8/3200*L$25</f>
-        <v>402.11999999999995</v>
-      </c>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18">
+        <v>2010.5999999999997</v>
+      </c>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17">
         <f t="shared" ref="N29" si="37">N27/4096/8/3200*N$25</f>
-        <v>437.40000000000003</v>
-      </c>
-      <c r="O29" s="18"/>
-      <c r="P29" s="18">
+        <v>2187.0000000000005</v>
+      </c>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17">
         <f t="shared" ref="P29" si="38">P27/4096/8/3200*P$25</f>
-        <v>482.7</v>
-      </c>
-      <c r="Q29" s="18"/>
+        <v>2413.5</v>
+      </c>
+      <c r="Q29" s="17"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="17">
+      <c r="B30" s="18">
         <v>1</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17">
+      <c r="C30" s="18"/>
+      <c r="D30" s="18">
         <v>1</v>
       </c>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17">
+      <c r="E30" s="18"/>
+      <c r="F30" s="18">
         <v>1</v>
       </c>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17">
+      <c r="G30" s="18"/>
+      <c r="H30" s="18">
         <v>1</v>
       </c>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17">
+      <c r="I30" s="18"/>
+      <c r="J30" s="18">
         <v>1</v>
       </c>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17">
+      <c r="K30" s="18"/>
+      <c r="L30" s="18">
         <v>1</v>
       </c>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17">
+      <c r="M30" s="18"/>
+      <c r="N30" s="18">
         <v>1</v>
       </c>
-      <c r="O30" s="17"/>
-      <c r="P30" s="17">
+      <c r="O30" s="18"/>
+      <c r="P30" s="18">
         <v>1</v>
       </c>
-      <c r="Q30" s="17"/>
+      <c r="Q30" s="18"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="16">
+      <c r="B31" s="21">
         <f>(B28+B29*B30)/86400</f>
-        <v>2.549305555555555E-4</v>
-      </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16">
+        <v>6.3732638888888888E-4</v>
+      </c>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21">
         <f t="shared" ref="D31:F31" si="39">(D28+D29*D30)/86400</f>
-        <v>2.8717592592592597E-4</v>
-      </c>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16">
+        <v>7.1793981481481481E-4</v>
+      </c>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21">
         <f t="shared" si="39"/>
-        <v>8.515E-3</v>
-      </c>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16">
+        <v>4.2575000000000002E-2</v>
+      </c>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21">
         <f>(H28+H29*H30+J28)/86400</f>
-        <v>4.9901388888888886E-3</v>
-      </c>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16">
+        <v>2.4950694444444442E-2</v>
+      </c>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21">
         <f>(J28+J29*J30+L28)/86400</f>
-        <v>4.628819444444445E-3</v>
-      </c>
-      <c r="K31" s="16"/>
-      <c r="L31" s="16">
+        <v>2.3144097222222222E-2</v>
+      </c>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21">
         <f t="shared" ref="L31:P31" si="40">(L28+L29*L30)/86400</f>
-        <v>5.063263888888888E-3</v>
-      </c>
-      <c r="M31" s="16"/>
-      <c r="N31" s="16">
+        <v>2.531631944444444E-2</v>
+      </c>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21">
         <f t="shared" si="40"/>
-        <v>5.8399305555555565E-3</v>
-      </c>
-      <c r="O31" s="16"/>
-      <c r="P31" s="16">
+        <v>2.9199652777777783E-2</v>
+      </c>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21">
         <f t="shared" si="40"/>
-        <v>6.132291666666667E-3</v>
-      </c>
-      <c r="Q31" s="16"/>
-      <c r="R31" s="18"/>
-      <c r="S31" s="18"/>
+        <v>3.0661458333333336E-2</v>
+      </c>
+      <c r="Q31" s="21"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="17"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="E32" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="110">
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="R24:S24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="P31:Q31"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="F26:G26"/>
@@ -2737,50 +2739,48 @@
     <mergeCell ref="F25:G25"/>
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="J25:K25"/>
-    <mergeCell ref="R31:S31"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="P31:Q31"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2829,14 +2829,14 @@
       <c r="A1" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="L1" s="21" t="s">
+      <c r="E1" s="16"/>
+      <c r="L1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="21"/>
+      <c r="M1" s="16"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2845,10 +2845,10 @@
       <c r="B2">
         <v>9481</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="21"/>
+      <c r="E2" s="16"/>
       <c r="F2">
         <v>19.909876918386299</v>
       </c>
@@ -2863,10 +2863,10 @@
         <f>MAX(F4,1/F4)</f>
         <v>11.830135875287004</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="21"/>
+      <c r="M2" s="16"/>
       <c r="N2">
         <v>42.926477759350803</v>
       </c>
@@ -2889,10 +2889,10 @@
       <c r="B3">
         <v>20</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="21"/>
+      <c r="E3" s="16"/>
       <c r="F3">
         <v>17</v>
       </c>
@@ -2903,10 +2903,10 @@
         <f>$B4*F5/300000000*1000000000000000</f>
         <v>52300.882458116022</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="21"/>
+      <c r="M3" s="16"/>
       <c r="N3">
         <v>-29.5</v>
       </c>
@@ -2925,10 +2925,10 @@
       <c r="B4" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="21"/>
+      <c r="E4" s="16"/>
       <c r="F4">
         <f>SIN(RADIANS(F2+F3))/SIN(RADIANS(F2-F3))</f>
         <v>11.830135875287004</v>
@@ -2944,10 +2944,10 @@
         <f>I3/$B7</f>
         <v>13.075220614529005</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="21"/>
+      <c r="M4" s="16"/>
       <c r="N4">
         <f>SIN(RADIANS(N2+N3))/SIN(RADIANS(N2-N3))</f>
         <v>0.24356450463759297</v>
@@ -2971,18 +2971,18 @@
       <c r="B5" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="21"/>
+      <c r="E5" s="16"/>
       <c r="F5">
         <f>ABS((COS(RADIANS(F2-F3))-COS(RADIANS(F2+F3)))/SIN(RADIANS(F2-F3)))</f>
         <v>3.9225661843587014</v>
       </c>
-      <c r="L5" s="21" t="s">
+      <c r="L5" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="21"/>
+      <c r="M5" s="16"/>
       <c r="N5">
         <f>ABS((COS(RADIANS(N2-N3))-COS(RADIANS(N2+N3)))/SIN(RADIANS(N2-N3)))</f>
         <v>0.70357494464450898</v>
@@ -3008,10 +3008,10 @@
         <f>B3/10</f>
         <v>2</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="21"/>
+      <c r="E8" s="16"/>
       <c r="F8" s="1">
         <v>5.9999999999999997E-7</v>
       </c>
@@ -3031,10 +3031,10 @@
         <f>4/B8</f>
         <v>2</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="21"/>
+      <c r="E9" s="16"/>
       <c r="F9" s="7">
         <f>SUM(28:28)/86400</f>
         <v>0.1360213888888889</v>
@@ -3048,20 +3048,20 @@
         <f>MIN(B9/400,0.001)</f>
         <v>1E-3</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="21"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="7">
         <f>SUM(31:31)-F9</f>
         <v>1.3155878472222222</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="21"/>
+      <c r="E11" s="16"/>
       <c r="F11" s="10">
         <f>SUM(31:31)</f>
         <v>1.451609236111111</v>
@@ -3096,56 +3096,56 @@
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21" t="s">
+      <c r="C16" s="16"/>
+      <c r="D16" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21" t="s">
+      <c r="E16" s="16"/>
+      <c r="F16" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21" t="s">
+      <c r="G16" s="16"/>
+      <c r="H16" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21" t="s">
+      <c r="I16" s="16"/>
+      <c r="J16" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21" t="s">
+      <c r="K16" s="16"/>
+      <c r="L16" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21" t="s">
+      <c r="M16" s="16"/>
+      <c r="N16" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="O16" s="21"/>
-      <c r="P16" s="21" t="s">
+      <c r="O16" s="16"/>
+      <c r="P16" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="21" t="s">
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="S16" s="21"/>
-      <c r="T16" s="21" t="s">
+      <c r="S16" s="16"/>
+      <c r="T16" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="U16" s="21"/>
-      <c r="V16" s="21" t="s">
+      <c r="U16" s="16"/>
+      <c r="V16" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="W16" s="21"/>
-      <c r="X16" s="21" t="s">
+      <c r="W16" s="16"/>
+      <c r="X16" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="Y16" s="21"/>
-      <c r="Z16" s="21"/>
-      <c r="AA16" s="21"/>
+      <c r="Y16" s="16"/>
+      <c r="Z16" s="16"/>
+      <c r="AA16" s="16"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
@@ -3563,259 +3563,259 @@
       <c r="A21" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="17">
         <v>722.7</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18">
+      <c r="C21" s="17"/>
+      <c r="D21" s="17">
         <f>B21*J2</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18">
+      <c r="E21" s="17"/>
+      <c r="F21" s="17">
         <f>D21</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18">
+      <c r="G21" s="17"/>
+      <c r="H21" s="17">
         <f>F21</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18">
+      <c r="I21" s="17"/>
+      <c r="J21" s="17">
         <f>H21/J2</f>
         <v>722.7</v>
       </c>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18">
+      <c r="K21" s="17"/>
+      <c r="L21" s="17">
         <v>722.86</v>
       </c>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18">
+      <c r="M21" s="17"/>
+      <c r="N21" s="17">
         <v>722.85</v>
       </c>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18">
+      <c r="O21" s="17"/>
+      <c r="P21" s="17">
         <v>176.54</v>
       </c>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18">
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17">
         <v>14.28</v>
       </c>
-      <c r="S21" s="18"/>
-      <c r="T21" s="18">
+      <c r="S21" s="17"/>
+      <c r="T21" s="17">
         <v>175.15</v>
       </c>
-      <c r="U21" s="18"/>
-      <c r="V21" s="18">
+      <c r="U21" s="17"/>
+      <c r="V21" s="17">
         <v>173.04</v>
       </c>
-      <c r="W21" s="18"/>
-      <c r="X21" s="18">
+      <c r="W21" s="17"/>
+      <c r="X21" s="17">
         <v>173.07</v>
       </c>
-      <c r="Y21" s="18"/>
-      <c r="Z21" s="17"/>
-      <c r="AA21" s="17"/>
+      <c r="Y21" s="17"/>
+      <c r="Z21" s="18"/>
+      <c r="AA21" s="18"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="17">
+      <c r="B22" s="18">
         <f>B12</f>
         <v>512</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17">
+      <c r="C22" s="18"/>
+      <c r="D22" s="18">
         <f>B22*I2</f>
         <v>6144</v>
       </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17">
+      <c r="E22" s="18"/>
+      <c r="F22" s="18">
         <f>D22</f>
         <v>6144</v>
       </c>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17">
+      <c r="G22" s="18"/>
+      <c r="H22" s="18">
         <f>F22</f>
         <v>6144</v>
       </c>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17">
+      <c r="I22" s="18"/>
+      <c r="J22" s="18">
         <f t="shared" ref="J22:J24" si="23">H22</f>
         <v>6144</v>
       </c>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17">
+      <c r="K22" s="18"/>
+      <c r="L22" s="18">
         <f>J22</f>
         <v>6144</v>
       </c>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17">
+      <c r="M22" s="18"/>
+      <c r="N22" s="18">
         <f>L22*Q2*4</f>
         <v>98304</v>
       </c>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17">
+      <c r="O22" s="18"/>
+      <c r="P22" s="18">
         <f>N22</f>
         <v>98304</v>
       </c>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="17">
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18">
         <f t="shared" ref="R22:R24" si="24">P22</f>
         <v>98304</v>
       </c>
-      <c r="S22" s="17"/>
-      <c r="T22" s="17">
+      <c r="S22" s="18"/>
+      <c r="T22" s="18">
         <f t="shared" ref="T22:T24" si="25">R22</f>
         <v>98304</v>
       </c>
-      <c r="U22" s="17"/>
-      <c r="V22" s="17">
+      <c r="U22" s="18"/>
+      <c r="V22" s="18">
         <f>T22</f>
         <v>98304</v>
       </c>
-      <c r="W22" s="17"/>
-      <c r="X22" s="17">
+      <c r="W22" s="18"/>
+      <c r="X22" s="18">
         <f t="shared" ref="X22:X23" si="26">V22</f>
         <v>98304</v>
       </c>
-      <c r="Y22" s="17"/>
-      <c r="Z22" s="17"/>
-      <c r="AA22" s="17"/>
+      <c r="Y22" s="18"/>
+      <c r="Z22" s="18"/>
+      <c r="AA22" s="18"/>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="18">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17">
+      <c r="C23" s="18"/>
+      <c r="D23" s="18">
         <f t="shared" ref="D23" si="27">B23</f>
         <v>8</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17">
+      <c r="E23" s="18"/>
+      <c r="F23" s="18">
         <f t="shared" ref="F23" si="28">D23</f>
         <v>8</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17">
+      <c r="G23" s="18"/>
+      <c r="H23" s="18">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17">
+      <c r="I23" s="18"/>
+      <c r="J23" s="18">
         <f t="shared" si="23"/>
         <v>8</v>
       </c>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17">
+      <c r="K23" s="18"/>
+      <c r="L23" s="18">
         <f t="shared" ref="L23:L24" si="29">J23</f>
         <v>8</v>
       </c>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17">
+      <c r="M23" s="18"/>
+      <c r="N23" s="18">
         <f t="shared" ref="N23" si="30">L23</f>
         <v>8</v>
       </c>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17">
+      <c r="O23" s="18"/>
+      <c r="P23" s="18">
         <f>N23</f>
         <v>8</v>
       </c>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17">
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18">
         <f t="shared" si="24"/>
         <v>8</v>
       </c>
-      <c r="S23" s="17"/>
-      <c r="T23" s="17">
+      <c r="S23" s="18"/>
+      <c r="T23" s="18">
         <f t="shared" si="25"/>
         <v>8</v>
       </c>
-      <c r="U23" s="17"/>
-      <c r="V23" s="17">
+      <c r="U23" s="18"/>
+      <c r="V23" s="18">
         <f>T23</f>
         <v>8</v>
       </c>
-      <c r="W23" s="17"/>
-      <c r="X23" s="17">
+      <c r="W23" s="18"/>
+      <c r="X23" s="18">
         <f t="shared" si="26"/>
         <v>8</v>
       </c>
-      <c r="Y23" s="17"/>
-      <c r="Z23" s="17"/>
-      <c r="AA23" s="17"/>
+      <c r="Y23" s="18"/>
+      <c r="Z23" s="18"/>
+      <c r="AA23" s="18"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="17">
+      <c r="B24" s="18">
         <f>B14</f>
         <v>2000</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17">
+      <c r="C24" s="18"/>
+      <c r="D24" s="18">
         <f>B24*I4</f>
         <v>26000</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17">
+      <c r="E24" s="18"/>
+      <c r="F24" s="18">
         <f>D24</f>
         <v>26000</v>
       </c>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17">
+      <c r="G24" s="18"/>
+      <c r="H24" s="18">
         <f t="shared" ref="H24" si="31">F24</f>
         <v>26000</v>
       </c>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17">
+      <c r="I24" s="18"/>
+      <c r="J24" s="18">
         <f t="shared" si="23"/>
         <v>26000</v>
       </c>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17">
+      <c r="K24" s="18"/>
+      <c r="L24" s="18">
         <f t="shared" si="29"/>
         <v>26000</v>
       </c>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17">
+      <c r="M24" s="18"/>
+      <c r="N24" s="18">
         <f>L24</f>
         <v>26000</v>
       </c>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17">
+      <c r="O24" s="18"/>
+      <c r="P24" s="18">
         <f t="shared" ref="P24" si="32">N24</f>
         <v>26000</v>
       </c>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="17">
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18">
         <f t="shared" si="24"/>
         <v>26000</v>
       </c>
-      <c r="S24" s="17"/>
-      <c r="T24" s="17">
+      <c r="S24" s="18"/>
+      <c r="T24" s="18">
         <f t="shared" si="25"/>
         <v>26000</v>
       </c>
-      <c r="U24" s="17"/>
-      <c r="V24" s="17">
+      <c r="U24" s="18"/>
+      <c r="V24" s="18">
         <f t="shared" ref="V24" si="33">T24</f>
         <v>26000</v>
       </c>
-      <c r="W24" s="17"/>
-      <c r="X24" s="17">
+      <c r="W24" s="18"/>
+      <c r="X24" s="18">
         <f>V24*2</f>
         <v>52000</v>
       </c>
-      <c r="Y24" s="17"/>
+      <c r="Y24" s="18"/>
       <c r="Z24" s="5"/>
       <c r="AA24" s="5"/>
     </row>
@@ -3823,66 +3823,66 @@
       <c r="A25" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="20">
+      <c r="B25" s="19">
         <f>B22*B23*B24</f>
         <v>8192000</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20">
+      <c r="C25" s="19"/>
+      <c r="D25" s="19">
         <f>D22*D23*D24</f>
         <v>1277952000</v>
       </c>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20">
+      <c r="E25" s="19"/>
+      <c r="F25" s="19">
         <f t="shared" ref="F25" si="34">F22*F23*F24</f>
         <v>1277952000</v>
       </c>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20">
+      <c r="G25" s="19"/>
+      <c r="H25" s="19">
         <f t="shared" ref="H25" si="35">H22*H23*H24</f>
         <v>1277952000</v>
       </c>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20">
+      <c r="I25" s="19"/>
+      <c r="J25" s="19">
         <f t="shared" ref="J25" si="36">J22*J23*J24</f>
         <v>1277952000</v>
       </c>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20">
+      <c r="K25" s="19"/>
+      <c r="L25" s="19">
         <f>L22*L23*L24</f>
         <v>1277952000</v>
       </c>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20">
+      <c r="M25" s="19"/>
+      <c r="N25" s="19">
         <f t="shared" ref="N25:X25" si="37">N22*N23*N24</f>
         <v>20447232000</v>
       </c>
-      <c r="O25" s="20"/>
-      <c r="P25" s="20">
+      <c r="O25" s="19"/>
+      <c r="P25" s="19">
         <f t="shared" si="37"/>
         <v>20447232000</v>
       </c>
-      <c r="Q25" s="20"/>
-      <c r="R25" s="20">
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19">
         <f t="shared" si="37"/>
         <v>20447232000</v>
       </c>
-      <c r="S25" s="20"/>
-      <c r="T25" s="20">
+      <c r="S25" s="19"/>
+      <c r="T25" s="19">
         <f t="shared" si="37"/>
         <v>20447232000</v>
       </c>
-      <c r="U25" s="20"/>
-      <c r="V25" s="20">
+      <c r="U25" s="19"/>
+      <c r="V25" s="19">
         <f t="shared" si="37"/>
         <v>20447232000</v>
       </c>
-      <c r="W25" s="20"/>
-      <c r="X25" s="20">
+      <c r="W25" s="19"/>
+      <c r="X25" s="19">
         <f t="shared" si="37"/>
         <v>40894464000</v>
       </c>
-      <c r="Y25" s="20"/>
+      <c r="Y25" s="19"/>
       <c r="Z25" s="8"/>
       <c r="AA25" s="8"/>
     </row>
@@ -3890,431 +3890,434 @@
       <c r="A26" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="19">
+      <c r="B26" s="20">
         <f>0.191+9.964+1.804+1.666</f>
         <v>13.625000000000002</v>
       </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19">
+      <c r="C26" s="20"/>
+      <c r="D26" s="20">
         <v>25.887</v>
       </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19">
+      <c r="E26" s="20"/>
+      <c r="F26" s="20">
         <v>21.568000000000001</v>
       </c>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19">
+      <c r="G26" s="20"/>
+      <c r="H26" s="20">
         <v>21.541</v>
       </c>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19">
+      <c r="I26" s="20"/>
+      <c r="J26" s="20">
         <v>9.1859999999999999</v>
       </c>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19">
+      <c r="K26" s="20"/>
+      <c r="L26" s="20">
         <v>1.1519999999999999</v>
       </c>
-      <c r="M26" s="19"/>
-      <c r="N26" s="19">
+      <c r="M26" s="20"/>
+      <c r="N26" s="20">
         <v>14.536</v>
       </c>
-      <c r="O26" s="19"/>
-      <c r="P26" s="19">
+      <c r="O26" s="20"/>
+      <c r="P26" s="20">
         <v>5.0839999999999996</v>
       </c>
-      <c r="Q26" s="19"/>
-      <c r="R26" s="19">
+      <c r="Q26" s="20"/>
+      <c r="R26" s="20">
         <f>0.874+3.15</f>
         <v>4.024</v>
       </c>
-      <c r="S26" s="19"/>
-      <c r="T26" s="19">
+      <c r="S26" s="20"/>
+      <c r="T26" s="20">
         <v>5.891</v>
       </c>
-      <c r="U26" s="19"/>
-      <c r="V26" s="19">
+      <c r="U26" s="20"/>
+      <c r="V26" s="20">
         <v>11.195</v>
       </c>
-      <c r="W26" s="19"/>
-      <c r="X26" s="19">
+      <c r="W26" s="20"/>
+      <c r="X26" s="20">
         <v>7.8550000000000004</v>
       </c>
-      <c r="Y26" s="19"/>
+      <c r="Y26" s="20"/>
     </row>
     <row r="27" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="19">
+      <c r="B27" s="20">
         <f>19.37+17.15</f>
         <v>36.519999999999996</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19">
+      <c r="C27" s="20"/>
+      <c r="D27" s="20">
         <v>146.75</v>
       </c>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19">
+      <c r="E27" s="20"/>
+      <c r="F27" s="20">
         <v>180.85</v>
       </c>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19">
+      <c r="G27" s="20"/>
+      <c r="H27" s="20">
         <v>166.69</v>
       </c>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19">
+      <c r="I27" s="20"/>
+      <c r="J27" s="20">
         <v>128.34</v>
       </c>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19">
+      <c r="K27" s="20"/>
+      <c r="L27" s="20">
         <v>23.66</v>
       </c>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19">
+      <c r="M27" s="20"/>
+      <c r="N27" s="20">
         <v>108.08</v>
       </c>
-      <c r="O27" s="19"/>
-      <c r="P27" s="19">
+      <c r="O27" s="20"/>
+      <c r="P27" s="20">
         <v>62.75</v>
       </c>
-      <c r="Q27" s="19"/>
-      <c r="R27" s="19">
+      <c r="Q27" s="20"/>
+      <c r="R27" s="20">
         <v>56.74</v>
       </c>
-      <c r="S27" s="19"/>
-      <c r="T27" s="19">
+      <c r="S27" s="20"/>
+      <c r="T27" s="20">
         <v>67.02</v>
       </c>
-      <c r="U27" s="19"/>
-      <c r="V27" s="19">
+      <c r="U27" s="20"/>
+      <c r="V27" s="20">
         <v>72.900000000000006</v>
       </c>
-      <c r="W27" s="19"/>
-      <c r="X27" s="19">
+      <c r="W27" s="20"/>
+      <c r="X27" s="20">
         <v>80.45</v>
       </c>
-      <c r="Y27" s="19"/>
+      <c r="Y27" s="20"/>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="17">
         <f>B26/512/8/2000*B$25</f>
         <v>13.625000000000002</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18">
+      <c r="C28" s="17"/>
+      <c r="D28" s="17">
         <f>D26/6144/8/4000*D$25</f>
         <v>168.2655</v>
       </c>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18">
+      <c r="E28" s="17"/>
+      <c r="F28" s="17">
         <f t="shared" ref="F28:F29" si="38">F26/6144/8/4000*F$25</f>
         <v>140.19200000000001</v>
       </c>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18">
+      <c r="G28" s="17"/>
+      <c r="H28" s="17">
         <f t="shared" ref="H28:H29" si="39">H26/6144/8/4000*H$25</f>
         <v>140.01650000000001</v>
       </c>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18">
+      <c r="I28" s="17"/>
+      <c r="J28" s="17">
         <f t="shared" ref="J28:J29" si="40">J26/6144/8/4000*J$25</f>
         <v>59.708999999999996</v>
       </c>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18">
+      <c r="K28" s="17"/>
+      <c r="L28" s="17">
         <f>L26/512/8/1600*L$25</f>
         <v>224.64</v>
       </c>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18">
+      <c r="M28" s="17"/>
+      <c r="N28" s="17">
         <f>N26/4096/8/3200*N$25</f>
         <v>2834.52</v>
       </c>
-      <c r="O28" s="18"/>
-      <c r="P28" s="18">
+      <c r="O28" s="17"/>
+      <c r="P28" s="17">
         <f t="shared" ref="P28:P29" si="41">P26/4096/8/3200*P$25</f>
         <v>991.37999999999988</v>
       </c>
-      <c r="Q28" s="18"/>
-      <c r="R28" s="18">
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17">
         <f t="shared" ref="R28:R29" si="42">R26/4096/8/3200*R$25</f>
         <v>784.68</v>
       </c>
-      <c r="S28" s="18"/>
-      <c r="T28" s="18">
+      <c r="S28" s="17"/>
+      <c r="T28" s="17">
         <f t="shared" ref="T28:T29" si="43">T26/4096/8/3200*T$25</f>
         <v>1148.7449999999999</v>
       </c>
-      <c r="U28" s="18"/>
-      <c r="V28" s="18">
+      <c r="U28" s="17"/>
+      <c r="V28" s="17">
         <f t="shared" ref="V28:V29" si="44">V26/4096/8/3200*V$25</f>
         <v>2183.0250000000001</v>
       </c>
-      <c r="W28" s="18"/>
-      <c r="X28" s="18">
+      <c r="W28" s="17"/>
+      <c r="X28" s="17">
         <f t="shared" ref="X28:X29" si="45">X26/4096/8/3200*X$25</f>
         <v>3063.4500000000003</v>
       </c>
-      <c r="Y28" s="18"/>
+      <c r="Y28" s="17"/>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="18">
+      <c r="B29" s="17">
         <f>B27/512/8/2000*B$25</f>
         <v>36.519999999999996</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18">
+      <c r="C29" s="17"/>
+      <c r="D29" s="17">
         <f>D27/6144/8/4000*D$25</f>
         <v>953.875</v>
       </c>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18">
+      <c r="E29" s="17"/>
+      <c r="F29" s="17">
         <f t="shared" si="38"/>
         <v>1175.5250000000001</v>
       </c>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18">
+      <c r="G29" s="17"/>
+      <c r="H29" s="17">
         <f t="shared" si="39"/>
         <v>1083.4849999999999</v>
       </c>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18">
+      <c r="I29" s="17"/>
+      <c r="J29" s="17">
         <f t="shared" si="40"/>
         <v>834.20999999999992</v>
       </c>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18">
+      <c r="K29" s="17"/>
+      <c r="L29" s="17">
         <f>L27/512/8/1600*L$25</f>
         <v>4613.7</v>
       </c>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18">
+      <c r="M29" s="17"/>
+      <c r="N29" s="17">
         <f>N27/4096/8/3200*N$25</f>
         <v>21075.599999999999</v>
       </c>
-      <c r="O29" s="18"/>
-      <c r="P29" s="18">
+      <c r="O29" s="17"/>
+      <c r="P29" s="17">
         <f t="shared" si="41"/>
         <v>12236.249999999998</v>
       </c>
-      <c r="Q29" s="18"/>
-      <c r="R29" s="18">
+      <c r="Q29" s="17"/>
+      <c r="R29" s="17">
         <f t="shared" si="42"/>
         <v>11064.300000000001</v>
       </c>
-      <c r="S29" s="18"/>
-      <c r="T29" s="18">
+      <c r="S29" s="17"/>
+      <c r="T29" s="17">
         <f t="shared" si="43"/>
         <v>13068.899999999998</v>
       </c>
-      <c r="U29" s="18"/>
-      <c r="V29" s="18">
+      <c r="U29" s="17"/>
+      <c r="V29" s="17">
         <f t="shared" si="44"/>
         <v>14215.500000000002</v>
       </c>
-      <c r="W29" s="18"/>
-      <c r="X29" s="18">
+      <c r="W29" s="17"/>
+      <c r="X29" s="17">
         <f t="shared" si="45"/>
         <v>31375.5</v>
       </c>
-      <c r="Y29" s="18"/>
+      <c r="Y29" s="17"/>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="17">
+      <c r="B30" s="18">
         <v>1</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17">
+      <c r="C30" s="18"/>
+      <c r="D30" s="18">
         <v>1</v>
       </c>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17">
+      <c r="E30" s="18"/>
+      <c r="F30" s="18">
         <v>1</v>
       </c>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17">
+      <c r="G30" s="18"/>
+      <c r="H30" s="18">
         <v>1</v>
       </c>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17">
+      <c r="I30" s="18"/>
+      <c r="J30" s="18">
         <v>1</v>
       </c>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17">
+      <c r="K30" s="18"/>
+      <c r="L30" s="18">
         <v>1</v>
       </c>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17">
+      <c r="M30" s="18"/>
+      <c r="N30" s="18">
         <v>1</v>
       </c>
-      <c r="O30" s="17"/>
-      <c r="P30" s="17">
+      <c r="O30" s="18"/>
+      <c r="P30" s="18">
         <v>1</v>
       </c>
-      <c r="Q30" s="17"/>
-      <c r="R30" s="17">
+      <c r="Q30" s="18"/>
+      <c r="R30" s="18">
         <v>1</v>
       </c>
-      <c r="S30" s="17"/>
-      <c r="T30" s="17">
+      <c r="S30" s="18"/>
+      <c r="T30" s="18">
         <v>1</v>
       </c>
-      <c r="U30" s="17"/>
-      <c r="V30" s="17">
+      <c r="U30" s="18"/>
+      <c r="V30" s="18">
         <v>1</v>
       </c>
-      <c r="W30" s="17"/>
-      <c r="X30" s="17">
+      <c r="W30" s="18"/>
+      <c r="X30" s="18">
         <v>1</v>
       </c>
-      <c r="Y30" s="17"/>
-      <c r="Z30" s="18"/>
-      <c r="AA30" s="18"/>
+      <c r="Y30" s="18"/>
+      <c r="Z30" s="17"/>
+      <c r="AA30" s="17"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="16">
+      <c r="B31" s="21">
         <f>(B28+B29*B30)/86400</f>
         <v>5.8038194444444435E-4</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16">
+      <c r="C31" s="21"/>
+      <c r="D31" s="21">
         <f t="shared" ref="D31:F31" si="46">(D28+D29*D30)/86400</f>
         <v>1.2987737268518517E-2</v>
       </c>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16">
+      <c r="E31" s="21"/>
+      <c r="F31" s="21">
         <f t="shared" si="46"/>
         <v>1.5228206018518519E-2</v>
       </c>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16">
+      <c r="G31" s="21"/>
+      <c r="H31" s="21">
         <f t="shared" ref="H31" si="47">(H28+H29*H30)/86400</f>
         <v>1.4160896990740739E-2</v>
       </c>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16">
+      <c r="I31" s="21"/>
+      <c r="J31" s="21">
         <f t="shared" ref="J31" si="48">(J28+J29*J30)/86400</f>
         <v>1.034628472222222E-2</v>
       </c>
-      <c r="K31" s="16"/>
-      <c r="L31" s="16">
+      <c r="K31" s="21"/>
+      <c r="L31" s="21">
         <f t="shared" ref="L31:N31" si="49">(L28+L29*L30)/86400</f>
         <v>5.5999305555555559E-2</v>
       </c>
-      <c r="M31" s="16"/>
-      <c r="N31" s="16">
+      <c r="M31" s="21"/>
+      <c r="N31" s="21">
         <f t="shared" si="49"/>
         <v>0.27673749999999997</v>
       </c>
-      <c r="O31" s="16"/>
-      <c r="P31" s="16">
+      <c r="O31" s="21"/>
+      <c r="P31" s="21">
         <f>(P28+P29*P30+R28)/86400</f>
         <v>0.16217951388888885</v>
       </c>
-      <c r="Q31" s="16"/>
-      <c r="R31" s="16">
+      <c r="Q31" s="21"/>
+      <c r="R31" s="21">
         <f>(R28+R29*R30+T28)/86400</f>
         <v>0.15043663194444448</v>
       </c>
-      <c r="S31" s="16"/>
-      <c r="T31" s="16">
+      <c r="S31" s="21"/>
+      <c r="T31" s="21">
         <f t="shared" ref="T31:X31" si="50">(T28+T29*T30)/86400</f>
         <v>0.16455607638888886</v>
       </c>
-      <c r="U31" s="16"/>
-      <c r="V31" s="16">
+      <c r="U31" s="21"/>
+      <c r="V31" s="21">
         <f t="shared" si="50"/>
         <v>0.18979774305555558</v>
       </c>
-      <c r="W31" s="16"/>
-      <c r="X31" s="16">
+      <c r="W31" s="21"/>
+      <c r="X31" s="21">
         <f t="shared" si="50"/>
         <v>0.39859895833333331</v>
       </c>
-      <c r="Y31" s="16"/>
+      <c r="Y31" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="163">
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="X16:Y16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="T21:U21"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="X21:Y21"/>
-    <mergeCell ref="Z21:AA21"/>
-    <mergeCell ref="X22:Y22"/>
-    <mergeCell ref="Z22:AA22"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="P31:Q31"/>
+    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="T31:U31"/>
+    <mergeCell ref="V31:W31"/>
+    <mergeCell ref="X31:Y31"/>
+    <mergeCell ref="V28:W28"/>
+    <mergeCell ref="X28:Y28"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="R29:S29"/>
+    <mergeCell ref="V29:W29"/>
+    <mergeCell ref="X29:Y29"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="R30:S30"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="X30:Y30"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="X25:Y25"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="R26:S26"/>
+    <mergeCell ref="V26:W26"/>
+    <mergeCell ref="X26:Y26"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="R27:S27"/>
+    <mergeCell ref="V27:W27"/>
+    <mergeCell ref="X27:Y27"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="T29:U29"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="T28:U28"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="T26:U26"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="T27:U27"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="R25:S25"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="R28:S28"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="J30:K30"/>
     <mergeCell ref="X23:Y23"/>
@@ -4339,77 +4342,74 @@
     <mergeCell ref="T25:U25"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="F26:G26"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="T29:U29"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="T28:U28"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="T26:U26"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="T27:U27"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="R25:S25"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="R28:S28"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="X25:Y25"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="R26:S26"/>
-    <mergeCell ref="V26:W26"/>
-    <mergeCell ref="X26:Y26"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="R27:S27"/>
-    <mergeCell ref="V27:W27"/>
-    <mergeCell ref="X27:Y27"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="P31:Q31"/>
-    <mergeCell ref="R31:S31"/>
-    <mergeCell ref="T31:U31"/>
-    <mergeCell ref="V31:W31"/>
-    <mergeCell ref="X31:Y31"/>
-    <mergeCell ref="V28:W28"/>
-    <mergeCell ref="X28:Y28"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="R29:S29"/>
-    <mergeCell ref="V29:W29"/>
-    <mergeCell ref="X29:Y29"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="R30:S30"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="X30:Y30"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="T21:U21"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="X21:Y21"/>
+    <mergeCell ref="Z21:AA21"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="X16:Y16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update: HRM-mirror simulation parameter optimization
</commit_message>
<xml_diff>
--- a/Sampling_Resolution_Calculator.xlsx
+++ b/Sampling_Resolution_Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nanw0\GoogleDrive\SLAC\SLAC-Diling\11. 21 Winter\DXS optics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C425473C-AFF6-47E7-ABAA-7E280437DDEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFE9810-1CC1-42FB-974B-4B724277ADFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="735" windowWidth="17580" windowHeight="15090" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HHLM" sheetId="10" r:id="rId1"/>
@@ -1630,7 +1630,7 @@
   <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1694,7 +1694,7 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>25</v>
@@ -1732,11 +1732,11 @@
       </c>
       <c r="I4" s="2">
         <f>MAX(ROUND(2*I3/$B7,0),1)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J4">
         <f>I3/$B7</f>
-        <v>2.9315622693521211</v>
+        <v>1.4657811346760605</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -1765,7 +1765,7 @@
       </c>
       <c r="B7">
         <f>B8*B14</f>
-        <v>4000</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
@@ -1774,7 +1774,7 @@
       </c>
       <c r="B8">
         <f>B3/10</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>20</v>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="I8" s="9">
         <f>22122874/1024/1024/3072/8/26000*MAX(25:25)</f>
-        <v>103.86715932992787</v>
+        <v>20.773431865985575</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
@@ -1797,7 +1797,7 @@
       </c>
       <c r="B9">
         <f>4/B8</f>
-        <v>2</v>
+        <v>0.4</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>52</v>
@@ -1805,7 +1805,7 @@
       <c r="E9" s="16"/>
       <c r="F9" s="7">
         <f>SUM(28:28)/86400</f>
-        <v>1.7098032407407406E-2</v>
+        <v>3.4652546296296298E-3</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
@@ -1814,7 +1814,7 @@
       </c>
       <c r="B10">
         <f>MIN(B9/800,0.001)</f>
-        <v>1E-3</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>53</v>
@@ -1822,7 +1822,7 @@
       <c r="E10" s="16"/>
       <c r="F10" s="7">
         <f>SUM(31:31)-F9</f>
-        <v>0.16010445601851853</v>
+        <v>3.2246296296296301E-2</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
@@ -1832,7 +1832,7 @@
       <c r="E11" s="16"/>
       <c r="F11" s="10">
         <f>SUM(31:31)</f>
-        <v>0.17720248842592592</v>
+        <v>3.5711550925925928E-2</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
@@ -1860,7 +1860,7 @@
       </c>
       <c r="B14">
         <f>B9/B10</f>
-        <v>2000</v>
+        <v>800</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
@@ -2050,19 +2050,19 @@
       </c>
       <c r="B19" s="2">
         <f>B7</f>
-        <v>4000</v>
+        <v>8000</v>
       </c>
       <c r="C19" s="2">
         <f>B8</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D19" s="2">
         <f>E19*D24</f>
-        <v>4000</v>
+        <v>8000</v>
       </c>
       <c r="E19" s="2">
         <f>C19</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F19" s="2">
         <f>G19*F24</f>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="G19" s="2">
         <f>E19</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H19" s="2">
         <f>I19*H24</f>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="I19" s="2">
         <f>G19</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J19" s="2">
         <f>K19*J24</f>
@@ -2086,7 +2086,7 @@
       </c>
       <c r="K19" s="2">
         <f>I19</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L19" s="2">
         <f>M19*L24</f>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="M19" s="2">
         <f>K19</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="N19" s="2">
         <f>O19*N24</f>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="O19" s="2">
         <f>M19</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="P19" s="2">
         <f>Q19*P24</f>
@@ -2110,7 +2110,7 @@
       </c>
       <c r="Q19" s="2">
         <f>O19</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
@@ -2121,23 +2121,23 @@
       </c>
       <c r="B20" s="2">
         <f>B9*1000</f>
-        <v>2000</v>
+        <v>400</v>
       </c>
       <c r="C20" s="2">
         <f>B10*1000</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D20" s="2">
         <f>$B20*$C19/E19</f>
-        <v>2000</v>
+        <v>400</v>
       </c>
       <c r="E20" s="2">
         <f>$B19*$C20/D19</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F20" s="2">
         <f>$B20*$C19/G19</f>
-        <v>2000</v>
+        <v>400</v>
       </c>
       <c r="G20" s="2">
         <f>$B19*$C20/F19</f>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="H20" s="2">
         <f t="shared" ref="H20" si="6">$B20*$C19/I19</f>
-        <v>2000</v>
+        <v>400</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" ref="I20" si="7">$B19*$C20/H19</f>
@@ -2153,7 +2153,7 @@
       </c>
       <c r="J20" s="2">
         <f t="shared" ref="J20" si="8">$B20*$C19/K19</f>
-        <v>2000</v>
+        <v>400</v>
       </c>
       <c r="K20" s="2">
         <f t="shared" ref="K20" si="9">$B19*$C20/J19</f>
@@ -2161,7 +2161,7 @@
       </c>
       <c r="L20" s="2">
         <f t="shared" ref="L20" si="10">$B20*$C19/M19</f>
-        <v>2000</v>
+        <v>400</v>
       </c>
       <c r="M20" s="2">
         <f t="shared" ref="M20" si="11">$B19*$C20/L19</f>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="N20" s="2">
         <f t="shared" ref="N20" si="12">$B20*$C19/O19</f>
-        <v>2000</v>
+        <v>400</v>
       </c>
       <c r="O20" s="2">
         <f t="shared" ref="O20" si="13">$B19*$C20/N19</f>
@@ -2177,7 +2177,7 @@
       </c>
       <c r="P20" s="2">
         <f t="shared" ref="P20" si="14">$B20*$C19/Q19</f>
-        <v>2000</v>
+        <v>400</v>
       </c>
       <c r="Q20" s="2">
         <f t="shared" ref="Q20" si="15">$B19*$C20/P19</f>
@@ -2325,42 +2325,42 @@
       </c>
       <c r="B24" s="18">
         <f>B14</f>
-        <v>2000</v>
+        <v>800</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="18">
         <f t="shared" si="19"/>
-        <v>2000</v>
+        <v>800</v>
       </c>
       <c r="E24" s="18"/>
       <c r="F24" s="18">
         <f>D24*I4</f>
-        <v>12000</v>
+        <v>2400</v>
       </c>
       <c r="G24" s="18"/>
       <c r="H24" s="18">
         <f t="shared" ref="H24" si="21">F24</f>
-        <v>12000</v>
+        <v>2400</v>
       </c>
       <c r="I24" s="18"/>
       <c r="J24" s="18">
         <f t="shared" si="16"/>
-        <v>12000</v>
+        <v>2400</v>
       </c>
       <c r="K24" s="18"/>
       <c r="L24" s="18">
         <f t="shared" si="17"/>
-        <v>12000</v>
+        <v>2400</v>
       </c>
       <c r="M24" s="18"/>
       <c r="N24" s="18">
         <f t="shared" ref="N24" si="22">L24</f>
-        <v>12000</v>
+        <v>2400</v>
       </c>
       <c r="O24" s="18"/>
       <c r="P24" s="18">
         <f>N24</f>
-        <v>12000</v>
+        <v>2400</v>
       </c>
       <c r="Q24" s="18"/>
       <c r="R24" s="18"/>
@@ -2372,42 +2372,42 @@
       </c>
       <c r="B25" s="19">
         <f>B22*B23*B24</f>
-        <v>16384000</v>
+        <v>6553600</v>
       </c>
       <c r="C25" s="19"/>
       <c r="D25" s="19">
         <f>D22*D23*D24</f>
-        <v>16384000</v>
+        <v>6553600</v>
       </c>
       <c r="E25" s="19"/>
       <c r="F25" s="19">
         <f t="shared" ref="F25" si="23">F22*F23*F24</f>
-        <v>3145728000</v>
+        <v>629145600</v>
       </c>
       <c r="G25" s="19"/>
       <c r="H25" s="19">
         <f t="shared" ref="H25" si="24">H22*H23*H24</f>
-        <v>3145728000</v>
+        <v>629145600</v>
       </c>
       <c r="I25" s="19"/>
       <c r="J25" s="19">
         <f t="shared" ref="J25" si="25">J22*J23*J24</f>
-        <v>3145728000</v>
+        <v>629145600</v>
       </c>
       <c r="K25" s="19"/>
       <c r="L25" s="19">
         <f t="shared" ref="L25" si="26">L22*L23*L24</f>
-        <v>3145728000</v>
+        <v>629145600</v>
       </c>
       <c r="M25" s="19"/>
       <c r="N25" s="19">
         <f t="shared" ref="N25" si="27">N22*N23*N24</f>
-        <v>3145728000</v>
+        <v>629145600</v>
       </c>
       <c r="O25" s="19"/>
       <c r="P25" s="19">
         <f t="shared" ref="P25" si="28">P22*P23*P24</f>
-        <v>3145728000</v>
+        <v>629145600</v>
       </c>
       <c r="Q25" s="19"/>
       <c r="R25" s="13"/>
@@ -2498,42 +2498,42 @@
       </c>
       <c r="B28" s="17">
         <f>B26/512/8/1600*B$25</f>
-        <v>16.84</v>
+        <v>6.7360000000000007</v>
       </c>
       <c r="C28" s="17"/>
       <c r="D28" s="17">
         <f>D26/512/8/1600*D$25</f>
-        <v>2.88</v>
+        <v>1.1519999999999999</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="17">
         <f>F26/4096/8/3200*F$25</f>
-        <v>436.08</v>
+        <v>87.215999999999994</v>
       </c>
       <c r="G28" s="17"/>
       <c r="H28" s="17">
         <f t="shared" ref="H28" si="29">H26/4096/8/3200*H$25</f>
-        <v>152.51999999999998</v>
+        <v>30.503999999999998</v>
       </c>
       <c r="I28" s="17"/>
       <c r="J28" s="17">
         <f t="shared" ref="J28" si="30">J26/4096/8/3200*J$25</f>
-        <v>120.72</v>
+        <v>24.143999999999998</v>
       </c>
       <c r="K28" s="17"/>
       <c r="L28" s="17">
         <f t="shared" ref="L28" si="31">L26/4096/8/3200*L$25</f>
-        <v>176.73</v>
+        <v>35.345999999999997</v>
       </c>
       <c r="M28" s="17"/>
       <c r="N28" s="17">
         <f t="shared" ref="N28" si="32">N26/4096/8/3200*N$25</f>
-        <v>335.85</v>
+        <v>67.17</v>
       </c>
       <c r="O28" s="17"/>
       <c r="P28" s="17">
         <f t="shared" ref="P28" si="33">P26/4096/8/3200*P$25</f>
-        <v>235.65000000000003</v>
+        <v>47.13</v>
       </c>
       <c r="Q28" s="17"/>
     </row>
@@ -2543,42 +2543,42 @@
       </c>
       <c r="B29" s="17">
         <f>B27/512/8/1600*B$25</f>
-        <v>38.224999999999994</v>
+        <v>15.289999999999997</v>
       </c>
       <c r="C29" s="17"/>
       <c r="D29" s="17">
         <f>D27/512/8/1600*D$25</f>
-        <v>59.15</v>
+        <v>23.66</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="17">
         <f>F27/4096/8/3200*F$25</f>
-        <v>3242.4</v>
+        <v>648.48</v>
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="17">
         <f t="shared" ref="H29" si="34">H27/4096/8/3200*H$25</f>
-        <v>1882.4999999999998</v>
+        <v>376.49999999999994</v>
       </c>
       <c r="I29" s="17"/>
       <c r="J29" s="17">
         <f t="shared" ref="J29" si="35">J27/4096/8/3200*J$25</f>
-        <v>1702.2</v>
+        <v>340.44</v>
       </c>
       <c r="K29" s="17"/>
       <c r="L29" s="17">
         <f t="shared" ref="L29" si="36">L27/4096/8/3200*L$25</f>
-        <v>2010.5999999999997</v>
+        <v>402.11999999999995</v>
       </c>
       <c r="M29" s="17"/>
       <c r="N29" s="17">
         <f t="shared" ref="N29" si="37">N27/4096/8/3200*N$25</f>
-        <v>2187.0000000000005</v>
+        <v>437.40000000000003</v>
       </c>
       <c r="O29" s="17"/>
       <c r="P29" s="17">
         <f t="shared" ref="P29" si="38">P27/4096/8/3200*P$25</f>
-        <v>2413.5</v>
+        <v>482.7</v>
       </c>
       <c r="Q29" s="17"/>
     </row>
@@ -2625,42 +2625,42 @@
       </c>
       <c r="B31" s="21">
         <f>(B28+B29*B30)/86400</f>
-        <v>6.3732638888888888E-4</v>
+        <v>2.549305555555555E-4</v>
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="21">
         <f t="shared" ref="D31:F31" si="39">(D28+D29*D30)/86400</f>
-        <v>7.1793981481481481E-4</v>
+        <v>2.8717592592592597E-4</v>
       </c>
       <c r="E31" s="21"/>
       <c r="F31" s="21">
         <f t="shared" si="39"/>
-        <v>4.2575000000000002E-2</v>
+        <v>8.515E-3</v>
       </c>
       <c r="G31" s="21"/>
       <c r="H31" s="21">
         <f>(H28+H29*H30+J28)/86400</f>
-        <v>2.4950694444444442E-2</v>
+        <v>4.9901388888888886E-3</v>
       </c>
       <c r="I31" s="21"/>
       <c r="J31" s="21">
         <f>(J28+J29*J30+L28)/86400</f>
-        <v>2.3144097222222222E-2</v>
+        <v>4.628819444444445E-3</v>
       </c>
       <c r="K31" s="21"/>
       <c r="L31" s="21">
         <f t="shared" ref="L31:P31" si="40">(L28+L29*L30)/86400</f>
-        <v>2.531631944444444E-2</v>
+        <v>5.063263888888888E-3</v>
       </c>
       <c r="M31" s="21"/>
       <c r="N31" s="21">
         <f t="shared" si="40"/>
-        <v>2.9199652777777783E-2</v>
+        <v>5.8399305555555565E-3</v>
       </c>
       <c r="O31" s="21"/>
       <c r="P31" s="21">
         <f t="shared" si="40"/>
-        <v>3.0661458333333336E-2</v>
+        <v>6.132291666666667E-3</v>
       </c>
       <c r="Q31" s="21"/>
       <c r="R31" s="17"/>

</xml_diff>

<commit_message>
Update: thermal deformation for 1, 3, 10, 20, 40W lasers
</commit_message>
<xml_diff>
--- a/Sampling_Resolution_Calculator.xlsx
+++ b/Sampling_Resolution_Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nanw0\GoogleDrive\SLAC\SLAC-Diling\11. 21 Winter\DXS optics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFE9810-1CC1-42FB-974B-4B724277ADFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFFE0E2-96BA-41EB-8274-FBC8C2E888C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="945" yWindow="555" windowWidth="25335" windowHeight="20370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HHLM" sheetId="10" r:id="rId1"/>
@@ -482,22 +482,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -782,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9ED2467-9A32-4D0C-9EF6-BA646B0CE237}">
   <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -808,10 +808,10 @@
       <c r="A1" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="16"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -820,10 +820,10 @@
       <c r="B2">
         <v>9481</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="16"/>
+      <c r="E2" s="21"/>
       <c r="F2">
         <v>19.909876918386299</v>
       </c>
@@ -846,10 +846,10 @@
       <c r="B3">
         <v>20</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="16"/>
+      <c r="E3" s="21"/>
       <c r="F3">
         <v>17</v>
       </c>
@@ -868,10 +868,10 @@
       <c r="B4" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="16"/>
+      <c r="E4" s="21"/>
       <c r="F4">
         <f>SIN(RADIANS(F2+F3))/SIN(RADIANS(F2-F3))</f>
         <v>11.830135875287004</v>
@@ -895,10 +895,10 @@
       <c r="B5" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="16"/>
+      <c r="E5" s="21"/>
       <c r="F5">
         <f>ABS((COS(RADIANS(F2-F3))-COS(RADIANS(F2+F3)))/SIN(RADIANS(F2-F3)))</f>
         <v>3.9225661843587014</v>
@@ -924,10 +924,10 @@
         <f>B3/10</f>
         <v>2</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="16"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="1">
         <v>5.9999999999999997E-7</v>
       </c>
@@ -947,10 +947,10 @@
         <f>4/B8</f>
         <v>2</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="16"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="7">
         <f>SUM(28:28)/86400</f>
         <v>6.0394444444444445E-3</v>
@@ -964,20 +964,20 @@
         <f>MIN(B9/400,0.001)</f>
         <v>1E-3</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="16"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="7">
         <f>SUM(31:31)-F9</f>
         <v>4.7264062499999995E-2</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="16"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="10">
         <f>SUM(31:31)</f>
         <v>5.330350694444444E-2</v>
@@ -1015,26 +1015,26 @@
       <c r="A16" t="s">
         <v>89</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16" t="s">
+      <c r="C16" s="21"/>
+      <c r="D16" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16" t="s">
+      <c r="E16" s="21"/>
+      <c r="F16" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16" t="s">
+      <c r="G16" s="21"/>
+      <c r="H16" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16" t="s">
+      <c r="I16" s="21"/>
+      <c r="J16" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="K16" s="16"/>
+      <c r="K16" s="21"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
@@ -1228,317 +1228,317 @@
       <c r="A21" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="17">
+      <c r="B21" s="18">
         <v>722.7</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17">
+      <c r="C21" s="18"/>
+      <c r="D21" s="18">
         <f>B21*J2</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17">
+      <c r="E21" s="18"/>
+      <c r="F21" s="18">
         <f>D21</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17">
+      <c r="G21" s="18"/>
+      <c r="H21" s="18">
         <f>F21</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17">
+      <c r="I21" s="18"/>
+      <c r="J21" s="18">
         <f>H21/J2</f>
         <v>722.7</v>
       </c>
-      <c r="K21" s="17"/>
+      <c r="K21" s="18"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="17">
         <f>B12</f>
         <v>512</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18">
+      <c r="C22" s="17"/>
+      <c r="D22" s="17">
         <f>B22*I2</f>
         <v>6144</v>
       </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18">
+      <c r="E22" s="17"/>
+      <c r="F22" s="17">
         <f>D22</f>
         <v>6144</v>
       </c>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18">
+      <c r="G22" s="17"/>
+      <c r="H22" s="17">
         <f>F22</f>
         <v>6144</v>
       </c>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18">
+      <c r="I22" s="17"/>
+      <c r="J22" s="17">
         <f t="shared" ref="J22:J24" si="7">H22</f>
         <v>6144</v>
       </c>
-      <c r="K22" s="18"/>
+      <c r="K22" s="17"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="17">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18">
+      <c r="C23" s="17"/>
+      <c r="D23" s="17">
         <f t="shared" ref="D23" si="8">B23</f>
         <v>8</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18">
+      <c r="E23" s="17"/>
+      <c r="F23" s="17">
         <f t="shared" ref="F23" si="9">D23</f>
         <v>8</v>
       </c>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18">
+      <c r="G23" s="17"/>
+      <c r="H23" s="17">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18">
+      <c r="I23" s="17"/>
+      <c r="J23" s="17">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="K23" s="18"/>
+      <c r="K23" s="17"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="17">
         <f>B14</f>
         <v>2000</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18">
+      <c r="C24" s="17"/>
+      <c r="D24" s="17">
         <f>B24*I4</f>
         <v>26000</v>
       </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18">
+      <c r="E24" s="17"/>
+      <c r="F24" s="17">
         <f>D24</f>
         <v>26000</v>
       </c>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18">
+      <c r="G24" s="17"/>
+      <c r="H24" s="17">
         <f t="shared" ref="H24" si="10">F24</f>
         <v>26000</v>
       </c>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18">
+      <c r="I24" s="17"/>
+      <c r="J24" s="17">
         <f t="shared" si="7"/>
         <v>26000</v>
       </c>
-      <c r="K24" s="18"/>
+      <c r="K24" s="17"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="20">
         <f>B22*B23*B24</f>
         <v>8192000</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19">
+      <c r="C25" s="20"/>
+      <c r="D25" s="20">
         <f>D22*D23*D24</f>
         <v>1277952000</v>
       </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19">
+      <c r="E25" s="20"/>
+      <c r="F25" s="20">
         <f t="shared" ref="F25" si="11">F22*F23*F24</f>
         <v>1277952000</v>
       </c>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19">
+      <c r="G25" s="20"/>
+      <c r="H25" s="20">
         <f t="shared" ref="H25" si="12">H22*H23*H24</f>
         <v>1277952000</v>
       </c>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19">
+      <c r="I25" s="20"/>
+      <c r="J25" s="20">
         <f t="shared" ref="J25" si="13">J22*J23*J24</f>
         <v>1277952000</v>
       </c>
-      <c r="K25" s="19"/>
+      <c r="K25" s="20"/>
     </row>
     <row r="26" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" s="19">
         <f>0.191+9.964+1.804+1.666</f>
         <v>13.625000000000002</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20">
+      <c r="C26" s="19"/>
+      <c r="D26" s="19">
         <v>25.887</v>
       </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20">
+      <c r="E26" s="19"/>
+      <c r="F26" s="19">
         <v>21.568000000000001</v>
       </c>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20">
+      <c r="G26" s="19"/>
+      <c r="H26" s="19">
         <v>21.541</v>
       </c>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20">
+      <c r="I26" s="19"/>
+      <c r="J26" s="19">
         <v>9.1859999999999999</v>
       </c>
-      <c r="K26" s="20"/>
+      <c r="K26" s="19"/>
     </row>
     <row r="27" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="20">
+      <c r="B27" s="19">
         <f>19.37+17.15</f>
         <v>36.519999999999996</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20">
+      <c r="C27" s="19"/>
+      <c r="D27" s="19">
         <v>146.75</v>
       </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20">
+      <c r="E27" s="19"/>
+      <c r="F27" s="19">
         <v>180.85</v>
       </c>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20">
+      <c r="G27" s="19"/>
+      <c r="H27" s="19">
         <v>166.69</v>
       </c>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20">
+      <c r="I27" s="19"/>
+      <c r="J27" s="19">
         <v>128.34</v>
       </c>
-      <c r="K27" s="20"/>
+      <c r="K27" s="19"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="17">
+      <c r="B28" s="18">
         <f>B26/512/8/2000*B$25</f>
         <v>13.625000000000002</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17">
+      <c r="C28" s="18"/>
+      <c r="D28" s="18">
         <f>D26/6144/8/4000*D$25</f>
         <v>168.2655</v>
       </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17">
+      <c r="E28" s="18"/>
+      <c r="F28" s="18">
         <f t="shared" ref="F28" si="14">F26/6144/8/4000*F$25</f>
         <v>140.19200000000001</v>
       </c>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17">
+      <c r="G28" s="18"/>
+      <c r="H28" s="18">
         <f t="shared" ref="H28" si="15">H26/6144/8/4000*H$25</f>
         <v>140.01650000000001</v>
       </c>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17">
+      <c r="I28" s="18"/>
+      <c r="J28" s="18">
         <f t="shared" ref="J28" si="16">J26/6144/8/4000*J$25</f>
         <v>59.708999999999996</v>
       </c>
-      <c r="K28" s="17"/>
+      <c r="K28" s="18"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="17">
+      <c r="B29" s="18">
         <f>B27/512/8/2000*B$25</f>
         <v>36.519999999999996</v>
       </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17">
+      <c r="C29" s="18"/>
+      <c r="D29" s="18">
         <f>D27/6144/8/4000*D$25</f>
         <v>953.875</v>
       </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17">
+      <c r="E29" s="18"/>
+      <c r="F29" s="18">
         <f t="shared" ref="F29" si="17">F27/6144/8/4000*F$25</f>
         <v>1175.5250000000001</v>
       </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17">
+      <c r="G29" s="18"/>
+      <c r="H29" s="18">
         <f t="shared" ref="H29" si="18">H27/6144/8/4000*H$25</f>
         <v>1083.4849999999999</v>
       </c>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17">
+      <c r="I29" s="18"/>
+      <c r="J29" s="18">
         <f t="shared" ref="J29" si="19">J27/6144/8/4000*J$25</f>
         <v>834.20999999999992</v>
       </c>
-      <c r="K29" s="17"/>
+      <c r="K29" s="18"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="18">
+      <c r="B30" s="17">
         <v>1</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18">
+      <c r="C30" s="17"/>
+      <c r="D30" s="17">
         <v>1</v>
       </c>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18">
+      <c r="E30" s="17"/>
+      <c r="F30" s="17">
         <v>1</v>
       </c>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18">
+      <c r="G30" s="17"/>
+      <c r="H30" s="17">
         <v>1</v>
       </c>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18">
+      <c r="I30" s="17"/>
+      <c r="J30" s="17">
         <v>1</v>
       </c>
-      <c r="K30" s="18"/>
+      <c r="K30" s="17"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="21">
+      <c r="B31" s="16">
         <f>(B28+B29*B30)/86400</f>
         <v>5.8038194444444435E-4</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21">
+      <c r="C31" s="16"/>
+      <c r="D31" s="16">
         <f t="shared" ref="D31:F31" si="20">(D28+D29*D30)/86400</f>
         <v>1.2987737268518517E-2</v>
       </c>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21">
+      <c r="E31" s="16"/>
+      <c r="F31" s="16">
         <f t="shared" si="20"/>
         <v>1.5228206018518519E-2</v>
       </c>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21">
+      <c r="G31" s="16"/>
+      <c r="H31" s="16">
         <f t="shared" ref="H31" si="21">(H28+H29*H30)/86400</f>
         <v>1.4160896990740739E-2</v>
       </c>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21">
+      <c r="I31" s="16"/>
+      <c r="J31" s="16">
         <f t="shared" ref="J31" si="22">(J28+J29*J30)/86400</f>
         <v>1.034628472222222E-2</v>
       </c>
-      <c r="K31" s="21"/>
+      <c r="K31" s="16"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="E32" s="6"/>
@@ -1550,66 +1550,6 @@
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="F16:G16"/>
@@ -1619,6 +1559,66 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D8:E8"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1629,8 +1629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FDDF995-0054-48A7-B092-0C0EFEBE5F19}">
   <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1658,10 +1658,10 @@
       <c r="A1" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="16"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1670,10 +1670,10 @@
       <c r="B2">
         <v>9481</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="16"/>
+      <c r="E2" s="21"/>
       <c r="F2">
         <v>42.926477759350803</v>
       </c>
@@ -1694,12 +1694,12 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>100</v>
-      </c>
-      <c r="D3" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="16"/>
+      <c r="E3" s="21"/>
       <c r="F3">
         <v>-29.5</v>
       </c>
@@ -1719,10 +1719,10 @@
         <f>0.005</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="16"/>
+      <c r="E4" s="21"/>
       <c r="F4">
         <f>SIN(RADIANS(F2+F3))/SIN(RADIANS(F2-F3))</f>
         <v>0.24356450463759297</v>
@@ -1732,11 +1732,11 @@
       </c>
       <c r="I4" s="2">
         <f>MAX(ROUND(2*I3/$B7,0),1)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J4">
         <f>I3/$B7</f>
-        <v>1.4657811346760605</v>
+        <v>2.9315622693521211</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -1747,10 +1747,10 @@
         <f>0.005</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="16"/>
+      <c r="E5" s="21"/>
       <c r="F5">
         <f>ABS((COS(RADIANS(F2-F3))-COS(RADIANS(F2+F3)))/SIN(RADIANS(F2-F3)))</f>
         <v>0.70357494464450898</v>
@@ -1765,7 +1765,7 @@
       </c>
       <c r="B7">
         <f>B8*B14</f>
-        <v>8000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
@@ -1774,12 +1774,12 @@
       </c>
       <c r="B8">
         <f>B3/10</f>
-        <v>10</v>
-      </c>
-      <c r="D8" s="16" t="s">
+        <v>0.3</v>
+      </c>
+      <c r="D8" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="16"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="1">
         <v>5.9999999999999997E-7</v>
       </c>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="I8" s="9">
         <f>22122874/1024/1024/3072/8/26000*MAX(25:25)</f>
-        <v>20.773431865985575</v>
+        <v>692.4477288661858</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
@@ -1797,15 +1797,15 @@
       </c>
       <c r="B9">
         <f>4/B8</f>
-        <v>0.4</v>
-      </c>
-      <c r="D9" s="16" t="s">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="D9" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="16"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="7">
         <f>SUM(28:28)/86400</f>
-        <v>3.4652546296296298E-3</v>
+        <v>0.11398688271604938</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
@@ -1814,25 +1814,25 @@
       </c>
       <c r="B10">
         <f>MIN(B9/800,0.001)</f>
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="D10" s="16" t="s">
+        <v>1E-3</v>
+      </c>
+      <c r="D10" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="16"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="7">
         <f>SUM(31:31)-F9</f>
-        <v>3.2246296296296301E-2</v>
+        <v>1.0673630401234568</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="16"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="10">
         <f>SUM(31:31)</f>
-        <v>3.5711550925925928E-2</v>
+        <v>1.1813499228395061</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
@@ -1860,47 +1860,47 @@
       </c>
       <c r="B14">
         <f>B9/B10</f>
-        <v>800</v>
+        <v>13333.333333333334</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>88</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16" t="s">
+      <c r="C16" s="21"/>
+      <c r="D16" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16" t="s">
+      <c r="E16" s="21"/>
+      <c r="F16" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16" t="s">
+      <c r="G16" s="21"/>
+      <c r="H16" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16" t="s">
+      <c r="I16" s="21"/>
+      <c r="J16" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16" t="s">
+      <c r="K16" s="21"/>
+      <c r="L16" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16" t="s">
+      <c r="M16" s="21"/>
+      <c r="N16" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16" t="s">
+      <c r="O16" s="21"/>
+      <c r="P16" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="16"/>
-      <c r="S16" s="16"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="21"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
@@ -2050,19 +2050,19 @@
       </c>
       <c r="B19" s="2">
         <f>B7</f>
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="C19" s="2">
         <f>B8</f>
-        <v>10</v>
+        <v>0.3</v>
       </c>
       <c r="D19" s="2">
         <f>E19*D24</f>
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="E19" s="2">
         <f>C19</f>
-        <v>10</v>
+        <v>0.3</v>
       </c>
       <c r="F19" s="2">
         <f>G19*F24</f>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="G19" s="2">
         <f>E19</f>
-        <v>10</v>
+        <v>0.3</v>
       </c>
       <c r="H19" s="2">
         <f>I19*H24</f>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="I19" s="2">
         <f>G19</f>
-        <v>10</v>
+        <v>0.3</v>
       </c>
       <c r="J19" s="2">
         <f>K19*J24</f>
@@ -2086,7 +2086,7 @@
       </c>
       <c r="K19" s="2">
         <f>I19</f>
-        <v>10</v>
+        <v>0.3</v>
       </c>
       <c r="L19" s="2">
         <f>M19*L24</f>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="M19" s="2">
         <f>K19</f>
-        <v>10</v>
+        <v>0.3</v>
       </c>
       <c r="N19" s="2">
         <f>O19*N24</f>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="O19" s="2">
         <f>M19</f>
-        <v>10</v>
+        <v>0.3</v>
       </c>
       <c r="P19" s="2">
         <f>Q19*P24</f>
@@ -2110,7 +2110,7 @@
       </c>
       <c r="Q19" s="2">
         <f>O19</f>
-        <v>10</v>
+        <v>0.3</v>
       </c>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
@@ -2121,23 +2121,23 @@
       </c>
       <c r="B20" s="2">
         <f>B9*1000</f>
-        <v>400</v>
+        <v>13333.333333333334</v>
       </c>
       <c r="C20" s="2">
         <f>B10*1000</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D20" s="2">
         <f>$B20*$C19/E19</f>
-        <v>400</v>
+        <v>13333.333333333334</v>
       </c>
       <c r="E20" s="2">
         <f>$B19*$C20/D19</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F20" s="2">
         <f>$B20*$C19/G19</f>
-        <v>400</v>
+        <v>13333.333333333334</v>
       </c>
       <c r="G20" s="2">
         <f>$B19*$C20/F19</f>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="H20" s="2">
         <f t="shared" ref="H20" si="6">$B20*$C19/I19</f>
-        <v>400</v>
+        <v>13333.333333333334</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" ref="I20" si="7">$B19*$C20/H19</f>
@@ -2153,7 +2153,7 @@
       </c>
       <c r="J20" s="2">
         <f t="shared" ref="J20" si="8">$B20*$C19/K19</f>
-        <v>400</v>
+        <v>13333.333333333334</v>
       </c>
       <c r="K20" s="2">
         <f t="shared" ref="K20" si="9">$B19*$C20/J19</f>
@@ -2161,7 +2161,7 @@
       </c>
       <c r="L20" s="2">
         <f t="shared" ref="L20" si="10">$B20*$C19/M19</f>
-        <v>400</v>
+        <v>13333.333333333334</v>
       </c>
       <c r="M20" s="2">
         <f t="shared" ref="M20" si="11">$B19*$C20/L19</f>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="N20" s="2">
         <f t="shared" ref="N20" si="12">$B20*$C19/O19</f>
-        <v>400</v>
+        <v>13333.333333333334</v>
       </c>
       <c r="O20" s="2">
         <f t="shared" ref="O20" si="13">$B19*$C20/N19</f>
@@ -2177,7 +2177,7 @@
       </c>
       <c r="P20" s="2">
         <f t="shared" ref="P20" si="14">$B20*$C19/Q19</f>
-        <v>400</v>
+        <v>13333.333333333334</v>
       </c>
       <c r="Q20" s="2">
         <f t="shared" ref="Q20" si="15">$B19*$C20/P19</f>
@@ -2190,38 +2190,38 @@
       <c r="A21" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="17">
+      <c r="B21" s="18">
         <v>726.57</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17">
+      <c r="C21" s="18"/>
+      <c r="D21" s="18">
         <v>722.86</v>
       </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17">
+      <c r="E21" s="18"/>
+      <c r="F21" s="18">
         <v>722.85</v>
       </c>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17">
+      <c r="G21" s="18"/>
+      <c r="H21" s="18">
         <v>176.54</v>
       </c>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17">
+      <c r="I21" s="18"/>
+      <c r="J21" s="18">
         <v>14.28</v>
       </c>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17">
+      <c r="K21" s="18"/>
+      <c r="L21" s="18">
         <v>175.15</v>
       </c>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17">
+      <c r="M21" s="18"/>
+      <c r="N21" s="18">
         <v>173.04</v>
       </c>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17">
+      <c r="O21" s="18"/>
+      <c r="P21" s="18">
         <v>173.07</v>
       </c>
-      <c r="Q21" s="17"/>
+      <c r="Q21" s="18"/>
       <c r="R21" s="12"/>
       <c r="S21" s="12"/>
     </row>
@@ -2229,187 +2229,187 @@
       <c r="A22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="17">
         <f>B12</f>
         <v>1024</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18">
+      <c r="C22" s="17"/>
+      <c r="D22" s="17">
         <f>B22</f>
         <v>1024</v>
       </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18">
+      <c r="E22" s="17"/>
+      <c r="F22" s="17">
         <f>D22*I2*8</f>
         <v>32768</v>
       </c>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18">
+      <c r="G22" s="17"/>
+      <c r="H22" s="17">
         <f>F22</f>
         <v>32768</v>
       </c>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18">
+      <c r="I22" s="17"/>
+      <c r="J22" s="17">
         <f t="shared" ref="J22:J24" si="16">H22</f>
         <v>32768</v>
       </c>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18">
+      <c r="K22" s="17"/>
+      <c r="L22" s="17">
         <f t="shared" ref="L22:L24" si="17">J22</f>
         <v>32768</v>
       </c>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18">
+      <c r="M22" s="17"/>
+      <c r="N22" s="17">
         <f>L22</f>
         <v>32768</v>
       </c>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18">
+      <c r="O22" s="17"/>
+      <c r="P22" s="17">
         <f t="shared" ref="P22:P23" si="18">N22</f>
         <v>32768</v>
       </c>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="S22" s="17"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="17">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18">
+      <c r="C23" s="17"/>
+      <c r="D23" s="17">
         <f t="shared" ref="D23:D24" si="19">B23</f>
         <v>8</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18">
+      <c r="E23" s="17"/>
+      <c r="F23" s="17">
         <f t="shared" ref="F23" si="20">D23</f>
         <v>8</v>
       </c>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18">
+      <c r="G23" s="17"/>
+      <c r="H23" s="17">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18">
+      <c r="I23" s="17"/>
+      <c r="J23" s="17">
         <f t="shared" si="16"/>
         <v>8</v>
       </c>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18">
+      <c r="K23" s="17"/>
+      <c r="L23" s="17">
         <f t="shared" si="17"/>
         <v>8</v>
       </c>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18">
+      <c r="M23" s="17"/>
+      <c r="N23" s="17">
         <f>L23</f>
         <v>8</v>
       </c>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18">
+      <c r="O23" s="17"/>
+      <c r="P23" s="17">
         <f t="shared" si="18"/>
         <v>8</v>
       </c>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="17"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="17">
         <f>B14</f>
-        <v>800</v>
-      </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18">
+        <v>13333.333333333334</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17">
         <f t="shared" si="19"/>
-        <v>800</v>
-      </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18">
+        <v>13333.333333333334</v>
+      </c>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17">
         <f>D24*I4</f>
-        <v>2400</v>
-      </c>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18">
+        <v>80000</v>
+      </c>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17">
         <f t="shared" ref="H24" si="21">F24</f>
-        <v>2400</v>
-      </c>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18">
+        <v>80000</v>
+      </c>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17">
         <f t="shared" si="16"/>
-        <v>2400</v>
-      </c>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18">
+        <v>80000</v>
+      </c>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17">
         <f t="shared" si="17"/>
-        <v>2400</v>
-      </c>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18">
+        <v>80000</v>
+      </c>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17">
         <f t="shared" ref="N24" si="22">L24</f>
-        <v>2400</v>
-      </c>
-      <c r="O24" s="18"/>
-      <c r="P24" s="18">
+        <v>80000</v>
+      </c>
+      <c r="O24" s="17"/>
+      <c r="P24" s="17">
         <f>N24</f>
-        <v>2400</v>
-      </c>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18"/>
-      <c r="S24" s="18"/>
+        <v>80000</v>
+      </c>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="17"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="20">
         <f>B22*B23*B24</f>
-        <v>6553600</v>
-      </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19">
+        <v>109226666.66666667</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20">
         <f>D22*D23*D24</f>
-        <v>6553600</v>
-      </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19">
+        <v>109226666.66666667</v>
+      </c>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20">
         <f t="shared" ref="F25" si="23">F22*F23*F24</f>
-        <v>629145600</v>
-      </c>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19">
+        <v>20971520000</v>
+      </c>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20">
         <f t="shared" ref="H25" si="24">H22*H23*H24</f>
-        <v>629145600</v>
-      </c>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19">
+        <v>20971520000</v>
+      </c>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20">
         <f t="shared" ref="J25" si="25">J22*J23*J24</f>
-        <v>629145600</v>
-      </c>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19">
+        <v>20971520000</v>
+      </c>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20">
         <f t="shared" ref="L25" si="26">L22*L23*L24</f>
-        <v>629145600</v>
-      </c>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19">
+        <v>20971520000</v>
+      </c>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20">
         <f t="shared" ref="N25" si="27">N22*N23*N24</f>
-        <v>629145600</v>
-      </c>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19">
+        <v>20971520000</v>
+      </c>
+      <c r="O25" s="20"/>
+      <c r="P25" s="20">
         <f t="shared" ref="P25" si="28">P22*P23*P24</f>
-        <v>629145600</v>
-      </c>
-      <c r="Q25" s="19"/>
+        <v>20971520000</v>
+      </c>
+      <c r="Q25" s="20"/>
       <c r="R25" s="13"/>
       <c r="S25" s="13"/>
     </row>
@@ -2417,40 +2417,40 @@
       <c r="A26" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" s="19">
         <f>0.154+3.252+1.863+1.467</f>
         <v>6.7360000000000007</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20">
+      <c r="C26" s="19"/>
+      <c r="D26" s="19">
         <v>1.1519999999999999</v>
       </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20">
+      <c r="E26" s="19"/>
+      <c r="F26" s="19">
         <v>14.536</v>
       </c>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20">
+      <c r="G26" s="19"/>
+      <c r="H26" s="19">
         <v>5.0839999999999996</v>
       </c>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20">
+      <c r="I26" s="19"/>
+      <c r="J26" s="19">
         <f>0.874+3.15</f>
         <v>4.024</v>
       </c>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20">
+      <c r="K26" s="19"/>
+      <c r="L26" s="19">
         <v>5.891</v>
       </c>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20">
+      <c r="M26" s="19"/>
+      <c r="N26" s="19">
         <v>11.195</v>
       </c>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20">
+      <c r="O26" s="19"/>
+      <c r="P26" s="19">
         <v>7.8550000000000004</v>
       </c>
-      <c r="Q26" s="20"/>
+      <c r="Q26" s="19"/>
       <c r="R26" s="14"/>
       <c r="S26" s="14"/>
     </row>
@@ -2458,219 +2458,305 @@
       <c r="A27" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="20">
+      <c r="B27" s="19">
         <f>6.36+8.93</f>
         <v>15.29</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20">
+      <c r="C27" s="19"/>
+      <c r="D27" s="19">
         <v>23.66</v>
       </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20">
+      <c r="E27" s="19"/>
+      <c r="F27" s="19">
         <v>108.08</v>
       </c>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20">
+      <c r="G27" s="19"/>
+      <c r="H27" s="19">
         <v>62.75</v>
       </c>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20">
+      <c r="I27" s="19"/>
+      <c r="J27" s="19">
         <v>56.74</v>
       </c>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20">
+      <c r="K27" s="19"/>
+      <c r="L27" s="19">
         <v>67.02</v>
       </c>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20">
+      <c r="M27" s="19"/>
+      <c r="N27" s="19">
         <v>72.900000000000006</v>
       </c>
-      <c r="O27" s="20"/>
-      <c r="P27" s="20">
+      <c r="O27" s="19"/>
+      <c r="P27" s="19">
         <v>80.45</v>
       </c>
-      <c r="Q27" s="20"/>
+      <c r="Q27" s="19"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="17">
+      <c r="B28" s="18">
         <f>B26/512/8/1600*B$25</f>
-        <v>6.7360000000000007</v>
-      </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17">
+        <v>112.26666666666668</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18">
         <f>D26/512/8/1600*D$25</f>
-        <v>1.1519999999999999</v>
-      </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17">
+        <v>19.2</v>
+      </c>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18">
         <f>F26/4096/8/3200*F$25</f>
-        <v>87.215999999999994</v>
-      </c>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17">
+        <v>2907.2</v>
+      </c>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18">
         <f t="shared" ref="H28" si="29">H26/4096/8/3200*H$25</f>
-        <v>30.503999999999998</v>
-      </c>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17">
+        <v>1016.8</v>
+      </c>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18">
         <f t="shared" ref="J28" si="30">J26/4096/8/3200*J$25</f>
-        <v>24.143999999999998</v>
-      </c>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17">
+        <v>804.8</v>
+      </c>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18">
         <f t="shared" ref="L28" si="31">L26/4096/8/3200*L$25</f>
-        <v>35.345999999999997</v>
-      </c>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17">
+        <v>1178.2</v>
+      </c>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18">
         <f t="shared" ref="N28" si="32">N26/4096/8/3200*N$25</f>
-        <v>67.17</v>
-      </c>
-      <c r="O28" s="17"/>
-      <c r="P28" s="17">
+        <v>2239</v>
+      </c>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18">
         <f t="shared" ref="P28" si="33">P26/4096/8/3200*P$25</f>
-        <v>47.13</v>
-      </c>
-      <c r="Q28" s="17"/>
+        <v>1571.0000000000002</v>
+      </c>
+      <c r="Q28" s="18"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="17">
+      <c r="B29" s="18">
         <f>B27/512/8/1600*B$25</f>
-        <v>15.289999999999997</v>
-      </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17">
+        <v>254.83333333333331</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18">
         <f>D27/512/8/1600*D$25</f>
-        <v>23.66</v>
-      </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17">
+        <v>394.33333333333337</v>
+      </c>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18">
         <f>F27/4096/8/3200*F$25</f>
-        <v>648.48</v>
-      </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17">
+        <v>21616</v>
+      </c>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18">
         <f t="shared" ref="H29" si="34">H27/4096/8/3200*H$25</f>
-        <v>376.49999999999994</v>
-      </c>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17">
+        <v>12549.999999999998</v>
+      </c>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18">
         <f t="shared" ref="J29" si="35">J27/4096/8/3200*J$25</f>
-        <v>340.44</v>
-      </c>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17">
+        <v>11348</v>
+      </c>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18">
         <f t="shared" ref="L29" si="36">L27/4096/8/3200*L$25</f>
-        <v>402.11999999999995</v>
-      </c>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17">
+        <v>13403.999999999998</v>
+      </c>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18">
         <f t="shared" ref="N29" si="37">N27/4096/8/3200*N$25</f>
-        <v>437.40000000000003</v>
-      </c>
-      <c r="O29" s="17"/>
-      <c r="P29" s="17">
+        <v>14580.000000000002</v>
+      </c>
+      <c r="O29" s="18"/>
+      <c r="P29" s="18">
         <f t="shared" ref="P29" si="38">P27/4096/8/3200*P$25</f>
-        <v>482.7</v>
-      </c>
-      <c r="Q29" s="17"/>
+        <v>16090</v>
+      </c>
+      <c r="Q29" s="18"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="18">
+      <c r="B30" s="17">
         <v>1</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18">
+      <c r="C30" s="17"/>
+      <c r="D30" s="17">
         <v>1</v>
       </c>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18">
+      <c r="E30" s="17"/>
+      <c r="F30" s="17">
         <v>1</v>
       </c>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18">
+      <c r="G30" s="17"/>
+      <c r="H30" s="17">
         <v>1</v>
       </c>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18">
+      <c r="I30" s="17"/>
+      <c r="J30" s="17">
         <v>1</v>
       </c>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18">
+      <c r="K30" s="17"/>
+      <c r="L30" s="17">
         <v>1</v>
       </c>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18">
+      <c r="M30" s="17"/>
+      <c r="N30" s="17">
         <v>1</v>
       </c>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18">
+      <c r="O30" s="17"/>
+      <c r="P30" s="17">
         <v>1</v>
       </c>
-      <c r="Q30" s="18"/>
+      <c r="Q30" s="17"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="21">
+      <c r="B31" s="16">
         <f>(B28+B29*B30)/86400</f>
-        <v>2.549305555555555E-4</v>
-      </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21">
+        <v>4.2488425925925931E-3</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16">
         <f t="shared" ref="D31:F31" si="39">(D28+D29*D30)/86400</f>
-        <v>2.8717592592592597E-4</v>
-      </c>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21">
+        <v>4.7862654320987661E-3</v>
+      </c>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16">
         <f t="shared" si="39"/>
-        <v>8.515E-3</v>
-      </c>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21">
+        <v>0.28383333333333333</v>
+      </c>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16">
         <f>(H28+H29*H30+J28)/86400</f>
-        <v>4.9901388888888886E-3</v>
-      </c>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21">
+        <v>0.16633796296296294</v>
+      </c>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16">
         <f>(J28+J29*J30+L28)/86400</f>
-        <v>4.628819444444445E-3</v>
-      </c>
-      <c r="K31" s="21"/>
-      <c r="L31" s="21">
+        <v>0.15429398148148149</v>
+      </c>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16">
         <f t="shared" ref="L31:P31" si="40">(L28+L29*L30)/86400</f>
-        <v>5.063263888888888E-3</v>
-      </c>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21">
+        <v>0.16877546296296295</v>
+      </c>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16">
         <f t="shared" si="40"/>
-        <v>5.8399305555555565E-3</v>
-      </c>
-      <c r="O31" s="21"/>
-      <c r="P31" s="21">
+        <v>0.19466435185185185</v>
+      </c>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16">
         <f t="shared" si="40"/>
-        <v>6.132291666666667E-3</v>
-      </c>
-      <c r="Q31" s="21"/>
-      <c r="R31" s="17"/>
-      <c r="S31" s="17"/>
+        <v>0.20440972222222223</v>
+      </c>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="18"/>
+      <c r="S31" s="18"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="E32" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="110">
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="P31:Q31"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
     <mergeCell ref="N26:O26"/>
     <mergeCell ref="N27:O27"/>
     <mergeCell ref="P26:Q26"/>
@@ -2695,92 +2781,6 @@
     <mergeCell ref="F27:G27"/>
     <mergeCell ref="H27:I27"/>
     <mergeCell ref="J27:K27"/>
-    <mergeCell ref="R31:S31"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="P31:Q31"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="R24:S24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2793,7 +2793,7 @@
   <dimension ref="A1:AA31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Y31"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2829,14 +2829,14 @@
       <c r="A1" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="L1" s="16" t="s">
+      <c r="E1" s="21"/>
+      <c r="L1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="16"/>
+      <c r="M1" s="21"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2845,10 +2845,10 @@
       <c r="B2">
         <v>9481</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="16"/>
+      <c r="E2" s="21"/>
       <c r="F2">
         <v>19.909876918386299</v>
       </c>
@@ -2863,10 +2863,10 @@
         <f>MAX(F4,1/F4)</f>
         <v>11.830135875287004</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="16"/>
+      <c r="M2" s="21"/>
       <c r="N2">
         <v>42.926477759350803</v>
       </c>
@@ -2887,12 +2887,12 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>20</v>
-      </c>
-      <c r="D3" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="16"/>
+      <c r="E3" s="21"/>
       <c r="F3">
         <v>17</v>
       </c>
@@ -2903,10 +2903,10 @@
         <f>$B4*F5/300000000*1000000000000000</f>
         <v>52300.882458116022</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="L3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="16"/>
+      <c r="M3" s="21"/>
       <c r="N3">
         <v>-29.5</v>
       </c>
@@ -2925,10 +2925,10 @@
       <c r="B4" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="16"/>
+      <c r="E4" s="21"/>
       <c r="F4">
         <f>SIN(RADIANS(F2+F3))/SIN(RADIANS(F2-F3))</f>
         <v>11.830135875287004</v>
@@ -2944,10 +2944,10 @@
         <f>I3/$B7</f>
         <v>13.075220614529005</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="L4" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="16"/>
+      <c r="M4" s="21"/>
       <c r="N4">
         <f>SIN(RADIANS(N2+N3))/SIN(RADIANS(N2-N3))</f>
         <v>0.24356450463759297</v>
@@ -2971,18 +2971,18 @@
       <c r="B5" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="16"/>
+      <c r="E5" s="21"/>
       <c r="F5">
         <f>ABS((COS(RADIANS(F2-F3))-COS(RADIANS(F2+F3)))/SIN(RADIANS(F2-F3)))</f>
         <v>3.9225661843587014</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="L5" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="16"/>
+      <c r="M5" s="21"/>
       <c r="N5">
         <f>ABS((COS(RADIANS(N2-N3))-COS(RADIANS(N2+N3)))/SIN(RADIANS(N2-N3)))</f>
         <v>0.70357494464450898</v>
@@ -3006,12 +3006,12 @@
       </c>
       <c r="B8">
         <f>B3/10</f>
-        <v>2</v>
-      </c>
-      <c r="D8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="16"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="1">
         <v>5.9999999999999997E-7</v>
       </c>
@@ -3020,7 +3020,7 @@
       </c>
       <c r="I8" s="9">
         <f>22122874/1024/1024/3072/8/26000*MAX(25:25)</f>
-        <v>1350.2730712890623</v>
+        <v>450.09102376302076</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
@@ -3029,15 +3029,15 @@
       </c>
       <c r="B9">
         <f>4/B8</f>
-        <v>2</v>
-      </c>
-      <c r="D9" s="16" t="s">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D9" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="16"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="7">
         <f>SUM(28:28)/86400</f>
-        <v>0.1360213888888889</v>
+        <v>4.5340462962962964E-2</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
@@ -3048,23 +3048,23 @@
         <f>MIN(B9/400,0.001)</f>
         <v>1E-3</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="16"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="7">
         <f>SUM(31:31)-F9</f>
-        <v>1.3155878472222222</v>
+        <v>0.43852928240740741</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="16"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="10">
         <f>SUM(31:31)</f>
-        <v>1.451609236111111</v>
+        <v>0.48386974537037036</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
@@ -3092,60 +3092,60 @@
       </c>
       <c r="B14">
         <f>B9/B10</f>
-        <v>2000</v>
+        <v>666.66666666666663</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16" t="s">
+      <c r="C16" s="21"/>
+      <c r="D16" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16" t="s">
+      <c r="E16" s="21"/>
+      <c r="F16" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16" t="s">
+      <c r="G16" s="21"/>
+      <c r="H16" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16" t="s">
+      <c r="I16" s="21"/>
+      <c r="J16" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16" t="s">
+      <c r="K16" s="21"/>
+      <c r="L16" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16" t="s">
+      <c r="M16" s="21"/>
+      <c r="N16" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16" t="s">
+      <c r="O16" s="21"/>
+      <c r="P16" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="16" t="s">
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="S16" s="16"/>
-      <c r="T16" s="16" t="s">
+      <c r="S16" s="21"/>
+      <c r="T16" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="U16" s="16"/>
-      <c r="V16" s="16" t="s">
+      <c r="U16" s="21"/>
+      <c r="V16" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="W16" s="16"/>
-      <c r="X16" s="16" t="s">
+      <c r="W16" s="21"/>
+      <c r="X16" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="Y16" s="16"/>
-      <c r="Z16" s="16"/>
-      <c r="AA16" s="16"/>
+      <c r="Y16" s="21"/>
+      <c r="Z16" s="21"/>
+      <c r="AA16" s="21"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="C19" s="2">
         <f>B8</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D19" s="2">
         <f>E19*D24</f>
@@ -3371,7 +3371,7 @@
       </c>
       <c r="E19" s="2">
         <f>C19</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F19" s="2">
         <f>G19*F24</f>
@@ -3379,7 +3379,7 @@
       </c>
       <c r="G19" s="2">
         <f>E19</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H19" s="2">
         <f>I19*H24</f>
@@ -3387,7 +3387,7 @@
       </c>
       <c r="I19" s="2">
         <f>G19</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J19" s="2">
         <f>K19*J24</f>
@@ -3395,7 +3395,7 @@
       </c>
       <c r="K19" s="2">
         <f>I19</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L19" s="2">
         <f>M19*L24</f>
@@ -3403,7 +3403,7 @@
       </c>
       <c r="M19" s="2">
         <f>K19</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="N19" s="2">
         <f>O19*N24</f>
@@ -3411,7 +3411,7 @@
       </c>
       <c r="O19" s="2">
         <f>M19</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P19" s="2">
         <f>Q19*P24</f>
@@ -3419,7 +3419,7 @@
       </c>
       <c r="Q19" s="2">
         <f>O19</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="R19" s="2">
         <f>S19*R24</f>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="S19" s="2">
         <f>Q19</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="T19" s="2">
         <f>U19*T24</f>
@@ -3435,7 +3435,7 @@
       </c>
       <c r="U19" s="2">
         <f>S19</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="V19" s="2">
         <f>W19*V24</f>
@@ -3443,7 +3443,7 @@
       </c>
       <c r="W19" s="2">
         <f>U19</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="X19" s="2">
         <f>Y19*X24</f>
@@ -3451,7 +3451,7 @@
       </c>
       <c r="Y19" s="2">
         <f>W19</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
@@ -3462,7 +3462,7 @@
       </c>
       <c r="B20" s="2">
         <f>B9*1000</f>
-        <v>2000</v>
+        <v>666.66666666666663</v>
       </c>
       <c r="C20" s="2">
         <f>B10*1000</f>
@@ -3470,7 +3470,7 @@
       </c>
       <c r="D20" s="2">
         <f>$B20*$C19/E19</f>
-        <v>2000</v>
+        <v>666.66666666666663</v>
       </c>
       <c r="E20" s="2">
         <f>$B19*$C20/D19</f>
@@ -3478,7 +3478,7 @@
       </c>
       <c r="F20" s="2">
         <f>$B20*$C19/G19</f>
-        <v>2000</v>
+        <v>666.66666666666663</v>
       </c>
       <c r="G20" s="2">
         <f>$B19*$C20/F19</f>
@@ -3486,7 +3486,7 @@
       </c>
       <c r="H20" s="2">
         <f t="shared" ref="H20" si="9">$B20*$C19/I19</f>
-        <v>2000</v>
+        <v>666.66666666666663</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" ref="I20" si="10">$B19*$C20/H19</f>
@@ -3494,7 +3494,7 @@
       </c>
       <c r="J20" s="2">
         <f t="shared" ref="J20" si="11">$B20*$C19/K19</f>
-        <v>2000</v>
+        <v>666.66666666666663</v>
       </c>
       <c r="K20" s="2">
         <f t="shared" ref="K20" si="12">$B19*$C20/J19</f>
@@ -3502,7 +3502,7 @@
       </c>
       <c r="L20" s="2">
         <f>$B20*$C19/M19</f>
-        <v>2000</v>
+        <v>666.66666666666663</v>
       </c>
       <c r="M20" s="2">
         <f>$B19*$C20/L19</f>
@@ -3510,7 +3510,7 @@
       </c>
       <c r="N20" s="2">
         <f>$B20*$C19/O19</f>
-        <v>2000</v>
+        <v>666.66666666666663</v>
       </c>
       <c r="O20" s="2">
         <f>$B19*$C20/N19</f>
@@ -3518,7 +3518,7 @@
       </c>
       <c r="P20" s="2">
         <f t="shared" ref="P20" si="13">$B20*$C19/Q19</f>
-        <v>2000</v>
+        <v>666.66666666666663</v>
       </c>
       <c r="Q20" s="2">
         <f t="shared" ref="Q20" si="14">$B19*$C20/P19</f>
@@ -3526,7 +3526,7 @@
       </c>
       <c r="R20" s="2">
         <f t="shared" ref="R20" si="15">$B20*$C19/S19</f>
-        <v>2000</v>
+        <v>666.66666666666663</v>
       </c>
       <c r="S20" s="2">
         <f t="shared" ref="S20" si="16">$B19*$C20/R19</f>
@@ -3534,7 +3534,7 @@
       </c>
       <c r="T20" s="2">
         <f t="shared" ref="T20" si="17">$B20*$C19/U19</f>
-        <v>2000</v>
+        <v>666.66666666666663</v>
       </c>
       <c r="U20" s="2">
         <f t="shared" ref="U20" si="18">$B19*$C20/T19</f>
@@ -3542,7 +3542,7 @@
       </c>
       <c r="V20" s="2">
         <f t="shared" ref="V20" si="19">$B20*$C19/W19</f>
-        <v>2000</v>
+        <v>666.66666666666663</v>
       </c>
       <c r="W20" s="2">
         <f t="shared" ref="W20" si="20">$B19*$C20/V19</f>
@@ -3550,7 +3550,7 @@
       </c>
       <c r="X20" s="2">
         <f t="shared" ref="X20" si="21">$B20*$C19/Y19</f>
-        <v>2000</v>
+        <v>666.66666666666663</v>
       </c>
       <c r="Y20" s="2">
         <f t="shared" ref="Y20" si="22">$B19*$C20/X19</f>
@@ -3563,259 +3563,259 @@
       <c r="A21" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="17">
+      <c r="B21" s="18">
         <v>722.7</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17">
+      <c r="C21" s="18"/>
+      <c r="D21" s="18">
         <f>B21*J2</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17">
+      <c r="E21" s="18"/>
+      <c r="F21" s="18">
         <f>D21</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17">
+      <c r="G21" s="18"/>
+      <c r="H21" s="18">
         <f>F21</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17">
+      <c r="I21" s="18"/>
+      <c r="J21" s="18">
         <f>H21/J2</f>
         <v>722.7</v>
       </c>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17">
+      <c r="K21" s="18"/>
+      <c r="L21" s="18">
         <v>722.86</v>
       </c>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17">
+      <c r="M21" s="18"/>
+      <c r="N21" s="18">
         <v>722.85</v>
       </c>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17">
+      <c r="O21" s="18"/>
+      <c r="P21" s="18">
         <v>176.54</v>
       </c>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="17">
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18">
         <v>14.28</v>
       </c>
-      <c r="S21" s="17"/>
-      <c r="T21" s="17">
+      <c r="S21" s="18"/>
+      <c r="T21" s="18">
         <v>175.15</v>
       </c>
-      <c r="U21" s="17"/>
-      <c r="V21" s="17">
+      <c r="U21" s="18"/>
+      <c r="V21" s="18">
         <v>173.04</v>
       </c>
-      <c r="W21" s="17"/>
-      <c r="X21" s="17">
+      <c r="W21" s="18"/>
+      <c r="X21" s="18">
         <v>173.07</v>
       </c>
-      <c r="Y21" s="17"/>
-      <c r="Z21" s="18"/>
-      <c r="AA21" s="18"/>
+      <c r="Y21" s="18"/>
+      <c r="Z21" s="17"/>
+      <c r="AA21" s="17"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="17">
         <f>B12</f>
         <v>512</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18">
+      <c r="C22" s="17"/>
+      <c r="D22" s="17">
         <f>B22*I2</f>
         <v>6144</v>
       </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18">
+      <c r="E22" s="17"/>
+      <c r="F22" s="17">
         <f>D22</f>
         <v>6144</v>
       </c>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18">
+      <c r="G22" s="17"/>
+      <c r="H22" s="17">
         <f>F22</f>
         <v>6144</v>
       </c>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18">
+      <c r="I22" s="17"/>
+      <c r="J22" s="17">
         <f t="shared" ref="J22:J24" si="23">H22</f>
         <v>6144</v>
       </c>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18">
+      <c r="K22" s="17"/>
+      <c r="L22" s="17">
         <f>J22</f>
         <v>6144</v>
       </c>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18">
+      <c r="M22" s="17"/>
+      <c r="N22" s="17">
         <f>L22*Q2*4</f>
         <v>98304</v>
       </c>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18">
+      <c r="O22" s="17"/>
+      <c r="P22" s="17">
         <f>N22</f>
         <v>98304</v>
       </c>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18">
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17">
         <f t="shared" ref="R22:R24" si="24">P22</f>
         <v>98304</v>
       </c>
-      <c r="S22" s="18"/>
-      <c r="T22" s="18">
+      <c r="S22" s="17"/>
+      <c r="T22" s="17">
         <f t="shared" ref="T22:T24" si="25">R22</f>
         <v>98304</v>
       </c>
-      <c r="U22" s="18"/>
-      <c r="V22" s="18">
+      <c r="U22" s="17"/>
+      <c r="V22" s="17">
         <f>T22</f>
         <v>98304</v>
       </c>
-      <c r="W22" s="18"/>
-      <c r="X22" s="18">
+      <c r="W22" s="17"/>
+      <c r="X22" s="17">
         <f t="shared" ref="X22:X23" si="26">V22</f>
         <v>98304</v>
       </c>
-      <c r="Y22" s="18"/>
-      <c r="Z22" s="18"/>
-      <c r="AA22" s="18"/>
+      <c r="Y22" s="17"/>
+      <c r="Z22" s="17"/>
+      <c r="AA22" s="17"/>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="17">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18">
+      <c r="C23" s="17"/>
+      <c r="D23" s="17">
         <f t="shared" ref="D23" si="27">B23</f>
         <v>8</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18">
+      <c r="E23" s="17"/>
+      <c r="F23" s="17">
         <f t="shared" ref="F23" si="28">D23</f>
         <v>8</v>
       </c>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18">
+      <c r="G23" s="17"/>
+      <c r="H23" s="17">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18">
+      <c r="I23" s="17"/>
+      <c r="J23" s="17">
         <f t="shared" si="23"/>
         <v>8</v>
       </c>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18">
+      <c r="K23" s="17"/>
+      <c r="L23" s="17">
         <f t="shared" ref="L23:L24" si="29">J23</f>
         <v>8</v>
       </c>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18">
+      <c r="M23" s="17"/>
+      <c r="N23" s="17">
         <f t="shared" ref="N23" si="30">L23</f>
         <v>8</v>
       </c>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18">
+      <c r="O23" s="17"/>
+      <c r="P23" s="17">
         <f>N23</f>
         <v>8</v>
       </c>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18">
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17">
         <f t="shared" si="24"/>
         <v>8</v>
       </c>
-      <c r="S23" s="18"/>
-      <c r="T23" s="18">
+      <c r="S23" s="17"/>
+      <c r="T23" s="17">
         <f t="shared" si="25"/>
         <v>8</v>
       </c>
-      <c r="U23" s="18"/>
-      <c r="V23" s="18">
+      <c r="U23" s="17"/>
+      <c r="V23" s="17">
         <f>T23</f>
         <v>8</v>
       </c>
-      <c r="W23" s="18"/>
-      <c r="X23" s="18">
+      <c r="W23" s="17"/>
+      <c r="X23" s="17">
         <f t="shared" si="26"/>
         <v>8</v>
       </c>
-      <c r="Y23" s="18"/>
-      <c r="Z23" s="18"/>
-      <c r="AA23" s="18"/>
+      <c r="Y23" s="17"/>
+      <c r="Z23" s="17"/>
+      <c r="AA23" s="17"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="17">
         <f>B14</f>
-        <v>2000</v>
-      </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18">
+        <v>666.66666666666663</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17">
         <f>B24*I4</f>
-        <v>26000</v>
-      </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18">
+        <v>8666.6666666666661</v>
+      </c>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17">
         <f>D24</f>
-        <v>26000</v>
-      </c>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18">
+        <v>8666.6666666666661</v>
+      </c>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17">
         <f t="shared" ref="H24" si="31">F24</f>
-        <v>26000</v>
-      </c>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18">
+        <v>8666.6666666666661</v>
+      </c>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17">
         <f t="shared" si="23"/>
-        <v>26000</v>
-      </c>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18">
+        <v>8666.6666666666661</v>
+      </c>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17">
         <f t="shared" si="29"/>
-        <v>26000</v>
-      </c>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18">
+        <v>8666.6666666666661</v>
+      </c>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17">
         <f>L24</f>
-        <v>26000</v>
-      </c>
-      <c r="O24" s="18"/>
-      <c r="P24" s="18">
+        <v>8666.6666666666661</v>
+      </c>
+      <c r="O24" s="17"/>
+      <c r="P24" s="17">
         <f t="shared" ref="P24" si="32">N24</f>
-        <v>26000</v>
-      </c>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18">
+        <v>8666.6666666666661</v>
+      </c>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17">
         <f t="shared" si="24"/>
-        <v>26000</v>
-      </c>
-      <c r="S24" s="18"/>
-      <c r="T24" s="18">
+        <v>8666.6666666666661</v>
+      </c>
+      <c r="S24" s="17"/>
+      <c r="T24" s="17">
         <f t="shared" si="25"/>
-        <v>26000</v>
-      </c>
-      <c r="U24" s="18"/>
-      <c r="V24" s="18">
+        <v>8666.6666666666661</v>
+      </c>
+      <c r="U24" s="17"/>
+      <c r="V24" s="17">
         <f t="shared" ref="V24" si="33">T24</f>
-        <v>26000</v>
-      </c>
-      <c r="W24" s="18"/>
-      <c r="X24" s="18">
+        <v>8666.6666666666661</v>
+      </c>
+      <c r="W24" s="17"/>
+      <c r="X24" s="17">
         <f>V24*2</f>
-        <v>52000</v>
-      </c>
-      <c r="Y24" s="18"/>
+        <v>17333.333333333332</v>
+      </c>
+      <c r="Y24" s="17"/>
       <c r="Z24" s="5"/>
       <c r="AA24" s="5"/>
     </row>
@@ -3823,66 +3823,66 @@
       <c r="A25" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="20">
         <f>B22*B23*B24</f>
-        <v>8192000</v>
-      </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19">
+        <v>2730666.6666666665</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20">
         <f>D22*D23*D24</f>
-        <v>1277952000</v>
-      </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19">
+        <v>425984000</v>
+      </c>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20">
         <f t="shared" ref="F25" si="34">F22*F23*F24</f>
-        <v>1277952000</v>
-      </c>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19">
+        <v>425984000</v>
+      </c>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20">
         <f t="shared" ref="H25" si="35">H22*H23*H24</f>
-        <v>1277952000</v>
-      </c>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19">
+        <v>425984000</v>
+      </c>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20">
         <f t="shared" ref="J25" si="36">J22*J23*J24</f>
-        <v>1277952000</v>
-      </c>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19">
+        <v>425984000</v>
+      </c>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20">
         <f>L22*L23*L24</f>
-        <v>1277952000</v>
-      </c>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19">
+        <v>425984000</v>
+      </c>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20">
         <f t="shared" ref="N25:X25" si="37">N22*N23*N24</f>
-        <v>20447232000</v>
-      </c>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19">
+        <v>6815744000</v>
+      </c>
+      <c r="O25" s="20"/>
+      <c r="P25" s="20">
         <f t="shared" si="37"/>
-        <v>20447232000</v>
-      </c>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="19">
+        <v>6815744000</v>
+      </c>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="20">
         <f t="shared" si="37"/>
-        <v>20447232000</v>
-      </c>
-      <c r="S25" s="19"/>
-      <c r="T25" s="19">
+        <v>6815744000</v>
+      </c>
+      <c r="S25" s="20"/>
+      <c r="T25" s="20">
         <f t="shared" si="37"/>
-        <v>20447232000</v>
-      </c>
-      <c r="U25" s="19"/>
-      <c r="V25" s="19">
+        <v>6815744000</v>
+      </c>
+      <c r="U25" s="20"/>
+      <c r="V25" s="20">
         <f t="shared" si="37"/>
-        <v>20447232000</v>
-      </c>
-      <c r="W25" s="19"/>
-      <c r="X25" s="19">
+        <v>6815744000</v>
+      </c>
+      <c r="W25" s="20"/>
+      <c r="X25" s="20">
         <f t="shared" si="37"/>
-        <v>40894464000</v>
-      </c>
-      <c r="Y25" s="19"/>
+        <v>13631488000</v>
+      </c>
+      <c r="Y25" s="20"/>
       <c r="Z25" s="8"/>
       <c r="AA25" s="8"/>
     </row>
@@ -3890,410 +3890,455 @@
       <c r="A26" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" s="19">
         <f>0.191+9.964+1.804+1.666</f>
         <v>13.625000000000002</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20">
+      <c r="C26" s="19"/>
+      <c r="D26" s="19">
         <v>25.887</v>
       </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20">
+      <c r="E26" s="19"/>
+      <c r="F26" s="19">
         <v>21.568000000000001</v>
       </c>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20">
+      <c r="G26" s="19"/>
+      <c r="H26" s="19">
         <v>21.541</v>
       </c>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20">
+      <c r="I26" s="19"/>
+      <c r="J26" s="19">
         <v>9.1859999999999999</v>
       </c>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20">
+      <c r="K26" s="19"/>
+      <c r="L26" s="19">
         <v>1.1519999999999999</v>
       </c>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20">
+      <c r="M26" s="19"/>
+      <c r="N26" s="19">
         <v>14.536</v>
       </c>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20">
+      <c r="O26" s="19"/>
+      <c r="P26" s="19">
         <v>5.0839999999999996</v>
       </c>
-      <c r="Q26" s="20"/>
-      <c r="R26" s="20">
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19">
         <f>0.874+3.15</f>
         <v>4.024</v>
       </c>
-      <c r="S26" s="20"/>
-      <c r="T26" s="20">
+      <c r="S26" s="19"/>
+      <c r="T26" s="19">
         <v>5.891</v>
       </c>
-      <c r="U26" s="20"/>
-      <c r="V26" s="20">
+      <c r="U26" s="19"/>
+      <c r="V26" s="19">
         <v>11.195</v>
       </c>
-      <c r="W26" s="20"/>
-      <c r="X26" s="20">
+      <c r="W26" s="19"/>
+      <c r="X26" s="19">
         <v>7.8550000000000004</v>
       </c>
-      <c r="Y26" s="20"/>
+      <c r="Y26" s="19"/>
     </row>
     <row r="27" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="20">
+      <c r="B27" s="19">
         <f>19.37+17.15</f>
         <v>36.519999999999996</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20">
+      <c r="C27" s="19"/>
+      <c r="D27" s="19">
         <v>146.75</v>
       </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20">
+      <c r="E27" s="19"/>
+      <c r="F27" s="19">
         <v>180.85</v>
       </c>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20">
+      <c r="G27" s="19"/>
+      <c r="H27" s="19">
         <v>166.69</v>
       </c>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20">
+      <c r="I27" s="19"/>
+      <c r="J27" s="19">
         <v>128.34</v>
       </c>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20">
+      <c r="K27" s="19"/>
+      <c r="L27" s="19">
         <v>23.66</v>
       </c>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20">
+      <c r="M27" s="19"/>
+      <c r="N27" s="19">
         <v>108.08</v>
       </c>
-      <c r="O27" s="20"/>
-      <c r="P27" s="20">
+      <c r="O27" s="19"/>
+      <c r="P27" s="19">
         <v>62.75</v>
       </c>
-      <c r="Q27" s="20"/>
-      <c r="R27" s="20">
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19">
         <v>56.74</v>
       </c>
-      <c r="S27" s="20"/>
-      <c r="T27" s="20">
+      <c r="S27" s="19"/>
+      <c r="T27" s="19">
         <v>67.02</v>
       </c>
-      <c r="U27" s="20"/>
-      <c r="V27" s="20">
+      <c r="U27" s="19"/>
+      <c r="V27" s="19">
         <v>72.900000000000006</v>
       </c>
-      <c r="W27" s="20"/>
-      <c r="X27" s="20">
+      <c r="W27" s="19"/>
+      <c r="X27" s="19">
         <v>80.45</v>
       </c>
-      <c r="Y27" s="20"/>
+      <c r="Y27" s="19"/>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="17">
+      <c r="B28" s="18">
         <f>B26/512/8/2000*B$25</f>
-        <v>13.625000000000002</v>
-      </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17">
+        <v>4.541666666666667</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18">
         <f>D26/6144/8/4000*D$25</f>
-        <v>168.2655</v>
-      </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17">
+        <v>56.088499999999996</v>
+      </c>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18">
         <f t="shared" ref="F28:F29" si="38">F26/6144/8/4000*F$25</f>
-        <v>140.19200000000001</v>
-      </c>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17">
+        <v>46.730666666666671</v>
+      </c>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18">
         <f t="shared" ref="H28:H29" si="39">H26/6144/8/4000*H$25</f>
-        <v>140.01650000000001</v>
-      </c>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17">
+        <v>46.672166666666669</v>
+      </c>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18">
         <f t="shared" ref="J28:J29" si="40">J26/6144/8/4000*J$25</f>
-        <v>59.708999999999996</v>
-      </c>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17">
+        <v>19.902999999999999</v>
+      </c>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18">
         <f>L26/512/8/1600*L$25</f>
-        <v>224.64</v>
-      </c>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17">
+        <v>74.88</v>
+      </c>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18">
         <f>N26/4096/8/3200*N$25</f>
-        <v>2834.52</v>
-      </c>
-      <c r="O28" s="17"/>
-      <c r="P28" s="17">
+        <v>944.83999999999992</v>
+      </c>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18">
         <f t="shared" ref="P28:P29" si="41">P26/4096/8/3200*P$25</f>
-        <v>991.37999999999988</v>
-      </c>
-      <c r="Q28" s="17"/>
-      <c r="R28" s="17">
+        <v>330.46</v>
+      </c>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18">
         <f t="shared" ref="R28:R29" si="42">R26/4096/8/3200*R$25</f>
-        <v>784.68</v>
-      </c>
-      <c r="S28" s="17"/>
-      <c r="T28" s="17">
+        <v>261.56</v>
+      </c>
+      <c r="S28" s="18"/>
+      <c r="T28" s="18">
         <f t="shared" ref="T28:T29" si="43">T26/4096/8/3200*T$25</f>
-        <v>1148.7449999999999</v>
-      </c>
-      <c r="U28" s="17"/>
-      <c r="V28" s="17">
+        <v>382.91499999999996</v>
+      </c>
+      <c r="U28" s="18"/>
+      <c r="V28" s="18">
         <f t="shared" ref="V28:V29" si="44">V26/4096/8/3200*V$25</f>
-        <v>2183.0250000000001</v>
-      </c>
-      <c r="W28" s="17"/>
-      <c r="X28" s="17">
+        <v>727.67500000000007</v>
+      </c>
+      <c r="W28" s="18"/>
+      <c r="X28" s="18">
         <f t="shared" ref="X28:X29" si="45">X26/4096/8/3200*X$25</f>
-        <v>3063.4500000000003</v>
-      </c>
-      <c r="Y28" s="17"/>
+        <v>1021.1500000000001</v>
+      </c>
+      <c r="Y28" s="18"/>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="17">
+      <c r="B29" s="18">
         <f>B27/512/8/2000*B$25</f>
-        <v>36.519999999999996</v>
-      </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17">
+        <v>12.173333333333332</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18">
         <f>D27/6144/8/4000*D$25</f>
-        <v>953.875</v>
-      </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17">
+        <v>317.95833333333331</v>
+      </c>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18">
         <f t="shared" si="38"/>
-        <v>1175.5250000000001</v>
-      </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17">
+        <v>391.8416666666667</v>
+      </c>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18">
         <f t="shared" si="39"/>
-        <v>1083.4849999999999</v>
-      </c>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17">
+        <v>361.16166666666669</v>
+      </c>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18">
         <f t="shared" si="40"/>
-        <v>834.20999999999992</v>
-      </c>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17">
+        <v>278.07</v>
+      </c>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18">
         <f>L27/512/8/1600*L$25</f>
-        <v>4613.7</v>
-      </c>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17">
+        <v>1537.9</v>
+      </c>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18">
         <f>N27/4096/8/3200*N$25</f>
-        <v>21075.599999999999</v>
-      </c>
-      <c r="O29" s="17"/>
-      <c r="P29" s="17">
+        <v>7025.2</v>
+      </c>
+      <c r="O29" s="18"/>
+      <c r="P29" s="18">
         <f t="shared" si="41"/>
-        <v>12236.249999999998</v>
-      </c>
-      <c r="Q29" s="17"/>
-      <c r="R29" s="17">
+        <v>4078.7499999999995</v>
+      </c>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="18">
         <f t="shared" si="42"/>
-        <v>11064.300000000001</v>
-      </c>
-      <c r="S29" s="17"/>
-      <c r="T29" s="17">
+        <v>3688.1</v>
+      </c>
+      <c r="S29" s="18"/>
+      <c r="T29" s="18">
         <f t="shared" si="43"/>
-        <v>13068.899999999998</v>
-      </c>
-      <c r="U29" s="17"/>
-      <c r="V29" s="17">
+        <v>4356.2999999999993</v>
+      </c>
+      <c r="U29" s="18"/>
+      <c r="V29" s="18">
         <f t="shared" si="44"/>
-        <v>14215.500000000002</v>
-      </c>
-      <c r="W29" s="17"/>
-      <c r="X29" s="17">
+        <v>4738.5000000000009</v>
+      </c>
+      <c r="W29" s="18"/>
+      <c r="X29" s="18">
         <f t="shared" si="45"/>
-        <v>31375.5</v>
-      </c>
-      <c r="Y29" s="17"/>
+        <v>10458.5</v>
+      </c>
+      <c r="Y29" s="18"/>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="18">
+      <c r="B30" s="17">
         <v>1</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18">
+      <c r="C30" s="17"/>
+      <c r="D30" s="17">
         <v>1</v>
       </c>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18">
+      <c r="E30" s="17"/>
+      <c r="F30" s="17">
         <v>1</v>
       </c>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18">
+      <c r="G30" s="17"/>
+      <c r="H30" s="17">
         <v>1</v>
       </c>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18">
+      <c r="I30" s="17"/>
+      <c r="J30" s="17">
         <v>1</v>
       </c>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18">
+      <c r="K30" s="17"/>
+      <c r="L30" s="17">
         <v>1</v>
       </c>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18">
+      <c r="M30" s="17"/>
+      <c r="N30" s="17">
         <v>1</v>
       </c>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18">
+      <c r="O30" s="17"/>
+      <c r="P30" s="17">
         <v>1</v>
       </c>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="18">
+      <c r="Q30" s="17"/>
+      <c r="R30" s="17">
         <v>1</v>
       </c>
-      <c r="S30" s="18"/>
-      <c r="T30" s="18">
+      <c r="S30" s="17"/>
+      <c r="T30" s="17">
         <v>1</v>
       </c>
-      <c r="U30" s="18"/>
-      <c r="V30" s="18">
+      <c r="U30" s="17"/>
+      <c r="V30" s="17">
         <v>1</v>
       </c>
-      <c r="W30" s="18"/>
-      <c r="X30" s="18">
+      <c r="W30" s="17"/>
+      <c r="X30" s="17">
         <v>1</v>
       </c>
-      <c r="Y30" s="18"/>
-      <c r="Z30" s="17"/>
-      <c r="AA30" s="17"/>
+      <c r="Y30" s="17"/>
+      <c r="Z30" s="18"/>
+      <c r="AA30" s="18"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="21">
+      <c r="B31" s="16">
         <f>(B28+B29*B30)/86400</f>
-        <v>5.8038194444444435E-4</v>
-      </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21">
+        <v>1.9346064814814814E-4</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16">
         <f t="shared" ref="D31:F31" si="46">(D28+D29*D30)/86400</f>
-        <v>1.2987737268518517E-2</v>
-      </c>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21">
+        <v>4.3292457561728394E-3</v>
+      </c>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16">
         <f t="shared" si="46"/>
-        <v>1.5228206018518519E-2</v>
-      </c>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21">
+        <v>5.0760686728395068E-3</v>
+      </c>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16">
         <f t="shared" ref="H31" si="47">(H28+H29*H30)/86400</f>
-        <v>1.4160896990740739E-2</v>
-      </c>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21">
+        <v>4.7202989969135807E-3</v>
+      </c>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16">
         <f t="shared" ref="J31" si="48">(J28+J29*J30)/86400</f>
-        <v>1.034628472222222E-2</v>
-      </c>
-      <c r="K31" s="21"/>
-      <c r="L31" s="21">
+        <v>3.4487615740740741E-3</v>
+      </c>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16">
         <f t="shared" ref="L31:N31" si="49">(L28+L29*L30)/86400</f>
-        <v>5.5999305555555559E-2</v>
-      </c>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21">
+        <v>1.8666435185185189E-2</v>
+      </c>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16">
         <f t="shared" si="49"/>
-        <v>0.27673749999999997</v>
-      </c>
-      <c r="O31" s="21"/>
-      <c r="P31" s="21">
+        <v>9.2245833333333332E-2</v>
+      </c>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16">
         <f>(P28+P29*P30+R28)/86400</f>
-        <v>0.16217951388888885</v>
-      </c>
-      <c r="Q31" s="21"/>
-      <c r="R31" s="21">
+        <v>5.4059837962962959E-2</v>
+      </c>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16">
         <f>(R28+R29*R30+T28)/86400</f>
-        <v>0.15043663194444448</v>
-      </c>
-      <c r="S31" s="21"/>
-      <c r="T31" s="21">
+        <v>5.014554398148148E-2</v>
+      </c>
+      <c r="S31" s="16"/>
+      <c r="T31" s="16">
         <f t="shared" ref="T31:X31" si="50">(T28+T29*T30)/86400</f>
-        <v>0.16455607638888886</v>
-      </c>
-      <c r="U31" s="21"/>
-      <c r="V31" s="21">
+        <v>5.4852025462962951E-2</v>
+      </c>
+      <c r="U31" s="16"/>
+      <c r="V31" s="16">
         <f t="shared" si="50"/>
-        <v>0.18979774305555558</v>
-      </c>
-      <c r="W31" s="21"/>
-      <c r="X31" s="21">
+        <v>6.326591435185186E-2</v>
+      </c>
+      <c r="W31" s="16"/>
+      <c r="X31" s="16">
         <f t="shared" si="50"/>
-        <v>0.39859895833333331</v>
-      </c>
-      <c r="Y31" s="21"/>
+        <v>0.13286631944444444</v>
+      </c>
+      <c r="Y31" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="163">
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="P31:Q31"/>
-    <mergeCell ref="R31:S31"/>
-    <mergeCell ref="T31:U31"/>
-    <mergeCell ref="V31:W31"/>
-    <mergeCell ref="X31:Y31"/>
-    <mergeCell ref="V28:W28"/>
-    <mergeCell ref="X28:Y28"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="R29:S29"/>
-    <mergeCell ref="V29:W29"/>
-    <mergeCell ref="X29:Y29"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="R30:S30"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="X30:Y30"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="X25:Y25"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="R26:S26"/>
-    <mergeCell ref="V26:W26"/>
-    <mergeCell ref="X26:Y26"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="R27:S27"/>
-    <mergeCell ref="V27:W27"/>
-    <mergeCell ref="X27:Y27"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="X16:Y16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="T21:U21"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="X21:Y21"/>
+    <mergeCell ref="Z21:AA21"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="Z23:AA23"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="Z30:AA30"/>
+    <mergeCell ref="X24:Y24"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="T25:U25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="D29:E29"/>
@@ -4318,98 +4363,53 @@
     <mergeCell ref="N28:O28"/>
     <mergeCell ref="P28:Q28"/>
     <mergeCell ref="R28:S28"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="Z23:AA23"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="R24:S24"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="Z30:AA30"/>
-    <mergeCell ref="X24:Y24"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="T25:U25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="T21:U21"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="X21:Y21"/>
-    <mergeCell ref="Z21:AA21"/>
-    <mergeCell ref="X22:Y22"/>
-    <mergeCell ref="Z22:AA22"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="X16:Y16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="X25:Y25"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="R26:S26"/>
+    <mergeCell ref="V26:W26"/>
+    <mergeCell ref="X26:Y26"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="R27:S27"/>
+    <mergeCell ref="V27:W27"/>
+    <mergeCell ref="X27:Y27"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="P31:Q31"/>
+    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="T31:U31"/>
+    <mergeCell ref="V31:W31"/>
+    <mergeCell ref="X31:Y31"/>
+    <mergeCell ref="V28:W28"/>
+    <mergeCell ref="X28:Y28"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="R29:S29"/>
+    <mergeCell ref="V29:W29"/>
+    <mergeCell ref="X29:Y29"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="R30:S30"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="X30:Y30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4422,7 +4422,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update: mirror simulation results
</commit_message>
<xml_diff>
--- a/Sampling_Resolution_Calculator.xlsx
+++ b/Sampling_Resolution_Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nanw0\GoogleDrive\SLAC\SLAC-Diling\11. 21 Winter\DXS optics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFFE0E2-96BA-41EB-8274-FBC8C2E888C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA39B5B-5D9D-4A0C-9BE1-11A9A0167A5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="555" windowWidth="25335" windowHeight="20370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="285" windowWidth="29040" windowHeight="15465" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HHLM" sheetId="10" r:id="rId1"/>
@@ -482,22 +482,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -782,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9ED2467-9A32-4D0C-9EF6-BA646B0CE237}">
   <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -808,10 +808,10 @@
       <c r="A1" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="21"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -820,10 +820,10 @@
       <c r="B2">
         <v>9481</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="21"/>
+      <c r="E2" s="16"/>
       <c r="F2">
         <v>19.909876918386299</v>
       </c>
@@ -846,10 +846,10 @@
       <c r="B3">
         <v>20</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="21"/>
+      <c r="E3" s="16"/>
       <c r="F3">
         <v>17</v>
       </c>
@@ -868,10 +868,10 @@
       <c r="B4" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="21"/>
+      <c r="E4" s="16"/>
       <c r="F4">
         <f>SIN(RADIANS(F2+F3))/SIN(RADIANS(F2-F3))</f>
         <v>11.830135875287004</v>
@@ -895,10 +895,10 @@
       <c r="B5" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="21"/>
+      <c r="E5" s="16"/>
       <c r="F5">
         <f>ABS((COS(RADIANS(F2-F3))-COS(RADIANS(F2+F3)))/SIN(RADIANS(F2-F3)))</f>
         <v>3.9225661843587014</v>
@@ -924,10 +924,10 @@
         <f>B3/10</f>
         <v>2</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="21"/>
+      <c r="E8" s="16"/>
       <c r="F8" s="1">
         <v>5.9999999999999997E-7</v>
       </c>
@@ -947,10 +947,10 @@
         <f>4/B8</f>
         <v>2</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="21"/>
+      <c r="E9" s="16"/>
       <c r="F9" s="7">
         <f>SUM(28:28)/86400</f>
         <v>6.0394444444444445E-3</v>
@@ -964,20 +964,20 @@
         <f>MIN(B9/400,0.001)</f>
         <v>1E-3</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="21"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="7">
         <f>SUM(31:31)-F9</f>
         <v>4.7264062499999995E-2</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="21"/>
+      <c r="E11" s="16"/>
       <c r="F11" s="10">
         <f>SUM(31:31)</f>
         <v>5.330350694444444E-2</v>
@@ -1015,26 +1015,26 @@
       <c r="A16" t="s">
         <v>89</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21" t="s">
+      <c r="C16" s="16"/>
+      <c r="D16" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21" t="s">
+      <c r="E16" s="16"/>
+      <c r="F16" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21" t="s">
+      <c r="G16" s="16"/>
+      <c r="H16" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21" t="s">
+      <c r="I16" s="16"/>
+      <c r="J16" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="K16" s="21"/>
+      <c r="K16" s="16"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
@@ -1228,317 +1228,317 @@
       <c r="A21" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="17">
         <v>722.7</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18">
+      <c r="C21" s="17"/>
+      <c r="D21" s="17">
         <f>B21*J2</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18">
+      <c r="E21" s="17"/>
+      <c r="F21" s="17">
         <f>D21</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18">
+      <c r="G21" s="17"/>
+      <c r="H21" s="17">
         <f>F21</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18">
+      <c r="I21" s="17"/>
+      <c r="J21" s="17">
         <f>H21/J2</f>
         <v>722.7</v>
       </c>
-      <c r="K21" s="18"/>
+      <c r="K21" s="17"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="17">
+      <c r="B22" s="18">
         <f>B12</f>
         <v>512</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17">
+      <c r="C22" s="18"/>
+      <c r="D22" s="18">
         <f>B22*I2</f>
         <v>6144</v>
       </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17">
+      <c r="E22" s="18"/>
+      <c r="F22" s="18">
         <f>D22</f>
         <v>6144</v>
       </c>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17">
+      <c r="G22" s="18"/>
+      <c r="H22" s="18">
         <f>F22</f>
         <v>6144</v>
       </c>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17">
+      <c r="I22" s="18"/>
+      <c r="J22" s="18">
         <f t="shared" ref="J22:J24" si="7">H22</f>
         <v>6144</v>
       </c>
-      <c r="K22" s="17"/>
+      <c r="K22" s="18"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="18">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17">
+      <c r="C23" s="18"/>
+      <c r="D23" s="18">
         <f t="shared" ref="D23" si="8">B23</f>
         <v>8</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17">
+      <c r="E23" s="18"/>
+      <c r="F23" s="18">
         <f t="shared" ref="F23" si="9">D23</f>
         <v>8</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17">
+      <c r="G23" s="18"/>
+      <c r="H23" s="18">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17">
+      <c r="I23" s="18"/>
+      <c r="J23" s="18">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="K23" s="17"/>
+      <c r="K23" s="18"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="17">
+      <c r="B24" s="18">
         <f>B14</f>
         <v>2000</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17">
+      <c r="C24" s="18"/>
+      <c r="D24" s="18">
         <f>B24*I4</f>
         <v>26000</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17">
+      <c r="E24" s="18"/>
+      <c r="F24" s="18">
         <f>D24</f>
         <v>26000</v>
       </c>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17">
+      <c r="G24" s="18"/>
+      <c r="H24" s="18">
         <f t="shared" ref="H24" si="10">F24</f>
         <v>26000</v>
       </c>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17">
+      <c r="I24" s="18"/>
+      <c r="J24" s="18">
         <f t="shared" si="7"/>
         <v>26000</v>
       </c>
-      <c r="K24" s="17"/>
+      <c r="K24" s="18"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="20">
+      <c r="B25" s="19">
         <f>B22*B23*B24</f>
         <v>8192000</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20">
+      <c r="C25" s="19"/>
+      <c r="D25" s="19">
         <f>D22*D23*D24</f>
         <v>1277952000</v>
       </c>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20">
+      <c r="E25" s="19"/>
+      <c r="F25" s="19">
         <f t="shared" ref="F25" si="11">F22*F23*F24</f>
         <v>1277952000</v>
       </c>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20">
+      <c r="G25" s="19"/>
+      <c r="H25" s="19">
         <f t="shared" ref="H25" si="12">H22*H23*H24</f>
         <v>1277952000</v>
       </c>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20">
+      <c r="I25" s="19"/>
+      <c r="J25" s="19">
         <f t="shared" ref="J25" si="13">J22*J23*J24</f>
         <v>1277952000</v>
       </c>
-      <c r="K25" s="20"/>
+      <c r="K25" s="19"/>
     </row>
     <row r="26" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="19">
+      <c r="B26" s="20">
         <f>0.191+9.964+1.804+1.666</f>
         <v>13.625000000000002</v>
       </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19">
+      <c r="C26" s="20"/>
+      <c r="D26" s="20">
         <v>25.887</v>
       </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19">
+      <c r="E26" s="20"/>
+      <c r="F26" s="20">
         <v>21.568000000000001</v>
       </c>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19">
+      <c r="G26" s="20"/>
+      <c r="H26" s="20">
         <v>21.541</v>
       </c>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19">
+      <c r="I26" s="20"/>
+      <c r="J26" s="20">
         <v>9.1859999999999999</v>
       </c>
-      <c r="K26" s="19"/>
+      <c r="K26" s="20"/>
     </row>
     <row r="27" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="19">
+      <c r="B27" s="20">
         <f>19.37+17.15</f>
         <v>36.519999999999996</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19">
+      <c r="C27" s="20"/>
+      <c r="D27" s="20">
         <v>146.75</v>
       </c>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19">
+      <c r="E27" s="20"/>
+      <c r="F27" s="20">
         <v>180.85</v>
       </c>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19">
+      <c r="G27" s="20"/>
+      <c r="H27" s="20">
         <v>166.69</v>
       </c>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19">
+      <c r="I27" s="20"/>
+      <c r="J27" s="20">
         <v>128.34</v>
       </c>
-      <c r="K27" s="19"/>
+      <c r="K27" s="20"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="17">
         <f>B26/512/8/2000*B$25</f>
         <v>13.625000000000002</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18">
+      <c r="C28" s="17"/>
+      <c r="D28" s="17">
         <f>D26/6144/8/4000*D$25</f>
         <v>168.2655</v>
       </c>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18">
+      <c r="E28" s="17"/>
+      <c r="F28" s="17">
         <f t="shared" ref="F28" si="14">F26/6144/8/4000*F$25</f>
         <v>140.19200000000001</v>
       </c>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18">
+      <c r="G28" s="17"/>
+      <c r="H28" s="17">
         <f t="shared" ref="H28" si="15">H26/6144/8/4000*H$25</f>
         <v>140.01650000000001</v>
       </c>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18">
+      <c r="I28" s="17"/>
+      <c r="J28" s="17">
         <f t="shared" ref="J28" si="16">J26/6144/8/4000*J$25</f>
         <v>59.708999999999996</v>
       </c>
-      <c r="K28" s="18"/>
+      <c r="K28" s="17"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="18">
+      <c r="B29" s="17">
         <f>B27/512/8/2000*B$25</f>
         <v>36.519999999999996</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18">
+      <c r="C29" s="17"/>
+      <c r="D29" s="17">
         <f>D27/6144/8/4000*D$25</f>
         <v>953.875</v>
       </c>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18">
+      <c r="E29" s="17"/>
+      <c r="F29" s="17">
         <f t="shared" ref="F29" si="17">F27/6144/8/4000*F$25</f>
         <v>1175.5250000000001</v>
       </c>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18">
+      <c r="G29" s="17"/>
+      <c r="H29" s="17">
         <f t="shared" ref="H29" si="18">H27/6144/8/4000*H$25</f>
         <v>1083.4849999999999</v>
       </c>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18">
+      <c r="I29" s="17"/>
+      <c r="J29" s="17">
         <f t="shared" ref="J29" si="19">J27/6144/8/4000*J$25</f>
         <v>834.20999999999992</v>
       </c>
-      <c r="K29" s="18"/>
+      <c r="K29" s="17"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="17">
+      <c r="B30" s="18">
         <v>1</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17">
+      <c r="C30" s="18"/>
+      <c r="D30" s="18">
         <v>1</v>
       </c>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17">
+      <c r="E30" s="18"/>
+      <c r="F30" s="18">
         <v>1</v>
       </c>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17">
+      <c r="G30" s="18"/>
+      <c r="H30" s="18">
         <v>1</v>
       </c>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17">
+      <c r="I30" s="18"/>
+      <c r="J30" s="18">
         <v>1</v>
       </c>
-      <c r="K30" s="17"/>
+      <c r="K30" s="18"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="16">
+      <c r="B31" s="21">
         <f>(B28+B29*B30)/86400</f>
         <v>5.8038194444444435E-4</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16">
+      <c r="C31" s="21"/>
+      <c r="D31" s="21">
         <f t="shared" ref="D31:F31" si="20">(D28+D29*D30)/86400</f>
         <v>1.2987737268518517E-2</v>
       </c>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16">
+      <c r="E31" s="21"/>
+      <c r="F31" s="21">
         <f t="shared" si="20"/>
         <v>1.5228206018518519E-2</v>
       </c>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16">
+      <c r="G31" s="21"/>
+      <c r="H31" s="21">
         <f t="shared" ref="H31" si="21">(H28+H29*H30)/86400</f>
         <v>1.4160896990740739E-2</v>
       </c>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16">
+      <c r="I31" s="21"/>
+      <c r="J31" s="21">
         <f t="shared" ref="J31" si="22">(J28+J29*J30)/86400</f>
         <v>1.034628472222222E-2</v>
       </c>
-      <c r="K31" s="16"/>
+      <c r="K31" s="21"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="E32" s="6"/>
@@ -1550,6 +1550,66 @@
     </row>
   </sheetData>
   <mergeCells count="69">
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="F16:G16"/>
@@ -1559,66 +1619,6 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:K31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1629,8 +1629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FDDF995-0054-48A7-B092-0C0EFEBE5F19}">
   <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1658,10 +1658,10 @@
       <c r="A1" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="21"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1670,10 +1670,10 @@
       <c r="B2">
         <v>9481</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="21"/>
+      <c r="E2" s="16"/>
       <c r="F2">
         <v>42.926477759350803</v>
       </c>
@@ -1694,12 +1694,12 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="D3" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="21"/>
+      <c r="E3" s="16"/>
       <c r="F3">
         <v>-29.5</v>
       </c>
@@ -1719,10 +1719,10 @@
         <f>0.005</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="21"/>
+      <c r="E4" s="16"/>
       <c r="F4">
         <f>SIN(RADIANS(F2+F3))/SIN(RADIANS(F2-F3))</f>
         <v>0.24356450463759297</v>
@@ -1747,10 +1747,10 @@
         <f>0.005</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="21"/>
+      <c r="E5" s="16"/>
       <c r="F5">
         <f>ABS((COS(RADIANS(F2-F3))-COS(RADIANS(F2+F3)))/SIN(RADIANS(F2-F3)))</f>
         <v>0.70357494464450898</v>
@@ -1774,12 +1774,12 @@
       </c>
       <c r="B8">
         <f>B3/10</f>
-        <v>0.3</v>
-      </c>
-      <c r="D8" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="21"/>
+      <c r="E8" s="16"/>
       <c r="F8" s="1">
         <v>5.9999999999999997E-7</v>
       </c>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="I8" s="9">
         <f>22122874/1024/1024/3072/8/26000*MAX(25:25)</f>
-        <v>692.4477288661858</v>
+        <v>51.933579664963936</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
@@ -1797,15 +1797,15 @@
       </c>
       <c r="B9">
         <f>4/B8</f>
-        <v>13.333333333333334</v>
-      </c>
-      <c r="D9" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="21"/>
+      <c r="E9" s="16"/>
       <c r="F9" s="7">
         <f>SUM(28:28)/86400</f>
-        <v>0.11398688271604938</v>
+        <v>8.6631365740740748E-3</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
@@ -1816,23 +1816,23 @@
         <f>MIN(B9/800,0.001)</f>
         <v>1E-3</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="21"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="7">
         <f>SUM(31:31)-F9</f>
-        <v>1.0673630401234568</v>
+        <v>8.0615740740740738E-2</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="21"/>
+      <c r="E11" s="16"/>
       <c r="F11" s="10">
         <f>SUM(31:31)</f>
-        <v>1.1813499228395061</v>
+        <v>8.927887731481482E-2</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
@@ -1860,47 +1860,47 @@
       </c>
       <c r="B14">
         <f>B9/B10</f>
-        <v>13333.333333333334</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>88</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21" t="s">
+      <c r="C16" s="16"/>
+      <c r="D16" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21" t="s">
+      <c r="E16" s="16"/>
+      <c r="F16" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21" t="s">
+      <c r="G16" s="16"/>
+      <c r="H16" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21" t="s">
+      <c r="I16" s="16"/>
+      <c r="J16" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21" t="s">
+      <c r="K16" s="16"/>
+      <c r="L16" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21" t="s">
+      <c r="M16" s="16"/>
+      <c r="N16" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="O16" s="21"/>
-      <c r="P16" s="21" t="s">
+      <c r="O16" s="16"/>
+      <c r="P16" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="21"/>
-      <c r="S16" s="21"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
@@ -1924,7 +1924,7 @@
       </c>
       <c r="F17" s="2">
         <f>G17*F22</f>
-        <v>62492.182816763183</v>
+        <v>31246.091408381591</v>
       </c>
       <c r="G17" s="2">
         <f>E17*F4</f>
@@ -1932,7 +1932,7 @@
       </c>
       <c r="H17" s="2">
         <f>I17*H22</f>
-        <v>62492.182816763183</v>
+        <v>31246.091408381591</v>
       </c>
       <c r="I17" s="2">
         <f>G17</f>
@@ -1940,7 +1940,7 @@
       </c>
       <c r="J17" s="2">
         <f>K17*J22</f>
-        <v>4580.5778859244456</v>
+        <v>2290.2889429622228</v>
       </c>
       <c r="K17" s="2">
         <f>I17/13.64286</f>
@@ -1948,7 +1948,7 @@
       </c>
       <c r="L17" s="2">
         <f>M17*L22</f>
-        <v>62492.182816763183</v>
+        <v>31246.091408381591</v>
       </c>
       <c r="M17" s="2">
         <f>I17</f>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="N17" s="2">
         <f>O17*N22</f>
-        <v>256573.44</v>
+        <v>128286.72</v>
       </c>
       <c r="O17" s="2">
         <f>M17/F4</f>
@@ -1964,7 +1964,7 @@
       </c>
       <c r="P17" s="2">
         <f t="shared" ref="P17:P18" si="0">N17</f>
-        <v>256573.44</v>
+        <v>128286.72</v>
       </c>
       <c r="Q17" s="2">
         <f>P17/P22</f>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="C19" s="2">
         <f>B8</f>
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="D19" s="2">
         <f>E19*D24</f>
@@ -2062,7 +2062,7 @@
       </c>
       <c r="E19" s="2">
         <f>C19</f>
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="F19" s="2">
         <f>G19*F24</f>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="G19" s="2">
         <f>E19</f>
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="H19" s="2">
         <f>I19*H24</f>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="I19" s="2">
         <f>G19</f>
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="J19" s="2">
         <f>K19*J24</f>
@@ -2086,7 +2086,7 @@
       </c>
       <c r="K19" s="2">
         <f>I19</f>
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="L19" s="2">
         <f>M19*L24</f>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="M19" s="2">
         <f>K19</f>
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="N19" s="2">
         <f>O19*N24</f>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="O19" s="2">
         <f>M19</f>
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="P19" s="2">
         <f>Q19*P24</f>
@@ -2110,7 +2110,7 @@
       </c>
       <c r="Q19" s="2">
         <f>O19</f>
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
@@ -2121,7 +2121,7 @@
       </c>
       <c r="B20" s="2">
         <f>B9*1000</f>
-        <v>13333.333333333334</v>
+        <v>2000</v>
       </c>
       <c r="C20" s="2">
         <f>B10*1000</f>
@@ -2129,7 +2129,7 @@
       </c>
       <c r="D20" s="2">
         <f>$B20*$C19/E19</f>
-        <v>13333.333333333334</v>
+        <v>2000</v>
       </c>
       <c r="E20" s="2">
         <f>$B19*$C20/D19</f>
@@ -2137,7 +2137,7 @@
       </c>
       <c r="F20" s="2">
         <f>$B20*$C19/G19</f>
-        <v>13333.333333333334</v>
+        <v>2000</v>
       </c>
       <c r="G20" s="2">
         <f>$B19*$C20/F19</f>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="H20" s="2">
         <f t="shared" ref="H20" si="6">$B20*$C19/I19</f>
-        <v>13333.333333333334</v>
+        <v>2000</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" ref="I20" si="7">$B19*$C20/H19</f>
@@ -2153,7 +2153,7 @@
       </c>
       <c r="J20" s="2">
         <f t="shared" ref="J20" si="8">$B20*$C19/K19</f>
-        <v>13333.333333333334</v>
+        <v>2000</v>
       </c>
       <c r="K20" s="2">
         <f t="shared" ref="K20" si="9">$B19*$C20/J19</f>
@@ -2161,7 +2161,7 @@
       </c>
       <c r="L20" s="2">
         <f t="shared" ref="L20" si="10">$B20*$C19/M19</f>
-        <v>13333.333333333334</v>
+        <v>2000</v>
       </c>
       <c r="M20" s="2">
         <f t="shared" ref="M20" si="11">$B19*$C20/L19</f>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="N20" s="2">
         <f t="shared" ref="N20" si="12">$B20*$C19/O19</f>
-        <v>13333.333333333334</v>
+        <v>2000</v>
       </c>
       <c r="O20" s="2">
         <f t="shared" ref="O20" si="13">$B19*$C20/N19</f>
@@ -2177,7 +2177,7 @@
       </c>
       <c r="P20" s="2">
         <f t="shared" ref="P20" si="14">$B20*$C19/Q19</f>
-        <v>13333.333333333334</v>
+        <v>2000</v>
       </c>
       <c r="Q20" s="2">
         <f t="shared" ref="Q20" si="15">$B19*$C20/P19</f>
@@ -2190,38 +2190,38 @@
       <c r="A21" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="17">
         <v>726.57</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18">
+      <c r="C21" s="17"/>
+      <c r="D21" s="17">
         <v>722.86</v>
       </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18">
+      <c r="E21" s="17"/>
+      <c r="F21" s="17">
         <v>722.85</v>
       </c>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18">
+      <c r="G21" s="17"/>
+      <c r="H21" s="17">
         <v>176.54</v>
       </c>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18">
+      <c r="I21" s="17"/>
+      <c r="J21" s="17">
         <v>14.28</v>
       </c>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18">
+      <c r="K21" s="17"/>
+      <c r="L21" s="17">
         <v>175.15</v>
       </c>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18">
+      <c r="M21" s="17"/>
+      <c r="N21" s="17">
         <v>173.04</v>
       </c>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18">
+      <c r="O21" s="17"/>
+      <c r="P21" s="17">
         <v>173.07</v>
       </c>
-      <c r="Q21" s="18"/>
+      <c r="Q21" s="17"/>
       <c r="R21" s="12"/>
       <c r="S21" s="12"/>
     </row>
@@ -2229,187 +2229,187 @@
       <c r="A22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="17">
+      <c r="B22" s="18">
         <f>B12</f>
         <v>1024</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17">
+      <c r="C22" s="18"/>
+      <c r="D22" s="18">
         <f>B22</f>
         <v>1024</v>
       </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17">
-        <f>D22*I2*8</f>
-        <v>32768</v>
-      </c>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17">
+      <c r="E22" s="18"/>
+      <c r="F22" s="18">
+        <f>D22*I2*4</f>
+        <v>16384</v>
+      </c>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18">
         <f>F22</f>
-        <v>32768</v>
-      </c>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17">
+        <v>16384</v>
+      </c>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18">
         <f t="shared" ref="J22:J24" si="16">H22</f>
-        <v>32768</v>
-      </c>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17">
+        <v>16384</v>
+      </c>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18">
         <f t="shared" ref="L22:L24" si="17">J22</f>
-        <v>32768</v>
-      </c>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17">
+        <v>16384</v>
+      </c>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18">
         <f>L22</f>
-        <v>32768</v>
-      </c>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17">
+        <v>16384</v>
+      </c>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18">
         <f t="shared" ref="P22:P23" si="18">N22</f>
-        <v>32768</v>
-      </c>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="17"/>
+        <v>16384</v>
+      </c>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="18"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="18">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17">
+      <c r="C23" s="18"/>
+      <c r="D23" s="18">
         <f t="shared" ref="D23:D24" si="19">B23</f>
         <v>8</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17">
+      <c r="E23" s="18"/>
+      <c r="F23" s="18">
         <f t="shared" ref="F23" si="20">D23</f>
         <v>8</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17">
+      <c r="G23" s="18"/>
+      <c r="H23" s="18">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17">
+      <c r="I23" s="18"/>
+      <c r="J23" s="18">
         <f t="shared" si="16"/>
         <v>8</v>
       </c>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17">
+      <c r="K23" s="18"/>
+      <c r="L23" s="18">
         <f t="shared" si="17"/>
         <v>8</v>
       </c>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17">
+      <c r="M23" s="18"/>
+      <c r="N23" s="18">
         <f>L23</f>
         <v>8</v>
       </c>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17">
+      <c r="O23" s="18"/>
+      <c r="P23" s="18">
         <f t="shared" si="18"/>
         <v>8</v>
       </c>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="17"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="17">
+      <c r="B24" s="18">
         <f>B14</f>
-        <v>13333.333333333334</v>
-      </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17">
+        <v>2000</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18">
         <f t="shared" si="19"/>
-        <v>13333.333333333334</v>
-      </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17">
+        <v>2000</v>
+      </c>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18">
         <f>D24*I4</f>
-        <v>80000</v>
-      </c>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17">
+        <v>12000</v>
+      </c>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18">
         <f t="shared" ref="H24" si="21">F24</f>
-        <v>80000</v>
-      </c>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17">
+        <v>12000</v>
+      </c>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18">
         <f t="shared" si="16"/>
-        <v>80000</v>
-      </c>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17">
+        <v>12000</v>
+      </c>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18">
         <f t="shared" si="17"/>
-        <v>80000</v>
-      </c>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17">
+        <v>12000</v>
+      </c>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18">
         <f t="shared" ref="N24" si="22">L24</f>
-        <v>80000</v>
-      </c>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17">
+        <v>12000</v>
+      </c>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18">
         <f>N24</f>
-        <v>80000</v>
-      </c>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="17"/>
-      <c r="S24" s="17"/>
+        <v>12000</v>
+      </c>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="20">
+      <c r="B25" s="19">
         <f>B22*B23*B24</f>
-        <v>109226666.66666667</v>
-      </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20">
+        <v>16384000</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19">
         <f>D22*D23*D24</f>
-        <v>109226666.66666667</v>
-      </c>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20">
+        <v>16384000</v>
+      </c>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19">
         <f t="shared" ref="F25" si="23">F22*F23*F24</f>
-        <v>20971520000</v>
-      </c>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20">
+        <v>1572864000</v>
+      </c>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19">
         <f t="shared" ref="H25" si="24">H22*H23*H24</f>
-        <v>20971520000</v>
-      </c>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20">
+        <v>1572864000</v>
+      </c>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19">
         <f t="shared" ref="J25" si="25">J22*J23*J24</f>
-        <v>20971520000</v>
-      </c>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20">
+        <v>1572864000</v>
+      </c>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19">
         <f t="shared" ref="L25" si="26">L22*L23*L24</f>
-        <v>20971520000</v>
-      </c>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20">
+        <v>1572864000</v>
+      </c>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19">
         <f t="shared" ref="N25" si="27">N22*N23*N24</f>
-        <v>20971520000</v>
-      </c>
-      <c r="O25" s="20"/>
-      <c r="P25" s="20">
+        <v>1572864000</v>
+      </c>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19">
         <f t="shared" ref="P25" si="28">P22*P23*P24</f>
-        <v>20971520000</v>
-      </c>
-      <c r="Q25" s="20"/>
+        <v>1572864000</v>
+      </c>
+      <c r="Q25" s="19"/>
       <c r="R25" s="13"/>
       <c r="S25" s="13"/>
     </row>
@@ -2417,40 +2417,40 @@
       <c r="A26" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="19">
+      <c r="B26" s="20">
         <f>0.154+3.252+1.863+1.467</f>
         <v>6.7360000000000007</v>
       </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19">
+      <c r="C26" s="20"/>
+      <c r="D26" s="20">
         <v>1.1519999999999999</v>
       </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19">
+      <c r="E26" s="20"/>
+      <c r="F26" s="20">
         <v>14.536</v>
       </c>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19">
+      <c r="G26" s="20"/>
+      <c r="H26" s="20">
         <v>5.0839999999999996</v>
       </c>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19">
+      <c r="I26" s="20"/>
+      <c r="J26" s="20">
         <f>0.874+3.15</f>
         <v>4.024</v>
       </c>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19">
+      <c r="K26" s="20"/>
+      <c r="L26" s="20">
         <v>5.891</v>
       </c>
-      <c r="M26" s="19"/>
-      <c r="N26" s="19">
+      <c r="M26" s="20"/>
+      <c r="N26" s="20">
         <v>11.195</v>
       </c>
-      <c r="O26" s="19"/>
-      <c r="P26" s="19">
+      <c r="O26" s="20"/>
+      <c r="P26" s="20">
         <v>7.8550000000000004</v>
       </c>
-      <c r="Q26" s="19"/>
+      <c r="Q26" s="20"/>
       <c r="R26" s="14"/>
       <c r="S26" s="14"/>
     </row>
@@ -2458,261 +2458,263 @@
       <c r="A27" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="19">
+      <c r="B27" s="20">
         <f>6.36+8.93</f>
         <v>15.29</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19">
+      <c r="C27" s="20"/>
+      <c r="D27" s="20">
         <v>23.66</v>
       </c>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19">
+      <c r="E27" s="20"/>
+      <c r="F27" s="20">
         <v>108.08</v>
       </c>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19">
+      <c r="G27" s="20"/>
+      <c r="H27" s="20">
         <v>62.75</v>
       </c>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19">
+      <c r="I27" s="20"/>
+      <c r="J27" s="20">
         <v>56.74</v>
       </c>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19">
+      <c r="K27" s="20"/>
+      <c r="L27" s="20">
         <v>67.02</v>
       </c>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19">
+      <c r="M27" s="20"/>
+      <c r="N27" s="20">
         <v>72.900000000000006</v>
       </c>
-      <c r="O27" s="19"/>
-      <c r="P27" s="19">
+      <c r="O27" s="20"/>
+      <c r="P27" s="20">
         <v>80.45</v>
       </c>
-      <c r="Q27" s="19"/>
+      <c r="Q27" s="20"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="17">
         <f>B26/512/8/1600*B$25</f>
-        <v>112.26666666666668</v>
-      </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18">
+        <v>16.84</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17">
         <f>D26/512/8/1600*D$25</f>
-        <v>19.2</v>
-      </c>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18">
+        <v>2.88</v>
+      </c>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17">
         <f>F26/4096/8/3200*F$25</f>
-        <v>2907.2</v>
-      </c>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18">
+        <v>218.04</v>
+      </c>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17">
         <f t="shared" ref="H28" si="29">H26/4096/8/3200*H$25</f>
-        <v>1016.8</v>
-      </c>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18">
+        <v>76.259999999999991</v>
+      </c>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17">
         <f t="shared" ref="J28" si="30">J26/4096/8/3200*J$25</f>
-        <v>804.8</v>
-      </c>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18">
+        <v>60.36</v>
+      </c>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17">
         <f t="shared" ref="L28" si="31">L26/4096/8/3200*L$25</f>
-        <v>1178.2</v>
-      </c>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18">
+        <v>88.364999999999995</v>
+      </c>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17">
         <f t="shared" ref="N28" si="32">N26/4096/8/3200*N$25</f>
-        <v>2239</v>
-      </c>
-      <c r="O28" s="18"/>
-      <c r="P28" s="18">
+        <v>167.92500000000001</v>
+      </c>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17">
         <f t="shared" ref="P28" si="33">P26/4096/8/3200*P$25</f>
-        <v>1571.0000000000002</v>
-      </c>
-      <c r="Q28" s="18"/>
+        <v>117.82500000000002</v>
+      </c>
+      <c r="Q28" s="17"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="18">
+      <c r="B29" s="17">
         <f>B27/512/8/1600*B$25</f>
-        <v>254.83333333333331</v>
-      </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18">
+        <v>38.224999999999994</v>
+      </c>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17">
         <f>D27/512/8/1600*D$25</f>
-        <v>394.33333333333337</v>
-      </c>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18">
+        <v>59.15</v>
+      </c>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17">
         <f>F27/4096/8/3200*F$25</f>
-        <v>21616</v>
-      </c>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18">
+        <v>1621.2</v>
+      </c>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17">
         <f t="shared" ref="H29" si="34">H27/4096/8/3200*H$25</f>
-        <v>12549.999999999998</v>
-      </c>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18">
+        <v>941.24999999999989</v>
+      </c>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17">
         <f t="shared" ref="J29" si="35">J27/4096/8/3200*J$25</f>
-        <v>11348</v>
-      </c>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18">
+        <v>851.1</v>
+      </c>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17">
         <f t="shared" ref="L29" si="36">L27/4096/8/3200*L$25</f>
-        <v>13403.999999999998</v>
-      </c>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18">
+        <v>1005.2999999999998</v>
+      </c>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17">
         <f t="shared" ref="N29" si="37">N27/4096/8/3200*N$25</f>
-        <v>14580.000000000002</v>
-      </c>
-      <c r="O29" s="18"/>
-      <c r="P29" s="18">
+        <v>1093.5000000000002</v>
+      </c>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17">
         <f t="shared" ref="P29" si="38">P27/4096/8/3200*P$25</f>
-        <v>16090</v>
-      </c>
-      <c r="Q29" s="18"/>
+        <v>1206.75</v>
+      </c>
+      <c r="Q29" s="17"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="17">
+      <c r="B30" s="18">
         <v>1</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17">
+      <c r="C30" s="18"/>
+      <c r="D30" s="18">
         <v>1</v>
       </c>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17">
+      <c r="E30" s="18"/>
+      <c r="F30" s="18">
         <v>1</v>
       </c>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17">
+      <c r="G30" s="18"/>
+      <c r="H30" s="18">
         <v>1</v>
       </c>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17">
+      <c r="I30" s="18"/>
+      <c r="J30" s="18">
         <v>1</v>
       </c>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17">
+      <c r="K30" s="18"/>
+      <c r="L30" s="18">
         <v>1</v>
       </c>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17">
+      <c r="M30" s="18"/>
+      <c r="N30" s="18">
         <v>1</v>
       </c>
-      <c r="O30" s="17"/>
-      <c r="P30" s="17">
+      <c r="O30" s="18"/>
+      <c r="P30" s="18">
         <v>1</v>
       </c>
-      <c r="Q30" s="17"/>
+      <c r="Q30" s="18"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="16">
+      <c r="B31" s="21">
         <f>(B28+B29*B30)/86400</f>
-        <v>4.2488425925925931E-3</v>
-      </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16">
+        <v>6.3732638888888888E-4</v>
+      </c>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21">
         <f t="shared" ref="D31:F31" si="39">(D28+D29*D30)/86400</f>
-        <v>4.7862654320987661E-3</v>
-      </c>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16">
+        <v>7.1793981481481481E-4</v>
+      </c>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21">
         <f t="shared" si="39"/>
-        <v>0.28383333333333333</v>
-      </c>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16">
+        <v>2.1287500000000001E-2</v>
+      </c>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21">
         <f>(H28+H29*H30+J28)/86400</f>
-        <v>0.16633796296296294</v>
-      </c>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16">
+        <v>1.2475347222222221E-2</v>
+      </c>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21">
         <f>(J28+J29*J30+L28)/86400</f>
-        <v>0.15429398148148149</v>
-      </c>
-      <c r="K31" s="16"/>
-      <c r="L31" s="16">
+        <v>1.1572048611111111E-2</v>
+      </c>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21">
         <f t="shared" ref="L31:P31" si="40">(L28+L29*L30)/86400</f>
-        <v>0.16877546296296295</v>
-      </c>
-      <c r="M31" s="16"/>
-      <c r="N31" s="16">
+        <v>1.265815972222222E-2</v>
+      </c>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21">
         <f t="shared" si="40"/>
-        <v>0.19466435185185185</v>
-      </c>
-      <c r="O31" s="16"/>
-      <c r="P31" s="16">
+        <v>1.4599826388888891E-2</v>
+      </c>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21">
         <f t="shared" si="40"/>
-        <v>0.20440972222222223</v>
-      </c>
-      <c r="Q31" s="16"/>
-      <c r="R31" s="18"/>
-      <c r="S31" s="18"/>
+        <v>1.5330729166666668E-2</v>
+      </c>
+      <c r="Q31" s="21"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="17"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="E32" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="110">
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="R24:S24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="P31:Q31"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="F26:G26"/>
@@ -2737,50 +2739,48 @@
     <mergeCell ref="F25:G25"/>
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="J25:K25"/>
-    <mergeCell ref="R31:S31"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="P31:Q31"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2793,7 +2793,8 @@
   <dimension ref="A1:AA31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N22" sqref="N22:O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2829,14 +2830,14 @@
       <c r="A1" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="L1" s="21" t="s">
+      <c r="E1" s="16"/>
+      <c r="L1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="21"/>
+      <c r="M1" s="16"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2845,10 +2846,10 @@
       <c r="B2">
         <v>9481</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="21"/>
+      <c r="E2" s="16"/>
       <c r="F2">
         <v>19.909876918386299</v>
       </c>
@@ -2863,10 +2864,10 @@
         <f>MAX(F4,1/F4)</f>
         <v>11.830135875287004</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="21"/>
+      <c r="M2" s="16"/>
       <c r="N2">
         <v>42.926477759350803</v>
       </c>
@@ -2887,12 +2888,12 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>60</v>
-      </c>
-      <c r="D3" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="21"/>
+      <c r="E3" s="16"/>
       <c r="F3">
         <v>17</v>
       </c>
@@ -2903,10 +2904,10 @@
         <f>$B4*F5/300000000*1000000000000000</f>
         <v>52300.882458116022</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="21"/>
+      <c r="M3" s="16"/>
       <c r="N3">
         <v>-29.5</v>
       </c>
@@ -2925,10 +2926,10 @@
       <c r="B4" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="21"/>
+      <c r="E4" s="16"/>
       <c r="F4">
         <f>SIN(RADIANS(F2+F3))/SIN(RADIANS(F2-F3))</f>
         <v>11.830135875287004</v>
@@ -2944,10 +2945,10 @@
         <f>I3/$B7</f>
         <v>13.075220614529005</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="21"/>
+      <c r="M4" s="16"/>
       <c r="N4">
         <f>SIN(RADIANS(N2+N3))/SIN(RADIANS(N2-N3))</f>
         <v>0.24356450463759297</v>
@@ -2971,18 +2972,18 @@
       <c r="B5" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="21"/>
+      <c r="E5" s="16"/>
       <c r="F5">
         <f>ABS((COS(RADIANS(F2-F3))-COS(RADIANS(F2+F3)))/SIN(RADIANS(F2-F3)))</f>
         <v>3.9225661843587014</v>
       </c>
-      <c r="L5" s="21" t="s">
+      <c r="L5" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="21"/>
+      <c r="M5" s="16"/>
       <c r="N5">
         <f>ABS((COS(RADIANS(N2-N3))-COS(RADIANS(N2+N3)))/SIN(RADIANS(N2-N3)))</f>
         <v>0.70357494464450898</v>
@@ -3006,12 +3007,12 @@
       </c>
       <c r="B8">
         <f>B3/10</f>
-        <v>6</v>
-      </c>
-      <c r="D8" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="21"/>
+      <c r="E8" s="16"/>
       <c r="F8" s="1">
         <v>5.9999999999999997E-7</v>
       </c>
@@ -3020,7 +3021,7 @@
       </c>
       <c r="I8" s="9">
         <f>22122874/1024/1024/3072/8/26000*MAX(25:25)</f>
-        <v>450.09102376302076</v>
+        <v>270.05461425781249</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
@@ -3029,15 +3030,15 @@
       </c>
       <c r="B9">
         <f>4/B8</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="D9" s="21" t="s">
+        <v>0.4</v>
+      </c>
+      <c r="D9" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="21"/>
+      <c r="E9" s="16"/>
       <c r="F9" s="7">
         <f>SUM(28:28)/86400</f>
-        <v>4.5340462962962964E-2</v>
+        <v>2.7204277777777775E-2</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
@@ -3048,23 +3049,23 @@
         <f>MIN(B9/400,0.001)</f>
         <v>1E-3</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="21"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="7">
         <f>SUM(31:31)-F9</f>
-        <v>0.43852928240740741</v>
+        <v>0.26311756944444442</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="21"/>
+      <c r="E11" s="16"/>
       <c r="F11" s="10">
         <f>SUM(31:31)</f>
-        <v>0.48386974537037036</v>
+        <v>0.29032184722222221</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
@@ -3092,60 +3093,60 @@
       </c>
       <c r="B14">
         <f>B9/B10</f>
-        <v>666.66666666666663</v>
+        <v>400</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21" t="s">
+      <c r="C16" s="16"/>
+      <c r="D16" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21" t="s">
+      <c r="E16" s="16"/>
+      <c r="F16" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21" t="s">
+      <c r="G16" s="16"/>
+      <c r="H16" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21" t="s">
+      <c r="I16" s="16"/>
+      <c r="J16" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21" t="s">
+      <c r="K16" s="16"/>
+      <c r="L16" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21" t="s">
+      <c r="M16" s="16"/>
+      <c r="N16" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="O16" s="21"/>
-      <c r="P16" s="21" t="s">
+      <c r="O16" s="16"/>
+      <c r="P16" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="21" t="s">
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="S16" s="21"/>
-      <c r="T16" s="21" t="s">
+      <c r="S16" s="16"/>
+      <c r="T16" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="U16" s="21"/>
-      <c r="V16" s="21" t="s">
+      <c r="U16" s="16"/>
+      <c r="V16" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="W16" s="21"/>
-      <c r="X16" s="21" t="s">
+      <c r="W16" s="16"/>
+      <c r="X16" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="Y16" s="21"/>
-      <c r="Z16" s="21"/>
-      <c r="AA16" s="21"/>
+      <c r="Y16" s="16"/>
+      <c r="Z16" s="16"/>
+      <c r="AA16" s="16"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
@@ -3363,7 +3364,7 @@
       </c>
       <c r="C19" s="2">
         <f>B8</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D19" s="2">
         <f>E19*D24</f>
@@ -3371,7 +3372,7 @@
       </c>
       <c r="E19" s="2">
         <f>C19</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F19" s="2">
         <f>G19*F24</f>
@@ -3379,7 +3380,7 @@
       </c>
       <c r="G19" s="2">
         <f>E19</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H19" s="2">
         <f>I19*H24</f>
@@ -3387,7 +3388,7 @@
       </c>
       <c r="I19" s="2">
         <f>G19</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J19" s="2">
         <f>K19*J24</f>
@@ -3395,7 +3396,7 @@
       </c>
       <c r="K19" s="2">
         <f>I19</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="L19" s="2">
         <f>M19*L24</f>
@@ -3403,7 +3404,7 @@
       </c>
       <c r="M19" s="2">
         <f>K19</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="N19" s="2">
         <f>O19*N24</f>
@@ -3411,7 +3412,7 @@
       </c>
       <c r="O19" s="2">
         <f>M19</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="P19" s="2">
         <f>Q19*P24</f>
@@ -3419,7 +3420,7 @@
       </c>
       <c r="Q19" s="2">
         <f>O19</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="R19" s="2">
         <f>S19*R24</f>
@@ -3427,7 +3428,7 @@
       </c>
       <c r="S19" s="2">
         <f>Q19</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="T19" s="2">
         <f>U19*T24</f>
@@ -3435,7 +3436,7 @@
       </c>
       <c r="U19" s="2">
         <f>S19</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="V19" s="2">
         <f>W19*V24</f>
@@ -3443,7 +3444,7 @@
       </c>
       <c r="W19" s="2">
         <f>U19</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="X19" s="2">
         <f>Y19*X24</f>
@@ -3451,7 +3452,7 @@
       </c>
       <c r="Y19" s="2">
         <f>W19</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
@@ -3462,7 +3463,7 @@
       </c>
       <c r="B20" s="2">
         <f>B9*1000</f>
-        <v>666.66666666666663</v>
+        <v>400</v>
       </c>
       <c r="C20" s="2">
         <f>B10*1000</f>
@@ -3470,7 +3471,7 @@
       </c>
       <c r="D20" s="2">
         <f>$B20*$C19/E19</f>
-        <v>666.66666666666663</v>
+        <v>400</v>
       </c>
       <c r="E20" s="2">
         <f>$B19*$C20/D19</f>
@@ -3478,7 +3479,7 @@
       </c>
       <c r="F20" s="2">
         <f>$B20*$C19/G19</f>
-        <v>666.66666666666663</v>
+        <v>400</v>
       </c>
       <c r="G20" s="2">
         <f>$B19*$C20/F19</f>
@@ -3486,7 +3487,7 @@
       </c>
       <c r="H20" s="2">
         <f t="shared" ref="H20" si="9">$B20*$C19/I19</f>
-        <v>666.66666666666663</v>
+        <v>400</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" ref="I20" si="10">$B19*$C20/H19</f>
@@ -3494,7 +3495,7 @@
       </c>
       <c r="J20" s="2">
         <f t="shared" ref="J20" si="11">$B20*$C19/K19</f>
-        <v>666.66666666666663</v>
+        <v>400</v>
       </c>
       <c r="K20" s="2">
         <f t="shared" ref="K20" si="12">$B19*$C20/J19</f>
@@ -3502,7 +3503,7 @@
       </c>
       <c r="L20" s="2">
         <f>$B20*$C19/M19</f>
-        <v>666.66666666666663</v>
+        <v>400</v>
       </c>
       <c r="M20" s="2">
         <f>$B19*$C20/L19</f>
@@ -3510,7 +3511,7 @@
       </c>
       <c r="N20" s="2">
         <f>$B20*$C19/O19</f>
-        <v>666.66666666666663</v>
+        <v>400</v>
       </c>
       <c r="O20" s="2">
         <f>$B19*$C20/N19</f>
@@ -3518,7 +3519,7 @@
       </c>
       <c r="P20" s="2">
         <f t="shared" ref="P20" si="13">$B20*$C19/Q19</f>
-        <v>666.66666666666663</v>
+        <v>400</v>
       </c>
       <c r="Q20" s="2">
         <f t="shared" ref="Q20" si="14">$B19*$C20/P19</f>
@@ -3526,7 +3527,7 @@
       </c>
       <c r="R20" s="2">
         <f t="shared" ref="R20" si="15">$B20*$C19/S19</f>
-        <v>666.66666666666663</v>
+        <v>400</v>
       </c>
       <c r="S20" s="2">
         <f t="shared" ref="S20" si="16">$B19*$C20/R19</f>
@@ -3534,7 +3535,7 @@
       </c>
       <c r="T20" s="2">
         <f t="shared" ref="T20" si="17">$B20*$C19/U19</f>
-        <v>666.66666666666663</v>
+        <v>400</v>
       </c>
       <c r="U20" s="2">
         <f t="shared" ref="U20" si="18">$B19*$C20/T19</f>
@@ -3542,7 +3543,7 @@
       </c>
       <c r="V20" s="2">
         <f t="shared" ref="V20" si="19">$B20*$C19/W19</f>
-        <v>666.66666666666663</v>
+        <v>400</v>
       </c>
       <c r="W20" s="2">
         <f t="shared" ref="W20" si="20">$B19*$C20/V19</f>
@@ -3550,7 +3551,7 @@
       </c>
       <c r="X20" s="2">
         <f t="shared" ref="X20" si="21">$B20*$C19/Y19</f>
-        <v>666.66666666666663</v>
+        <v>400</v>
       </c>
       <c r="Y20" s="2">
         <f t="shared" ref="Y20" si="22">$B19*$C20/X19</f>
@@ -3563,259 +3564,259 @@
       <c r="A21" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="17">
         <v>722.7</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18">
+      <c r="C21" s="17"/>
+      <c r="D21" s="17">
         <f>B21*J2</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18">
+      <c r="E21" s="17"/>
+      <c r="F21" s="17">
         <f>D21</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18">
+      <c r="G21" s="17"/>
+      <c r="H21" s="17">
         <f>F21</f>
         <v>8549.6391970699187</v>
       </c>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18">
+      <c r="I21" s="17"/>
+      <c r="J21" s="17">
         <f>H21/J2</f>
         <v>722.7</v>
       </c>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18">
+      <c r="K21" s="17"/>
+      <c r="L21" s="17">
         <v>722.86</v>
       </c>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18">
+      <c r="M21" s="17"/>
+      <c r="N21" s="17">
         <v>722.85</v>
       </c>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18">
+      <c r="O21" s="17"/>
+      <c r="P21" s="17">
         <v>176.54</v>
       </c>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18">
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17">
         <v>14.28</v>
       </c>
-      <c r="S21" s="18"/>
-      <c r="T21" s="18">
+      <c r="S21" s="17"/>
+      <c r="T21" s="17">
         <v>175.15</v>
       </c>
-      <c r="U21" s="18"/>
-      <c r="V21" s="18">
+      <c r="U21" s="17"/>
+      <c r="V21" s="17">
         <v>173.04</v>
       </c>
-      <c r="W21" s="18"/>
-      <c r="X21" s="18">
+      <c r="W21" s="17"/>
+      <c r="X21" s="17">
         <v>173.07</v>
       </c>
-      <c r="Y21" s="18"/>
-      <c r="Z21" s="17"/>
-      <c r="AA21" s="17"/>
+      <c r="Y21" s="17"/>
+      <c r="Z21" s="18"/>
+      <c r="AA21" s="18"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="17">
+      <c r="B22" s="18">
         <f>B12</f>
         <v>512</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17">
+      <c r="C22" s="18"/>
+      <c r="D22" s="18">
         <f>B22*I2</f>
         <v>6144</v>
       </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17">
+      <c r="E22" s="18"/>
+      <c r="F22" s="18">
         <f>D22</f>
         <v>6144</v>
       </c>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17">
+      <c r="G22" s="18"/>
+      <c r="H22" s="18">
         <f>F22</f>
         <v>6144</v>
       </c>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17">
+      <c r="I22" s="18"/>
+      <c r="J22" s="18">
         <f t="shared" ref="J22:J24" si="23">H22</f>
         <v>6144</v>
       </c>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17">
+      <c r="K22" s="18"/>
+      <c r="L22" s="18">
         <f>J22</f>
         <v>6144</v>
       </c>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17">
+      <c r="M22" s="18"/>
+      <c r="N22" s="18">
         <f>L22*Q2*4</f>
         <v>98304</v>
       </c>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17">
+      <c r="O22" s="18"/>
+      <c r="P22" s="18">
         <f>N22</f>
         <v>98304</v>
       </c>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="17">
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18">
         <f t="shared" ref="R22:R24" si="24">P22</f>
         <v>98304</v>
       </c>
-      <c r="S22" s="17"/>
-      <c r="T22" s="17">
+      <c r="S22" s="18"/>
+      <c r="T22" s="18">
         <f t="shared" ref="T22:T24" si="25">R22</f>
         <v>98304</v>
       </c>
-      <c r="U22" s="17"/>
-      <c r="V22" s="17">
+      <c r="U22" s="18"/>
+      <c r="V22" s="18">
         <f>T22</f>
         <v>98304</v>
       </c>
-      <c r="W22" s="17"/>
-      <c r="X22" s="17">
+      <c r="W22" s="18"/>
+      <c r="X22" s="18">
         <f t="shared" ref="X22:X23" si="26">V22</f>
         <v>98304</v>
       </c>
-      <c r="Y22" s="17"/>
-      <c r="Z22" s="17"/>
-      <c r="AA22" s="17"/>
+      <c r="Y22" s="18"/>
+      <c r="Z22" s="18"/>
+      <c r="AA22" s="18"/>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="18">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17">
+      <c r="C23" s="18"/>
+      <c r="D23" s="18">
         <f t="shared" ref="D23" si="27">B23</f>
         <v>8</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17">
+      <c r="E23" s="18"/>
+      <c r="F23" s="18">
         <f t="shared" ref="F23" si="28">D23</f>
         <v>8</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17">
+      <c r="G23" s="18"/>
+      <c r="H23" s="18">
         <f>B13</f>
         <v>8</v>
       </c>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17">
+      <c r="I23" s="18"/>
+      <c r="J23" s="18">
         <f t="shared" si="23"/>
         <v>8</v>
       </c>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17">
+      <c r="K23" s="18"/>
+      <c r="L23" s="18">
         <f t="shared" ref="L23:L24" si="29">J23</f>
         <v>8</v>
       </c>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17">
+      <c r="M23" s="18"/>
+      <c r="N23" s="18">
         <f t="shared" ref="N23" si="30">L23</f>
         <v>8</v>
       </c>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17">
+      <c r="O23" s="18"/>
+      <c r="P23" s="18">
         <f>N23</f>
         <v>8</v>
       </c>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17">
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18">
         <f t="shared" si="24"/>
         <v>8</v>
       </c>
-      <c r="S23" s="17"/>
-      <c r="T23" s="17">
+      <c r="S23" s="18"/>
+      <c r="T23" s="18">
         <f t="shared" si="25"/>
         <v>8</v>
       </c>
-      <c r="U23" s="17"/>
-      <c r="V23" s="17">
+      <c r="U23" s="18"/>
+      <c r="V23" s="18">
         <f>T23</f>
         <v>8</v>
       </c>
-      <c r="W23" s="17"/>
-      <c r="X23" s="17">
+      <c r="W23" s="18"/>
+      <c r="X23" s="18">
         <f t="shared" si="26"/>
         <v>8</v>
       </c>
-      <c r="Y23" s="17"/>
-      <c r="Z23" s="17"/>
-      <c r="AA23" s="17"/>
+      <c r="Y23" s="18"/>
+      <c r="Z23" s="18"/>
+      <c r="AA23" s="18"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="17">
+      <c r="B24" s="18">
         <f>B14</f>
-        <v>666.66666666666663</v>
-      </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17">
+        <v>400</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18">
         <f>B24*I4</f>
-        <v>8666.6666666666661</v>
-      </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17">
+        <v>5200</v>
+      </c>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18">
         <f>D24</f>
-        <v>8666.6666666666661</v>
-      </c>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17">
+        <v>5200</v>
+      </c>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18">
         <f t="shared" ref="H24" si="31">F24</f>
-        <v>8666.6666666666661</v>
-      </c>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17">
+        <v>5200</v>
+      </c>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18">
         <f t="shared" si="23"/>
-        <v>8666.6666666666661</v>
-      </c>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17">
+        <v>5200</v>
+      </c>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18">
         <f t="shared" si="29"/>
-        <v>8666.6666666666661</v>
-      </c>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17">
+        <v>5200</v>
+      </c>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18">
         <f>L24</f>
-        <v>8666.6666666666661</v>
-      </c>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17">
+        <v>5200</v>
+      </c>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18">
         <f t="shared" ref="P24" si="32">N24</f>
-        <v>8666.6666666666661</v>
-      </c>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="17">
+        <v>5200</v>
+      </c>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18">
         <f t="shared" si="24"/>
-        <v>8666.6666666666661</v>
-      </c>
-      <c r="S24" s="17"/>
-      <c r="T24" s="17">
+        <v>5200</v>
+      </c>
+      <c r="S24" s="18"/>
+      <c r="T24" s="18">
         <f t="shared" si="25"/>
-        <v>8666.6666666666661</v>
-      </c>
-      <c r="U24" s="17"/>
-      <c r="V24" s="17">
+        <v>5200</v>
+      </c>
+      <c r="U24" s="18"/>
+      <c r="V24" s="18">
         <f t="shared" ref="V24" si="33">T24</f>
-        <v>8666.6666666666661</v>
-      </c>
-      <c r="W24" s="17"/>
-      <c r="X24" s="17">
+        <v>5200</v>
+      </c>
+      <c r="W24" s="18"/>
+      <c r="X24" s="18">
         <f>V24*2</f>
-        <v>17333.333333333332</v>
-      </c>
-      <c r="Y24" s="17"/>
+        <v>10400</v>
+      </c>
+      <c r="Y24" s="18"/>
       <c r="Z24" s="5"/>
       <c r="AA24" s="5"/>
     </row>
@@ -3823,66 +3824,66 @@
       <c r="A25" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="20">
+      <c r="B25" s="19">
         <f>B22*B23*B24</f>
-        <v>2730666.6666666665</v>
-      </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20">
+        <v>1638400</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19">
         <f>D22*D23*D24</f>
-        <v>425984000</v>
-      </c>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20">
+        <v>255590400</v>
+      </c>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19">
         <f t="shared" ref="F25" si="34">F22*F23*F24</f>
-        <v>425984000</v>
-      </c>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20">
+        <v>255590400</v>
+      </c>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19">
         <f t="shared" ref="H25" si="35">H22*H23*H24</f>
-        <v>425984000</v>
-      </c>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20">
+        <v>255590400</v>
+      </c>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19">
         <f t="shared" ref="J25" si="36">J22*J23*J24</f>
-        <v>425984000</v>
-      </c>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20">
+        <v>255590400</v>
+      </c>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19">
         <f>L22*L23*L24</f>
-        <v>425984000</v>
-      </c>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20">
+        <v>255590400</v>
+      </c>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19">
         <f t="shared" ref="N25:X25" si="37">N22*N23*N24</f>
-        <v>6815744000</v>
-      </c>
-      <c r="O25" s="20"/>
-      <c r="P25" s="20">
+        <v>4089446400</v>
+      </c>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19">
         <f t="shared" si="37"/>
-        <v>6815744000</v>
-      </c>
-      <c r="Q25" s="20"/>
-      <c r="R25" s="20">
+        <v>4089446400</v>
+      </c>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19">
         <f t="shared" si="37"/>
-        <v>6815744000</v>
-      </c>
-      <c r="S25" s="20"/>
-      <c r="T25" s="20">
+        <v>4089446400</v>
+      </c>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19">
         <f t="shared" si="37"/>
-        <v>6815744000</v>
-      </c>
-      <c r="U25" s="20"/>
-      <c r="V25" s="20">
+        <v>4089446400</v>
+      </c>
+      <c r="U25" s="19"/>
+      <c r="V25" s="19">
         <f t="shared" si="37"/>
-        <v>6815744000</v>
-      </c>
-      <c r="W25" s="20"/>
-      <c r="X25" s="20">
+        <v>4089446400</v>
+      </c>
+      <c r="W25" s="19"/>
+      <c r="X25" s="19">
         <f t="shared" si="37"/>
-        <v>13631488000</v>
-      </c>
-      <c r="Y25" s="20"/>
+        <v>8178892800</v>
+      </c>
+      <c r="Y25" s="19"/>
       <c r="Z25" s="8"/>
       <c r="AA25" s="8"/>
     </row>
@@ -3890,431 +3891,434 @@
       <c r="A26" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="19">
+      <c r="B26" s="20">
         <f>0.191+9.964+1.804+1.666</f>
         <v>13.625000000000002</v>
       </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19">
+      <c r="C26" s="20"/>
+      <c r="D26" s="20">
         <v>25.887</v>
       </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19">
+      <c r="E26" s="20"/>
+      <c r="F26" s="20">
         <v>21.568000000000001</v>
       </c>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19">
+      <c r="G26" s="20"/>
+      <c r="H26" s="20">
         <v>21.541</v>
       </c>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19">
+      <c r="I26" s="20"/>
+      <c r="J26" s="20">
         <v>9.1859999999999999</v>
       </c>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19">
+      <c r="K26" s="20"/>
+      <c r="L26" s="20">
         <v>1.1519999999999999</v>
       </c>
-      <c r="M26" s="19"/>
-      <c r="N26" s="19">
+      <c r="M26" s="20"/>
+      <c r="N26" s="20">
         <v>14.536</v>
       </c>
-      <c r="O26" s="19"/>
-      <c r="P26" s="19">
+      <c r="O26" s="20"/>
+      <c r="P26" s="20">
         <v>5.0839999999999996</v>
       </c>
-      <c r="Q26" s="19"/>
-      <c r="R26" s="19">
+      <c r="Q26" s="20"/>
+      <c r="R26" s="20">
         <f>0.874+3.15</f>
         <v>4.024</v>
       </c>
-      <c r="S26" s="19"/>
-      <c r="T26" s="19">
+      <c r="S26" s="20"/>
+      <c r="T26" s="20">
         <v>5.891</v>
       </c>
-      <c r="U26" s="19"/>
-      <c r="V26" s="19">
+      <c r="U26" s="20"/>
+      <c r="V26" s="20">
         <v>11.195</v>
       </c>
-      <c r="W26" s="19"/>
-      <c r="X26" s="19">
+      <c r="W26" s="20"/>
+      <c r="X26" s="20">
         <v>7.8550000000000004</v>
       </c>
-      <c r="Y26" s="19"/>
+      <c r="Y26" s="20"/>
     </row>
     <row r="27" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="19">
+      <c r="B27" s="20">
         <f>19.37+17.15</f>
         <v>36.519999999999996</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19">
+      <c r="C27" s="20"/>
+      <c r="D27" s="20">
         <v>146.75</v>
       </c>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19">
+      <c r="E27" s="20"/>
+      <c r="F27" s="20">
         <v>180.85</v>
       </c>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19">
+      <c r="G27" s="20"/>
+      <c r="H27" s="20">
         <v>166.69</v>
       </c>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19">
+      <c r="I27" s="20"/>
+      <c r="J27" s="20">
         <v>128.34</v>
       </c>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19">
+      <c r="K27" s="20"/>
+      <c r="L27" s="20">
         <v>23.66</v>
       </c>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19">
+      <c r="M27" s="20"/>
+      <c r="N27" s="20">
         <v>108.08</v>
       </c>
-      <c r="O27" s="19"/>
-      <c r="P27" s="19">
+      <c r="O27" s="20"/>
+      <c r="P27" s="20">
         <v>62.75</v>
       </c>
-      <c r="Q27" s="19"/>
-      <c r="R27" s="19">
+      <c r="Q27" s="20"/>
+      <c r="R27" s="20">
         <v>56.74</v>
       </c>
-      <c r="S27" s="19"/>
-      <c r="T27" s="19">
+      <c r="S27" s="20"/>
+      <c r="T27" s="20">
         <v>67.02</v>
       </c>
-      <c r="U27" s="19"/>
-      <c r="V27" s="19">
+      <c r="U27" s="20"/>
+      <c r="V27" s="20">
         <v>72.900000000000006</v>
       </c>
-      <c r="W27" s="19"/>
-      <c r="X27" s="19">
+      <c r="W27" s="20"/>
+      <c r="X27" s="20">
         <v>80.45</v>
       </c>
-      <c r="Y27" s="19"/>
+      <c r="Y27" s="20"/>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="17">
         <f>B26/512/8/2000*B$25</f>
-        <v>4.541666666666667</v>
-      </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18">
+        <v>2.7250000000000005</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17">
         <f>D26/6144/8/4000*D$25</f>
-        <v>56.088499999999996</v>
-      </c>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18">
+        <v>33.653099999999995</v>
+      </c>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17">
         <f t="shared" ref="F28:F29" si="38">F26/6144/8/4000*F$25</f>
-        <v>46.730666666666671</v>
-      </c>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18">
+        <v>28.038400000000003</v>
+      </c>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17">
         <f t="shared" ref="H28:H29" si="39">H26/6144/8/4000*H$25</f>
-        <v>46.672166666666669</v>
-      </c>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18">
+        <v>28.003300000000003</v>
+      </c>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17">
         <f t="shared" ref="J28:J29" si="40">J26/6144/8/4000*J$25</f>
-        <v>19.902999999999999</v>
-      </c>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18">
+        <v>11.941799999999999</v>
+      </c>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17">
         <f>L26/512/8/1600*L$25</f>
-        <v>74.88</v>
-      </c>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18">
+        <v>44.927999999999997</v>
+      </c>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17">
         <f>N26/4096/8/3200*N$25</f>
-        <v>944.83999999999992</v>
-      </c>
-      <c r="O28" s="18"/>
-      <c r="P28" s="18">
+        <v>566.904</v>
+      </c>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17">
         <f t="shared" ref="P28:P29" si="41">P26/4096/8/3200*P$25</f>
-        <v>330.46</v>
-      </c>
-      <c r="Q28" s="18"/>
-      <c r="R28" s="18">
+        <v>198.27599999999998</v>
+      </c>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17">
         <f t="shared" ref="R28:R29" si="42">R26/4096/8/3200*R$25</f>
-        <v>261.56</v>
-      </c>
-      <c r="S28" s="18"/>
-      <c r="T28" s="18">
+        <v>156.93599999999998</v>
+      </c>
+      <c r="S28" s="17"/>
+      <c r="T28" s="17">
         <f t="shared" ref="T28:T29" si="43">T26/4096/8/3200*T$25</f>
-        <v>382.91499999999996</v>
-      </c>
-      <c r="U28" s="18"/>
-      <c r="V28" s="18">
+        <v>229.749</v>
+      </c>
+      <c r="U28" s="17"/>
+      <c r="V28" s="17">
         <f t="shared" ref="V28:V29" si="44">V26/4096/8/3200*V$25</f>
-        <v>727.67500000000007</v>
-      </c>
-      <c r="W28" s="18"/>
-      <c r="X28" s="18">
+        <v>436.60500000000002</v>
+      </c>
+      <c r="W28" s="17"/>
+      <c r="X28" s="17">
         <f t="shared" ref="X28:X29" si="45">X26/4096/8/3200*X$25</f>
-        <v>1021.1500000000001</v>
-      </c>
-      <c r="Y28" s="18"/>
+        <v>612.69000000000005</v>
+      </c>
+      <c r="Y28" s="17"/>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="18">
+      <c r="B29" s="17">
         <f>B27/512/8/2000*B$25</f>
-        <v>12.173333333333332</v>
-      </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18">
+        <v>7.3039999999999994</v>
+      </c>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17">
         <f>D27/6144/8/4000*D$25</f>
-        <v>317.95833333333331</v>
-      </c>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18">
+        <v>190.77499999999998</v>
+      </c>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17">
         <f t="shared" si="38"/>
-        <v>391.8416666666667</v>
-      </c>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18">
+        <v>235.10500000000002</v>
+      </c>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17">
         <f t="shared" si="39"/>
-        <v>361.16166666666669</v>
-      </c>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18">
+        <v>216.697</v>
+      </c>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17">
         <f t="shared" si="40"/>
-        <v>278.07</v>
-      </c>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18">
+        <v>166.84199999999998</v>
+      </c>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17">
         <f>L27/512/8/1600*L$25</f>
-        <v>1537.9</v>
-      </c>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18">
+        <v>922.74</v>
+      </c>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17">
         <f>N27/4096/8/3200*N$25</f>
-        <v>7025.2</v>
-      </c>
-      <c r="O29" s="18"/>
-      <c r="P29" s="18">
+        <v>4215.12</v>
+      </c>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17">
         <f t="shared" si="41"/>
-        <v>4078.7499999999995</v>
-      </c>
-      <c r="Q29" s="18"/>
-      <c r="R29" s="18">
+        <v>2447.25</v>
+      </c>
+      <c r="Q29" s="17"/>
+      <c r="R29" s="17">
         <f t="shared" si="42"/>
-        <v>3688.1</v>
-      </c>
-      <c r="S29" s="18"/>
-      <c r="T29" s="18">
+        <v>2212.86</v>
+      </c>
+      <c r="S29" s="17"/>
+      <c r="T29" s="17">
         <f t="shared" si="43"/>
-        <v>4356.2999999999993</v>
-      </c>
-      <c r="U29" s="18"/>
-      <c r="V29" s="18">
+        <v>2613.7799999999997</v>
+      </c>
+      <c r="U29" s="17"/>
+      <c r="V29" s="17">
         <f t="shared" si="44"/>
-        <v>4738.5000000000009</v>
-      </c>
-      <c r="W29" s="18"/>
-      <c r="X29" s="18">
+        <v>2843.1000000000004</v>
+      </c>
+      <c r="W29" s="17"/>
+      <c r="X29" s="17">
         <f t="shared" si="45"/>
-        <v>10458.5</v>
-      </c>
-      <c r="Y29" s="18"/>
+        <v>6275.1</v>
+      </c>
+      <c r="Y29" s="17"/>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="17">
+      <c r="B30" s="18">
         <v>1</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17">
+      <c r="C30" s="18"/>
+      <c r="D30" s="18">
         <v>1</v>
       </c>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17">
+      <c r="E30" s="18"/>
+      <c r="F30" s="18">
         <v>1</v>
       </c>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17">
+      <c r="G30" s="18"/>
+      <c r="H30" s="18">
         <v>1</v>
       </c>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17">
+      <c r="I30" s="18"/>
+      <c r="J30" s="18">
         <v>1</v>
       </c>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17">
+      <c r="K30" s="18"/>
+      <c r="L30" s="18">
         <v>1</v>
       </c>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17">
+      <c r="M30" s="18"/>
+      <c r="N30" s="18">
         <v>1</v>
       </c>
-      <c r="O30" s="17"/>
-      <c r="P30" s="17">
+      <c r="O30" s="18"/>
+      <c r="P30" s="18">
         <v>1</v>
       </c>
-      <c r="Q30" s="17"/>
-      <c r="R30" s="17">
+      <c r="Q30" s="18"/>
+      <c r="R30" s="18">
         <v>1</v>
       </c>
-      <c r="S30" s="17"/>
-      <c r="T30" s="17">
+      <c r="S30" s="18"/>
+      <c r="T30" s="18">
         <v>1</v>
       </c>
-      <c r="U30" s="17"/>
-      <c r="V30" s="17">
+      <c r="U30" s="18"/>
+      <c r="V30" s="18">
         <v>1</v>
       </c>
-      <c r="W30" s="17"/>
-      <c r="X30" s="17">
+      <c r="W30" s="18"/>
+      <c r="X30" s="18">
         <v>1</v>
       </c>
-      <c r="Y30" s="17"/>
-      <c r="Z30" s="18"/>
-      <c r="AA30" s="18"/>
+      <c r="Y30" s="18"/>
+      <c r="Z30" s="17"/>
+      <c r="AA30" s="17"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="16">
+      <c r="B31" s="21">
         <f>(B28+B29*B30)/86400</f>
-        <v>1.9346064814814814E-4</v>
-      </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16">
+        <v>1.1607638888888888E-4</v>
+      </c>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21">
         <f t="shared" ref="D31:F31" si="46">(D28+D29*D30)/86400</f>
-        <v>4.3292457561728394E-3</v>
-      </c>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16">
+        <v>2.5975474537037035E-3</v>
+      </c>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21">
         <f t="shared" si="46"/>
-        <v>5.0760686728395068E-3</v>
-      </c>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16">
+        <v>3.0456412037037041E-3</v>
+      </c>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21">
         <f t="shared" ref="H31" si="47">(H28+H29*H30)/86400</f>
-        <v>4.7202989969135807E-3</v>
-      </c>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16">
+        <v>2.8321793981481483E-3</v>
+      </c>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21">
         <f t="shared" ref="J31" si="48">(J28+J29*J30)/86400</f>
-        <v>3.4487615740740741E-3</v>
-      </c>
-      <c r="K31" s="16"/>
-      <c r="L31" s="16">
+        <v>2.0692569444444443E-3</v>
+      </c>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21">
         <f t="shared" ref="L31:N31" si="49">(L28+L29*L30)/86400</f>
-        <v>1.8666435185185189E-2</v>
-      </c>
-      <c r="M31" s="16"/>
-      <c r="N31" s="16">
+        <v>1.1199861111111112E-2</v>
+      </c>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21">
         <f t="shared" si="49"/>
-        <v>9.2245833333333332E-2</v>
-      </c>
-      <c r="O31" s="16"/>
-      <c r="P31" s="16">
+        <v>5.5347499999999994E-2</v>
+      </c>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21">
         <f>(P28+P29*P30+R28)/86400</f>
-        <v>5.4059837962962959E-2</v>
-      </c>
-      <c r="Q31" s="16"/>
-      <c r="R31" s="16">
+        <v>3.2435902777777775E-2</v>
+      </c>
+      <c r="Q31" s="21"/>
+      <c r="R31" s="21">
         <f>(R28+R29*R30+T28)/86400</f>
-        <v>5.014554398148148E-2</v>
-      </c>
-      <c r="S31" s="16"/>
-      <c r="T31" s="16">
+        <v>3.0087326388888891E-2</v>
+      </c>
+      <c r="S31" s="21"/>
+      <c r="T31" s="21">
         <f t="shared" ref="T31:X31" si="50">(T28+T29*T30)/86400</f>
-        <v>5.4852025462962951E-2</v>
-      </c>
-      <c r="U31" s="16"/>
-      <c r="V31" s="16">
+        <v>3.2911215277777774E-2</v>
+      </c>
+      <c r="U31" s="21"/>
+      <c r="V31" s="21">
         <f t="shared" si="50"/>
-        <v>6.326591435185186E-2</v>
-      </c>
-      <c r="W31" s="16"/>
-      <c r="X31" s="16">
+        <v>3.7959548611111116E-2</v>
+      </c>
+      <c r="W31" s="21"/>
+      <c r="X31" s="21">
         <f t="shared" si="50"/>
-        <v>0.13286631944444444</v>
-      </c>
-      <c r="Y31" s="16"/>
+        <v>7.9719791666666678E-2</v>
+      </c>
+      <c r="Y31" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="163">
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="X16:Y16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="T21:U21"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="X21:Y21"/>
-    <mergeCell ref="Z21:AA21"/>
-    <mergeCell ref="X22:Y22"/>
-    <mergeCell ref="Z22:AA22"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="P31:Q31"/>
+    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="T31:U31"/>
+    <mergeCell ref="V31:W31"/>
+    <mergeCell ref="X31:Y31"/>
+    <mergeCell ref="V28:W28"/>
+    <mergeCell ref="X28:Y28"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="R29:S29"/>
+    <mergeCell ref="V29:W29"/>
+    <mergeCell ref="X29:Y29"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="R30:S30"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="X30:Y30"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="X25:Y25"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="R26:S26"/>
+    <mergeCell ref="V26:W26"/>
+    <mergeCell ref="X26:Y26"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="R27:S27"/>
+    <mergeCell ref="V27:W27"/>
+    <mergeCell ref="X27:Y27"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="T29:U29"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="T28:U28"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="T26:U26"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="T27:U27"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="R25:S25"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="R28:S28"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="J30:K30"/>
     <mergeCell ref="X23:Y23"/>
@@ -4339,77 +4343,74 @@
     <mergeCell ref="T25:U25"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="F26:G26"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="T29:U29"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="T28:U28"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="T26:U26"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="T27:U27"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="R25:S25"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="R28:S28"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="X25:Y25"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="R26:S26"/>
-    <mergeCell ref="V26:W26"/>
-    <mergeCell ref="X26:Y26"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="R27:S27"/>
-    <mergeCell ref="V27:W27"/>
-    <mergeCell ref="X27:Y27"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="P31:Q31"/>
-    <mergeCell ref="R31:S31"/>
-    <mergeCell ref="T31:U31"/>
-    <mergeCell ref="V31:W31"/>
-    <mergeCell ref="X31:Y31"/>
-    <mergeCell ref="V28:W28"/>
-    <mergeCell ref="X28:Y28"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="R29:S29"/>
-    <mergeCell ref="V29:W29"/>
-    <mergeCell ref="X29:Y29"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="R30:S30"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="X30:Y30"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="T21:U21"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="X21:Y21"/>
+    <mergeCell ref="Z21:AA21"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="X16:Y16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>